<commit_message>
Validate SKU code visible
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34642\git\TA245\JD_IC_TestAutomationTA245\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\37605\git\JD_IC_TestAutomation\JD_IC_TestAutomation\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCF0F49-A13B-4DA2-9A4A-7314E9A4EFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09EE7E9-5E18-40A8-80FA-1481A717F938}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ic_NavigetoWishlist++" sheetId="41" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3815" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3858" uniqueCount="557">
   <si>
     <t>TCID</t>
   </si>
@@ -1717,16 +1717,38 @@
   </si>
   <si>
     <t>Sourav.Banerjee@itcinfotech.com</t>
+  </si>
+  <si>
+    <t>Validate SKU code visible</t>
+  </si>
+  <si>
+    <t>Get_SKU_Code</t>
+  </si>
+  <si>
+    <t>validationRequired</t>
+  </si>
+  <si>
+    <t>No_wishlist</t>
+  </si>
+  <si>
+    <t>Bluetooth Music Receiver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1907,75 +1929,77 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
@@ -2377,12 +2401,12 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2468,17 +2492,17 @@
       <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="22"/>
+    <col min="3" max="3" width="22.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.26953125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -2572,19 +2596,19 @@
       <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.26953125" style="22" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="22"/>
+    <col min="9" max="9" width="11.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2696,16 +2720,16 @@
       <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.54296875" style="22" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="22"/>
+    <col min="7" max="7" width="18.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2812,7 +2836,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -2865,7 +2889,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -2906,7 +2930,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -3079,7 +3103,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -3694,7 +3718,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:29">
       <c r="A1" t="s">
@@ -5934,13 +5958,13 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6397,7 +6421,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -6573,7 +6597,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
@@ -6630,17 +6654,17 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7285,7 +7309,7 @@
       <selection activeCell="C12" sqref="C12:D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -7524,11 +7548,11 @@
       <selection activeCell="D9" sqref="D9:E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -8186,7 +8210,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -8411,13 +8435,13 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -8689,10 +8713,10 @@
       <selection activeCell="C10" sqref="C10:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8982,7 +9006,7 @@
       <selection activeCell="C14" sqref="C14:E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -9303,7 +9327,7 @@
       <selection activeCell="C33" sqref="C33:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -9945,7 +9969,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -10182,7 +10206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -10282,7 +10306,7 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="22" t="s">
@@ -10319,7 +10343,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -10394,13 +10418,13 @@
       <selection activeCell="C11" sqref="C11:E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10686,7 +10710,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -10814,7 +10838,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -10932,7 +10956,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -10973,7 +10997,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -11480,7 +11504,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" t="s">
@@ -12142,7 +12166,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -12287,7 +12311,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -12482,7 +12506,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -12614,22 +12638,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="F12" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="78" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="139.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="139.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12652,13 +12677,16 @@
         <v>544</v>
       </c>
       <c r="H1" t="s">
+        <v>554</v>
+      </c>
+      <c r="I1" t="s">
         <v>215</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>136</v>
       </c>
@@ -12681,13 +12709,16 @@
         <v>546</v>
       </c>
       <c r="H2" t="s">
+        <v>555</v>
+      </c>
+      <c r="I2" t="s">
         <v>101</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>143</v>
       </c>
@@ -12710,13 +12741,16 @@
         <v>546</v>
       </c>
       <c r="H3" t="s">
+        <v>555</v>
+      </c>
+      <c r="I3" t="s">
         <v>101</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>145</v>
       </c>
@@ -12739,13 +12773,16 @@
         <v>546</v>
       </c>
       <c r="H4" t="s">
+        <v>555</v>
+      </c>
+      <c r="I4" t="s">
         <v>223</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>147</v>
       </c>
@@ -12768,13 +12805,16 @@
         <v>546</v>
       </c>
       <c r="H5" t="s">
+        <v>555</v>
+      </c>
+      <c r="I5" t="s">
         <v>101</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>162</v>
       </c>
@@ -12797,13 +12837,16 @@
         <v>546</v>
       </c>
       <c r="H6" t="s">
+        <v>555</v>
+      </c>
+      <c r="I6" t="s">
         <v>101</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -12826,13 +12869,16 @@
         <v>546</v>
       </c>
       <c r="H7" t="s">
+        <v>555</v>
+      </c>
+      <c r="I7" t="s">
         <v>101</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -12855,13 +12901,16 @@
         <v>546</v>
       </c>
       <c r="H8" t="s">
+        <v>555</v>
+      </c>
+      <c r="I8" t="s">
         <v>101</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -12884,13 +12933,16 @@
         <v>546</v>
       </c>
       <c r="H9" t="s">
+        <v>555</v>
+      </c>
+      <c r="I9" t="s">
         <v>101</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -12913,13 +12965,16 @@
         <v>546</v>
       </c>
       <c r="H10" t="s">
+        <v>555</v>
+      </c>
+      <c r="I10" t="s">
         <v>228</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -12942,13 +12997,16 @@
         <v>546</v>
       </c>
       <c r="H11" t="s">
+        <v>555</v>
+      </c>
+      <c r="I11" t="s">
         <v>223</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -12971,13 +13029,16 @@
         <v>546</v>
       </c>
       <c r="H12" t="s">
+        <v>555</v>
+      </c>
+      <c r="I12" t="s">
         <v>230</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>93</v>
       </c>
@@ -13000,13 +13061,16 @@
         <v>546</v>
       </c>
       <c r="H13" t="s">
+        <v>555</v>
+      </c>
+      <c r="I13" t="s">
         <v>101</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -13029,13 +13093,16 @@
         <v>546</v>
       </c>
       <c r="H14" t="s">
+        <v>555</v>
+      </c>
+      <c r="I14" t="s">
         <v>101</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -13058,13 +13125,16 @@
         <v>546</v>
       </c>
       <c r="H15" t="s">
+        <v>555</v>
+      </c>
+      <c r="I15" t="s">
         <v>101</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -13087,13 +13157,16 @@
         <v>546</v>
       </c>
       <c r="H16" t="s">
+        <v>555</v>
+      </c>
+      <c r="I16" t="s">
         <v>101</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>65</v>
       </c>
@@ -13116,13 +13189,16 @@
         <v>546</v>
       </c>
       <c r="H17" t="s">
+        <v>555</v>
+      </c>
+      <c r="I17" t="s">
         <v>101</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -13145,13 +13221,16 @@
         <v>546</v>
       </c>
       <c r="H18" t="s">
+        <v>555</v>
+      </c>
+      <c r="I18" t="s">
         <v>101</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>69</v>
       </c>
@@ -13174,13 +13253,16 @@
         <v>546</v>
       </c>
       <c r="H19" t="s">
+        <v>555</v>
+      </c>
+      <c r="I19" t="s">
         <v>101</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -13203,13 +13285,16 @@
         <v>546</v>
       </c>
       <c r="H20" t="s">
+        <v>555</v>
+      </c>
+      <c r="I20" t="s">
         <v>101</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>80</v>
       </c>
@@ -13232,13 +13317,16 @@
         <v>546</v>
       </c>
       <c r="H21" t="s">
+        <v>555</v>
+      </c>
+      <c r="I21" t="s">
         <v>101</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>83</v>
       </c>
@@ -13261,13 +13349,16 @@
         <v>546</v>
       </c>
       <c r="H22" t="s">
+        <v>555</v>
+      </c>
+      <c r="I22" t="s">
         <v>101</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -13290,13 +13381,16 @@
         <v>546</v>
       </c>
       <c r="H23" t="s">
+        <v>555</v>
+      </c>
+      <c r="I23" t="s">
         <v>101</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -13319,13 +13413,16 @@
         <v>546</v>
       </c>
       <c r="H24" t="s">
+        <v>555</v>
+      </c>
+      <c r="I24" t="s">
         <v>101</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>156</v>
       </c>
@@ -13348,13 +13445,16 @@
         <v>546</v>
       </c>
       <c r="H25" t="s">
+        <v>555</v>
+      </c>
+      <c r="I25" t="s">
         <v>101</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>158</v>
       </c>
@@ -13377,13 +13477,16 @@
         <v>546</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>47</v>
       </c>
@@ -13406,13 +13509,16 @@
         <v>546</v>
       </c>
       <c r="H27" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>48</v>
       </c>
@@ -13435,13 +13541,16 @@
         <v>546</v>
       </c>
       <c r="H28" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="I28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>49</v>
       </c>
@@ -13464,13 +13573,16 @@
         <v>546</v>
       </c>
       <c r="H29" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>50</v>
       </c>
@@ -13493,13 +13605,16 @@
         <v>546</v>
       </c>
       <c r="H30" t="s">
-        <v>8</v>
+        <v>555</v>
       </c>
       <c r="I30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>52</v>
       </c>
@@ -13522,22 +13637,58 @@
         <v>545</v>
       </c>
       <c r="H31" t="s">
+        <v>555</v>
+      </c>
+      <c r="I31" t="s">
         <v>548</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>552</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>217</v>
+      </c>
+      <c r="E32" t="s">
+        <v>556</v>
+      </c>
+      <c r="F32" t="s">
+        <v>543</v>
+      </c>
+      <c r="G32" t="s">
+        <v>553</v>
+      </c>
+      <c r="H32" t="s">
+        <v>555</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31" xr:uid="{5CD818F2-7DF9-4D2A-BFD9-3AE0D352B9FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{5CD818F2-7DF9-4D2A-BFD9-3AE0D352B9FD}">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31" xr:uid="{DFF07F52-7F3F-471C-B6F1-F0586C11D30A}">
-      <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G1048576" xr:uid="{A25B3CDA-76F6-48A2-81AB-4F94865E9D4A}">
+      <formula1>"Add_To_Cart,Add_To_Wishlist,Get_SKU_Code"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13547,7 +13698,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -13683,7 +13834,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -13819,7 +13970,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -13951,27 +14102,27 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Q48"/>
+  <dimension ref="A1:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="79.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="28.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="27.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="2"/>
+    <col min="10" max="11" width="28.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="27.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -15413,8 +15564,8 @@
       <c r="D47" s="35" t="s">
         <v>549</v>
       </c>
-      <c r="E47" s="32" t="s">
-        <v>94</v>
+      <c r="E47" s="37" t="s">
+        <v>64</v>
       </c>
       <c r="G47" s="32" t="s">
         <v>535</v>
@@ -15436,8 +15587,8 @@
       <c r="D48" s="35" t="s">
         <v>550</v>
       </c>
-      <c r="E48" s="36" t="s">
-        <v>94</v>
+      <c r="E48" s="38" t="s">
+        <v>64</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>535</v>
@@ -15451,6 +15602,26 @@
       <c r="J48" s="35" t="s">
         <v>539</v>
       </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="2">
+        <v>53</v>
+      </c>
+      <c r="B49" t="s">
+        <v>552</v>
+      </c>
+      <c r="D49" t="s">
+        <v>552</v>
+      </c>
+      <c r="E49" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>377</v>
+      </c>
+      <c r="H49" s="4"/>
+      <c r="I49" s="33"/>
+      <c r="J49" s="35"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I2">
@@ -15538,13 +15709,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="22"/>
+    <col min="1" max="1" width="9.1796875" style="22"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="22"/>
+    <col min="3" max="3" width="11.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -15614,11 +15785,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="22"/>
-    <col min="4" max="4" width="15.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="22"/>
+    <col min="1" max="3" width="9.1796875" style="22"/>
+    <col min="4" max="4" width="15.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15668,30 +15839,30 @@
       <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.453125" style="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.1796875" style="22" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="22"/>
-    <col min="14" max="14" width="23.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.85546875" style="22" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="22"/>
+    <col min="13" max="13" width="9.1796875" style="22"/>
+    <col min="14" max="14" width="23.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.81640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1796875" style="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -15903,21 +16074,21 @@
       <selection activeCell="A2" sqref="A2:J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="22" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" style="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.26953125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" style="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1796875" style="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="22" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="22"/>
+    <col min="12" max="12" width="17.7265625" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>

<commit_message>
Pushing latest code for fix testNG issues
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\34642\git\TA245\JD_IC_TestAutomationTA245\src\test\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCF0F49-A13B-4DA2-9A4A-7314E9A4EFDE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ic_NavigetoWishlist++" sheetId="41" r:id="rId1"/>
@@ -61,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3815" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3815" uniqueCount="554">
   <si>
     <t>TCID</t>
   </si>
@@ -1717,16 +1711,36 @@
   </si>
   <si>
     <t>Sourav.Banerjee@itcinfotech.com</t>
+  </si>
+  <si>
+    <t>Click_the_IC_logo_to_go_home_page</t>
+  </si>
+  <si>
+    <t>Validating_the_minimum_search_characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1907,84 +1921,85 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2 2" xfId="3"/>
   </cellStyles>
   <dxfs count="5">
     <dxf>
@@ -2093,7 +2108,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2126,26 +2141,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2178,23 +2176,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2370,7 +2351,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B197FA4-789E-4E7E-B874-0B9B3EEE48E1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2448,20 +2429,20 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{8B610BF8-80B5-4E4F-800A-BBCF0ADA6178}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{BBC5B614-36C8-467E-85E9-21877CF6A5B4}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{83BAA6B4-2AF2-41FF-AA92-468715D569A4}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2565,7 +2546,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2689,7 +2670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2807,7 +2788,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2860,7 +2841,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2901,7 +2882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3074,7 +3055,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3689,7 +3670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -5927,7 +5908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
@@ -6392,7 +6373,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6566,7 +6547,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5978DD-B5A2-422F-931F-0C277A87B7E5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6614,7 +6595,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3" xr:uid="{DCE38A74-3F09-4033-9113-0D40589180A4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C3">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6623,7 +6604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7278,7 +7259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7517,7 +7498,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8181,7 +8162,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -8404,7 +8385,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8682,7 +8663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8975,7 +8956,7 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9296,7 +9277,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -9940,7 +9921,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10177,7 +10158,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10275,7 +10256,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AC8B28F-0CEF-41FF-ACE0-A0ABFA59C5D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10314,7 +10295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10387,7 +10368,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10681,7 +10662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10809,7 +10790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10927,7 +10908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10968,7 +10949,7 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11475,7 +11456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12137,7 +12118,7 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12282,7 +12263,7 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12477,7 +12458,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -12613,7 +12594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView topLeftCell="A14" workbookViewId="0">
@@ -13530,10 +13511,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31" xr:uid="{5CD818F2-7DF9-4D2A-BFD9-3AE0D352B9FD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31" xr:uid="{DFF07F52-7F3F-471C-B6F1-F0586C11D30A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13542,7 +13523,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13678,7 +13659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13814,7 +13795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13950,11 +13931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14984,15 +14965,15 @@
       <c r="A33" s="9">
         <v>40</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>408</v>
+      <c r="B33" s="37" t="s">
+        <v>552</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>64</v>
+      <c r="E33" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="G33" s="3" t="s">
         <v>409</v>
@@ -15009,7 +14990,7 @@
       <c r="D34" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="E34" s="3" t="s">
+      <c r="E34" s="36" t="s">
         <v>64</v>
       </c>
       <c r="G34" s="3" t="s">
@@ -15037,8 +15018,8 @@
       <c r="A36" s="20">
         <v>43</v>
       </c>
-      <c r="B36" s="21" t="s">
-        <v>414</v>
+      <c r="B36" s="3" t="s">
+        <v>553</v>
       </c>
       <c r="C36" s="2">
         <v>181</v>
@@ -15046,8 +15027,8 @@
       <c r="D36" s="21" t="s">
         <v>414</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>64</v>
+      <c r="E36" s="36" t="s">
+        <v>94</v>
       </c>
       <c r="G36" s="9" t="s">
         <v>415</v>
@@ -15413,8 +15394,8 @@
       <c r="D47" s="35" t="s">
         <v>549</v>
       </c>
-      <c r="E47" s="32" t="s">
-        <v>94</v>
+      <c r="E47" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="G47" s="32" t="s">
         <v>535</v>
@@ -15436,8 +15417,8 @@
       <c r="D48" s="35" t="s">
         <v>550</v>
       </c>
-      <c r="E48" s="36" t="s">
-        <v>94</v>
+      <c r="E48" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="G48" s="32" t="s">
         <v>535</v>
@@ -15469,63 +15450,63 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G29" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="G22:G23" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="H22" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
-    <hyperlink ref="H23" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
-    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
-    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
-    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
-    <hyperlink ref="J2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
-    <hyperlink ref="J3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
-    <hyperlink ref="J4" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
-    <hyperlink ref="J5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
-    <hyperlink ref="J6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
-    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
-    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
-    <hyperlink ref="H37" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
-    <hyperlink ref="H38" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
-    <hyperlink ref="I37" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
-    <hyperlink ref="I38" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
-    <hyperlink ref="J37" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
-    <hyperlink ref="J38" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
-    <hyperlink ref="K37" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
-    <hyperlink ref="K38" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
-    <hyperlink ref="L37" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
-    <hyperlink ref="L38" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
-    <hyperlink ref="G38" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
-    <hyperlink ref="G39" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
-    <hyperlink ref="O43" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
-    <hyperlink ref="P45" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
-    <hyperlink ref="I44" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
-    <hyperlink ref="G44" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
-    <hyperlink ref="H45" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
-    <hyperlink ref="J44" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
-    <hyperlink ref="K44" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
-    <hyperlink ref="L44" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
-    <hyperlink ref="M44" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
-    <hyperlink ref="N44" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
-    <hyperlink ref="O44" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
-    <hyperlink ref="Q44" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
-    <hyperlink ref="G45:G46" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
-    <hyperlink ref="H48" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{4E22FA89-343A-4DCB-B1C9-A8A8B5A7C70C}"/>
+    <hyperlink ref="G29" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G22:G23" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H22" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H23" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J2" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J3" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J4" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J5" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J6" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="I8:I9" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="I7" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="H37" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="H38" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I37" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="I38" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J37" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="J38" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="K37" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="K38" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="L37" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="L38" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G38" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G39" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="O43" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="P45" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="I44" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="G44" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H45" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J44" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K44" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L44" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M44" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N44" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O44" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="Q44" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G45:G46" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H48" location="'ProductSearch++'!A1" display="ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -15533,7 +15514,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15609,7 +15590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -15661,7 +15642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
@@ -15896,7 +15877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
updating DataTable2 to add setModule
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -3105,11 +3105,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E37" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E55" sqref="E55"/>
+      <selection pane="bottomRight" activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3199,7 +3199,7 @@
         <v>123</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" s="55"/>
       <c r="G2" s="57" t="s">
@@ -16164,8 +16164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17074,21 +17074,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17241,14 +17241,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -17261,6 +17253,14 @@
     <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updateding main to add TA255
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="596">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1909,6 +1909,18 @@
   </si>
   <si>
     <t>Samsung Toner D105L</t>
+  </si>
+  <si>
+    <t>Wish List - Validate Multiple Products can be added to Wish List</t>
+  </si>
+  <si>
+    <t>Wishlist - Validate product can be added to Wishlist</t>
+  </si>
+  <si>
+    <t>Samsung Toner D105L#Xbox One Stealth 600 Gaming Headsets#Volkano Earphones With Mic Stannic Series Black</t>
+  </si>
+  <si>
+    <t>1#1#1</t>
   </si>
 </sst>
 </file>
@@ -3103,13 +3115,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q55"/>
+  <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G55" sqref="G55"/>
+      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5149,8 +5161,8 @@
       <c r="D55" s="75" t="s">
         <v>583</v>
       </c>
-      <c r="E55" s="75" t="s">
-        <v>8</v>
+      <c r="E55" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="G55" s="11" t="s">
         <v>472</v>
@@ -5166,13 +5178,39 @@
       </c>
       <c r="K55" s="76" t="s">
         <v>584</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" s="74" customFormat="1">
+      <c r="A56" s="74">
+        <v>55</v>
+      </c>
+      <c r="B56" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="D56" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="E56" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H56" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B56:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B57:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5386,6 +5424,10 @@
     <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
     <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
     <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
+    <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G56" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H56" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I56" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12131,11 +12173,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12186,6 +12226,17 @@
         <v>583</v>
       </c>
       <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>87</v>
       </c>
     </row>
@@ -12202,11 +12253,9 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
-    </sheetView>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13192,6 +13241,38 @@
         <v>373</v>
       </c>
     </row>
+    <row r="32" spans="1:12" s="35" customFormat="1">
+      <c r="A32" s="35">
+        <v>55</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>593</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E32" s="35" t="s">
+        <v>594</v>
+      </c>
+      <c r="F32" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G32" s="35" t="s">
+        <v>470</v>
+      </c>
+      <c r="H32" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="I32" s="35" t="s">
+        <v>595</v>
+      </c>
+      <c r="J32" s="35" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -13204,16 +13285,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G32 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D32:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D33:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H32">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15080,11 +15161,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -15151,6 +15230,20 @@
         <v>496</v>
       </c>
     </row>
+    <row r="5" spans="1:4" s="35" customFormat="1">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="44" priority="2"/>
@@ -15159,7 +15252,7 @@
     <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 D5">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16162,11 +16255,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -16272,6 +16363,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="74">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>493</v>
+      </c>
+      <c r="G5" s="35">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="42" priority="2"/>
@@ -16280,7 +16394,7 @@
     <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 D5">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16288,8 +16402,10 @@
     <hyperlink ref="E2" r:id="rId1"/>
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -17074,21 +17190,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17241,6 +17357,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -17253,14 +17377,6 @@
     <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating main to add TA257
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
-    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId2"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId3"/>
-    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId4"/>
+    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId2"/>
+    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId3"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId4"/>
     <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId5"/>
     <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId6"/>
     <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId7"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2564" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="598">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1921,6 +1921,12 @@
   </si>
   <si>
     <t>1#1#1</t>
+  </si>
+  <si>
+    <t>Wish List - Validate Add All to Cart</t>
+  </si>
+  <si>
+    <t>Samsung Toner D105L#Volkano Earphones With Mic Stannic Series Black</t>
   </si>
 </sst>
 </file>
@@ -3115,13 +3121,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q56"/>
+  <dimension ref="A1:Q57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B56" sqref="B56"/>
+      <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5190,8 +5196,8 @@
       <c r="D56" s="75" t="s">
         <v>592</v>
       </c>
-      <c r="E56" s="75" t="s">
-        <v>8</v>
+      <c r="E56" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="G56" s="11" t="s">
         <v>472</v>
@@ -5204,13 +5210,42 @@
       </c>
       <c r="J56" s="11" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" s="74" customFormat="1">
+      <c r="A57" s="74">
+        <v>56</v>
+      </c>
+      <c r="B57" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="D57" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="J57" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K57" s="11" t="s">
+        <v>473</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B57:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B58:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5428,6 +5463,11 @@
     <hyperlink ref="G56" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
     <hyperlink ref="H56" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
     <hyperlink ref="I56" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8685,57 +8725,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="42"/>
-    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>588</v>
-      </c>
       <c r="D1" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="42">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="62">
+        <v>52</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="62">
+        <v>53</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74">
         <v>54</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B4" s="75" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>590</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>591</v>
-      </c>
-      <c r="E2" s="42">
-        <v>11</v>
+      <c r="D4" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="35" customFormat="1">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="74">
+        <v>56</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>496</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
-      <formula1>"All_product,Specific_product"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
+      <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12173,87 +12283,66 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="42"/>
+    <col min="1" max="2" width="9.140625" style="42"/>
+    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
+      <c r="B1" s="42" t="s">
+        <v>35</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="62">
-        <v>52</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>471</v>
+        <v>588</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="42">
+        <v>54</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>87</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="62">
-        <v>53</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="74">
-        <v>54</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>583</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="35">
-        <v>55</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>592</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>87</v>
+        <v>590</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="E2" s="42">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
-  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>"All_product,Specific_product"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -13273,6 +13362,38 @@
         <v>373</v>
       </c>
     </row>
+    <row r="33" spans="1:10" s="35" customFormat="1">
+      <c r="A33" s="35">
+        <v>56</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>596</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>597</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G33" s="35" t="s">
+        <v>470</v>
+      </c>
+      <c r="H33" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="I33" s="35" t="s">
+        <v>477</v>
+      </c>
+      <c r="J33" s="35" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -13285,16 +13406,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G32 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G33 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D33:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D34:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H32">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H33">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15161,20 +15282,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="42" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="42"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:3">
       <c r="A1" s="42" t="s">
         <v>34</v>
       </c>
@@ -15184,11 +15304,8 @@
       <c r="C1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="42" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="62">
         <v>52</v>
       </c>
@@ -15198,11 +15315,8 @@
       <c r="C2" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="62">
         <v>53</v>
       </c>
@@ -15212,11 +15326,8 @@
       <c r="C3" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="74">
         <v>54</v>
       </c>
@@ -15226,11 +15337,8 @@
       <c r="C4" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="35" customFormat="1">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="35">
         <v>55</v>
       </c>
@@ -15240,8 +15348,16 @@
       <c r="C5" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="35" t="s">
-        <v>496</v>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -15251,11 +15367,6 @@
   <conditionalFormatting sqref="A2:A3">
     <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 D5">
-      <formula1>"All,Specific"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -16255,7 +16366,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -16386,6 +16497,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>493</v>
+      </c>
+      <c r="G6" s="35">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="42" priority="2"/>
@@ -16394,7 +16528,7 @@
     <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4 D5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
@@ -16403,9 +16537,10 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updating main to add TA265_TA266_TA271
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -8,50 +8,51 @@
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
-    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId2"/>
-    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId3"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId4"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId5"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId6"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId7"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId8"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId9"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId10"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId11"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId12"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId13"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId14"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId15"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId16"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId17"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId18"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId19"/>
-    <sheet name="Suites" sheetId="22" r:id="rId20"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId21"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId22"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId23"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId24"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId25"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId26"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId27"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId28"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId29"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId30"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId31"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId32"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId33"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId34"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId35"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId36"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId37"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId38"/>
-    <sheet name="Russels" sheetId="26" r:id="rId39"/>
-    <sheet name="Login++" sheetId="25" r:id="rId40"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId41"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId42"/>
-    <sheet name="Preferred Store" sheetId="68" r:id="rId43"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId44"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId45"/>
+    <sheet name="ClearCart++" sheetId="70" r:id="rId2"/>
+    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId3"/>
+    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId4"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId5"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId6"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId7"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId8"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId9"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId10"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId11"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId12"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId13"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId14"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId15"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId16"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId17"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId18"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId19"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId20"/>
+    <sheet name="Suites" sheetId="22" r:id="rId21"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId22"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId23"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId24"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId25"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId26"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId27"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId28"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId29"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId30"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId31"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId32"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId33"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId34"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId35"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId36"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId37"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId38"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId39"/>
+    <sheet name="Russels" sheetId="26" r:id="rId40"/>
+    <sheet name="Login++" sheetId="25" r:id="rId41"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId42"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId43"/>
+    <sheet name="Preferred Store" sheetId="68" r:id="rId44"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId45"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId46"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="606">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1927,6 +1928,30 @@
   </si>
   <si>
     <t>Samsung Toner D105L#Volkano Earphones With Mic Stannic Series Black</t>
+  </si>
+  <si>
+    <t>ClearCart</t>
+  </si>
+  <si>
+    <t>Cart - Add One Item to the Cart and Verify</t>
+  </si>
+  <si>
+    <t>Cart - Add the same Item multiple Times and Verify</t>
+  </si>
+  <si>
+    <t>Clear cart</t>
+  </si>
+  <si>
+    <t>Leverch</t>
+  </si>
+  <si>
+    <t>Password@124</t>
+  </si>
+  <si>
+    <t>Volkano Phonic Bluetooth Headphones Black VK-2002BK</t>
+  </si>
+  <si>
+    <t>No_wishlist</t>
   </si>
 </sst>
 </file>
@@ -2098,7 +2123,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2272,6 +2297,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3121,13 +3147,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K57" sqref="K57"/>
+      <selection pane="bottomRight" activeCell="E56" sqref="E56:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5222,8 +5248,8 @@
       <c r="D57" s="75" t="s">
         <v>596</v>
       </c>
-      <c r="E57" s="75" t="s">
-        <v>8</v>
+      <c r="E57" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="G57" s="11" t="s">
         <v>472</v>
@@ -5239,13 +5265,92 @@
       </c>
       <c r="K57" s="11" t="s">
         <v>473</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="74" customFormat="1">
+      <c r="A58" s="74">
+        <v>57</v>
+      </c>
+      <c r="B58" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="C58" s="74">
+        <v>265</v>
+      </c>
+      <c r="D58" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="E58" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="H58" s="76" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" s="74" customFormat="1">
+      <c r="A59" s="74">
+        <v>58</v>
+      </c>
+      <c r="B59" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C59" s="74">
+        <v>271</v>
+      </c>
+      <c r="D59" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="E59" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G59" s="76" t="s">
+        <v>598</v>
+      </c>
+      <c r="H59" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="I59" s="75"/>
+    </row>
+    <row r="60" spans="1:15" s="74" customFormat="1">
+      <c r="A60" s="74">
+        <v>59</v>
+      </c>
+      <c r="B60" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C60" s="74">
+        <v>266</v>
+      </c>
+      <c r="D60" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="E60" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G60" s="76" t="s">
+        <v>598</v>
+      </c>
+      <c r="H60" s="76" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B61:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5468,6 +5573,11 @@
     <hyperlink ref="H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
     <hyperlink ref="I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
     <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H59" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5475,6 +5585,174 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="42" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>435</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>436</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>437</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>438</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>439</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>440</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>441</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>442</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>443</v>
+      </c>
+      <c r="M1" s="42" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="66">
+        <v>46</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>478</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>403</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>445</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>446</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>447</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>399</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>448</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>408</v>
+      </c>
+      <c r="M2" s="42" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="66">
+        <v>47</v>
+      </c>
+      <c r="B3" s="67" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>403</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>445</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>446</v>
+      </c>
+      <c r="G3" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>447</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>399</v>
+      </c>
+      <c r="J3" s="47" t="s">
+        <v>448</v>
+      </c>
+      <c r="K3" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>408</v>
+      </c>
+      <c r="M3" s="42" t="s">
+        <v>449</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+      <formula1>"Female,Male"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -5605,7 +5883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -5763,7 +6041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -5902,7 +6180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -6176,7 +6454,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -6247,7 +6525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6304,7 +6582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -6423,7 +6701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -6870,7 +7148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -8261,7 +8539,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="47.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="74">
+        <v>57</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="74">
+        <v>58</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="74">
+        <v>59</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -8723,136 +9066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="62">
-        <v>52</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>471</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="62">
-        <v>53</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="74">
-        <v>54</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>583</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="35" customFormat="1">
-      <c r="A5" s="35">
-        <v>55</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>592</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="74">
-        <v>56</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="74">
-        <v>56</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C7" s="42">
-        <v>2</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
-      <formula1>"All,Specific"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9017,7 +9231,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -9606,7 +9820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -9843,7 +10057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -10458,7 +10672,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -10705,7 +10919,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -10912,7 +11126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -11172,7 +11386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -11461,7 +11675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
@@ -12116,7 +12330,136 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="62">
+        <v>52</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="62">
+        <v>53</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74">
+        <v>54</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="35" customFormat="1">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="74">
+        <v>56</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
+      <formula1>"All,Specific"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -12281,70 +12624,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="42"/>
-    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>588</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="42">
-        <v>54</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>590</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>591</v>
-      </c>
-      <c r="E2" s="42">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
-      <formula1>"All_product,Specific_product"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
-  <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:B35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13394,6 +13680,70 @@
         <v>373</v>
       </c>
     </row>
+    <row r="34" spans="1:10" s="35" customFormat="1">
+      <c r="A34" s="74">
+        <v>58</v>
+      </c>
+      <c r="B34" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C34" s="35">
+        <v>1</v>
+      </c>
+      <c r="D34" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="F34" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="G34" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="H34" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I34" s="35">
+        <v>3</v>
+      </c>
+      <c r="J34" s="35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" s="35" customFormat="1">
+      <c r="A35" s="74">
+        <v>59</v>
+      </c>
+      <c r="B35" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C35" s="35">
+        <v>1</v>
+      </c>
+      <c r="D35" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="F35" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="G35" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="H35" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I35" s="35">
+        <v>1</v>
+      </c>
+      <c r="J35" s="35">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -13406,16 +13756,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G33 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F35">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D34:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D36:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H35">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13425,7 +13775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -13528,7 +13878,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -13611,11 +13961,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13866,11 +14218,21 @@
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="19"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
+      <c r="A15" s="74">
+        <v>57</v>
+      </c>
+      <c r="B15" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>603</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="19"/>
@@ -13901,13 +14263,14 @@
     <hyperlink ref="E12" r:id="rId8"/>
     <hyperlink ref="E13" r:id="rId9"/>
     <hyperlink ref="E14" r:id="rId10"/>
+    <hyperlink ref="E15" r:id="rId11" display="Password@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -14019,7 +14382,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -14117,7 +14480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -14163,7 +14526,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -14472,7 +14835,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -15175,7 +15538,66 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="42"/>
+    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>588</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="42">
+        <v>54</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>590</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="E2" s="42">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>"All_product,Specific_product"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -15280,98 +15702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="62">
-        <v>52</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>471</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="62">
-        <v>53</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="74">
-        <v>54</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>583</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="35">
-        <v>55</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>592</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="74">
-        <v>56</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C6" s="42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -15575,7 +15906,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -15679,7 +16010,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -15783,7 +16114,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
@@ -16156,7 +16487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16260,7 +16591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16365,6 +16696,97 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="62">
+        <v>52</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="62">
+        <v>53</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="74">
+        <v>54</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -16544,7 +16966,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -16999,7 +17421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -17093,7 +17515,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -17156,190 +17578,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="42" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>435</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>436</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>437</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>438</v>
-      </c>
-      <c r="H1" s="42" t="s">
-        <v>439</v>
-      </c>
-      <c r="I1" s="42" t="s">
-        <v>440</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>441</v>
-      </c>
-      <c r="K1" s="42" t="s">
-        <v>442</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>443</v>
-      </c>
-      <c r="M1" s="42" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="66">
-        <v>46</v>
-      </c>
-      <c r="B2" s="63" t="s">
-        <v>478</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>403</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>445</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>446</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>447</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>399</v>
-      </c>
-      <c r="J2" s="47" t="s">
-        <v>448</v>
-      </c>
-      <c r="K2" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="L2" s="42" t="s">
-        <v>408</v>
-      </c>
-      <c r="M2" s="42" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="66">
-        <v>47</v>
-      </c>
-      <c r="B3" s="67" t="s">
-        <v>488</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>403</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>445</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>446</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>447</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>399</v>
-      </c>
-      <c r="J3" s="47" t="s">
-        <v>448</v>
-      </c>
-      <c r="K3" s="42" t="s">
-        <v>362</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>408</v>
-      </c>
-      <c r="M3" s="42" t="s">
-        <v>449</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
-      <formula1>"Female,Male"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17492,14 +17746,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -17512,6 +17758,14 @@
     <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updating main to add TA270
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="606">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="608">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1952,6 +1952,12 @@
   </si>
   <si>
     <t>No_wishlist</t>
+  </si>
+  <si>
+    <t>Cart - Validate Quantity can be increased in Cart</t>
+  </si>
+  <si>
+    <t>IncreaseQuanityInCart</t>
   </si>
 </sst>
 </file>
@@ -3147,13 +3153,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q60"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E56" sqref="E56:E57"/>
+      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5280,8 +5286,8 @@
       <c r="D58" s="75" t="s">
         <v>601</v>
       </c>
-      <c r="E58" s="75" t="s">
-        <v>8</v>
+      <c r="E58" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F58" s="77" t="s">
         <v>602</v>
@@ -5306,8 +5312,8 @@
       <c r="D59" s="75" t="s">
         <v>600</v>
       </c>
-      <c r="E59" s="75" t="s">
-        <v>8</v>
+      <c r="E59" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F59" s="77" t="s">
         <v>602</v>
@@ -5333,8 +5339,8 @@
       <c r="D60" s="75" t="s">
         <v>599</v>
       </c>
-      <c r="E60" s="75" t="s">
-        <v>8</v>
+      <c r="E60" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F60" s="77" t="s">
         <v>602</v>
@@ -5344,13 +5350,39 @@
       </c>
       <c r="H60" s="76" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" s="74" customFormat="1">
+      <c r="A61" s="74">
+        <v>60</v>
+      </c>
+      <c r="B61" s="75" t="s">
+        <v>606</v>
+      </c>
+      <c r="C61" s="74">
+        <v>270</v>
+      </c>
+      <c r="D61" s="75" t="s">
+        <v>606</v>
+      </c>
+      <c r="E61" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G61" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="H61" s="75" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B61:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B62:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5578,6 +5610,7 @@
     <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
     <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12626,11 +12659,9 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34:B35"/>
-    </sheetView>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13744,6 +13775,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="36" spans="1:10" s="35" customFormat="1">
+      <c r="A36" s="74">
+        <v>60</v>
+      </c>
+      <c r="B36" s="75" t="s">
+        <v>606</v>
+      </c>
+      <c r="C36" s="35">
+        <v>1</v>
+      </c>
+      <c r="D36" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E36" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="F36" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="G36" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="H36" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I36" s="35">
+        <v>1</v>
+      </c>
+      <c r="J36" s="35">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -13756,16 +13819,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G36 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D36:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D37:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H36">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17588,15 +17651,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17745,6 +17799,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
@@ -17763,14 +17826,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17787,4 +17842,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA272 sheet to main
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="27" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="612">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1958,6 +1958,18 @@
   </si>
   <si>
     <t>IncreaseQuanityInCart</t>
+  </si>
+  <si>
+    <t>Cart - Remove some items from the cart and verify</t>
+  </si>
+  <si>
+    <t>RemoveArticleFromCart</t>
+  </si>
+  <si>
+    <t>Remove one quantity from cart adding 3 articles</t>
+  </si>
+  <si>
+    <t>Bluetooth Music Receiver#JBL Earphones T110 Blue#Basic Monitor Riser</t>
   </si>
 </sst>
 </file>
@@ -2129,7 +2141,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2304,6 +2316,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3153,13 +3168,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q61"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5378,11 +5393,31 @@
         <v>607</v>
       </c>
     </row>
+    <row r="62" spans="1:15" s="74" customFormat="1">
+      <c r="A62" s="74">
+        <v>61</v>
+      </c>
+      <c r="B62" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="D62" s="75" t="s">
+        <v>608</v>
+      </c>
+      <c r="E62" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="H62" s="75" t="s">
+        <v>609</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B62:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B63:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5611,6 +5646,7 @@
     <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
     <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12659,9 +12695,11 @@
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -13807,6 +13845,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="37" spans="1:10" s="35" customFormat="1" ht="30">
+      <c r="A37" s="35">
+        <v>61</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>610</v>
+      </c>
+      <c r="C37" s="35">
+        <v>1</v>
+      </c>
+      <c r="D37" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="78" t="s">
+        <v>611</v>
+      </c>
+      <c r="F37" s="35" t="s">
+        <v>465</v>
+      </c>
+      <c r="G37" s="35" t="s">
+        <v>466</v>
+      </c>
+      <c r="H37" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I37" s="35" t="s">
+        <v>595</v>
+      </c>
+      <c r="J37" s="35">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -13819,16 +13889,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G36 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D37:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D38:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17651,6 +17721,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17799,15 +17878,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
@@ -17826,6 +17896,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17842,12 +17920,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA305 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,55 +4,56 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="27" activeTab="30"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
-    <sheet name="ClearCart++" sheetId="70" r:id="rId2"/>
-    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId3"/>
-    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId4"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId5"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId6"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId7"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId8"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId9"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId10"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId11"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId12"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId13"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId14"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId15"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId16"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId17"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId18"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId19"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId20"/>
-    <sheet name="Suites" sheetId="22" r:id="rId21"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId22"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId23"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId24"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId25"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId26"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId27"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId28"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId29"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId30"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId31"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId32"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId33"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId34"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId35"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId36"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId37"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId38"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId39"/>
-    <sheet name="Russels" sheetId="26" r:id="rId40"/>
-    <sheet name="Login++" sheetId="25" r:id="rId41"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId42"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId43"/>
-    <sheet name="Preferred Store" sheetId="68" r:id="rId44"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId45"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId46"/>
+    <sheet name="ic_invalidCredslogin++" sheetId="71" r:id="rId2"/>
+    <sheet name="ClearCart++" sheetId="70" r:id="rId3"/>
+    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId4"/>
+    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId5"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId6"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId7"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId8"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId9"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId10"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId11"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId12"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId13"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId14"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId15"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId16"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId17"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId18"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId19"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId20"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId21"/>
+    <sheet name="Suites" sheetId="22" r:id="rId22"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId23"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId24"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId25"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId26"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId27"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId28"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId29"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId30"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId31"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId32"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId33"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId34"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId35"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId36"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId37"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId38"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId39"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId40"/>
+    <sheet name="Russels" sheetId="26" r:id="rId41"/>
+    <sheet name="Login++" sheetId="25" r:id="rId42"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId43"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId44"/>
+    <sheet name="Preferred Store" sheetId="68" r:id="rId45"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId46"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId47"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -126,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="618">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1970,6 +1971,24 @@
   </si>
   <si>
     <t>Bluetooth Music Receiver#JBL Earphones T110 Blue#Basic Monitor Riser</t>
+  </si>
+  <si>
+    <t>Invalid login creditials</t>
+  </si>
+  <si>
+    <t>ic_invalidCredslogin</t>
+  </si>
+  <si>
+    <t>Password@</t>
+  </si>
+  <si>
+    <t>LouieGBynumjourrapide.com</t>
+  </si>
+  <si>
+    <t>PasswordFlag</t>
+  </si>
+  <si>
+    <t>UsernameFlag</t>
   </si>
 </sst>
 </file>
@@ -3168,13 +3187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q62"/>
+  <dimension ref="A1:Q64"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G62" sqref="G62"/>
+      <selection pane="bottomRight" activeCell="A63" sqref="A63:B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5413,11 +5432,51 @@
         <v>609</v>
       </c>
     </row>
+    <row r="63" spans="1:15" s="74" customFormat="1">
+      <c r="A63" s="74">
+        <v>62</v>
+      </c>
+      <c r="B63" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C63" s="74">
+        <v>305</v>
+      </c>
+      <c r="D63" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="E63" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" s="74" customFormat="1">
+      <c r="A64" s="74">
+        <v>63</v>
+      </c>
+      <c r="B64" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C64" s="74">
+        <v>305</v>
+      </c>
+      <c r="D64" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="E64" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>613</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B65:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5655,6 +5714,69 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>450</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="63">
+        <v>48</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>452</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
@@ -5821,7 +5943,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -5952,7 +6074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -6110,7 +6232,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -6249,7 +6371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -6523,7 +6645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -6594,7 +6716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6651,7 +6773,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -6770,7 +6892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -7217,7 +7339,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="20.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="42"/>
+    <col min="4" max="4" width="13.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="42" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>616</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="74">
+        <v>62</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="74">
+        <v>63</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -8608,72 +8828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="42"/>
-    <col min="2" max="2" width="47.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="74">
-        <v>57</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>601</v>
-      </c>
-      <c r="C2" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="74">
-        <v>58</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>600</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="74">
-        <v>59</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>599</v>
-      </c>
-      <c r="C4" s="42">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -9135,7 +9290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9300,7 +9455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -9889,7 +10044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -10126,7 +10281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -10741,7 +10896,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -10988,7 +11143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -11195,7 +11350,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -11455,7 +11610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -11744,7 +11899,72 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="47.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="74">
+        <v>57</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="74">
+        <v>58</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="74">
+        <v>59</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
@@ -12399,136 +12619,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="62">
-        <v>52</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>471</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="62">
-        <v>53</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="74">
-        <v>54</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>583</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="35" customFormat="1">
-      <c r="A5" s="35">
-        <v>55</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>592</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="74">
-        <v>56</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="74">
-        <v>56</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C7" s="42">
-        <v>2</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
-      <formula1>"All,Specific"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -12693,12 +12784,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13724,8 +13815,8 @@
       <c r="B33" s="35" t="s">
         <v>596</v>
       </c>
-      <c r="C33" s="35" t="s">
-        <v>87</v>
+      <c r="C33" s="35">
+        <v>1</v>
       </c>
       <c r="D33" s="35" t="s">
         <v>152</v>
@@ -13908,7 +13999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -14011,7 +14102,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -14094,7 +14185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
@@ -14403,7 +14494,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -14515,7 +14606,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -14613,7 +14704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -14659,7 +14750,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -14968,7 +15059,136 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="62">
+        <v>52</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="62">
+        <v>53</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74">
+        <v>54</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="35" customFormat="1">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="74">
+        <v>56</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
+      <formula1>"All,Specific"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -15671,66 +15891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="42"/>
-    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>588</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>589</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="42">
-        <v>54</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>590</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>591</v>
-      </c>
-      <c r="E2" s="42">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
-      <formula1>"All_product,Specific_product"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -15835,7 +15996,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -16039,7 +16200,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16143,7 +16304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16247,7 +16408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
@@ -16620,7 +16781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16724,7 +16885,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16830,6 +16991,65 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="42"/>
+    <col min="3" max="3" width="20.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>588</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>589</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="42">
+        <v>54</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>590</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>591</v>
+      </c>
+      <c r="E2" s="42">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+      <formula1>"All_product,Specific_product"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16919,7 +17139,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
@@ -17099,7 +17319,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
@@ -17554,7 +17774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -17648,79 +17868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>450</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="63">
-        <v>48</v>
-      </c>
-      <c r="B2" s="67" t="s">
-        <v>341</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>451</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>452</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -17729,7 +17877,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -17878,24 +18026,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -17903,7 +18043,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -17920,4 +18060,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA309 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="30" activeTab="34"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2679" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="620">
   <si>
     <t>testSuitID</t>
   </si>
@@ -1989,6 +1989,12 @@
   </si>
   <si>
     <t>UsernameFlag</t>
+  </si>
+  <si>
+    <t>Validate the password is not visible</t>
+  </si>
+  <si>
+    <t>icPasswordSecured</t>
   </si>
 </sst>
 </file>
@@ -3187,13 +3193,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q64"/>
+  <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E43" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A63" sqref="A63:B64"/>
+      <selection pane="bottomRight" activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5399,8 +5405,8 @@
       <c r="D61" s="75" t="s">
         <v>606</v>
       </c>
-      <c r="E61" s="75" t="s">
-        <v>8</v>
+      <c r="E61" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F61" s="77" t="s">
         <v>602</v>
@@ -5422,8 +5428,11 @@
       <c r="D62" s="75" t="s">
         <v>608</v>
       </c>
-      <c r="E62" s="75" t="s">
-        <v>8</v>
+      <c r="E62" s="55" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" s="77" t="s">
+        <v>602</v>
       </c>
       <c r="G62" s="76" t="s">
         <v>31</v>
@@ -5446,7 +5455,10 @@
         <v>612</v>
       </c>
       <c r="E63" s="75" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F63" s="77" t="s">
+        <v>210</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>613</v>
@@ -5468,15 +5480,41 @@
       <c r="E64" s="75" t="s">
         <v>8</v>
       </c>
+      <c r="F64" s="77" t="s">
+        <v>210</v>
+      </c>
       <c r="G64" s="11" t="s">
         <v>613</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" s="74" customFormat="1">
+      <c r="A65" s="74">
+        <v>64</v>
+      </c>
+      <c r="B65" s="75" t="s">
+        <v>618</v>
+      </c>
+      <c r="C65" s="74">
+        <v>309</v>
+      </c>
+      <c r="D65" s="75" t="s">
+        <v>618</v>
+      </c>
+      <c r="E65" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F65" s="77" t="s">
+        <v>210</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>619</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B65:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B66:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -7343,7 +7381,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
@@ -14189,8 +14227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14449,7 +14487,7 @@
         <v>601</v>
       </c>
       <c r="C15" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>180</v>
@@ -14459,11 +14497,21 @@
       </c>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" s="19"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
+      <c r="A16" s="74">
+        <v>64</v>
+      </c>
+      <c r="B16" s="75" t="s">
+        <v>618</v>
+      </c>
+      <c r="C16" s="19">
+        <v>1</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>603</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -14488,9 +14536,10 @@
     <hyperlink ref="E13" r:id="rId9"/>
     <hyperlink ref="E14" r:id="rId10"/>
     <hyperlink ref="E15" r:id="rId11" display="Password@123"/>
+    <hyperlink ref="E16" r:id="rId12" display="Password@123"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -17869,12 +17918,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18027,18 +18076,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18063,18 +18121,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA315 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="36" activeTab="36"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="628">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2007,6 +2007,18 @@
   </si>
   <si>
     <t>icVerifyForgotPass</t>
+  </si>
+  <si>
+    <t>Validating the new password setting email sent</t>
+  </si>
+  <si>
+    <t>icEmailSentVerification</t>
+  </si>
+  <si>
+    <t>jdg123auto@gmail.com</t>
+  </si>
+  <si>
+    <t>Xpath@123</t>
   </si>
 </sst>
 </file>
@@ -3205,13 +3217,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E43" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A67" sqref="A67:B67"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5499,7 +5511,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="65" spans="1:7" s="74" customFormat="1">
+    <row r="65" spans="1:8" s="74" customFormat="1">
       <c r="A65" s="74">
         <v>64</v>
       </c>
@@ -5522,7 +5534,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="1:7" s="74" customFormat="1">
+    <row r="66" spans="1:8" s="74" customFormat="1">
       <c r="A66" s="74">
         <v>65</v>
       </c>
@@ -5535,8 +5547,8 @@
       <c r="D66" s="75" t="s">
         <v>620</v>
       </c>
-      <c r="E66" s="75" t="s">
-        <v>8</v>
+      <c r="E66" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F66" s="75" t="s">
         <v>210</v>
@@ -5545,7 +5557,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="67" spans="1:7" s="74" customFormat="1">
+    <row r="67" spans="1:8" s="74" customFormat="1">
       <c r="A67" s="74">
         <v>66</v>
       </c>
@@ -5558,21 +5570,47 @@
       <c r="D67" s="74" t="s">
         <v>622</v>
       </c>
-      <c r="E67" s="75" t="s">
-        <v>8</v>
+      <c r="E67" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F67" s="75" t="s">
         <v>210</v>
       </c>
       <c r="G67" s="77" t="s">
         <v>623</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" s="74" customFormat="1">
+      <c r="A68" s="74">
+        <v>67</v>
+      </c>
+      <c r="B68" s="75" t="s">
+        <v>624</v>
+      </c>
+      <c r="C68" s="74">
+        <v>318</v>
+      </c>
+      <c r="D68" s="75" t="s">
+        <v>624</v>
+      </c>
+      <c r="E68" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="75" t="s">
+        <v>210</v>
+      </c>
+      <c r="G68" s="74" t="s">
+        <v>623</v>
+      </c>
+      <c r="H68" s="75" t="s">
+        <v>625</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B68:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B69:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -14733,16 +14771,16 @@
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -14754,78 +14792,110 @@
     <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>183</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="1" customFormat="1">
+    <row r="2" spans="1:12" s="1" customFormat="1">
       <c r="A2" s="1">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="35"/>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:12">
       <c r="A3" s="1">
         <v>16</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="H3" s="1">
+      <c r="F3"/>
+      <c r="I3" s="1">
         <v>500</v>
       </c>
     </row>
+    <row r="4" spans="1:12">
+      <c r="A4" s="74">
+        <v>67</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>624</v>
+      </c>
+      <c r="C4" s="35">
+        <v>1</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>626</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14880,7 +14950,7 @@
   <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15315,19 +15385,19 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S12"/>
+  <dimension ref="A1:S13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="O5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="44" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="43.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -16055,18 +16125,77 @@
         <v>93</v>
       </c>
     </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="74">
+        <v>67</v>
+      </c>
+      <c r="B13" s="75" t="s">
+        <v>624</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" s="14">
+        <v>2222227</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="N13" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="O13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="P13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="S13" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K13">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12 O2:S12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I13 O2:S13">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M13">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L13">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18053,12 +18182,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18211,27 +18340,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18256,9 +18376,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA331 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="36" activeTab="36"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="28" activeTab="31"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2745" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2758" uniqueCount="631">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2019,6 +2019,15 @@
   </si>
   <si>
     <t>Xpath@123</t>
+  </si>
+  <si>
+    <t>Validate SKU code visible</t>
+  </si>
+  <si>
+    <t>Bluetooth Music Receiver</t>
+  </si>
+  <si>
+    <t>Get_SKU_Code</t>
   </si>
 </sst>
 </file>
@@ -2190,7 +2199,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2368,6 +2377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3217,13 +3227,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q68"/>
+  <dimension ref="A1:Q69"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomRight" activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5511,7 +5521,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="65" spans="1:8" s="74" customFormat="1">
+    <row r="65" spans="1:10" s="74" customFormat="1">
       <c r="A65" s="74">
         <v>64</v>
       </c>
@@ -5534,7 +5544,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="1:8" s="74" customFormat="1">
+    <row r="66" spans="1:10" s="74" customFormat="1">
       <c r="A66" s="74">
         <v>65</v>
       </c>
@@ -5557,7 +5567,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="74" customFormat="1">
+    <row r="67" spans="1:10" s="74" customFormat="1">
       <c r="A67" s="74">
         <v>66</v>
       </c>
@@ -5580,7 +5590,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="68" spans="1:8" s="74" customFormat="1">
+    <row r="68" spans="1:10" s="74" customFormat="1">
       <c r="A68" s="74">
         <v>67</v>
       </c>
@@ -5605,12 +5615,38 @@
       <c r="H68" s="75" t="s">
         <v>625</v>
       </c>
+    </row>
+    <row r="69" spans="1:10" s="74" customFormat="1">
+      <c r="A69" s="74">
+        <v>68</v>
+      </c>
+      <c r="B69" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="C69" s="74">
+        <v>331</v>
+      </c>
+      <c r="D69" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="E69" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F69" s="75" t="s">
+        <v>210</v>
+      </c>
+      <c r="G69" s="76" t="s">
+        <v>31</v>
+      </c>
+      <c r="H69" s="11"/>
+      <c r="I69" s="79"/>
+      <c r="J69" s="79"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B69:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B70:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5840,6 +5876,7 @@
     <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
     <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12920,10 +12957,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD39"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14102,6 +14139,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="38" spans="1:10" s="35" customFormat="1">
+      <c r="A38" s="74">
+        <v>68</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>628</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E38" s="35" t="s">
+        <v>629</v>
+      </c>
+      <c r="F38" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G38" s="35" t="s">
+        <v>630</v>
+      </c>
+      <c r="H38" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I38" s="35">
+        <v>1</v>
+      </c>
+      <c r="J38" s="35" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -14113,18 +14182,21 @@
   <conditionalFormatting sqref="A30">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D38:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D39:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38">
+      <formula1>"Add_To_Cart,Add_To_Wishlist,Get_SKU_Code"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14773,7 +14845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -15476,7 +15548,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30">
+    <row r="2" spans="1:19">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -15535,7 +15607,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30">
+    <row r="3" spans="1:19">
       <c r="A3" s="19">
         <v>2</v>
       </c>
@@ -15594,7 +15666,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="30">
+    <row r="4" spans="1:19">
       <c r="A4" s="19">
         <v>3</v>
       </c>
@@ -15771,7 +15843,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="45">
+    <row r="7" spans="1:19" ht="30">
       <c r="A7" s="19">
         <v>21</v>
       </c>
@@ -15889,7 +15961,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45">
+    <row r="9" spans="1:19" ht="30">
       <c r="A9" s="19">
         <v>23</v>
       </c>
@@ -15948,7 +16020,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="45">
+    <row r="10" spans="1:19" ht="30">
       <c r="A10" s="19">
         <v>24</v>
       </c>
@@ -18182,12 +18254,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18340,18 +18412,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18376,18 +18457,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA335 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="28" activeTab="31"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2758" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="635">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2028,6 +2028,18 @@
   </si>
   <si>
     <t>Get_SKU_Code</t>
+  </si>
+  <si>
+    <t>Compare products</t>
+  </si>
+  <si>
+    <t>CompareProducts</t>
+  </si>
+  <si>
+    <t>Bluetooth Music Receiver#JBL Tune600 Black</t>
+  </si>
+  <si>
+    <t>Add_To_Compare</t>
   </si>
 </sst>
 </file>
@@ -3227,13 +3239,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q69"/>
+  <dimension ref="A1:Q70"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G69" sqref="G69"/>
+      <selection pane="bottomRight" activeCell="E67" sqref="E67:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5603,8 +5615,8 @@
       <c r="D68" s="75" t="s">
         <v>624</v>
       </c>
-      <c r="E68" s="75" t="s">
-        <v>8</v>
+      <c r="E68" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F68" s="75" t="s">
         <v>210</v>
@@ -5629,8 +5641,8 @@
       <c r="D69" s="35" t="s">
         <v>628</v>
       </c>
-      <c r="E69" s="75" t="s">
-        <v>8</v>
+      <c r="E69" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F69" s="75" t="s">
         <v>210</v>
@@ -5641,12 +5653,35 @@
       <c r="H69" s="11"/>
       <c r="I69" s="79"/>
       <c r="J69" s="79"/>
+    </row>
+    <row r="70" spans="1:10" s="74" customFormat="1">
+      <c r="A70" s="74">
+        <v>69</v>
+      </c>
+      <c r="B70" s="75" t="s">
+        <v>631</v>
+      </c>
+      <c r="C70" s="74">
+        <v>335</v>
+      </c>
+      <c r="D70" s="75" t="s">
+        <v>631</v>
+      </c>
+      <c r="E70" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="G70" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="H70" s="74" t="s">
+        <v>632</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B70:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B71:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5664,6 +5699,11 @@
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
     <cfRule type="duplicateValues" dxfId="47" priority="12"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D70">
+      <formula1>$K$2:$K$18</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
     <hyperlink ref="J3" location="'SapCustomer++'!A1" display="SapCustomer"/>
@@ -12957,10 +12997,10 @@
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:B38"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14171,6 +14211,38 @@
         <v>373</v>
       </c>
     </row>
+    <row r="39" spans="1:10" s="35" customFormat="1">
+      <c r="A39" s="35">
+        <v>69</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>631</v>
+      </c>
+      <c r="C39" s="35">
+        <v>1</v>
+      </c>
+      <c r="D39" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E39" s="35" t="s">
+        <v>633</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>634</v>
+      </c>
+      <c r="H39" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I39" s="35" t="s">
+        <v>477</v>
+      </c>
+      <c r="J39" s="35">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -14182,14 +14254,14 @@
   <conditionalFormatting sqref="A30">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F39">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D39:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D40:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37">
@@ -14197,6 +14269,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38">
       <formula1>"Add_To_Cart,Add_To_Wishlist,Get_SKU_Code"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G39">
+      <formula1>"Add_To_Cart,Add_To_Wishlist,Get_SKU_Code,Add_To_Compare"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18254,12 +18329,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18412,27 +18487,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18457,9 +18523,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA262 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -8,52 +8,54 @@
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
-    <sheet name="ic_invalidCredslogin++" sheetId="71" r:id="rId2"/>
-    <sheet name="ClearCart++" sheetId="70" r:id="rId3"/>
-    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId4"/>
-    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId5"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId6"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId7"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId8"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId9"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId10"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId11"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId12"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId13"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId14"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId15"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId16"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId17"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId18"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId19"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId20"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId21"/>
-    <sheet name="Suites" sheetId="22" r:id="rId22"/>
-    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId23"/>
-    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId24"/>
-    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId25"/>
-    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId26"/>
-    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId27"/>
-    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId28"/>
-    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId29"/>
-    <sheet name="Login_magento++" sheetId="35" r:id="rId30"/>
-    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId31"/>
-    <sheet name="ProductSearch++" sheetId="33" r:id="rId32"/>
-    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId33"/>
-    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId34"/>
-    <sheet name="ic_login++" sheetId="44" r:id="rId35"/>
-    <sheet name="DB_connection_master++" sheetId="47" r:id="rId36"/>
-    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId37"/>
-    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId38"/>
-    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId39"/>
-    <sheet name="accountCreation++" sheetId="39" r:id="rId40"/>
-    <sheet name="Russels" sheetId="26" r:id="rId41"/>
-    <sheet name="Login++" sheetId="25" r:id="rId42"/>
-    <sheet name="Bradlows" sheetId="27" r:id="rId43"/>
-    <sheet name="Rochester" sheetId="28" r:id="rId44"/>
-    <sheet name="Preferred Store" sheetId="68" r:id="rId45"/>
-    <sheet name="Sleepmasters" sheetId="29" r:id="rId46"/>
-    <sheet name="HiFiCorp" sheetId="30" r:id="rId47"/>
+    <sheet name="icEmailWishlistverification++" sheetId="73" r:id="rId2"/>
+    <sheet name="SendWishlistToEmail++" sheetId="72" r:id="rId3"/>
+    <sheet name="ic_invalidCredslogin++" sheetId="71" r:id="rId4"/>
+    <sheet name="ClearCart++" sheetId="70" r:id="rId5"/>
+    <sheet name="ic_verifyWishlistItem++" sheetId="66" r:id="rId6"/>
+    <sheet name="IC_WishlistToCart++" sheetId="69" r:id="rId7"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId8"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId9"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId10"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId11"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId12"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId13"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId14"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId15"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId16"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId17"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId18"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId19"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId20"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId21"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId22"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId23"/>
+    <sheet name="Suites" sheetId="22" r:id="rId24"/>
+    <sheet name="PayUPagePayment++" sheetId="31" r:id="rId25"/>
+    <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId26"/>
+    <sheet name="deliveryPopulation++" sheetId="34" r:id="rId27"/>
+    <sheet name="icGiftCardPurchase++" sheetId="43" r:id="rId28"/>
+    <sheet name="SAP_OrderRelated++" sheetId="46" r:id="rId29"/>
+    <sheet name="GenerateOrderSAPnumber++" sheetId="38" r:id="rId30"/>
+    <sheet name="OrderStatusSearch++" sheetId="36" r:id="rId31"/>
+    <sheet name="Login_magento++" sheetId="35" r:id="rId32"/>
+    <sheet name="ic_RetriveOrderID++" sheetId="53" r:id="rId33"/>
+    <sheet name="ProductSearch++" sheetId="33" r:id="rId34"/>
+    <sheet name="icRedeemGiftCard++" sheetId="48" r:id="rId35"/>
+    <sheet name="VeriyGiftcardUsableity++" sheetId="49" r:id="rId36"/>
+    <sheet name="ic_login++" sheetId="44" r:id="rId37"/>
+    <sheet name="DB_connection_master++" sheetId="47" r:id="rId38"/>
+    <sheet name="icGiftCardVerificationSender++" sheetId="45" r:id="rId39"/>
+    <sheet name="ic_CashDepositPayment++" sheetId="41" r:id="rId40"/>
+    <sheet name="CreateaccountBackend++" sheetId="40" r:id="rId41"/>
+    <sheet name="accountCreation++" sheetId="39" r:id="rId42"/>
+    <sheet name="Russels" sheetId="26" r:id="rId43"/>
+    <sheet name="Login++" sheetId="25" r:id="rId44"/>
+    <sheet name="Bradlows" sheetId="27" r:id="rId45"/>
+    <sheet name="Rochester" sheetId="28" r:id="rId46"/>
+    <sheet name="Preferred Store" sheetId="68" r:id="rId47"/>
+    <sheet name="Sleepmasters" sheetId="29" r:id="rId48"/>
+    <sheet name="HiFiCorp" sheetId="30" r:id="rId49"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -127,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="644">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2040,6 +2042,33 @@
   </si>
   <si>
     <t>Add_To_Compare</t>
+  </si>
+  <si>
+    <t>Wish List - Validate Mail for Wish List Share</t>
+  </si>
+  <si>
+    <t>SendWishlistToEmail</t>
+  </si>
+  <si>
+    <t>icEmailWishlistverification</t>
+  </si>
+  <si>
+    <t>Sourave</t>
+  </si>
+  <si>
+    <t>R300 Wallet top-up for purchases on PlayStation Store</t>
+  </si>
+  <si>
+    <t>Email_To_Share</t>
+  </si>
+  <si>
+    <t>TimeOut</t>
+  </si>
+  <si>
+    <t>waitTimeForEmailInSec</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -3239,13 +3268,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q70"/>
+  <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E52" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E67" sqref="E67:E69"/>
+      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5533,7 +5562,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="74" customFormat="1">
+    <row r="65" spans="1:12" s="74" customFormat="1">
       <c r="A65" s="74">
         <v>64</v>
       </c>
@@ -5556,7 +5585,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="74" customFormat="1">
+    <row r="66" spans="1:12" s="74" customFormat="1">
       <c r="A66" s="74">
         <v>65</v>
       </c>
@@ -5579,7 +5608,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="74" customFormat="1">
+    <row r="67" spans="1:12" s="74" customFormat="1">
       <c r="A67" s="74">
         <v>66</v>
       </c>
@@ -5602,7 +5631,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="74" customFormat="1">
+    <row r="68" spans="1:12" s="74" customFormat="1">
       <c r="A68" s="74">
         <v>67</v>
       </c>
@@ -5628,7 +5657,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="74" customFormat="1">
+    <row r="69" spans="1:12" s="74" customFormat="1">
       <c r="A69" s="74">
         <v>68</v>
       </c>
@@ -5654,7 +5683,7 @@
       <c r="I69" s="79"/>
       <c r="J69" s="79"/>
     </row>
-    <row r="70" spans="1:10" s="74" customFormat="1">
+    <row r="70" spans="1:12" s="74" customFormat="1">
       <c r="A70" s="74">
         <v>69</v>
       </c>
@@ -5675,13 +5704,51 @@
       </c>
       <c r="H70" s="74" t="s">
         <v>632</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" s="74" customFormat="1">
+      <c r="A71" s="35">
+        <v>70</v>
+      </c>
+      <c r="B71" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C71" s="74">
+        <v>265</v>
+      </c>
+      <c r="D71" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="E71" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="77" t="s">
+        <v>638</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="H71" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="I71" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="J71" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K71" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="L71" s="76" t="s">
+        <v>637</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="53" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B71:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B72:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="52" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -5700,7 +5767,7 @@
     <cfRule type="duplicateValues" dxfId="47" priority="12"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D70">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D70:D71">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
   </dataValidations>
@@ -5917,6 +5984,12 @@
     <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch"/>
     <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J71" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="K71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
+    <hyperlink ref="L71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -5924,6 +5997,555 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="68" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" style="68" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="68" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="68" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="68"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="69" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="69" t="s">
+        <v>480</v>
+      </c>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="69" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="69" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="69">
+        <v>25</v>
+      </c>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="69">
+        <v>26</v>
+      </c>
+      <c r="B5" s="69"/>
+      <c r="C5" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="69">
+        <v>29</v>
+      </c>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="55">
+        <v>1</v>
+      </c>
+      <c r="B7" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="C7" s="69">
+        <v>1</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="55">
+        <v>2</v>
+      </c>
+      <c r="B8" s="55" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="69">
+        <v>1</v>
+      </c>
+      <c r="D8" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="55">
+        <v>3</v>
+      </c>
+      <c r="B9" s="55" t="s">
+        <v>240</v>
+      </c>
+      <c r="C9" s="69">
+        <v>1</v>
+      </c>
+      <c r="D9" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="55">
+        <v>4</v>
+      </c>
+      <c r="B10" s="55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="69">
+        <v>1</v>
+      </c>
+      <c r="D10" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="55">
+        <v>5</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" s="69">
+        <v>1</v>
+      </c>
+      <c r="D11" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="55">
+        <v>6</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>237</v>
+      </c>
+      <c r="C12" s="69">
+        <v>1</v>
+      </c>
+      <c r="D12" s="69" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30">
+      <c r="A13" s="55">
+        <v>7</v>
+      </c>
+      <c r="B13" s="55" t="s">
+        <v>243</v>
+      </c>
+      <c r="C13" s="69">
+        <v>1</v>
+      </c>
+      <c r="D13" s="69" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30">
+      <c r="A14" s="55">
+        <v>8</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="C14" s="69">
+        <v>1</v>
+      </c>
+      <c r="D14" s="69" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="55">
+        <v>9</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>231</v>
+      </c>
+      <c r="C15" s="69">
+        <v>1</v>
+      </c>
+      <c r="D15" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="55">
+        <v>10</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>233</v>
+      </c>
+      <c r="C16" s="69">
+        <v>1</v>
+      </c>
+      <c r="D16" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="55">
+        <v>11</v>
+      </c>
+      <c r="B17" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="69">
+        <v>1</v>
+      </c>
+      <c r="D17" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="55">
+        <v>12</v>
+      </c>
+      <c r="B18" s="55" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="69">
+        <v>1</v>
+      </c>
+      <c r="D18" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="55">
+        <v>13</v>
+      </c>
+      <c r="B19" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="C19" s="69">
+        <v>1</v>
+      </c>
+      <c r="D19" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="55">
+        <v>14</v>
+      </c>
+      <c r="B20" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="C20" s="69">
+        <v>1</v>
+      </c>
+      <c r="D20" s="69" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="55">
+        <v>15</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>245</v>
+      </c>
+      <c r="C21" s="69">
+        <v>1</v>
+      </c>
+      <c r="D21" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="55">
+        <v>16</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>246</v>
+      </c>
+      <c r="C22" s="69">
+        <v>1</v>
+      </c>
+      <c r="D22" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="55">
+        <v>17</v>
+      </c>
+      <c r="B23" s="55" t="s">
+        <v>247</v>
+      </c>
+      <c r="C23" s="69">
+        <v>1</v>
+      </c>
+      <c r="D23" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="55">
+        <v>18</v>
+      </c>
+      <c r="B24" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="C24" s="69">
+        <v>1</v>
+      </c>
+      <c r="D24" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="55">
+        <v>19</v>
+      </c>
+      <c r="B25" s="55" t="s">
+        <v>249</v>
+      </c>
+      <c r="C25" s="69">
+        <v>1</v>
+      </c>
+      <c r="D25" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="55">
+        <v>20</v>
+      </c>
+      <c r="B26" s="55" t="s">
+        <v>295</v>
+      </c>
+      <c r="C26" s="69">
+        <v>1</v>
+      </c>
+      <c r="D26" s="69" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="55">
+        <v>31</v>
+      </c>
+      <c r="B27" s="55" t="s">
+        <v>208</v>
+      </c>
+      <c r="C27" s="69">
+        <v>1</v>
+      </c>
+      <c r="D27" s="69" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="63">
+        <v>39</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>345</v>
+      </c>
+      <c r="C28" s="69">
+        <v>1</v>
+      </c>
+      <c r="D28" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="63">
+        <v>40</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>346</v>
+      </c>
+      <c r="C29" s="69">
+        <v>1</v>
+      </c>
+      <c r="D29" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="63">
+        <v>41</v>
+      </c>
+      <c r="B30" s="63" t="s">
+        <v>347</v>
+      </c>
+      <c r="C30" s="69">
+        <v>1</v>
+      </c>
+      <c r="D30" s="69" t="s">
+        <v>458</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A7:A26">
+    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:B26">
+    <cfRule type="duplicateValues" dxfId="39" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27">
+    <cfRule type="duplicateValues" dxfId="38" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:A30">
+    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:B30">
+    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>453</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="44">
+        <v>47</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>342</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="44">
+        <v>48</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>343</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="44">
+        <v>49</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>457</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -5986,7 +6608,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -6154,7 +6776,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
@@ -6285,7 +6907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -6443,7 +7065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -6582,7 +7204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
@@ -6856,7 +7478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -6927,7 +7549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -6984,7 +7606,108 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="42"/>
+    <col min="4" max="4" width="23.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="42"/>
+    <col min="9" max="9" width="29.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>187</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>183</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="42" t="s">
+        <v>191</v>
+      </c>
+      <c r="I1" s="42" t="s">
+        <v>642</v>
+      </c>
+      <c r="J1" s="42" t="s">
+        <v>185</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="L1" s="42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="35">
+        <v>70</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="I2" s="42" t="s">
+        <v>643</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>362</v>
+      </c>
+      <c r="L2" s="42" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -7103,7 +7826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC7"/>
   <sheetViews>
@@ -7550,105 +8273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="42"/>
-    <col min="2" max="2" width="20.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="42"/>
-    <col min="4" max="4" width="13.140625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="42" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>617</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="42" t="s">
-        <v>616</v>
-      </c>
-      <c r="G1" s="42" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="74">
-        <v>62</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>612</v>
-      </c>
-      <c r="C2" s="42">
-        <v>1</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>615</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="74">
-        <v>63</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>612</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>417</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>614</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -9039,7 +9664,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -9501,7 +10126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
@@ -9666,7 +10291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J19"/>
   <sheetViews>
@@ -10255,7 +10880,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -10492,7 +11117,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
@@ -11107,7 +11732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
@@ -11354,7 +11979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
@@ -11561,7 +12186,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>640</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="35">
+        <v>70</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C2" s="75">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="E2" s="42">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -11821,7 +12499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -12110,72 +12788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.140625" style="42"/>
-    <col min="2" max="2" width="47.42578125" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="74">
-        <v>57</v>
-      </c>
-      <c r="B2" s="75" t="s">
-        <v>601</v>
-      </c>
-      <c r="C2" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="74">
-        <v>58</v>
-      </c>
-      <c r="B3" s="75" t="s">
-        <v>600</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="74">
-        <v>59</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>599</v>
-      </c>
-      <c r="C4" s="42">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
@@ -12830,7 +13443,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
@@ -12995,13 +13608,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
-    </sheetView>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -14243,6 +14854,38 @@
         <v>6</v>
       </c>
     </row>
+    <row r="40" spans="1:10" s="35" customFormat="1">
+      <c r="A40" s="35">
+        <v>70</v>
+      </c>
+      <c r="B40" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="E40" s="35" t="s">
+        <v>639</v>
+      </c>
+      <c r="F40" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G40" s="35" t="s">
+        <v>470</v>
+      </c>
+      <c r="H40" s="35" t="s">
+        <v>586</v>
+      </c>
+      <c r="I40" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40" s="35" t="s">
+        <v>373</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -14255,16 +14898,16 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30 G40">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F39">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D40:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D41:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37 H40">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38">
@@ -14280,7 +14923,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -14383,7 +15026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -14466,7 +15109,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -14804,7 +15447,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -14916,7 +15559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L4"/>
   <sheetViews>
@@ -15046,7 +15689,105 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="20.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="42"/>
+    <col min="4" max="4" width="13.140625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="42" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="42" t="s">
+        <v>616</v>
+      </c>
+      <c r="G1" s="42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="74">
+        <v>62</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="74">
+        <v>63</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>612</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>417</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -15092,7 +15833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L13"/>
   <sheetViews>
@@ -15401,136 +16142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="62">
-        <v>52</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>471</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="62">
-        <v>53</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>475</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="74">
-        <v>54</v>
-      </c>
-      <c r="B4" s="75" t="s">
-        <v>583</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="35" customFormat="1">
-      <c r="A5" s="35">
-        <v>55</v>
-      </c>
-      <c r="B5" s="75" t="s">
-        <v>592</v>
-      </c>
-      <c r="C5" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="74">
-        <v>56</v>
-      </c>
-      <c r="B6" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C6" s="42">
-        <v>1</v>
-      </c>
-      <c r="D6" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="74">
-        <v>56</v>
-      </c>
-      <c r="B7" s="75" t="s">
-        <v>596</v>
-      </c>
-      <c r="C7" s="42">
-        <v>2</v>
-      </c>
-      <c r="D7" s="35" t="s">
-        <v>496</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5 D6:D7">
-      <formula1>"All,Specific"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S13"/>
   <sheetViews>
@@ -16351,7 +16963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -16456,7 +17068,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -16660,7 +17272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16764,7 +17376,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -16868,7 +17480,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
@@ -17241,7 +17853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -17345,7 +17957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
@@ -17451,6 +18063,214 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="42"/>
+    <col min="2" max="2" width="47.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="74">
+        <v>57</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="74">
+        <v>58</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>600</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="74">
+        <v>59</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>599</v>
+      </c>
+      <c r="C4" s="42">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" style="42" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="42"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="62">
+        <v>52</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>471</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="62">
+        <v>53</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="74">
+        <v>54</v>
+      </c>
+      <c r="B4" s="75" t="s">
+        <v>583</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="35" customFormat="1">
+      <c r="A5" s="35">
+        <v>55</v>
+      </c>
+      <c r="B5" s="75" t="s">
+        <v>592</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="74">
+        <v>56</v>
+      </c>
+      <c r="B6" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C6" s="42">
+        <v>1</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="74">
+        <v>56</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>596</v>
+      </c>
+      <c r="C7" s="42">
+        <v>2</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="35">
+        <v>70</v>
+      </c>
+      <c r="B8" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C8" s="42">
+        <v>1</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>496</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D8">
+      <formula1>"All,Specific"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -17508,9 +18328,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17588,6 +18408,17 @@
         <v>87</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="35">
+        <v>70</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="44" priority="2"/>
@@ -17599,9 +18430,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -17755,6 +18586,29 @@
         <v>11</v>
       </c>
     </row>
+    <row r="7" spans="1:7" s="35" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A7" s="35">
+        <v>70</v>
+      </c>
+      <c r="B7" s="75" t="s">
+        <v>635</v>
+      </c>
+      <c r="C7" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>491</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>493</v>
+      </c>
+      <c r="G7" s="35">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
     <cfRule type="duplicateValues" dxfId="42" priority="2"/>
@@ -17763,7 +18617,7 @@
     <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17773,568 +18627,20 @@
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="E5" r:id="rId4"/>
     <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="68" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" style="68" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="68" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" style="68" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="68"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="69" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="69" t="s">
-        <v>480</v>
-      </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="69" t="s">
-        <v>481</v>
-      </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="69" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="69">
-        <v>25</v>
-      </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="69">
-        <v>26</v>
-      </c>
-      <c r="B5" s="69"/>
-      <c r="C5" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="69">
-        <v>29</v>
-      </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="55">
-        <v>1</v>
-      </c>
-      <c r="B7" s="55" t="s">
-        <v>238</v>
-      </c>
-      <c r="C7" s="69">
-        <v>1</v>
-      </c>
-      <c r="D7" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="55">
-        <v>2</v>
-      </c>
-      <c r="B8" s="55" t="s">
-        <v>239</v>
-      </c>
-      <c r="C8" s="69">
-        <v>1</v>
-      </c>
-      <c r="D8" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="55">
-        <v>3</v>
-      </c>
-      <c r="B9" s="55" t="s">
-        <v>240</v>
-      </c>
-      <c r="C9" s="69">
-        <v>1</v>
-      </c>
-      <c r="D9" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="55">
-        <v>4</v>
-      </c>
-      <c r="B10" s="55" t="s">
-        <v>241</v>
-      </c>
-      <c r="C10" s="69">
-        <v>1</v>
-      </c>
-      <c r="D10" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="55">
-        <v>5</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>242</v>
-      </c>
-      <c r="C11" s="69">
-        <v>1</v>
-      </c>
-      <c r="D11" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="55">
-        <v>6</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>237</v>
-      </c>
-      <c r="C12" s="69">
-        <v>1</v>
-      </c>
-      <c r="D12" s="69" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30">
-      <c r="A13" s="55">
-        <v>7</v>
-      </c>
-      <c r="B13" s="55" t="s">
-        <v>243</v>
-      </c>
-      <c r="C13" s="69">
-        <v>1</v>
-      </c>
-      <c r="D13" s="69" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="30">
-      <c r="A14" s="55">
-        <v>8</v>
-      </c>
-      <c r="B14" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="C14" s="69">
-        <v>1</v>
-      </c>
-      <c r="D14" s="69" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="55">
-        <v>9</v>
-      </c>
-      <c r="B15" s="55" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="69">
-        <v>1</v>
-      </c>
-      <c r="D15" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="55">
-        <v>10</v>
-      </c>
-      <c r="B16" s="55" t="s">
-        <v>233</v>
-      </c>
-      <c r="C16" s="69">
-        <v>1</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="55">
-        <v>11</v>
-      </c>
-      <c r="B17" s="55" t="s">
-        <v>234</v>
-      </c>
-      <c r="C17" s="69">
-        <v>1</v>
-      </c>
-      <c r="D17" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="55">
-        <v>12</v>
-      </c>
-      <c r="B18" s="55" t="s">
-        <v>235</v>
-      </c>
-      <c r="C18" s="69">
-        <v>1</v>
-      </c>
-      <c r="D18" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="55">
-        <v>13</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="69">
-        <v>1</v>
-      </c>
-      <c r="D19" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="55">
-        <v>14</v>
-      </c>
-      <c r="B20" s="55" t="s">
-        <v>285</v>
-      </c>
-      <c r="C20" s="69">
-        <v>1</v>
-      </c>
-      <c r="D20" s="69" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="55">
-        <v>15</v>
-      </c>
-      <c r="B21" s="55" t="s">
-        <v>245</v>
-      </c>
-      <c r="C21" s="69">
-        <v>1</v>
-      </c>
-      <c r="D21" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="55">
-        <v>16</v>
-      </c>
-      <c r="B22" s="55" t="s">
-        <v>246</v>
-      </c>
-      <c r="C22" s="69">
-        <v>1</v>
-      </c>
-      <c r="D22" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="55">
-        <v>17</v>
-      </c>
-      <c r="B23" s="55" t="s">
-        <v>247</v>
-      </c>
-      <c r="C23" s="69">
-        <v>1</v>
-      </c>
-      <c r="D23" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="55">
-        <v>18</v>
-      </c>
-      <c r="B24" s="55" t="s">
-        <v>248</v>
-      </c>
-      <c r="C24" s="69">
-        <v>1</v>
-      </c>
-      <c r="D24" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="55">
-        <v>19</v>
-      </c>
-      <c r="B25" s="55" t="s">
-        <v>249</v>
-      </c>
-      <c r="C25" s="69">
-        <v>1</v>
-      </c>
-      <c r="D25" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="55">
-        <v>20</v>
-      </c>
-      <c r="B26" s="55" t="s">
-        <v>295</v>
-      </c>
-      <c r="C26" s="69">
-        <v>1</v>
-      </c>
-      <c r="D26" s="69" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="55">
-        <v>31</v>
-      </c>
-      <c r="B27" s="55" t="s">
-        <v>208</v>
-      </c>
-      <c r="C27" s="69">
-        <v>1</v>
-      </c>
-      <c r="D27" s="69" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="63">
-        <v>39</v>
-      </c>
-      <c r="B28" s="63" t="s">
-        <v>345</v>
-      </c>
-      <c r="C28" s="69">
-        <v>1</v>
-      </c>
-      <c r="D28" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="63">
-        <v>40</v>
-      </c>
-      <c r="B29" s="63" t="s">
-        <v>346</v>
-      </c>
-      <c r="C29" s="69">
-        <v>1</v>
-      </c>
-      <c r="D29" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="63">
-        <v>41</v>
-      </c>
-      <c r="B30" s="63" t="s">
-        <v>347</v>
-      </c>
-      <c r="C30" s="69">
-        <v>1</v>
-      </c>
-      <c r="D30" s="69" t="s">
-        <v>458</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A7:A26">
-    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:B26">
-    <cfRule type="duplicateValues" dxfId="39" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="38" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="37" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:A30">
-    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28:B30">
-    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="42" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="42" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="42" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="42" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="42"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="42" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>453</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="44">
-        <v>47</v>
-      </c>
-      <c r="B2" s="44" t="s">
-        <v>342</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="44">
-        <v>48</v>
-      </c>
-      <c r="B3" s="44" t="s">
-        <v>343</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="44">
-        <v>49</v>
-      </c>
-      <c r="B4" s="44" t="s">
-        <v>344</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>457</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18487,18 +18793,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18523,18 +18838,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating main to add TA278 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="658">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2053,9 +2053,6 @@
     <t>icEmailWishlistverification</t>
   </si>
   <si>
-    <t>Sourave</t>
-  </si>
-  <si>
     <t>R300 Wallet top-up for purchases on PlayStation Store</t>
   </si>
   <si>
@@ -2069,6 +2066,51 @@
   </si>
   <si>
     <t>500</t>
+  </si>
+  <si>
+    <t>Verify Message after submit email on Forgot Password Page</t>
+  </si>
+  <si>
+    <t>Login Page - verify Mail is received for Forget Password</t>
+  </si>
+  <si>
+    <t>Bongi, getting 0 emails</t>
+  </si>
+  <si>
+    <t>Sourave, share button not showing</t>
+  </si>
+  <si>
+    <t>Cart redirection to Cart details page TA275</t>
+  </si>
+  <si>
+    <t>Cart redirection to cart details page</t>
+  </si>
+  <si>
+    <t>RedirectToProdDetailPageFromCart</t>
+  </si>
+  <si>
+    <t>Redeem gift cart with invalid coupon code TA277</t>
+  </si>
+  <si>
+    <t>Redeem gift cart with invalid coupon code</t>
+  </si>
+  <si>
+    <t>giftCardWithInvalidCouponCode</t>
+  </si>
+  <si>
+    <t>Registered user add items to cart-Logout to login again and confirm cart TA278</t>
+  </si>
+  <si>
+    <t>Registered user add items to cart-Logout to login again and confirm cart</t>
+  </si>
+  <si>
+    <t>ic_logout</t>
+  </si>
+  <si>
+    <t>verifyCart</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2170,7 +2212,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2192,6 +2234,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2240,7 +2288,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2419,6 +2467,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2427,7 +2482,17 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="54">
+  <dxfs count="55">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3268,13 +3333,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q71"/>
+  <dimension ref="A1:Q74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E71" sqref="E71"/>
+      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3284,7 +3349,7 @@
     <col min="3" max="3" width="20.140625" style="63" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="89.42578125" style="63" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="63" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="63" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="63" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" style="63" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29" style="63" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.140625" style="63" bestFit="1" customWidth="1"/>
@@ -3297,7 +3362,7 @@
     <col min="18" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" ht="30">
       <c r="A1" s="43" t="s">
         <v>15</v>
       </c>
@@ -5193,7 +5258,7 @@
       <c r="O49" s="64"/>
     </row>
     <row r="50" spans="1:15" s="45" customFormat="1">
-      <c r="A50" s="44">
+      <c r="A50" s="62">
         <v>49</v>
       </c>
       <c r="B50" s="44" t="s">
@@ -5205,7 +5270,7 @@
       <c r="D50" s="44" t="s">
         <v>342</v>
       </c>
-      <c r="E50" s="45" t="s">
+      <c r="E50" s="55" t="s">
         <v>9</v>
       </c>
       <c r="G50" s="73" t="s">
@@ -5214,7 +5279,7 @@
       <c r="H50" s="44"/>
     </row>
     <row r="51" spans="1:15" s="45" customFormat="1">
-      <c r="A51" s="44">
+      <c r="A51" s="62">
         <v>50</v>
       </c>
       <c r="B51" s="44" t="s">
@@ -5226,7 +5291,7 @@
       <c r="D51" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="E51" s="45" t="s">
+      <c r="E51" s="55" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="73" t="s">
@@ -5235,7 +5300,7 @@
       <c r="H51" s="44"/>
     </row>
     <row r="52" spans="1:15" s="45" customFormat="1">
-      <c r="A52" s="44">
+      <c r="A52" s="62">
         <v>51</v>
       </c>
       <c r="B52" s="44" t="s">
@@ -5247,7 +5312,7 @@
       <c r="D52" s="44" t="s">
         <v>344</v>
       </c>
-      <c r="E52" s="45" t="s">
+      <c r="E52" s="55" t="s">
         <v>9</v>
       </c>
       <c r="G52" s="73" t="s">
@@ -5259,7 +5324,7 @@
       <c r="A53" s="62">
         <v>52</v>
       </c>
-      <c r="B53" s="62" t="s">
+      <c r="B53" s="80" t="s">
         <v>471</v>
       </c>
       <c r="D53" s="62" t="s">
@@ -5305,7 +5370,7 @@
       </c>
     </row>
     <row r="55" spans="1:15" s="74" customFormat="1">
-      <c r="A55" s="74">
+      <c r="A55" s="62">
         <v>54</v>
       </c>
       <c r="B55" s="75" t="s">
@@ -5334,10 +5399,10 @@
       </c>
     </row>
     <row r="56" spans="1:15" s="74" customFormat="1">
-      <c r="A56" s="74">
+      <c r="A56" s="62">
         <v>55</v>
       </c>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="83" t="s">
         <v>592</v>
       </c>
       <c r="D56" s="75" t="s">
@@ -5360,10 +5425,10 @@
       </c>
     </row>
     <row r="57" spans="1:15" s="74" customFormat="1">
-      <c r="A57" s="74">
+      <c r="A57" s="62">
         <v>56</v>
       </c>
-      <c r="B57" s="75" t="s">
+      <c r="B57" s="82" t="s">
         <v>596</v>
       </c>
       <c r="D57" s="75" t="s">
@@ -5389,10 +5454,10 @@
       </c>
     </row>
     <row r="58" spans="1:15" s="74" customFormat="1">
-      <c r="A58" s="74">
+      <c r="A58" s="62">
         <v>57</v>
       </c>
-      <c r="B58" s="75" t="s">
+      <c r="B58" s="81" t="s">
         <v>601</v>
       </c>
       <c r="C58" s="74">
@@ -5415,7 +5480,7 @@
       </c>
     </row>
     <row r="59" spans="1:15" s="74" customFormat="1">
-      <c r="A59" s="74">
+      <c r="A59" s="62">
         <v>58</v>
       </c>
       <c r="B59" s="75" t="s">
@@ -5442,10 +5507,10 @@
       <c r="I59" s="75"/>
     </row>
     <row r="60" spans="1:15" s="74" customFormat="1">
-      <c r="A60" s="74">
+      <c r="A60" s="62">
         <v>59</v>
       </c>
-      <c r="B60" s="75" t="s">
+      <c r="B60" s="81" t="s">
         <v>599</v>
       </c>
       <c r="C60" s="74">
@@ -5468,10 +5533,10 @@
       </c>
     </row>
     <row r="61" spans="1:15" s="74" customFormat="1">
-      <c r="A61" s="74">
+      <c r="A61" s="62">
         <v>60</v>
       </c>
-      <c r="B61" s="75" t="s">
+      <c r="B61" s="82" t="s">
         <v>606</v>
       </c>
       <c r="C61" s="74">
@@ -5494,10 +5559,10 @@
       </c>
     </row>
     <row r="62" spans="1:15" s="74" customFormat="1">
-      <c r="A62" s="74">
+      <c r="A62" s="62">
         <v>61</v>
       </c>
-      <c r="B62" s="75" t="s">
+      <c r="B62" s="82" t="s">
         <v>608</v>
       </c>
       <c r="D62" s="75" t="s">
@@ -5517,7 +5582,7 @@
       </c>
     </row>
     <row r="63" spans="1:15" s="74" customFormat="1">
-      <c r="A63" s="74">
+      <c r="A63" s="62">
         <v>62</v>
       </c>
       <c r="B63" s="75" t="s">
@@ -5540,7 +5605,7 @@
       </c>
     </row>
     <row r="64" spans="1:15" s="74" customFormat="1">
-      <c r="A64" s="74">
+      <c r="A64" s="62">
         <v>63</v>
       </c>
       <c r="B64" s="75" t="s">
@@ -5562,8 +5627,8 @@
         <v>613</v>
       </c>
     </row>
-    <row r="65" spans="1:12" s="74" customFormat="1">
-      <c r="A65" s="74">
+    <row r="65" spans="1:13" s="74" customFormat="1">
+      <c r="A65" s="62">
         <v>64</v>
       </c>
       <c r="B65" s="75" t="s">
@@ -5585,11 +5650,11 @@
         <v>619</v>
       </c>
     </row>
-    <row r="66" spans="1:12" s="74" customFormat="1">
-      <c r="A66" s="74">
+    <row r="66" spans="1:13" s="74" customFormat="1">
+      <c r="A66" s="62">
         <v>65</v>
       </c>
-      <c r="B66" s="75" t="s">
+      <c r="B66" s="77" t="s">
         <v>620</v>
       </c>
       <c r="C66" s="74">
@@ -5608,18 +5673,18 @@
         <v>621</v>
       </c>
     </row>
-    <row r="67" spans="1:12" s="74" customFormat="1">
-      <c r="A67" s="74">
+    <row r="67" spans="1:13" s="74" customFormat="1">
+      <c r="A67" s="62">
         <v>66</v>
       </c>
-      <c r="B67" s="74" t="s">
-        <v>622</v>
+      <c r="B67" s="81" t="s">
+        <v>643</v>
       </c>
       <c r="C67" s="74">
         <v>315</v>
       </c>
-      <c r="D67" s="74" t="s">
-        <v>622</v>
+      <c r="D67" s="75" t="s">
+        <v>643</v>
       </c>
       <c r="E67" s="55" t="s">
         <v>9</v>
@@ -5631,34 +5696,34 @@
         <v>623</v>
       </c>
     </row>
-    <row r="68" spans="1:12" s="74" customFormat="1">
-      <c r="A68" s="74">
+    <row r="68" spans="1:13" s="74" customFormat="1">
+      <c r="A68" s="62">
         <v>67</v>
       </c>
-      <c r="B68" s="75" t="s">
-        <v>624</v>
+      <c r="B68" s="77" t="s">
+        <v>644</v>
       </c>
       <c r="C68" s="74">
         <v>318</v>
       </c>
       <c r="D68" s="75" t="s">
-        <v>624</v>
+        <v>644</v>
       </c>
       <c r="E68" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="F68" s="75" t="s">
-        <v>210</v>
-      </c>
-      <c r="G68" s="74" t="s">
+        <v>8</v>
+      </c>
+      <c r="F68" s="77" t="s">
+        <v>645</v>
+      </c>
+      <c r="G68" s="77" t="s">
         <v>623</v>
       </c>
-      <c r="H68" s="75" t="s">
+      <c r="H68" s="35" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="69" spans="1:12" s="74" customFormat="1">
-      <c r="A69" s="74">
+    <row r="69" spans="1:13" s="74" customFormat="1">
+      <c r="A69" s="62">
         <v>68</v>
       </c>
       <c r="B69" s="35" t="s">
@@ -5683,11 +5748,11 @@
       <c r="I69" s="79"/>
       <c r="J69" s="79"/>
     </row>
-    <row r="70" spans="1:12" s="74" customFormat="1">
-      <c r="A70" s="74">
+    <row r="70" spans="1:13" s="74" customFormat="1">
+      <c r="A70" s="62">
         <v>69</v>
       </c>
-      <c r="B70" s="75" t="s">
+      <c r="B70" s="81" t="s">
         <v>631</v>
       </c>
       <c r="C70" s="74">
@@ -5696,8 +5761,8 @@
       <c r="D70" s="75" t="s">
         <v>631</v>
       </c>
-      <c r="E70" s="75" t="s">
-        <v>8</v>
+      <c r="E70" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="G70" s="79" t="s">
         <v>31</v>
@@ -5706,11 +5771,11 @@
         <v>632</v>
       </c>
     </row>
-    <row r="71" spans="1:12" s="74" customFormat="1">
-      <c r="A71" s="35">
+    <row r="71" spans="1:13" s="74" customFormat="1">
+      <c r="A71" s="62">
         <v>70</v>
       </c>
-      <c r="B71" s="75" t="s">
+      <c r="B71" s="35" t="s">
         <v>635</v>
       </c>
       <c r="C71" s="74">
@@ -5719,11 +5784,11 @@
       <c r="D71" s="75" t="s">
         <v>635</v>
       </c>
-      <c r="E71" s="75" t="s">
-        <v>8</v>
+      <c r="E71" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F71" s="77" t="s">
-        <v>638</v>
+        <v>646</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>472</v>
@@ -5744,29 +5809,131 @@
         <v>637</v>
       </c>
     </row>
+    <row r="72" spans="1:13" s="74" customFormat="1">
+      <c r="A72" s="74">
+        <v>30</v>
+      </c>
+      <c r="B72" s="75" t="s">
+        <v>647</v>
+      </c>
+      <c r="C72" s="74">
+        <v>275</v>
+      </c>
+      <c r="D72" s="75" t="s">
+        <v>648</v>
+      </c>
+      <c r="E72" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G72" s="77" t="s">
+        <v>657</v>
+      </c>
+      <c r="H72" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="I72" s="74" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" s="74" customFormat="1">
+      <c r="A73" s="74">
+        <v>31</v>
+      </c>
+      <c r="B73" s="75" t="s">
+        <v>650</v>
+      </c>
+      <c r="C73" s="74">
+        <v>277</v>
+      </c>
+      <c r="D73" s="75" t="s">
+        <v>651</v>
+      </c>
+      <c r="E73" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F73" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G73" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="H73" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="I73" s="75" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" s="84" customFormat="1">
+      <c r="A74" s="84">
+        <v>32</v>
+      </c>
+      <c r="B74" s="79" t="s">
+        <v>653</v>
+      </c>
+      <c r="C74" s="84">
+        <v>278</v>
+      </c>
+      <c r="D74" s="79" t="s">
+        <v>654</v>
+      </c>
+      <c r="E74" s="79" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G74" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="H74" s="79" t="s">
+        <v>598</v>
+      </c>
+      <c r="I74" s="79" t="s">
+        <v>31</v>
+      </c>
+      <c r="J74" s="75" t="s">
+        <v>350</v>
+      </c>
+      <c r="K74" s="79" t="s">
+        <v>655</v>
+      </c>
+      <c r="L74" s="79" t="s">
+        <v>165</v>
+      </c>
+      <c r="M74" s="79" t="s">
+        <v>656</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="53" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B72:B1048576 B1:B31 B33:B49">
-    <cfRule type="duplicateValues" dxfId="52" priority="11"/>
+  <conditionalFormatting sqref="B75:B1048576 B1:B31 B33:B49">
+    <cfRule type="duplicateValues" dxfId="53" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="51" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="49" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="47" priority="12"/>
+  <conditionalFormatting sqref="A2:A31 A33:A49">
+    <cfRule type="duplicateValues" dxfId="48" priority="13"/>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <conditionalFormatting sqref="A50:A71">
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D70:D71">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
@@ -7610,9 +7777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -7649,7 +7814,7 @@
         <v>191</v>
       </c>
       <c r="I1" s="42" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="J1" s="42" t="s">
         <v>185</v>
@@ -7687,7 +7852,7 @@
         <v>362</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="J2" s="42" t="s">
         <v>362</v>
@@ -12211,10 +12376,10 @@
         <v>35</v>
       </c>
       <c r="D1" s="42" t="s">
+        <v>639</v>
+      </c>
+      <c r="E1" s="42" t="s">
         <v>640</v>
-      </c>
-      <c r="E1" s="42" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -14868,7 +15033,7 @@
         <v>152</v>
       </c>
       <c r="E40" s="35" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F40" s="35" t="s">
         <v>469</v>
@@ -15564,15 +15729,14 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
updating main to add TA280 to main sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2853" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="662">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2110,7 +2110,19 @@
     <t>verifyCart</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>Validate product is out of stock</t>
+  </si>
+  <si>
+    <t>275-278 sheet</t>
+  </si>
+  <si>
+    <t>277-276 sheet</t>
+  </si>
+  <si>
+    <t>Ultra Link Keyboard And Mouse Combo KBM04</t>
+  </si>
+  <si>
+    <t>Validate_Out_Of_Stock</t>
   </si>
 </sst>
 </file>
@@ -3333,13 +3345,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q74"/>
+  <dimension ref="A1:Q75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G72" sqref="G72"/>
+      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5811,25 +5823,25 @@
     </row>
     <row r="72" spans="1:13" s="74" customFormat="1">
       <c r="A72" s="74">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="B72" s="75" t="s">
         <v>647</v>
       </c>
-      <c r="C72" s="74">
-        <v>275</v>
+      <c r="C72" s="77" t="s">
+        <v>658</v>
       </c>
       <c r="D72" s="75" t="s">
         <v>648</v>
       </c>
-      <c r="E72" s="79" t="s">
-        <v>8</v>
+      <c r="E72" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F72" s="77" t="s">
         <v>602</v>
       </c>
-      <c r="G72" s="77" t="s">
-        <v>657</v>
+      <c r="G72" s="75" t="s">
+        <v>31</v>
       </c>
       <c r="H72" s="75" t="s">
         <v>350</v>
@@ -5840,19 +5852,19 @@
     </row>
     <row r="73" spans="1:13" s="74" customFormat="1">
       <c r="A73" s="74">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="B73" s="75" t="s">
         <v>650</v>
       </c>
-      <c r="C73" s="74">
-        <v>277</v>
+      <c r="C73" s="77" t="s">
+        <v>659</v>
       </c>
       <c r="D73" s="75" t="s">
         <v>651</v>
       </c>
-      <c r="E73" s="79" t="s">
-        <v>8</v>
+      <c r="E73" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F73" s="77" t="s">
         <v>602</v>
@@ -5869,7 +5881,7 @@
     </row>
     <row r="74" spans="1:13" s="84" customFormat="1">
       <c r="A74" s="84">
-        <v>32</v>
+        <v>73</v>
       </c>
       <c r="B74" s="79" t="s">
         <v>653</v>
@@ -5880,8 +5892,8 @@
       <c r="D74" s="79" t="s">
         <v>654</v>
       </c>
-      <c r="E74" s="79" t="s">
-        <v>8</v>
+      <c r="E74" s="55" t="s">
+        <v>9</v>
       </c>
       <c r="F74" s="77" t="s">
         <v>602</v>
@@ -5907,12 +5919,40 @@
       <c r="M74" s="79" t="s">
         <v>656</v>
       </c>
+    </row>
+    <row r="75" spans="1:13" s="74" customFormat="1">
+      <c r="A75" s="74">
+        <v>74</v>
+      </c>
+      <c r="B75" s="75" t="s">
+        <v>657</v>
+      </c>
+      <c r="C75" s="74">
+        <v>280</v>
+      </c>
+      <c r="D75" s="75" t="s">
+        <v>657</v>
+      </c>
+      <c r="E75" s="75" t="s">
+        <v>8</v>
+      </c>
+      <c r="F75" s="77" t="s">
+        <v>602</v>
+      </c>
+      <c r="G75" s="75" t="s">
+        <v>31</v>
+      </c>
+      <c r="H75" s="75"/>
+      <c r="I75" s="75"/>
+      <c r="J75" s="75"/>
+      <c r="K75" s="75"/>
+      <c r="L75" s="75"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B53:B54">
     <cfRule type="duplicateValues" dxfId="54" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B75:B1048576 B1:B31 B33:B49">
+  <conditionalFormatting sqref="B76:B1048576 B1:B31 B33:B49">
     <cfRule type="duplicateValues" dxfId="53" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
@@ -13775,9 +13815,11 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -15051,6 +15093,38 @@
         <v>373</v>
       </c>
     </row>
+    <row r="41" spans="1:10" s="35" customFormat="1">
+      <c r="A41" s="35">
+        <v>74</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>657</v>
+      </c>
+      <c r="C41" s="35">
+        <v>1</v>
+      </c>
+      <c r="D41" s="35" t="s">
+        <v>499</v>
+      </c>
+      <c r="E41" s="78" t="s">
+        <v>660</v>
+      </c>
+      <c r="F41" s="35" t="s">
+        <v>469</v>
+      </c>
+      <c r="G41" s="35" t="s">
+        <v>661</v>
+      </c>
+      <c r="H41" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="I41" s="35">
+        <v>1</v>
+      </c>
+      <c r="J41" s="35">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B27:B29">
@@ -15062,17 +15136,17 @@
   <conditionalFormatting sqref="A30">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G37 H2:H30 G40">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F41">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D41:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D30 D42:D1048576">
       <formula1>$K$2:$K$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37 H40">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H31:H37 H40:H41">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G38">
@@ -15080,6 +15154,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G39">
       <formula1>"Add_To_Cart,Add_To_Wishlist,Get_SKU_Code,Add_To_Compare"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G41">
+      <formula1>"Add_To_Cart,Add_To_Wishlist,Validate_Out_Of_Stock"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18799,12 +18876,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18957,27 +19034,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19002,9 +19070,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixing error on main
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="26" activeTab="29"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2723" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="650">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2094,6 +2094,15 @@
   </si>
   <si>
     <t>Xpath@123</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Different delivery options to display on checkout</t>
+  </si>
+  <si>
+    <t>verifyDeliveryOption</t>
   </si>
 </sst>
 </file>
@@ -2302,7 +2311,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="148">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2653,6 +2662,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2661,7 +2671,37 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="85">
+  <dxfs count="88">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3812,13 +3852,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA72"/>
+  <dimension ref="A1:AA74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E59" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
+      <selection pane="bottomRight" activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6479,8 +6519,8 @@
       <c r="E72" s="144" t="s">
         <v>199</v>
       </c>
-      <c r="F72" s="144" t="s">
-        <v>8</v>
+      <c r="F72" s="127" t="s">
+        <v>9</v>
       </c>
       <c r="G72" s="144" t="s">
         <v>643</v>
@@ -6512,28 +6552,83 @@
       <c r="Z72" s="144"/>
       <c r="AA72" s="144"/>
     </row>
+    <row r="73" spans="1:27">
+      <c r="A73" s="62">
+        <v>72</v>
+      </c>
+      <c r="B73" s="67" t="s">
+        <v>647</v>
+      </c>
+      <c r="C73" s="62">
+        <v>328</v>
+      </c>
+      <c r="D73" s="67" t="s">
+        <v>647</v>
+      </c>
+      <c r="E73" s="68" t="s">
+        <v>507</v>
+      </c>
+      <c r="F73" s="127" t="s">
+        <v>9</v>
+      </c>
+      <c r="G73" s="58" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27">
+      <c r="A74" s="134">
+        <v>73</v>
+      </c>
+      <c r="B74" s="134" t="s">
+        <v>648</v>
+      </c>
+      <c r="C74" s="134">
+        <v>345</v>
+      </c>
+      <c r="D74" s="134" t="s">
+        <v>648</v>
+      </c>
+      <c r="E74" s="144" t="s">
+        <v>199</v>
+      </c>
+      <c r="F74" s="134" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="148" t="s">
+        <v>31</v>
+      </c>
+      <c r="H74" s="134" t="s">
+        <v>649</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:Q72"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="84" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="83" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="82" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="81" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="80" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="79" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="20"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B49 B1:B31 B55:B1048576">
-    <cfRule type="duplicateValues" dxfId="78" priority="73"/>
+  <conditionalFormatting sqref="B33:B49 B1:B31 B55:B72 B75:B1048576">
+    <cfRule type="duplicateValues" dxfId="81" priority="75"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74">
+    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D74">
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
@@ -6900,10 +6995,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="58" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="57" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -7027,10 +7122,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="56" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -7283,10 +7378,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
@@ -7378,10 +7473,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7435,10 +7530,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="50" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8168,22 +8263,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="48" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="47" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="46" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="44" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="43" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
@@ -8846,22 +8941,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="42" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="41" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="38" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="37" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
@@ -9321,10 +9416,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="36" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="35" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -9599,10 +9694,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="77" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="76" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10050,7 +10145,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10283,7 +10378,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11194,16 +11289,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="32" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="31" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="30" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -11375,16 +11470,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="27" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12021,7 +12116,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -12251,7 +12346,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12895,19 +12990,19 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13209,10 +13304,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="74" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -13225,13 +13320,13 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13986,15 +14081,50 @@
         <v>576</v>
       </c>
     </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="134">
+        <v>73</v>
+      </c>
+      <c r="B24" s="134" t="s">
+        <v>648</v>
+      </c>
+      <c r="C24" s="126" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="119" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="126" t="s">
+        <v>602</v>
+      </c>
+      <c r="F24" s="126" t="s">
+        <v>411</v>
+      </c>
+      <c r="G24" s="126" t="s">
+        <v>408</v>
+      </c>
+      <c r="H24" s="126" t="s">
+        <v>87</v>
+      </c>
+      <c r="I24" s="126" t="s">
+        <v>315</v>
+      </c>
+      <c r="J24" s="126" t="s">
+        <v>577</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A13">
     <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A13">
+  <conditionalFormatting sqref="B24">
     <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -14018,13 +14148,13 @@
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D23</xm:sqref>
+          <xm:sqref>D2:D24</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>D24:D1048576</xm:sqref>
+          <xm:sqref>D25:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -15208,10 +15338,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="73" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -18336,22 +18466,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="71" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="70" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="69" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="68" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -18658,7 +18788,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18718,10 +18848,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="64" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="63" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18878,10 +19008,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="62" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="61" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -19006,10 +19136,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="60" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="59" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -19176,21 +19306,21 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19213,14 +19343,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -19235,4 +19357,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
latest XL sheet included
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4044,10 +4044,10 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4147,7 +4147,7 @@
         <v>501</v>
       </c>
       <c r="F2" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="126" t="s">
         <v>108</v>
@@ -4187,7 +4187,7 @@
         <v>501</v>
       </c>
       <c r="F3" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="126" t="s">
         <v>108</v>
@@ -4228,7 +4228,7 @@
         <v>501</v>
       </c>
       <c r="F4" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="126" t="s">
         <v>108</v>
@@ -4267,7 +4267,7 @@
         <v>501</v>
       </c>
       <c r="F5" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="126" t="s">
         <v>108</v>
@@ -4308,7 +4308,7 @@
         <v>501</v>
       </c>
       <c r="F6" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="126" t="s">
         <v>108</v>
@@ -4349,7 +4349,7 @@
         <v>136</v>
       </c>
       <c r="F7" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="126" t="s">
         <v>86</v>
@@ -4388,7 +4388,7 @@
         <v>501</v>
       </c>
       <c r="F8" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="126" t="s">
         <v>86</v>
@@ -4427,7 +4427,7 @@
         <v>501</v>
       </c>
       <c r="F9" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="126" t="s">
         <v>86</v>
@@ -4464,7 +4464,7 @@
         <v>196</v>
       </c>
       <c r="F10" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="126" t="s">
         <v>86</v>
@@ -4503,7 +4503,7 @@
         <v>196</v>
       </c>
       <c r="F11" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="126" t="s">
         <v>86</v>
@@ -4542,7 +4542,7 @@
         <v>196</v>
       </c>
       <c r="F12" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="126" t="s">
         <v>86</v>
@@ -4581,7 +4581,7 @@
         <v>196</v>
       </c>
       <c r="F13" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="126" t="s">
         <v>86</v>
@@ -4620,7 +4620,7 @@
         <v>196</v>
       </c>
       <c r="F14" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="126" t="s">
         <v>86</v>
@@ -4659,7 +4659,7 @@
         <v>196</v>
       </c>
       <c r="F15" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="126" t="s">
         <v>86</v>
@@ -4698,7 +4698,7 @@
         <v>196</v>
       </c>
       <c r="F16" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="126" t="s">
         <v>154</v>
@@ -4741,7 +4741,7 @@
         <v>196</v>
       </c>
       <c r="F17" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="126" t="s">
         <v>154</v>
@@ -4784,7 +4784,7 @@
         <v>196</v>
       </c>
       <c r="F18" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="126" t="s">
         <v>154</v>
@@ -4827,7 +4827,7 @@
         <v>196</v>
       </c>
       <c r="F19" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="126" t="s">
         <v>154</v>
@@ -4870,7 +4870,7 @@
         <v>196</v>
       </c>
       <c r="F20" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="126" t="s">
         <v>154</v>
@@ -4913,7 +4913,7 @@
         <v>196</v>
       </c>
       <c r="F21" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="126" t="s">
         <v>154</v>
@@ -4954,7 +4954,7 @@
       </c>
       <c r="E22" s="124"/>
       <c r="F22" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="126" t="s">
         <v>108</v>
@@ -4984,7 +4984,7 @@
       </c>
       <c r="E23" s="124"/>
       <c r="F23" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="126" t="s">
         <v>108</v>
@@ -5014,7 +5014,7 @@
       </c>
       <c r="E24" s="124"/>
       <c r="F24" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="126" t="s">
         <v>108</v>
@@ -5044,7 +5044,7 @@
       </c>
       <c r="E25" s="124"/>
       <c r="F25" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" s="126" t="s">
         <v>108</v>
@@ -5074,7 +5074,7 @@
       </c>
       <c r="E26" s="124"/>
       <c r="F26" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="126" t="s">
         <v>108</v>
@@ -5104,7 +5104,7 @@
       </c>
       <c r="E27" s="124"/>
       <c r="F27" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G27" s="126" t="s">
         <v>31</v>
@@ -5150,7 +5150,7 @@
       </c>
       <c r="E28" s="125"/>
       <c r="F28" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G28" s="126" t="s">
         <v>31</v>
@@ -5196,7 +5196,7 @@
       </c>
       <c r="E29" s="125"/>
       <c r="F29" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G29" s="126" t="s">
         <v>31</v>
@@ -5242,7 +5242,7 @@
       </c>
       <c r="E30" s="125"/>
       <c r="F30" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G30" s="126" t="s">
         <v>31</v>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="E31" s="125"/>
       <c r="F31" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G31" s="126" t="s">
         <v>31</v>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="E32" s="125"/>
       <c r="F32" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G32" s="126" t="s">
         <v>31</v>
@@ -5385,7 +5385,7 @@
         <v>196</v>
       </c>
       <c r="F33" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G33" s="127" t="s">
         <v>155</v>
@@ -5431,7 +5431,7 @@
         <v>196</v>
       </c>
       <c r="F34" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G34" s="127" t="s">
         <v>154</v>
@@ -5480,7 +5480,7 @@
         <v>196</v>
       </c>
       <c r="F35" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G35" s="127" t="s">
         <v>155</v>
@@ -5524,7 +5524,7 @@
         <v>196</v>
       </c>
       <c r="F36" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="126" t="s">
         <v>31</v>
@@ -5564,7 +5564,7 @@
         <v>196</v>
       </c>
       <c r="F37" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G37" s="127" t="s">
         <v>154</v>
@@ -5606,7 +5606,7 @@
         <v>196</v>
       </c>
       <c r="F38" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G38" s="129" t="s">
         <v>86</v>
@@ -5640,7 +5640,7 @@
         <v>196</v>
       </c>
       <c r="F39" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G39" s="129" t="s">
         <v>86</v>
@@ -5670,7 +5670,7 @@
       </c>
       <c r="E40" s="125"/>
       <c r="F40" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G40" s="129" t="s">
         <v>154</v>
@@ -5725,7 +5725,7 @@
       </c>
       <c r="E41" s="125"/>
       <c r="F41" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G41" s="129" t="s">
         <v>154</v>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="E42" s="125"/>
       <c r="F42" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G42" s="129" t="s">
         <v>154</v>
@@ -5866,7 +5866,7 @@
       </c>
       <c r="E44" s="125"/>
       <c r="F44" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G44" s="130" t="s">
         <v>288</v>
@@ -5897,7 +5897,7 @@
         <v>196</v>
       </c>
       <c r="F45" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G45" s="130" t="s">
         <v>289</v>
@@ -5928,7 +5928,7 @@
         <v>196</v>
       </c>
       <c r="F46" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" s="133" t="s">
         <v>290</v>
@@ -5959,7 +5959,7 @@
         <v>196</v>
       </c>
       <c r="F47" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G47" s="129" t="s">
         <v>154</v>
@@ -6004,7 +6004,7 @@
         <v>136</v>
       </c>
       <c r="F48" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G48" s="129" t="s">
         <v>154</v>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="E49" s="125"/>
       <c r="F49" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G49" s="129" t="s">
         <v>296</v>
@@ -6066,7 +6066,7 @@
         <v>501</v>
       </c>
       <c r="F50" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G50" s="58" t="s">
         <v>297</v>
@@ -6090,7 +6090,7 @@
         <v>501</v>
       </c>
       <c r="F51" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G51" s="58" t="s">
         <v>297</v>
@@ -6114,7 +6114,7 @@
         <v>501</v>
       </c>
       <c r="F52" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" s="58" t="s">
         <v>297</v>
@@ -6136,7 +6136,7 @@
         <v>136</v>
       </c>
       <c r="F53" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G53" s="129" t="s">
         <v>407</v>
@@ -6163,7 +6163,7 @@
         <v>136</v>
       </c>
       <c r="F54" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G54" s="129" t="s">
         <v>407</v>
@@ -6191,7 +6191,7 @@
       </c>
       <c r="E55" s="57"/>
       <c r="F55" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G55" s="58" t="s">
         <v>407</v>
@@ -6227,7 +6227,7 @@
       </c>
       <c r="E56" s="57"/>
       <c r="F56" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G56" s="58" t="s">
         <v>407</v>
@@ -6260,7 +6260,7 @@
       </c>
       <c r="E57" s="57"/>
       <c r="F57" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G57" s="58" t="s">
         <v>407</v>
@@ -6299,7 +6299,7 @@
         <v>501</v>
       </c>
       <c r="F58" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G58" s="58" t="s">
         <v>154</v>
@@ -6332,7 +6332,7 @@
         <v>501</v>
       </c>
       <c r="F59" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G59" s="58" t="s">
         <v>576</v>
@@ -6365,7 +6365,7 @@
         <v>501</v>
       </c>
       <c r="F60" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G60" s="58" t="s">
         <v>576</v>
@@ -6398,7 +6398,7 @@
         <v>501</v>
       </c>
       <c r="F61" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G61" s="58" t="s">
         <v>31</v>
@@ -6429,7 +6429,7 @@
         <v>501</v>
       </c>
       <c r="F62" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G62" s="58" t="s">
         <v>31</v>
@@ -6462,7 +6462,7 @@
         <v>196</v>
       </c>
       <c r="F63" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G63" s="58" t="s">
         <v>580</v>
@@ -6493,7 +6493,7 @@
         <v>196</v>
       </c>
       <c r="F64" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G64" s="58" t="s">
         <v>580</v>
@@ -6524,7 +6524,7 @@
         <v>196</v>
       </c>
       <c r="F65" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G65" s="58" t="s">
         <v>581</v>
@@ -6552,7 +6552,7 @@
         <v>196</v>
       </c>
       <c r="F66" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G66" s="57" t="s">
         <v>582</v>
@@ -6580,7 +6580,7 @@
         <v>196</v>
       </c>
       <c r="F67" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G67" s="66" t="s">
         <v>583</v>
@@ -6608,7 +6608,7 @@
         <v>196</v>
       </c>
       <c r="F68" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G68" s="57" t="s">
         <v>583</v>
@@ -6638,7 +6638,7 @@
         <v>196</v>
       </c>
       <c r="F69" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G69" s="58" t="s">
         <v>31</v>
@@ -6664,7 +6664,7 @@
       </c>
       <c r="E70" s="57"/>
       <c r="F70" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G70" s="58" t="s">
         <v>31</v>
@@ -6694,7 +6694,7 @@
         <v>586</v>
       </c>
       <c r="F71" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G71" s="58" t="s">
         <v>407</v>
@@ -19276,15 +19276,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19433,6 +19424,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -19442,23 +19442,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19475,4 +19458,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TCID - 51, 57 Code Updates
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4E936-C1E8-43C0-99F9-F49264C50037}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -67,12 +68,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1D00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -89,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1D00-000002000000}">
       <text>
         <r>
           <rPr>
@@ -111,12 +112,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2A00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -2226,7 +2227,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2322,7 +2323,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2389,6 +2390,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -2434,7 +2459,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2799,12 +2824,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -2812,13 +2831,31 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="4"/>
-    <cellStyle name="Normal 3" xfId="3"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="92">
     <dxf>
@@ -3797,7 +3834,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3830,9 +3867,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3865,6 +3919,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4040,35 +4111,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="11" style="61" customWidth="1"/>
-    <col min="2" max="2" width="93.5703125" style="131" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7109375" style="131" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="131" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" style="131" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" style="131" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="131" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.7109375" style="131" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27.140625" style="131" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="31.42578125" style="131" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.140625" style="131" customWidth="1"/>
-    <col min="18" max="18" width="20.140625" style="131" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="131"/>
+    <col min="2" max="2" width="93.54296875" style="131" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7265625" style="131" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="131" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" style="131" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.7265625" style="131" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.54296875" style="131" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.453125" style="131" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7265625" style="131" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.453125" style="131" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.453125" style="131" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27.1796875" style="131" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="31.453125" style="131" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.1796875" style="131" customWidth="1"/>
+    <col min="18" max="18" width="20.1796875" style="131" customWidth="1"/>
+    <col min="19" max="16384" width="9.1796875" style="131"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4130,7 +4201,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30">
+    <row r="2" spans="1:19" ht="29">
       <c r="A2" s="137">
         <v>1</v>
       </c>
@@ -4170,7 +4241,7 @@
       <c r="O2" s="124"/>
       <c r="P2" s="124"/>
     </row>
-    <row r="3" spans="1:19" ht="30">
+    <row r="3" spans="1:19" ht="29">
       <c r="A3" s="137">
         <v>2</v>
       </c>
@@ -4211,7 +4282,7 @@
       <c r="P3" s="124"/>
       <c r="Q3" s="124"/>
     </row>
-    <row r="4" spans="1:19" ht="30">
+    <row r="4" spans="1:19" ht="29">
       <c r="A4" s="137">
         <v>3</v>
       </c>
@@ -4250,7 +4321,7 @@
       <c r="P4" s="124"/>
       <c r="Q4" s="124"/>
     </row>
-    <row r="5" spans="1:19" ht="30">
+    <row r="5" spans="1:19" ht="29">
       <c r="A5" s="137">
         <v>4</v>
       </c>
@@ -4291,7 +4362,7 @@
       <c r="P5" s="124"/>
       <c r="Q5" s="124"/>
     </row>
-    <row r="6" spans="1:19" ht="30">
+    <row r="6" spans="1:19" ht="29">
       <c r="A6" s="137">
         <v>5</v>
       </c>
@@ -4332,7 +4403,7 @@
       <c r="P6" s="124"/>
       <c r="Q6" s="124"/>
     </row>
-    <row r="7" spans="1:19" ht="30">
+    <row r="7" spans="1:19" ht="29">
       <c r="A7" s="137">
         <v>6</v>
       </c>
@@ -4371,7 +4442,7 @@
       <c r="P7" s="124"/>
       <c r="Q7" s="124"/>
     </row>
-    <row r="8" spans="1:19" ht="30">
+    <row r="8" spans="1:19" ht="29">
       <c r="A8" s="137">
         <v>7</v>
       </c>
@@ -4410,7 +4481,7 @@
       <c r="P8" s="124"/>
       <c r="Q8" s="124"/>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="29">
       <c r="A9" s="137">
         <v>8</v>
       </c>
@@ -4447,7 +4518,7 @@
       <c r="P9" s="124"/>
       <c r="Q9" s="124"/>
     </row>
-    <row r="10" spans="1:19" ht="30">
+    <row r="10" spans="1:19" ht="29">
       <c r="A10" s="137">
         <v>9</v>
       </c>
@@ -4486,7 +4557,7 @@
       <c r="P10" s="124"/>
       <c r="Q10" s="124"/>
     </row>
-    <row r="11" spans="1:19" ht="30">
+    <row r="11" spans="1:19" ht="29">
       <c r="A11" s="137">
         <v>10</v>
       </c>
@@ -4525,7 +4596,7 @@
       <c r="P11" s="124"/>
       <c r="Q11" s="124"/>
     </row>
-    <row r="12" spans="1:19" ht="30">
+    <row r="12" spans="1:19" ht="29">
       <c r="A12" s="137">
         <v>11</v>
       </c>
@@ -4564,7 +4635,7 @@
       <c r="P12" s="124"/>
       <c r="Q12" s="124"/>
     </row>
-    <row r="13" spans="1:19" ht="30">
+    <row r="13" spans="1:19" ht="29">
       <c r="A13" s="137">
         <v>12</v>
       </c>
@@ -4603,7 +4674,7 @@
       <c r="P13" s="124"/>
       <c r="Q13" s="124"/>
     </row>
-    <row r="14" spans="1:19" ht="30">
+    <row r="14" spans="1:19" ht="29">
       <c r="A14" s="140">
         <v>13</v>
       </c>
@@ -4642,7 +4713,7 @@
       <c r="P14" s="124"/>
       <c r="Q14" s="124"/>
     </row>
-    <row r="15" spans="1:19" ht="30">
+    <row r="15" spans="1:19" ht="29">
       <c r="A15" s="137">
         <v>14</v>
       </c>
@@ -4681,7 +4752,7 @@
       <c r="P15" s="124"/>
       <c r="Q15" s="124"/>
     </row>
-    <row r="16" spans="1:19" ht="30">
+    <row r="16" spans="1:19" ht="29">
       <c r="A16" s="149">
         <v>15</v>
       </c>
@@ -4724,7 +4795,7 @@
       <c r="P16" s="124"/>
       <c r="Q16" s="124"/>
     </row>
-    <row r="17" spans="1:17" ht="30">
+    <row r="17" spans="1:17" ht="29">
       <c r="A17" s="149">
         <v>16</v>
       </c>
@@ -4767,7 +4838,7 @@
       <c r="P17" s="124"/>
       <c r="Q17" s="124"/>
     </row>
-    <row r="18" spans="1:17" ht="30">
+    <row r="18" spans="1:17" ht="29">
       <c r="A18" s="149">
         <v>17</v>
       </c>
@@ -4810,7 +4881,7 @@
       <c r="P18" s="124"/>
       <c r="Q18" s="124"/>
     </row>
-    <row r="19" spans="1:17" ht="30">
+    <row r="19" spans="1:17" ht="29">
       <c r="A19" s="149">
         <v>18</v>
       </c>
@@ -4853,7 +4924,7 @@
       <c r="P19" s="124"/>
       <c r="Q19" s="124"/>
     </row>
-    <row r="20" spans="1:17" ht="30">
+    <row r="20" spans="1:17" ht="29">
       <c r="A20" s="149">
         <v>19</v>
       </c>
@@ -4896,7 +4967,7 @@
       <c r="P20" s="124"/>
       <c r="Q20" s="124"/>
     </row>
-    <row r="21" spans="1:17" ht="30">
+    <row r="21" spans="1:17" ht="29">
       <c r="A21" s="149">
         <v>20</v>
       </c>
@@ -5837,7 +5908,7 @@
         <v>196</v>
       </c>
       <c r="F43" s="124" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G43" s="130" t="s">
         <v>287</v>
@@ -5914,7 +5985,7 @@
       <c r="Q45" s="130"/>
     </row>
     <row r="46" spans="1:19">
-      <c r="A46" s="152">
+      <c r="A46" s="150">
         <v>45</v>
       </c>
       <c r="B46" s="133" t="s">
@@ -5945,7 +6016,7 @@
       <c r="Q46" s="130"/>
     </row>
     <row r="47" spans="1:19">
-      <c r="A47" s="153">
+      <c r="A47" s="151">
         <v>46</v>
       </c>
       <c r="B47" s="131" t="s">
@@ -5990,7 +6061,7 @@
       </c>
     </row>
     <row r="48" spans="1:19">
-      <c r="A48" s="153">
+      <c r="A48" s="151">
         <v>47</v>
       </c>
       <c r="B48" s="134" t="s">
@@ -6098,7 +6169,7 @@
       <c r="H51" s="123"/>
     </row>
     <row r="52" spans="1:16" s="57" customFormat="1">
-      <c r="A52" s="64">
+      <c r="A52" s="156">
         <v>51</v>
       </c>
       <c r="B52" s="123" t="s">
@@ -6114,7 +6185,7 @@
         <v>501</v>
       </c>
       <c r="F52" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G52" s="58" t="s">
         <v>297</v>
@@ -6122,7 +6193,7 @@
       <c r="H52" s="123"/>
     </row>
     <row r="53" spans="1:16" s="130" customFormat="1">
-      <c r="A53" s="63">
+      <c r="A53" s="157">
         <v>52</v>
       </c>
       <c r="B53" s="130" t="s">
@@ -6149,7 +6220,7 @@
       </c>
     </row>
     <row r="54" spans="1:16" s="130" customFormat="1">
-      <c r="A54" s="63">
+      <c r="A54" s="154">
         <v>53</v>
       </c>
       <c r="B54" s="130" t="s">
@@ -6179,7 +6250,7 @@
       </c>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="67">
+      <c r="A55" s="155">
         <v>54</v>
       </c>
       <c r="B55" s="65" t="s">
@@ -6215,7 +6286,7 @@
       <c r="P55" s="124"/>
     </row>
     <row r="56" spans="1:16">
-      <c r="A56" s="67">
+      <c r="A56" s="155">
         <v>55</v>
       </c>
       <c r="B56" s="65" t="s">
@@ -6248,7 +6319,7 @@
       <c r="O56" s="57"/>
     </row>
     <row r="57" spans="1:16">
-      <c r="A57" s="67">
+      <c r="A57" s="155">
         <v>56</v>
       </c>
       <c r="B57" s="65" t="s">
@@ -6283,7 +6354,7 @@
       <c r="O57" s="57"/>
     </row>
     <row r="58" spans="1:16">
-      <c r="A58" s="67">
+      <c r="A58" s="158">
         <v>57</v>
       </c>
       <c r="B58" s="65" t="s">
@@ -6316,7 +6387,7 @@
       <c r="O58" s="57"/>
     </row>
     <row r="59" spans="1:16">
-      <c r="A59" s="67">
+      <c r="A59" s="158">
         <v>58</v>
       </c>
       <c r="B59" s="65" t="s">
@@ -6349,7 +6420,7 @@
       <c r="O59" s="57"/>
     </row>
     <row r="60" spans="1:16">
-      <c r="A60" s="67">
+      <c r="A60" s="158">
         <v>59</v>
       </c>
       <c r="B60" s="65" t="s">
@@ -6382,7 +6453,7 @@
       <c r="O60" s="57"/>
     </row>
     <row r="61" spans="1:16">
-      <c r="A61" s="151">
+      <c r="A61" s="158">
         <v>60</v>
       </c>
       <c r="B61" s="65" t="s">
@@ -6415,7 +6486,7 @@
       <c r="O61" s="57"/>
     </row>
     <row r="62" spans="1:16">
-      <c r="A62" s="151">
+      <c r="A62" s="158">
         <v>61</v>
       </c>
       <c r="B62" s="65" t="s">
@@ -6446,7 +6517,7 @@
       <c r="O62" s="57"/>
     </row>
     <row r="63" spans="1:16">
-      <c r="A63" s="67">
+      <c r="A63" s="158">
         <v>62</v>
       </c>
       <c r="B63" s="70" t="s">
@@ -6477,10 +6548,10 @@
       <c r="O63" s="57"/>
     </row>
     <row r="64" spans="1:16">
-      <c r="A64" s="67">
+      <c r="A64" s="158">
         <v>63</v>
       </c>
-      <c r="B64" s="154" t="s">
+      <c r="B64" s="152" t="s">
         <v>692</v>
       </c>
       <c r="C64" s="67">
@@ -6508,7 +6579,7 @@
       <c r="O64" s="57"/>
     </row>
     <row r="65" spans="1:12">
-      <c r="A65" s="67">
+      <c r="A65" s="158">
         <v>64</v>
       </c>
       <c r="B65" s="71" t="s">
@@ -6536,7 +6607,7 @@
       <c r="L65" s="57"/>
     </row>
     <row r="66" spans="1:12">
-      <c r="A66" s="67">
+      <c r="A66" s="158">
         <v>65</v>
       </c>
       <c r="B66" s="65" t="s">
@@ -6564,7 +6635,7 @@
       <c r="L66" s="57"/>
     </row>
     <row r="67" spans="1:12">
-      <c r="A67" s="150">
+      <c r="A67" s="158">
         <v>66</v>
       </c>
       <c r="B67" s="65" t="s">
@@ -6592,7 +6663,7 @@
       <c r="L67" s="57"/>
     </row>
     <row r="68" spans="1:12">
-      <c r="A68" s="150">
+      <c r="A68" s="155">
         <v>67</v>
       </c>
       <c r="B68" s="65" t="s">
@@ -6622,7 +6693,7 @@
       <c r="L68" s="57"/>
     </row>
     <row r="69" spans="1:12">
-      <c r="A69" s="150">
+      <c r="A69" s="155">
         <v>68</v>
       </c>
       <c r="B69" s="65" t="s">
@@ -6650,7 +6721,7 @@
       <c r="L69" s="57"/>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="151">
+      <c r="A70" s="155">
         <v>69</v>
       </c>
       <c r="B70" s="65" t="s">
@@ -6678,7 +6749,7 @@
       <c r="L70" s="57"/>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="64">
+      <c r="A71" s="153">
         <v>70</v>
       </c>
       <c r="B71" s="65" t="s">
@@ -6747,239 +6818,239 @@
     <cfRule type="duplicateValues" dxfId="82" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
-    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
-    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
-    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
-    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
-    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
-    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
-    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
-    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
-    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="M40" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="H54" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
-    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
-    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact"/>
-    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
-    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
-    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
-    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
-    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
-    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
-    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
-    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="K2" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
-    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="J3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="J4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="J5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
-    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
-    <hyperlink ref="I2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
-    <hyperlink ref="I3:I6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
-    <hyperlink ref="J55" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
-    <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
-    <hyperlink ref="H59" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
-    <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart"/>
-    <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="J71" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="G71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="K71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
-    <hyperlink ref="L71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
-    <hyperlink ref="G56:G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
-    <hyperlink ref="H56:H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
-    <hyperlink ref="I56:I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
-    <hyperlink ref="G63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
-    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
-    <hyperlink ref="G70" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++"/>
-    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch"/>
-    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++"/>
-    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
-    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
-    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
-    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento"/>
-    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="N42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
-    <hyperlink ref="O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
-    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="Q40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="Q42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
-    <hyperlink ref="R40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
-    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="S40" location="'SapCustomer++'!A1" display="SapCustomer"/>
-    <hyperlink ref="S42" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="O31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="M40" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="H54" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="K2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="J3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="J4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="J5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="I2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="I3:I6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="J55" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="I55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
+    <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
+    <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-0000B7000000}"/>
+    <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
+    <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
+    <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
+    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-0000BB000000}"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
+    <hyperlink ref="H59" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000BD000000}"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
+    <hyperlink ref="H60" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000BF000000}"/>
+    <hyperlink ref="G59:G60" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0000-0000C0000000}"/>
+    <hyperlink ref="G61" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C1000000}"/>
+    <hyperlink ref="G62" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C2000000}"/>
+    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
+    <hyperlink ref="J71" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
+    <hyperlink ref="G71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
+    <hyperlink ref="H71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
+    <hyperlink ref="I71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
+    <hyperlink ref="K71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
+    <hyperlink ref="L71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
+    <hyperlink ref="G56:G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
+    <hyperlink ref="H56:H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-0000CB000000}"/>
+    <hyperlink ref="I56:I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
+    <hyperlink ref="G63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
+    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
+    <hyperlink ref="G70" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
+    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
+    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
+    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
+    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
+    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
+    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
+    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
+    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
+    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
+    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
+    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
+    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
+    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
+    <hyperlink ref="N40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
+    <hyperlink ref="N42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
+    <hyperlink ref="O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
+    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
+    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
+    <hyperlink ref="Q40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
+    <hyperlink ref="Q42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
+    <hyperlink ref="R40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
+    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
+    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
+    <hyperlink ref="S40" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
+    <hyperlink ref="S42" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6987,28 +7058,28 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.26953125" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="36"/>
+    <col min="10" max="10" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -7124,7 +7195,7 @@
     <cfRule type="duplicateValues" dxfId="61" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7132,7 +7203,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
           <x14:formula1>
             <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
           </x14:formula1>
@@ -7145,24 +7216,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.54296875" style="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="36"/>
+    <col min="8" max="8" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -7251,7 +7322,7 @@
     <cfRule type="duplicateValues" dxfId="59" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7261,38 +7332,38 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.453125" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1796875" style="36" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="36"/>
-    <col min="15" max="15" width="23.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="36"/>
+    <col min="14" max="14" width="9.1796875" style="36"/>
+    <col min="15" max="15" width="23.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -7507,25 +7578,25 @@
     <cfRule type="duplicateValues" dxfId="57" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{00000000-0002-0000-0B00-000001000000}">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{00000000-0002-0000-0B00-000002000000}">
       <formula1>"African,Asian,Coloured,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{00000000-0002-0000-0B00-000003000000}">
       <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{00000000-0002-0000-0B00-000004000000}">
       <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{00000000-0002-0000-0B00-000005000000}">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{00000000-0002-0000-0B00-000006000000}">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7535,22 +7606,22 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="36"/>
+    <col min="4" max="4" width="20.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7606,15 +7677,15 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="35"/>
@@ -7661,25 +7732,25 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.1796875" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.453125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.1796875" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="29"/>
+    <col min="10" max="16384" width="9.1796875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -7752,7 +7823,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7763,42 +7834,42 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="11" customWidth="1"/>
-    <col min="14" max="14" width="20.28515625" style="11" customWidth="1"/>
-    <col min="15" max="15" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.81640625" style="11" customWidth="1"/>
+    <col min="14" max="14" width="20.26953125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="31.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.453125" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.26953125" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.140625" style="11" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.5703125" style="11" customWidth="1"/>
-    <col min="31" max="16384" width="8.7109375" style="11"/>
+    <col min="27" max="27" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.1796875" style="11" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.54296875" style="11" customWidth="1"/>
+    <col min="31" max="16384" width="8.7265625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30">
+    <row r="1" spans="1:28">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -8402,64 +8473,64 @@
     <cfRule type="duplicateValues" dxfId="47" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7" xr:uid="{00000000-0002-0000-0F00-000001000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D5" r:id="rId5" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
+    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
+    <hyperlink ref="D5" r:id="rId5" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.5703125" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.54296875" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.1796875" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.453125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.7265625" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.26953125" style="12" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.140625" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.7109375" style="12"/>
+    <col min="28" max="28" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7265625" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -9081,7 +9152,7 @@
     <cfRule type="duplicateValues" dxfId="41" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9090,7 +9161,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9101,14 +9172,14 @@
       <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7109375" style="1"/>
+    <col min="4" max="4" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9544,7 +9615,7 @@
     <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1100-000000000000}">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9553,22 +9624,22 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9722,19 +9793,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" style="82" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="82"/>
+    <col min="4" max="16384" width="9.1796875" style="82"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -9826,24 +9897,24 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.26953125" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.54296875" style="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="38" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="38"/>
+    <col min="11" max="16384" width="9.1796875" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="55" customFormat="1">
@@ -10273,19 +10344,19 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10503,7 +10574,7 @@
     <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1400-000000000000}">
       <formula1>"payUcreditcard,Cash_Deposits"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10512,33 +10583,33 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.81640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="29">
       <c r="A1" s="37" t="s">
         <v>34</v>
       </c>
@@ -10788,7 +10859,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1" ht="30">
+    <row r="6" spans="1:16" s="4" customFormat="1">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -10838,7 +10909,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="30">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="29">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -11379,14 +11450,14 @@
     <cfRule type="duplicateValues" dxfId="33" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1"/>
-    <hyperlink ref="O3" r:id="rId2"/>
-    <hyperlink ref="O4" r:id="rId3"/>
-    <hyperlink ref="O5" r:id="rId4"/>
-    <hyperlink ref="O8" r:id="rId5"/>
-    <hyperlink ref="O6" r:id="rId6"/>
-    <hyperlink ref="O7" r:id="rId7"/>
-    <hyperlink ref="O9" r:id="rId8"/>
+    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
+    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
+    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-1500-000002000000}"/>
+    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-1500-000003000000}"/>
+    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-1500-000004000000}"/>
+    <hyperlink ref="O6" r:id="rId6" xr:uid="{00000000-0004-0000-1500-000005000000}"/>
+    <hyperlink ref="O7" r:id="rId7" xr:uid="{00000000-0004-0000-1500-000006000000}"/>
+    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-1500-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
@@ -11394,18 +11465,18 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="21.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="29"/>
+    <col min="1" max="1" width="21.1796875" style="29"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" style="29"/>
+    <col min="3" max="3" width="21.1796875" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -11425,7 +11496,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30">
+    <row r="2" spans="1:5" ht="29">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -11436,7 +11507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30">
+    <row r="3" spans="1:5" ht="29">
       <c r="A3" s="45">
         <v>2</v>
       </c>
@@ -11447,7 +11518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30">
+    <row r="4" spans="1:5">
       <c r="A4" s="45">
         <v>3</v>
       </c>
@@ -11458,7 +11529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30">
+    <row r="5" spans="1:5" ht="29">
       <c r="A5" s="45">
         <v>4</v>
       </c>
@@ -11469,7 +11540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="29">
       <c r="A6" s="45">
         <v>5</v>
       </c>
@@ -11524,7 +11595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5">
       <c r="A11" s="45">
         <v>19</v>
       </c>
@@ -11564,27 +11635,27 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.54296875" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="4" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -11729,29 +11800,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="H2" r:id="rId2"/>
-    <hyperlink ref="J3" r:id="rId3"/>
-    <hyperlink ref="H3" r:id="rId4"/>
-    <hyperlink ref="J4" r:id="rId5"/>
-    <hyperlink ref="H4" r:id="rId6"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-1700-000001000000}"/>
+    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-1700-000002000000}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-1700-000003000000}"/>
+    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-1700-000004000000}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-1700-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="39.7265625" style="11" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11768,7 +11839,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="29">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -11782,7 +11853,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="29">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -11796,7 +11867,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="29">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -11810,7 +11881,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="29">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -11824,7 +11895,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="29">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -11838,7 +11909,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="29">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -11894,7 +11965,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:4" ht="29">
       <c r="A11" s="143">
         <v>40</v>
       </c>
@@ -11908,7 +11979,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="45">
+    <row r="12" spans="1:4" ht="29">
       <c r="A12" s="61">
         <v>41</v>
       </c>
@@ -11978,21 +12049,21 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -12240,19 +12311,19 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="38"/>
+    <col min="5" max="5" width="13.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12332,7 +12403,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30">
+    <row r="6" spans="1:5" ht="29">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -12467,7 +12538,7 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12478,14 +12549,14 @@
       <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13124,7 +13195,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13134,13 +13205,13 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.26953125" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="11"/>
+    <col min="4" max="4" width="7.7265625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13157,7 +13228,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30">
+    <row r="2" spans="1:4" ht="29">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -13169,7 +13240,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:4" ht="45">
+    <row r="3" spans="1:4" ht="43.5">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -13181,7 +13252,7 @@
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="45">
+    <row r="4" spans="1:4" ht="43.5">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -13193,7 +13264,7 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="30">
+    <row r="5" spans="1:4" ht="29">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -13205,7 +13276,7 @@
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="30">
+    <row r="6" spans="1:4" ht="29">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -13217,7 +13288,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" ht="30">
+    <row r="7" spans="1:4" ht="29">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -13289,20 +13360,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="77" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="77" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" style="77" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="77" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="77" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="77"/>
+    <col min="4" max="4" width="19.26953125" style="77" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="77"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13425,7 +13494,7 @@
     <cfRule type="duplicateValues" dxfId="78" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -13434,33 +13503,33 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="83" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="83" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="83" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="83" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="83" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.5703125" style="83" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="83" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="83" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="83" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="83" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" style="83" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="83" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="83"/>
+    <col min="4" max="4" width="20.7265625" style="83" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.54296875" style="83" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="83" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.81640625" style="83" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="83" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7265625" style="83" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" style="83" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.26953125" style="83" customWidth="1"/>
+    <col min="12" max="16384" width="9.1796875" style="83"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
+    <row r="1" spans="1:11">
       <c r="A1" s="79" t="s">
         <v>34</v>
       </c>
@@ -13559,7 +13628,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11" ht="29">
       <c r="A4" s="84">
         <v>28</v>
       </c>
@@ -14071,7 +14140,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30">
+    <row r="20" spans="1:10" ht="29">
       <c r="A20" s="86">
         <v>61</v>
       </c>
@@ -14211,13 +14280,13 @@
     <cfRule type="duplicateValues" dxfId="17" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G13" xr:uid="{00000000-0002-0000-1D00-000000000000}">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F13" xr:uid="{00000000-0002-0000-1D00-000001000000}">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J13" xr:uid="{00000000-0002-0000-1D00-000002000000}">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -14227,13 +14296,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1D00-000003000000}">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1D00-000004000000}">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -14246,20 +14315,20 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14309,16 +14378,16 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -14417,21 +14486,21 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="31"/>
+    <col min="4" max="4" width="18.54296875" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7265625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14492,21 +14561,21 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -14576,21 +14645,21 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="97" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="97" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="97" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="97" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="97" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" style="97" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="97"/>
+    <col min="5" max="5" width="23.1796875" style="97" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="97"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14841,11 +14910,11 @@
       <c r="C15" s="95">
         <v>1</v>
       </c>
-      <c r="D15" s="95" t="s">
-        <v>169</v>
+      <c r="D15" s="94" t="s">
+        <v>664</v>
       </c>
       <c r="E15" s="94" t="s">
-        <v>168</v>
+        <v>677</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -14894,40 +14963,41 @@
     <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Password@123"/>
-    <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E9" r:id="rId3"/>
-    <hyperlink ref="E12" r:id="rId4" display="Password@123"/>
-    <hyperlink ref="E14" r:id="rId5"/>
-    <hyperlink ref="E15" r:id="rId6"/>
-    <hyperlink ref="E16" r:id="rId7"/>
-    <hyperlink ref="E17" r:id="rId8"/>
-    <hyperlink ref="D12" r:id="rId9"/>
-    <hyperlink ref="D13" r:id="rId10"/>
-    <hyperlink ref="E13" r:id="rId11" display="Password@123"/>
-    <hyperlink ref="E3" r:id="rId12" display="Password@123"/>
-    <hyperlink ref="E4" r:id="rId13" display="Password@123"/>
-    <hyperlink ref="E5" r:id="rId14" display="Password@123"/>
-    <hyperlink ref="E6" r:id="rId15" display="Password@123"/>
-    <hyperlink ref="E7" r:id="rId16" display="Password@123"/>
-    <hyperlink ref="E10" r:id="rId17" display="Password@123"/>
-    <hyperlink ref="E11" r:id="rId18" display="Password@123"/>
+    <hyperlink ref="E2" r:id="rId1" display="Password@123" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-2200-000001000000}"/>
+    <hyperlink ref="E9" r:id="rId3" xr:uid="{00000000-0004-0000-2200-000002000000}"/>
+    <hyperlink ref="E12" r:id="rId4" display="Password@123" xr:uid="{00000000-0004-0000-2200-000003000000}"/>
+    <hyperlink ref="E14" r:id="rId5" xr:uid="{00000000-0004-0000-2200-000004000000}"/>
+    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-2200-000006000000}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{00000000-0004-0000-2200-000007000000}"/>
+    <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-2200-000008000000}"/>
+    <hyperlink ref="E13" r:id="rId9" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000A000000}"/>
+    <hyperlink ref="E3" r:id="rId10" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000B000000}"/>
+    <hyperlink ref="E4" r:id="rId11" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000C000000}"/>
+    <hyperlink ref="E5" r:id="rId12" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000D000000}"/>
+    <hyperlink ref="E6" r:id="rId13" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000E000000}"/>
+    <hyperlink ref="E7" r:id="rId14" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000F000000}"/>
+    <hyperlink ref="E10" r:id="rId15" display="Password@123" xr:uid="{00000000-0004-0000-2200-000010000000}"/>
+    <hyperlink ref="E11" r:id="rId16" display="Password@123" xr:uid="{00000000-0004-0000-2200-000011000000}"/>
+    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-2200-000009000000}"/>
+    <hyperlink ref="D15" r:id="rId18" xr:uid="{81428C68-028B-4893-9B4A-CD71D7D22D03}"/>
+    <hyperlink ref="E15" r:id="rId19" display="Password@123" xr:uid="{7AE80BCF-FE0D-40EE-8F1D-4CCBC9DED593}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId19"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15034,22 +15104,22 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -15123,28 +15193,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1"/>
-    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-2400-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15187,27 +15257,27 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -15288,30 +15358,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="74" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.81640625" style="74" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="74" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="74" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="74" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="74" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="74" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="74" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="74"/>
+    <col min="8" max="16384" width="9.1796875" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -15483,38 +15551,38 @@
     <cfRule type="duplicateValues" dxfId="76" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="E5" r:id="rId4"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -15604,7 +15672,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -15612,26 +15680,26 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -15710,19 +15778,19 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -15739,7 +15807,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.6" customHeight="1">
+    <row r="2" spans="1:4" ht="24.65" customHeight="1">
       <c r="A2" s="3">
         <v>9</v>
       </c>
@@ -15750,7 +15818,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="112" customFormat="1" ht="24.6" customHeight="1">
+    <row r="3" spans="1:4" s="112" customFormat="1" ht="24.65" customHeight="1">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -15767,31 +15835,31 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30">
+    <row r="1" spans="1:12" ht="29">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -15897,7 +15965,7 @@
       </c>
       <c r="L3" s="16"/>
     </row>
-    <row r="4" spans="1:12" ht="30">
+    <row r="4" spans="1:12">
       <c r="A4" s="16">
         <v>8</v>
       </c>
@@ -16236,17 +16304,17 @@
     <cfRule type="duplicateValues" dxfId="6" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-2A00-000000000000}">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576" xr:uid="{00000000-0002-0000-2A00-000001000000}">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -16255,7 +16323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -16265,28 +16333,28 @@
       <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="122" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="122" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="122" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="122" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="122" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" style="122" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.5703125" style="122" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="122" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" style="122" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" style="122" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="122" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" style="122" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.54296875" style="122" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.453125" style="122" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.54296875" style="122" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" style="122" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" style="122" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" style="122" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" style="122" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" style="122" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.140625" style="122" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.5703125" style="122" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="122" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.42578125" style="122" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.42578125" style="122" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.140625" style="122" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="122"/>
+    <col min="12" max="12" width="20.81640625" style="122" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" style="122" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.26953125" style="122" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.1796875" style="122" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.54296875" style="122" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7265625" style="122" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.453125" style="122" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.453125" style="122" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.1796875" style="122" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.1796875" style="122"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -16785,7 +16853,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="30">
+    <row r="9" spans="1:20">
       <c r="A9" s="116">
         <v>23</v>
       </c>
@@ -16847,7 +16915,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="30">
+    <row r="10" spans="1:20">
       <c r="A10" s="116">
         <v>24</v>
       </c>
@@ -17291,21 +17359,21 @@
     <cfRule type="duplicateValues" dxfId="0" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-2B00-000000000000}">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 P2:T11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 P2:T11" xr:uid="{00000000-0002-0000-2B00-000001000000}">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11" xr:uid="{00000000-0002-0000-2B00-000002000000}">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11" xr:uid="{00000000-0002-0000-2B00-000003000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1"/>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -17313,21 +17381,21 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -17417,19 +17485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -17621,21 +17689,21 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -17725,21 +17793,21 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -17829,16 +17897,16 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -18202,20 +18270,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1796875" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="50"/>
+    <col min="5" max="16384" width="9.1796875" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -18594,7 +18662,7 @@
     <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
@@ -18603,21 +18671,21 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -18707,21 +18775,21 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -18811,21 +18879,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="36"/>
+    <col min="4" max="4" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18881,7 +18949,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="38">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="38" t="s">
         <v>523</v>
@@ -18905,21 +18973,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.453125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="36"/>
+    <col min="4" max="4" width="15.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18968,29 +19036,29 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.1796875" style="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="36"/>
+    <col min="13" max="13" width="17.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -19124,10 +19192,10 @@
     <cfRule type="duplicateValues" dxfId="65" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19136,25 +19204,25 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="36"/>
+    <col min="4" max="4" width="22.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1796875" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -19252,13 +19320,13 @@
     <cfRule type="duplicateValues" dxfId="63" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0800-000001000000}">
       <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0800-000002000000}">
       <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
TCID 7, 19 fix
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE4E936-C1E8-43C0-99F9-F49264C50037}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D45C13-D632-406D-9223-F69E01175BC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -135,7 +135,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2712" uniqueCount="694">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2119,9 +2119,6 @@
     <t>9601015800085</t>
   </si>
   <si>
-    <t>Joanna</t>
-  </si>
-  <si>
     <t>BaLastName</t>
   </si>
   <si>
@@ -2131,12 +2128,6 @@
     <t>BdFisrtname</t>
   </si>
   <si>
-    <t>BackendLastJo</t>
-  </si>
-  <si>
-    <t>9501015800087</t>
-  </si>
-  <si>
     <t>watlevi41@gmail.com</t>
   </si>
   <si>
@@ -2222,6 +2213,18 @@
   </si>
   <si>
     <t>Invalid_login_creditials_No_Username</t>
+  </si>
+  <si>
+    <t>Password001!</t>
+  </si>
+  <si>
+    <t>9104123240187</t>
+  </si>
+  <si>
+    <t>Janne</t>
+  </si>
+  <si>
+    <t>Louw</t>
   </si>
 </sst>
 </file>
@@ -4115,10 +4118,10 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G54" sqref="G54"/>
+      <selection pane="bottomRight" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -4195,14 +4198,14 @@
         <v>301</v>
       </c>
       <c r="R1" s="145" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="S1" s="145" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="29">
-      <c r="A2" s="137">
+      <c r="A2" s="140">
         <v>1</v>
       </c>
       <c r="B2" s="124" t="s">
@@ -4242,7 +4245,7 @@
       <c r="P2" s="124"/>
     </row>
     <row r="3" spans="1:19" ht="29">
-      <c r="A3" s="137">
+      <c r="A3" s="140">
         <v>2</v>
       </c>
       <c r="B3" s="124" t="s">
@@ -4283,7 +4286,7 @@
       <c r="Q3" s="124"/>
     </row>
     <row r="4" spans="1:19" ht="29">
-      <c r="A4" s="137">
+      <c r="A4" s="140">
         <v>3</v>
       </c>
       <c r="B4" s="124" t="s">
@@ -4322,7 +4325,7 @@
       <c r="Q4" s="124"/>
     </row>
     <row r="5" spans="1:19" ht="29">
-      <c r="A5" s="137">
+      <c r="A5" s="140">
         <v>4</v>
       </c>
       <c r="B5" s="124" t="s">
@@ -4363,7 +4366,7 @@
       <c r="Q5" s="124"/>
     </row>
     <row r="6" spans="1:19" ht="29">
-      <c r="A6" s="137">
+      <c r="A6" s="140">
         <v>5</v>
       </c>
       <c r="B6" s="124" t="s">
@@ -4535,7 +4538,7 @@
         <v>196</v>
       </c>
       <c r="F10" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="126" t="s">
         <v>86</v>
@@ -5303,13 +5306,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="124" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C30" s="69" t="s">
         <v>261</v>
       </c>
       <c r="D30" s="124" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E30" s="125"/>
       <c r="F30" s="124" t="s">
@@ -5349,13 +5352,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="124" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="C31" s="69" t="s">
         <v>261</v>
       </c>
       <c r="D31" s="124" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="E31" s="125"/>
       <c r="F31" s="124" t="s">
@@ -5380,7 +5383,7 @@
         <v>88</v>
       </c>
       <c r="M31" s="126" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="N31" s="126" t="s">
         <v>109</v>
@@ -6185,7 +6188,7 @@
         <v>501</v>
       </c>
       <c r="F52" s="124" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G52" s="58" t="s">
         <v>297</v>
@@ -6552,7 +6555,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="152" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="C64" s="67">
         <v>305</v>
@@ -7655,7 +7658,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>308</v>
@@ -8116,7 +8119,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="94" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>92</v>
@@ -8166,7 +8169,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="94" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>92</v>
@@ -10676,16 +10679,16 @@
         <v>396</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
       <c r="H2" s="25" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
       <c r="I2" s="25" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="J2" s="25" t="s">
         <v>76</v>
@@ -10697,16 +10700,16 @@
         <v>73</v>
       </c>
       <c r="M2" s="25" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="N2" s="25" t="s">
+        <v>667</v>
+      </c>
+      <c r="O2" s="26" t="s">
         <v>670</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="27" t="s">
         <v>673</v>
-      </c>
-      <c r="P2" s="27" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="4" customFormat="1">
@@ -10876,13 +10879,13 @@
         <v>396</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="I6" s="25" t="s">
         <v>74</v>
@@ -10897,16 +10900,16 @@
         <v>73</v>
       </c>
       <c r="M6" s="25" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
       <c r="N6" s="25" t="s">
         <v>74</v>
       </c>
       <c r="O6" s="26" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="7" spans="1:16" s="4" customFormat="1" ht="29">
@@ -12542,11 +12545,11 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="H2" sqref="H2"/>
       <selection pane="topRight" activeCell="H2" sqref="H2"/>
       <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
-      <selection pane="bottomRight" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -12678,7 +12681,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" ht="29">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -12692,7 +12695,7 @@
         <v>225504</v>
       </c>
       <c r="E8" s="116" t="s">
-        <v>635</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -12794,7 +12797,7 @@
         <v>225564</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -13578,7 +13581,7 @@
         <v>147</v>
       </c>
       <c r="E2" s="84" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F2" s="83" t="s">
         <v>401</v>
@@ -13706,7 +13709,7 @@
         <v>147</v>
       </c>
       <c r="E6" s="116" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F6" s="83" t="s">
         <v>401</v>
@@ -13834,7 +13837,7 @@
         <v>147</v>
       </c>
       <c r="E10" s="83" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F10" s="83" t="s">
         <v>405</v>
@@ -13866,7 +13869,7 @@
         <v>147</v>
       </c>
       <c r="E11" s="114" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F11" s="83" t="s">
         <v>401</v>
@@ -14122,7 +14125,7 @@
         <v>147</v>
       </c>
       <c r="E19" s="116" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
       <c r="F19" s="86" t="s">
         <v>401</v>
@@ -14154,7 +14157,7 @@
         <v>147</v>
       </c>
       <c r="E20" s="116" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="F20" s="86" t="s">
         <v>401</v>
@@ -14218,7 +14221,7 @@
         <v>147</v>
       </c>
       <c r="E22" s="86" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
       <c r="F22" s="86" t="s">
         <v>405</v>
@@ -14690,10 +14693,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="95" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E2" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -14707,10 +14710,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E3" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -14724,10 +14727,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E4" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -14741,10 +14744,10 @@
         <v>1</v>
       </c>
       <c r="D5" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E5" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -14758,10 +14761,10 @@
         <v>1</v>
       </c>
       <c r="D6" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E6" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -14775,10 +14778,10 @@
         <v>1</v>
       </c>
       <c r="D7" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -14826,10 +14829,10 @@
         <v>1</v>
       </c>
       <c r="D10" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E10" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -14843,10 +14846,10 @@
         <v>1</v>
       </c>
       <c r="D11" s="116" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="E11" s="94" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -14860,10 +14863,10 @@
         <v>1</v>
       </c>
       <c r="D12" s="94" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E12" s="94" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -14877,10 +14880,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="94" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E13" s="94" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -14911,10 +14914,10 @@
         <v>1</v>
       </c>
       <c r="D15" s="94" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E15" s="94" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -15826,7 +15829,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -15838,8 +15841,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -15942,10 +15945,10 @@
         <v>1</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>658</v>
+        <v>692</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>662</v>
+        <v>693</v>
       </c>
       <c r="F3" s="19" t="s">
         <v>126</v>
@@ -15954,7 +15957,7 @@
         <v>128</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>663</v>
+        <v>691</v>
       </c>
       <c r="I3" s="16"/>
       <c r="J3" s="16" t="s">
@@ -15976,10 +15979,10 @@
         <v>1</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F4" s="19" t="s">
         <v>126</v>
@@ -15989,7 +15992,7 @@
       </c>
       <c r="H4" s="24"/>
       <c r="I4" s="24" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>127</v>
@@ -16746,7 +16749,7 @@
         <v>95</v>
       </c>
       <c r="F7" s="139" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="G7" s="118" t="s">
         <v>116</v>

</xml_diff>

<commit_message>
demo update sheet for jenkins test
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4043,11 +4043,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F44" sqref="F44"/>
+      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -5928,7 +5928,7 @@
         <v>196</v>
       </c>
       <c r="F46" s="124" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G46" s="133" t="s">
         <v>290</v>
@@ -19276,15 +19276,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -19433,6 +19424,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
@@ -19442,23 +19442,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19475,4 +19458,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updating after leverchv2 commit
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BB7A2D-D301-491A-809A-2EAF7DAFC09E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -70,12 +69,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1D00-000001000000}">
+    <comment ref="E1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1D00-000002000000}">
+    <comment ref="H1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -114,12 +113,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2A00-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -137,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="719">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2299,12 +2298,15 @@
   </si>
   <si>
     <t>automation12@gmail.com</t>
+  </si>
+  <si>
+    <t>getnumberOfEmails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="14">
     <font>
       <sz val="11"/>
@@ -2928,9 +2930,9 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="116">
     <dxf>
@@ -4149,7 +4151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4182,26 +4184,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4234,23 +4219,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -4426,35 +4394,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F62" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F83" sqref="F83"/>
+      <selection pane="bottomRight" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="61" customWidth="1"/>
-    <col min="2" max="2" width="93.54296875" style="130" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7265625" style="130" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="130" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="130" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.26953125" style="130" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.54296875" style="130" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.7265625" style="130" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27.1796875" style="130" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.1796875" style="130" customWidth="1"/>
-    <col min="18" max="18" width="20.1796875" style="130" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="130"/>
+    <col min="2" max="2" width="93.5703125" style="130" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="130" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="130" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="130" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" style="130" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.5703125" style="130" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" style="130" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27.140625" style="130" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" style="130" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="130" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="130"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -4516,7 +4484,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="29">
+    <row r="2" spans="1:19" ht="30">
       <c r="A2" s="139">
         <v>1</v>
       </c>
@@ -4556,7 +4524,7 @@
       <c r="O2" s="123"/>
       <c r="P2" s="123"/>
     </row>
-    <row r="3" spans="1:19" ht="29">
+    <row r="3" spans="1:19" ht="30">
       <c r="A3" s="139">
         <v>2</v>
       </c>
@@ -4597,7 +4565,7 @@
       <c r="P3" s="123"/>
       <c r="Q3" s="123"/>
     </row>
-    <row r="4" spans="1:19" ht="29">
+    <row r="4" spans="1:19" ht="30">
       <c r="A4" s="139">
         <v>3</v>
       </c>
@@ -4636,7 +4604,7 @@
       <c r="P4" s="123"/>
       <c r="Q4" s="123"/>
     </row>
-    <row r="5" spans="1:19" ht="29">
+    <row r="5" spans="1:19" ht="30">
       <c r="A5" s="139">
         <v>4</v>
       </c>
@@ -4677,7 +4645,7 @@
       <c r="P5" s="123"/>
       <c r="Q5" s="123"/>
     </row>
-    <row r="6" spans="1:19" ht="29">
+    <row r="6" spans="1:19" ht="30">
       <c r="A6" s="139">
         <v>5</v>
       </c>
@@ -4718,7 +4686,7 @@
       <c r="P6" s="123"/>
       <c r="Q6" s="123"/>
     </row>
-    <row r="7" spans="1:19" ht="29">
+    <row r="7" spans="1:19" ht="30">
       <c r="A7" s="136">
         <v>6</v>
       </c>
@@ -4757,7 +4725,7 @@
       <c r="P7" s="123"/>
       <c r="Q7" s="123"/>
     </row>
-    <row r="8" spans="1:19" ht="29">
+    <row r="8" spans="1:19" ht="30">
       <c r="A8" s="136">
         <v>7</v>
       </c>
@@ -4796,7 +4764,7 @@
       <c r="P8" s="123"/>
       <c r="Q8" s="123"/>
     </row>
-    <row r="9" spans="1:19" ht="29">
+    <row r="9" spans="1:19" ht="30">
       <c r="A9" s="136">
         <v>8</v>
       </c>
@@ -4833,7 +4801,7 @@
       <c r="P9" s="123"/>
       <c r="Q9" s="123"/>
     </row>
-    <row r="10" spans="1:19" ht="29">
+    <row r="10" spans="1:19" ht="30">
       <c r="A10" s="136">
         <v>9</v>
       </c>
@@ -4872,7 +4840,7 @@
       <c r="P10" s="123"/>
       <c r="Q10" s="123"/>
     </row>
-    <row r="11" spans="1:19" ht="29">
+    <row r="11" spans="1:19" ht="30">
       <c r="A11" s="136">
         <v>10</v>
       </c>
@@ -4911,7 +4879,7 @@
       <c r="P11" s="123"/>
       <c r="Q11" s="123"/>
     </row>
-    <row r="12" spans="1:19" ht="29">
+    <row r="12" spans="1:19" ht="30">
       <c r="A12" s="136">
         <v>11</v>
       </c>
@@ -4950,7 +4918,7 @@
       <c r="P12" s="123"/>
       <c r="Q12" s="123"/>
     </row>
-    <row r="13" spans="1:19" ht="29">
+    <row r="13" spans="1:19" ht="30">
       <c r="A13" s="136">
         <v>12</v>
       </c>
@@ -4989,7 +4957,7 @@
       <c r="P13" s="123"/>
       <c r="Q13" s="123"/>
     </row>
-    <row r="14" spans="1:19" ht="29">
+    <row r="14" spans="1:19" ht="30">
       <c r="A14" s="139">
         <v>13</v>
       </c>
@@ -5028,7 +4996,7 @@
       <c r="P14" s="123"/>
       <c r="Q14" s="123"/>
     </row>
-    <row r="15" spans="1:19" ht="29">
+    <row r="15" spans="1:19" ht="30">
       <c r="A15" s="139">
         <v>14</v>
       </c>
@@ -5067,7 +5035,7 @@
       <c r="P15" s="123"/>
       <c r="Q15" s="123"/>
     </row>
-    <row r="16" spans="1:19" ht="29">
+    <row r="16" spans="1:19" ht="30">
       <c r="A16" s="146">
         <v>15</v>
       </c>
@@ -5110,7 +5078,7 @@
       <c r="P16" s="123"/>
       <c r="Q16" s="123"/>
     </row>
-    <row r="17" spans="1:17" ht="29">
+    <row r="17" spans="1:17" ht="30">
       <c r="A17" s="146">
         <v>16</v>
       </c>
@@ -5153,7 +5121,7 @@
       <c r="P17" s="123"/>
       <c r="Q17" s="123"/>
     </row>
-    <row r="18" spans="1:17" ht="29">
+    <row r="18" spans="1:17" ht="30">
       <c r="A18" s="146">
         <v>17</v>
       </c>
@@ -5196,7 +5164,7 @@
       <c r="P18" s="123"/>
       <c r="Q18" s="123"/>
     </row>
-    <row r="19" spans="1:17" ht="29">
+    <row r="19" spans="1:17" ht="30">
       <c r="A19" s="146">
         <v>18</v>
       </c>
@@ -5239,7 +5207,7 @@
       <c r="P19" s="123"/>
       <c r="Q19" s="123"/>
     </row>
-    <row r="20" spans="1:17" ht="29">
+    <row r="20" spans="1:17" ht="30">
       <c r="A20" s="146">
         <v>19</v>
       </c>
@@ -5282,7 +5250,7 @@
       <c r="P20" s="123"/>
       <c r="Q20" s="123"/>
     </row>
-    <row r="21" spans="1:17" ht="29">
+    <row r="21" spans="1:17" ht="30">
       <c r="A21" s="146">
         <v>20</v>
       </c>
@@ -6744,7 +6712,7 @@
       <c r="G59" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H59" s="58" t="s">
+      <c r="H59" s="111" t="s">
         <v>574</v>
       </c>
       <c r="I59" s="58" t="s">
@@ -6780,7 +6748,7 @@
       <c r="G60" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H60" s="58" t="s">
+      <c r="H60" s="111" t="s">
         <v>574</v>
       </c>
       <c r="I60" s="58" t="s">
@@ -6815,7 +6783,7 @@
       <c r="G61" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H61" s="58" t="s">
+      <c r="H61" s="111" t="s">
         <v>574</v>
       </c>
       <c r="I61" s="58" t="s">
@@ -6852,7 +6820,7 @@
       <c r="G62" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="H62" s="58" t="s">
+      <c r="H62" s="111" t="s">
         <v>574</v>
       </c>
       <c r="I62" s="58" t="s">
@@ -6891,7 +6859,7 @@
       <c r="G63" s="58" t="s">
         <v>578</v>
       </c>
-      <c r="H63" s="57"/>
+      <c r="H63" s="111"/>
       <c r="I63" s="57"/>
       <c r="J63" s="57"/>
       <c r="K63" s="57"/>
@@ -6922,7 +6890,7 @@
       <c r="G64" s="58" t="s">
         <v>578</v>
       </c>
-      <c r="H64" s="57"/>
+      <c r="H64" s="111"/>
       <c r="I64" s="57"/>
       <c r="J64" s="57"/>
       <c r="K64" s="57"/>
@@ -6953,7 +6921,7 @@
       <c r="G65" s="58" t="s">
         <v>579</v>
       </c>
-      <c r="H65" s="57"/>
+      <c r="H65" s="111"/>
       <c r="I65" s="57"/>
       <c r="J65" s="57"/>
       <c r="K65" s="57"/>
@@ -6981,7 +6949,7 @@
       <c r="G66" s="57" t="s">
         <v>580</v>
       </c>
-      <c r="H66" s="57"/>
+      <c r="H66" s="111"/>
       <c r="I66" s="57"/>
       <c r="J66" s="57"/>
       <c r="K66" s="57"/>
@@ -7009,7 +6977,7 @@
       <c r="G67" s="65" t="s">
         <v>581</v>
       </c>
-      <c r="H67" s="57"/>
+      <c r="H67" s="111"/>
       <c r="I67" s="57"/>
       <c r="J67" s="57"/>
       <c r="K67" s="57"/>
@@ -7019,7 +6987,7 @@
       <c r="A68" s="150">
         <v>67</v>
       </c>
-      <c r="B68" s="64" t="s">
+      <c r="B68" s="65" t="s">
         <v>620</v>
       </c>
       <c r="C68" s="66">
@@ -7034,16 +7002,19 @@
       <c r="F68" s="123" t="s">
         <v>9</v>
       </c>
-      <c r="G68" s="57" t="s">
+      <c r="G68" s="123" t="s">
+        <v>718</v>
+      </c>
+      <c r="H68" s="111" t="s">
         <v>581</v>
       </c>
-      <c r="H68" s="64" t="s">
+      <c r="I68" s="65" t="s">
         <v>582</v>
       </c>
-      <c r="I68" s="57"/>
       <c r="J68" s="57"/>
       <c r="K68" s="57"/>
       <c r="L68" s="57"/>
+      <c r="M68" s="57"/>
     </row>
     <row r="69" spans="1:13">
       <c r="A69" s="160">
@@ -7067,7 +7038,7 @@
       <c r="G69" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H69" s="58"/>
+      <c r="H69" s="111"/>
       <c r="I69" s="64"/>
       <c r="J69" s="64"/>
       <c r="K69" s="57"/>
@@ -7093,7 +7064,7 @@
       <c r="G70" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H70" s="57" t="s">
+      <c r="H70" s="111" t="s">
         <v>583</v>
       </c>
       <c r="I70" s="57"/>
@@ -7118,24 +7089,27 @@
         <v>584</v>
       </c>
       <c r="F71" s="123" t="s">
-        <v>9</v>
-      </c>
-      <c r="G71" s="58" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="123" t="s">
+        <v>718</v>
+      </c>
+      <c r="H71" s="58" t="s">
         <v>407</v>
       </c>
-      <c r="H71" s="58" t="s">
+      <c r="I71" s="112" t="s">
         <v>408</v>
       </c>
-      <c r="I71" s="58" t="s">
+      <c r="J71" s="58" t="s">
         <v>409</v>
       </c>
-      <c r="J71" s="58" t="s">
+      <c r="K71" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="K71" s="58" t="s">
+      <c r="L71" s="58" t="s">
         <v>585</v>
       </c>
-      <c r="L71" s="58" t="s">
+      <c r="M71" s="58" t="s">
         <v>586</v>
       </c>
     </row>
@@ -7157,6 +7131,7 @@
       <c r="G72" s="58" t="s">
         <v>712</v>
       </c>
+      <c r="H72" s="111"/>
     </row>
     <row r="73" spans="1:13">
       <c r="A73" s="163">
@@ -7176,6 +7151,7 @@
       <c r="G73" s="58" t="s">
         <v>714</v>
       </c>
+      <c r="H73" s="111"/>
     </row>
     <row r="74" spans="1:13">
       <c r="A74" s="151">
@@ -7199,6 +7175,7 @@
       <c r="G74" s="128" t="s">
         <v>695</v>
       </c>
+      <c r="H74" s="111"/>
     </row>
     <row r="75" spans="1:13">
       <c r="A75" s="153">
@@ -7218,7 +7195,7 @@
       <c r="G75" s="58" t="s">
         <v>31</v>
       </c>
-      <c r="H75" s="58" t="s">
+      <c r="H75" s="111" t="s">
         <v>574</v>
       </c>
       <c r="I75" s="57"/>
@@ -7464,253 +7441,252 @@
     <cfRule type="duplicateValues" dxfId="89" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="O31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
-    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
-    <hyperlink ref="M40" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="J54" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
-    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
-    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
-    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
-    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
-    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
-    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
-    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
-    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
-    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
-    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
-    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
-    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
-    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
-    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
-    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
-    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
-    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
-    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
-    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
-    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
-    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
-    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
-    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
-    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
-    <hyperlink ref="K2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
-    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
-    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
-    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
-    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
-    <hyperlink ref="J3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
-    <hyperlink ref="J4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
-    <hyperlink ref="J5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
-    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
-    <hyperlink ref="J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
-    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
-    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
-    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
-    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
-    <hyperlink ref="I2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
-    <hyperlink ref="I3:I6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
-    <hyperlink ref="J55" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
-    <hyperlink ref="I55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
-    <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000B6000000}"/>
-    <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart" xr:uid="{00000000-0004-0000-0000-0000B8000000}"/>
-    <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000B9000000}"/>
-    <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000BA000000}"/>
-    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0000-0000BC000000}"/>
-    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0000-0000BE000000}"/>
-    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C3000000}"/>
-    <hyperlink ref="J71" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000C4000000}"/>
-    <hyperlink ref="G71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000C5000000}"/>
-    <hyperlink ref="H71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0000-0000C6000000}"/>
-    <hyperlink ref="I71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000C7000000}"/>
-    <hyperlink ref="K71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail" xr:uid="{00000000-0004-0000-0000-0000C8000000}"/>
-    <hyperlink ref="L71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification" xr:uid="{00000000-0004-0000-0000-0000C9000000}"/>
-    <hyperlink ref="G56:G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-0000CA000000}"/>
-    <hyperlink ref="I56:I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-0000CC000000}"/>
-    <hyperlink ref="G63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-0000CD000000}"/>
-    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-0000CE000000}"/>
-    <hyperlink ref="G70" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000CF000000}"/>
-    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0000-0000D0000000}"/>
-    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000D1000000}"/>
-    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0000-0000D2000000}"/>
-    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0000-0000D3000000}"/>
-    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D4000000}"/>
-    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D5000000}"/>
-    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-0000D6000000}"/>
-    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-0000D7000000}"/>
-    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0000-0000D8000000}"/>
-    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-0000D9000000}"/>
-    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0000-0000DA000000}"/>
-    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0000-0000DB000000}"/>
-    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DC000000}"/>
-    <hyperlink ref="N40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DD000000}"/>
-    <hyperlink ref="N42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-0000DE000000}"/>
-    <hyperlink ref="O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-0000DF000000}"/>
-    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-0000E0000000}"/>
-    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E1000000}"/>
-    <hyperlink ref="Q40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E2000000}"/>
-    <hyperlink ref="Q42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0000-0000E3000000}"/>
-    <hyperlink ref="R40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-0000E4000000}"/>
-    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-0000E5000000}"/>
-    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E6000000}"/>
-    <hyperlink ref="S40" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E7000000}"/>
-    <hyperlink ref="S42" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0000-0000E8000000}"/>
-    <hyperlink ref="L54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{43F28687-BDD4-4576-9CB2-335425C70DAB}"/>
-    <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{F7B3758D-DA28-4354-BB8E-4C52273B9C3C}"/>
-    <hyperlink ref="H56:H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{23E952BA-0F16-4536-A7E8-246446D5A12E}"/>
-    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{8D6E5A07-449A-45E0-82D1-0BB597EC06AA}"/>
-    <hyperlink ref="H54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{0E18B1F8-9186-42F4-8530-23AF563BF6B2}"/>
-    <hyperlink ref="I54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{7B638116-682E-4260-A375-FDF510D5A2D9}"/>
-    <hyperlink ref="K54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{05E5242C-1360-4A14-B570-9DBB6D84B394}"/>
-    <hyperlink ref="G74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear" xr:uid="{569BCBC1-14CB-4BDD-94B1-584A32FF0AE5}"/>
-    <hyperlink ref="G78" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{277B8CC8-2F10-470D-A563-9D1039ED8B31}"/>
-    <hyperlink ref="G79" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{AC74479E-FD2D-4273-8B19-9B3413C0A200}"/>
-    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login" xr:uid="{7C96EF6F-8B2E-4FCF-AF61-B06CFD7806C5}"/>
-    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{1D3A9A1A-7D07-4F7C-BE71-0D31D834470D}"/>
-    <hyperlink ref="H59:H75" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{2EB727F0-993C-4694-B301-14FEC0916972}"/>
-    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{89385743-9000-4FE4-AE61-B98AF0084038}"/>
-    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{060EEFBD-D295-499C-8F6E-343759BD18E0}"/>
-    <hyperlink ref="G75" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{15A0E568-FF04-4796-B5EE-800E5CDA4B24}"/>
-    <hyperlink ref="G76:G77" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{AFD27A9B-6D46-4594-85DF-6C71EF2B60A0}"/>
-    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login" xr:uid="{75F0765E-3244-4F18-A287-F591941CB7B0}"/>
-    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{5A327A68-0FCA-42F7-8957-156F2007EBFE}"/>
-    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{7ABE5EF3-5D2B-4B5F-8EF1-D851A61018E9}"/>
-    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login" xr:uid="{50BB8B51-5D00-4A24-9C2A-0BD4DBEAD9BE}"/>
-    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login" xr:uid="{C4848167-EF5D-4FCE-8EAF-A0008D28F298}"/>
-    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{76E8D0DB-4DA5-4365-8969-4FA2E30707A0}"/>
-    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{F27235DF-7B56-4EA2-B612-B305C65AEFAA}"/>
+    <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G3" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H4" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G4" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H5" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G5" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H6" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G6" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G27" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L27" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G24" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G25" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G22" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G23" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G26" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="I27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G28" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G30" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="H30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L28" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L30" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="J30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="M30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="K30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="O30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G31" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="K31" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="L31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="J31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G29" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L29" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="I29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G32" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L32" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="P32" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H37" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H33" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="K33" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="M33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="G33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="J34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="M35" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="I48" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="J48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="M40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="M40:M42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="J54" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
+    <hyperlink ref="N32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="L48" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="K48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G53:G54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G35" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H35" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I35" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="J35" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K35" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L35" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G36" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="I36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="I37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="K36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="G50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="G50:G52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="H2" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K2" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G2" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="J2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K3" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K5" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="J3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K6" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="J6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="I2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="I3:I6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J55" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="K55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
+    <hyperlink ref="J56" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J57" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="G69" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K71" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="J71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="L71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
+    <hyperlink ref="M71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
+    <hyperlink ref="G56:G57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I56:I57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="G63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="G64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="G70" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M41" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="O42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="Q40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="Q42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="S41" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="S40" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="S42" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="H55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="H56:H57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="K57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="H54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="K54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="G74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear"/>
+    <hyperlink ref="G78" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G79" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G75" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G76:G77" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7718,29 +7694,29 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="36"/>
+    <col min="13" max="13" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -7874,10 +7850,10 @@
     <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0700-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7886,25 +7862,25 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="22.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -8002,13 +7978,13 @@
     <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0800-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0800-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8017,28 +7993,28 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="36"/>
+    <col min="10" max="10" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -8154,7 +8130,7 @@
     <cfRule type="duplicateValues" dxfId="66" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8162,7 +8138,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0900-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
           </x14:formula1>
@@ -8175,24 +8151,24 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="36"/>
+    <col min="8" max="8" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8281,7 +8257,7 @@
     <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8291,38 +8267,38 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="36"/>
-    <col min="15" max="15" width="23.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="36"/>
+    <col min="14" max="14" width="9.140625" style="36"/>
+    <col min="15" max="15" width="23.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -8537,25 +8513,25 @@
     <cfRule type="duplicateValues" dxfId="62" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{00000000-0002-0000-0B00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{00000000-0002-0000-0B00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
       <formula1>"African,Asian,Coloured,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{00000000-0002-0000-0B00-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
       <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{00000000-0002-0000-0B00-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{00000000-0002-0000-0B00-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{00000000-0002-0000-0B00-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8565,22 +8541,22 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="20.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -8636,15 +8612,15 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="35"/>
@@ -8691,25 +8667,25 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="29"/>
+    <col min="10" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -8782,7 +8758,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8793,42 +8769,42 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="20.26953125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="31.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.1796875" style="11" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" style="11" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="11"/>
+    <col min="27" max="27" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" style="11" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="30">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -9432,64 +9408,64 @@
     <cfRule type="duplicateValues" dxfId="52" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-0F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7" xr:uid="{00000000-0002-0000-0F00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0F00-000001000000}"/>
-    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0F00-000003000000}"/>
-    <hyperlink ref="D5" r:id="rId5" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-0F00-000004000000}"/>
+    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D5" r:id="rId5" display="original2Ic@automationjdg.co.za"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.7265625" style="12"/>
+    <col min="28" max="28" width="23.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7109375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -10111,7 +10087,7 @@
     <cfRule type="duplicateValues" dxfId="46" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-1000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10120,17 +10096,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31917AC-2077-42D8-B3AC-65F6F3A16B2E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -10163,14 +10139,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{3BB63F68-8DEB-48F8-8FF8-3285ECE8D5AD}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10181,14 +10157,14 @@
       <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -10624,7 +10600,7 @@
     <cfRule type="duplicateValues" dxfId="44" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -10633,22 +10609,22 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -10802,24 +10778,24 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="38" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="38"/>
+    <col min="11" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="55" customFormat="1">
@@ -11249,19 +11225,19 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11479,7 +11455,7 @@
     <cfRule type="duplicateValues" dxfId="42" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"payUcreditcard,Cash_Deposits"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11488,33 +11464,33 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="29">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A1" s="37" t="s">
         <v>34</v>
       </c>
@@ -11764,7 +11740,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
+    <row r="6" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -11814,7 +11790,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="29">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -12355,14 +12331,14 @@
     <cfRule type="duplicateValues" dxfId="38" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-1500-000002000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-1500-000003000000}"/>
-    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-1500-000004000000}"/>
-    <hyperlink ref="O6" r:id="rId6" xr:uid="{00000000-0004-0000-1500-000005000000}"/>
-    <hyperlink ref="O7" r:id="rId7" xr:uid="{00000000-0004-0000-1500-000006000000}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-1500-000007000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
+    <hyperlink ref="O8" r:id="rId5"/>
+    <hyperlink ref="O6" r:id="rId6"/>
+    <hyperlink ref="O7" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
@@ -12370,18 +12346,18 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="29"/>
+    <col min="1" max="1" width="21.140625" style="29"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" style="29"/>
+    <col min="3" max="3" width="21.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12401,7 +12377,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -12412,7 +12388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="45">
         <v>2</v>
       </c>
@@ -12423,7 +12399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="45">
         <v>3</v>
       </c>
@@ -12434,7 +12410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="45">
         <v>4</v>
       </c>
@@ -12445,7 +12421,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="45">
         <v>5</v>
       </c>
@@ -12500,7 +12476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="45">
         <v>19</v>
       </c>
@@ -12540,27 +12516,27 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="6"/>
+    <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -12705,29 +12681,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-1700-000001000000}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-1700-000002000000}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-1700-000003000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-1700-000004000000}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-1700-000005000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="J4" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7265625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="11" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -12744,7 +12720,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -12758,7 +12734,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="29">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -12772,7 +12748,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -12786,7 +12762,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -12800,7 +12776,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -12814,7 +12790,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -12870,7 +12846,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="142">
         <v>40</v>
       </c>
@@ -12884,7 +12860,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29">
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" s="61">
         <v>41</v>
       </c>
@@ -12954,21 +12930,21 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -13216,19 +13192,19 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="38"/>
+    <col min="5" max="5" width="13.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13308,7 +13284,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -13443,17 +13419,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A45F8140-A253-4D2D-9444-DDEA38E5F82B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13492,14 +13468,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{E4849886-E130-4931-AED9-3253BC3DFF99}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13510,14 +13486,14 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -13639,7 +13615,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="29">
+    <row r="8" spans="1:5" ht="30">
       <c r="A8" s="16">
         <v>7</v>
       </c>
@@ -13741,7 +13717,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="29">
+    <row r="14" spans="1:5" ht="30">
       <c r="A14" s="16">
         <v>13</v>
       </c>
@@ -14156,7 +14132,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14166,13 +14142,13 @@
       <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="11"/>
+    <col min="4" max="4" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -14189,7 +14165,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -14201,7 +14177,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:4" ht="43.5">
+    <row r="3" spans="1:4" ht="45">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -14213,7 +14189,7 @@
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="43.5">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -14225,7 +14201,7 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -14237,7 +14213,7 @@
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -14249,7 +14225,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -14321,7 +14297,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -14331,23 +14307,23 @@
       <selection pane="bottomRight" activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="82" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.54296875" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" style="82" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="82" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="82"/>
+    <col min="4" max="4" width="20.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="82" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="82"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="78" t="s">
         <v>34</v>
       </c>
@@ -14446,7 +14422,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="83">
         <v>28</v>
       </c>
@@ -15022,7 +14998,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="29">
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="85">
         <v>61</v>
       </c>
@@ -15247,7 +15223,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="113" customFormat="1" ht="29">
+    <row r="29" spans="1:11" s="113" customFormat="1" ht="30">
       <c r="A29" s="113">
         <v>78</v>
       </c>
@@ -15329,13 +15305,13 @@
     <cfRule type="duplicateValues" dxfId="20" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14" xr:uid="{00000000-0002-0000-1D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G14">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F14" xr:uid="{00000000-0002-0000-1D00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F14">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J14" xr:uid="{00000000-0002-0000-1D00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J14">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -15345,13 +15321,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1D00-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>D2:D30</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-1D00-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
@@ -15364,20 +15340,20 @@
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -15427,16 +15403,16 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -15535,21 +15511,21 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="31"/>
+    <col min="4" max="4" width="18.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15610,21 +15586,21 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15694,21 +15670,21 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="96" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="96" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="96" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="96" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="96" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" style="96" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="96"/>
+    <col min="5" max="5" width="23.140625" style="96" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="96"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16051,7 +16027,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14" customHeight="1">
+    <row r="21" spans="1:5" ht="14.1" customHeight="1">
       <c r="A21" s="57">
         <v>64</v>
       </c>
@@ -16134,33 +16110,33 @@
     <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Password@123" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
-    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-2200-000001000000}"/>
-    <hyperlink ref="E9" r:id="rId3" xr:uid="{00000000-0004-0000-2200-000002000000}"/>
-    <hyperlink ref="E12" r:id="rId4" display="Password@123" xr:uid="{00000000-0004-0000-2200-000003000000}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{00000000-0004-0000-2200-000004000000}"/>
-    <hyperlink ref="E21" r:id="rId6" xr:uid="{00000000-0004-0000-2200-000006000000}"/>
-    <hyperlink ref="E22" r:id="rId7" xr:uid="{00000000-0004-0000-2200-000007000000}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{00000000-0004-0000-2200-000008000000}"/>
-    <hyperlink ref="E13" r:id="rId9" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000A000000}"/>
-    <hyperlink ref="E3" r:id="rId10" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000B000000}"/>
-    <hyperlink ref="E4" r:id="rId11" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000C000000}"/>
-    <hyperlink ref="E5" r:id="rId12" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000D000000}"/>
-    <hyperlink ref="E6" r:id="rId13" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000E000000}"/>
-    <hyperlink ref="E7" r:id="rId14" display="Password@123" xr:uid="{00000000-0004-0000-2200-00000F000000}"/>
-    <hyperlink ref="E10" r:id="rId15" display="Password@123" xr:uid="{00000000-0004-0000-2200-000010000000}"/>
-    <hyperlink ref="E11" r:id="rId16" display="Password@123" xr:uid="{00000000-0004-0000-2200-000011000000}"/>
-    <hyperlink ref="D13" r:id="rId17" xr:uid="{00000000-0004-0000-2200-000009000000}"/>
-    <hyperlink ref="D16" r:id="rId18" xr:uid="{81428C68-028B-4893-9B4A-CD71D7D22D03}"/>
-    <hyperlink ref="E16" r:id="rId19" display="Password@123" xr:uid="{7AE80BCF-FE0D-40EE-8F1D-4CCBC9DED593}"/>
-    <hyperlink ref="D17" r:id="rId20" xr:uid="{90AEBB31-FE04-467A-971F-6F069860908F}"/>
-    <hyperlink ref="E17" r:id="rId21" display="Password@123" xr:uid="{0FA053E1-94DC-4378-9E2E-1156A759E150}"/>
-    <hyperlink ref="D18" r:id="rId22" xr:uid="{E53C6B61-E9DF-4B4D-A577-91D44E651E99}"/>
-    <hyperlink ref="D19" r:id="rId23" xr:uid="{CDDE7AF4-B91E-430A-BE1E-B69F5B97DDFA}"/>
-    <hyperlink ref="D20" r:id="rId24" xr:uid="{CB6A59C3-52AB-4E3F-B9CB-935599461DF5}"/>
-    <hyperlink ref="D23" r:id="rId25" xr:uid="{0DDA1C05-5398-4003-BFF4-6243B960F51E}"/>
-    <hyperlink ref="D24" r:id="rId26" xr:uid="{C6E10DCB-6923-4F2E-A74F-515095483F5D}"/>
-    <hyperlink ref="D15" r:id="rId27" xr:uid="{7A63D023-7686-45AD-93DB-5D1A9A83B3EC}"/>
+    <hyperlink ref="E2" r:id="rId1" display="Password@123"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E12" r:id="rId4" display="Password@123"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="E21" r:id="rId6"/>
+    <hyperlink ref="E22" r:id="rId7"/>
+    <hyperlink ref="D12" r:id="rId8"/>
+    <hyperlink ref="E13" r:id="rId9" display="Password@123"/>
+    <hyperlink ref="E3" r:id="rId10" display="Password@123"/>
+    <hyperlink ref="E4" r:id="rId11" display="Password@123"/>
+    <hyperlink ref="E5" r:id="rId12" display="Password@123"/>
+    <hyperlink ref="E6" r:id="rId13" display="Password@123"/>
+    <hyperlink ref="E7" r:id="rId14" display="Password@123"/>
+    <hyperlink ref="E10" r:id="rId15" display="Password@123"/>
+    <hyperlink ref="E11" r:id="rId16" display="Password@123"/>
+    <hyperlink ref="D13" r:id="rId17"/>
+    <hyperlink ref="D16" r:id="rId18"/>
+    <hyperlink ref="E16" r:id="rId19" display="Password@123"/>
+    <hyperlink ref="D17" r:id="rId20"/>
+    <hyperlink ref="E17" r:id="rId21" display="Password@123"/>
+    <hyperlink ref="D18" r:id="rId22"/>
+    <hyperlink ref="D19" r:id="rId23"/>
+    <hyperlink ref="D20" r:id="rId24"/>
+    <hyperlink ref="D23" r:id="rId25"/>
+    <hyperlink ref="D24" r:id="rId26"/>
+    <hyperlink ref="D15" r:id="rId27"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId28"/>
@@ -16168,15 +16144,15 @@
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -16344,22 +16320,22 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -16433,27 +16409,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-2400-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="81" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="81" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="81" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="81" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="81"/>
+    <col min="4" max="16384" width="9.140625" style="81"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -16546,20 +16522,20 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16602,27 +16578,27 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -16703,28 +16679,28 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -16814,7 +16790,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -16822,26 +16798,26 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:K3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -16886,7 +16862,7 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="112" t="s">
         <v>170</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -16913,26 +16889,65 @@
         <v>500</v>
       </c>
     </row>
+    <row r="4" spans="1:11" s="111" customFormat="1">
+      <c r="A4" s="111">
+        <v>67</v>
+      </c>
+      <c r="B4" s="111">
+        <v>1</v>
+      </c>
+      <c r="C4" s="112" t="s">
+        <v>170</v>
+      </c>
+      <c r="D4" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="H4" s="111">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="111" customFormat="1">
+      <c r="A5" s="111">
+        <v>70</v>
+      </c>
+      <c r="B5" s="111">
+        <v>1</v>
+      </c>
+      <c r="C5" s="112" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="H5" s="111">
+        <v>500</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -16949,7 +16964,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.65" customHeight="1">
+    <row r="2" spans="1:4" ht="24.6" customHeight="1">
       <c r="A2" s="3">
         <v>9</v>
       </c>
@@ -16960,7 +16975,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="111" customFormat="1" ht="24.65" customHeight="1">
+    <row r="3" spans="1:4" s="111" customFormat="1" ht="24.6" customHeight="1">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -16977,31 +16992,31 @@
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -17107,7 +17122,7 @@
       </c>
       <c r="L3" s="16"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="16">
         <v>8</v>
       </c>
@@ -17446,17 +17461,17 @@
     <cfRule type="duplicateValues" dxfId="6" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-2A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576" xr:uid="{00000000-0002-0000-2A00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-2A00-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -17465,38 +17480,38 @@
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
-  <dimension ref="A1:T30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomRight" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="121" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="121" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="121" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="121" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="121" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="121" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="121" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="121" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" style="121" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="121" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" style="121" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.26953125" style="121" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.1796875" style="121" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7265625" style="121" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.1796875" style="121" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="121"/>
+    <col min="12" max="12" width="20.85546875" style="121" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="121" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="121" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" style="121" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="121" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" style="121" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="121"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -17995,7 +18010,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" ht="30">
       <c r="A9" s="115">
         <v>23</v>
       </c>
@@ -18057,7 +18072,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="115">
         <v>24</v>
       </c>
@@ -18251,7 +18266,7 @@
         <v>3333333333</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:20">
       <c r="A17" s="123">
         <v>11</v>
       </c>
@@ -18265,7 +18280,7 @@
         <v>3333333333</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:20">
       <c r="A18" s="123">
         <v>12</v>
       </c>
@@ -18279,7 +18294,7 @@
         <v>3333333333</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:20">
       <c r="A19" s="123">
         <v>13</v>
       </c>
@@ -18293,7 +18308,7 @@
         <v>3333333333</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:20">
       <c r="A20" s="123">
         <v>14</v>
       </c>
@@ -18310,7 +18325,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:20">
       <c r="A21" s="123">
         <v>15</v>
       </c>
@@ -18327,7 +18342,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:20">
       <c r="A22" s="123">
         <v>16</v>
       </c>
@@ -18344,7 +18359,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:20">
       <c r="A23" s="123">
         <v>17</v>
       </c>
@@ -18361,7 +18376,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:20">
       <c r="A24" s="123">
         <v>18</v>
       </c>
@@ -18378,7 +18393,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:20">
       <c r="A25" s="123">
         <v>19</v>
       </c>
@@ -18395,7 +18410,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:20">
       <c r="A26" s="123">
         <v>20</v>
       </c>
@@ -18412,7 +18427,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:20">
       <c r="A27" s="123">
         <v>31</v>
       </c>
@@ -18429,7 +18444,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:20">
       <c r="A28" s="130">
         <v>39</v>
       </c>
@@ -18446,7 +18461,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:20">
       <c r="A29" s="130">
         <v>40</v>
       </c>
@@ -18463,7 +18478,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:20">
       <c r="A30" s="130">
         <v>41</v>
       </c>
@@ -18478,6 +18493,68 @@
       </c>
       <c r="L30" s="121" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="115">
+        <v>67</v>
+      </c>
+      <c r="B31" s="116" t="s">
+        <v>620</v>
+      </c>
+      <c r="C31" s="113">
+        <v>1</v>
+      </c>
+      <c r="D31" s="113" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="113" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="138" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="117" t="s">
+        <v>116</v>
+      </c>
+      <c r="H31" s="113" t="s">
+        <v>116</v>
+      </c>
+      <c r="I31" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="J31" s="113">
+        <v>2222227</v>
+      </c>
+      <c r="K31" s="118" t="s">
+        <v>642</v>
+      </c>
+      <c r="L31" s="113" t="s">
+        <v>115</v>
+      </c>
+      <c r="M31" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="N31" s="113" t="s">
+        <v>94</v>
+      </c>
+      <c r="O31" s="118" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" s="113" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q31" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="R31" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="S31" s="113" t="s">
+        <v>92</v>
+      </c>
+      <c r="T31" s="113" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -18501,21 +18578,21 @@
     <cfRule type="duplicateValues" dxfId="0" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11" xr:uid="{00000000-0002-0000-2B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L11 L31">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 P2:T11" xr:uid="{00000000-0002-0000-2B00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I11 P2:T11 I31 P31:T31">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11" xr:uid="{00000000-0002-0000-2B00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11 N31">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11" xr:uid="{00000000-0002-0000-2B00-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M31">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F7" r:id="rId1" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
+    <hyperlink ref="F7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -18523,21 +18600,21 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -18627,19 +18704,19 @@
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -18831,21 +18908,21 @@
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -18935,20 +19012,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="76" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" style="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="76"/>
+    <col min="4" max="4" width="19.28515625" style="76" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="76"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -19091,7 +19168,7 @@
     <cfRule type="duplicateValues" dxfId="83" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -19100,21 +19177,21 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -19204,16 +19281,16 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -19577,21 +19654,21 @@
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -19681,21 +19758,21 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -19785,23 +19862,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="73" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="73" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="73" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="73" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="73" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="73"/>
+    <col min="8" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -19997,35 +20072,35 @@
     <cfRule type="duplicateValues" dxfId="81" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com" xr:uid="{D16A3140-4CBC-4253-9C85-FAF9D1CB6F5C}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{B853E9E6-3548-4C36-8719-4B3DD1319787}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="50"/>
+    <col min="5" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -20404,7 +20479,7 @@
     <cfRule type="duplicateValues" dxfId="75" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
@@ -20413,21 +20488,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -20507,21 +20582,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -20570,12 +20645,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20728,27 +20803,18 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20773,9 +20839,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update to include keymanager structure
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -2728,7 +2728,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="175">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3145,7 +3145,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -4853,11 +4852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z93"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD2"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4960,7 +4959,7 @@
         <v>495</v>
       </c>
       <c r="F2" s="123" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="125" t="s">
         <v>108</v>
@@ -8249,8 +8248,8 @@
       <c r="E93" s="130" t="s">
         <v>195</v>
       </c>
-      <c r="F93" s="172" t="s">
-        <v>8</v>
+      <c r="F93" s="155" t="s">
+        <v>9</v>
       </c>
       <c r="G93" s="130" t="s">
         <v>777</v>
@@ -10227,13 +10226,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="130" customFormat="1">
-      <c r="A1" s="173" t="s">
+      <c r="A1" s="172" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="86" t="s">
         <v>518</v>
       </c>
-      <c r="C1" s="173" t="s">
+      <c r="C1" s="172" t="s">
         <v>215</v>
       </c>
       <c r="D1" s="86" t="s">
@@ -10295,7 +10294,7 @@
       <c r="B2" s="130" t="s">
         <v>496</v>
       </c>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="173" t="s">
         <v>249</v>
       </c>
       <c r="D2" s="130" t="s">
@@ -12217,7 +12216,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12262,7 +12261,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="111" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>9</v>
@@ -12283,7 +12282,7 @@
         <v>778</v>
       </c>
       <c r="C3" s="111" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="111" t="s">
         <v>9</v>
@@ -14316,7 +14315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updating testNG to use multiSuites, update Action.java->gettext to show on extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,33 +4,33 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="IC" sheetId="23" r:id="rId1"/>
-    <sheet name="EVS" sheetId="82" r:id="rId2"/>
-    <sheet name="evs_Login++" sheetId="81" r:id="rId3"/>
-    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId4"/>
-    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId5"/>
-    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId6"/>
-    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId7"/>
-    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId8"/>
-    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId9"/>
-    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId10"/>
-    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId11"/>
-    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId12"/>
-    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId13"/>
-    <sheet name="EnterContact++" sheetId="58" r:id="rId14"/>
-    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId15"/>
-    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId16"/>
-    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId17"/>
-    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId18"/>
-    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId19"/>
-    <sheet name="giftCardReport++" sheetId="54" r:id="rId20"/>
-    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId21"/>
-    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId22"/>
-    <sheet name="SapCustomer++" sheetId="50" r:id="rId23"/>
-    <sheet name="Suites" sheetId="22" r:id="rId24"/>
+    <sheet name="Suites" sheetId="22" r:id="rId1"/>
+    <sheet name="IC" sheetId="23" r:id="rId2"/>
+    <sheet name="EVS" sheetId="82" r:id="rId3"/>
+    <sheet name="evs_Login++" sheetId="81" r:id="rId4"/>
+    <sheet name="SapRSIGetDataFromSAPDB++" sheetId="80" r:id="rId5"/>
+    <sheet name="icInvalidEmailNewsLetter++" sheetId="77" r:id="rId6"/>
+    <sheet name="ic_SubscribeNewsletter++" sheetId="78" r:id="rId7"/>
+    <sheet name="ic_RemoveFromcart++" sheetId="67" r:id="rId8"/>
+    <sheet name="IC_ClearWishList++" sheetId="66" r:id="rId9"/>
+    <sheet name="ic_NavigetoWishlist++" sheetId="65" r:id="rId10"/>
+    <sheet name="Magento_UserInfoVerification++" sheetId="64" r:id="rId11"/>
+    <sheet name="IC_ProductsSortBy++" sheetId="63" r:id="rId12"/>
+    <sheet name="ic_SubscribeNews_DupliEmailID++" sheetId="62" r:id="rId13"/>
+    <sheet name="EnterSpouseInfor++" sheetId="61" r:id="rId14"/>
+    <sheet name="EnterContact++" sheetId="58" r:id="rId15"/>
+    <sheet name="CreditEnterAddressDetails++" sheetId="59" r:id="rId16"/>
+    <sheet name="CreditEnterEmploymentDetails++" sheetId="60" r:id="rId17"/>
+    <sheet name="EnterBasicDetails++" sheetId="57" r:id="rId18"/>
+    <sheet name="CreditStatusVerification++" sheetId="56" r:id="rId19"/>
+    <sheet name="CreditApp_NavigateFilter++" sheetId="55" r:id="rId20"/>
+    <sheet name="giftCardReport++" sheetId="54" r:id="rId21"/>
+    <sheet name="adminUserUpdate++" sheetId="52" r:id="rId22"/>
+    <sheet name="ICUpdateUser++" sheetId="51" r:id="rId23"/>
+    <sheet name="SapCustomer++" sheetId="50" r:id="rId24"/>
     <sheet name="PayUPagePayment++" sheetId="31" r:id="rId25"/>
     <sheet name="CheckoutpaymentOption++" sheetId="32" r:id="rId26"/>
     <sheet name="deliveryPopulation++" sheetId="34" r:id="rId27"/>
@@ -66,7 +66,7 @@
     <sheet name="HiFiCorp" sheetId="30" r:id="rId57"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IC!$A$1:$S$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IC!$A$1:$S$71</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -4850,13 +4850,1901 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" s="111" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A3" s="111">
+        <v>2</v>
+      </c>
+      <c r="B3" s="111" t="s">
+        <v>778</v>
+      </c>
+      <c r="C3" s="111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="111" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A4" s="111">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A5" s="111">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A6" s="111">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A7" s="111">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A8" s="111">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="73" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="73" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="73" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="73"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="73" t="s">
+        <v>414</v>
+      </c>
+      <c r="E1" s="73" t="s">
+        <v>82</v>
+      </c>
+      <c r="F1" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="73" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="72">
+        <v>52</v>
+      </c>
+      <c r="B2" s="72" t="s">
+        <v>530</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>417</v>
+      </c>
+      <c r="F2" s="73" t="s">
+        <v>418</v>
+      </c>
+      <c r="G2" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="72">
+        <v>53</v>
+      </c>
+      <c r="B3" s="72" t="s">
+        <v>529</v>
+      </c>
+      <c r="C3" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E3" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F3" s="73" t="s">
+        <v>666</v>
+      </c>
+      <c r="G3" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="57">
+        <v>54</v>
+      </c>
+      <c r="B4" s="64" t="s">
+        <v>606</v>
+      </c>
+      <c r="C4" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>666</v>
+      </c>
+      <c r="G4" s="73">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="57">
+        <v>55</v>
+      </c>
+      <c r="B5" s="64" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E5" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F5" s="90" t="s">
+        <v>666</v>
+      </c>
+      <c r="G5" s="71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="57">
+        <v>56</v>
+      </c>
+      <c r="B6" s="64" t="s">
+        <v>607</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E6" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F6" s="90" t="s">
+        <v>666</v>
+      </c>
+      <c r="G6" s="71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="71">
+        <v>70</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>619</v>
+      </c>
+      <c r="C7" s="73" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>416</v>
+      </c>
+      <c r="E7" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F7" s="90" t="s">
+        <v>666</v>
+      </c>
+      <c r="G7" s="71">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="90" customFormat="1">
+      <c r="A8" s="122">
+        <v>73</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>619</v>
+      </c>
+      <c r="C8" s="90">
+        <v>1</v>
+      </c>
+      <c r="D8" s="90" t="s">
+        <v>416</v>
+      </c>
+      <c r="E8" s="58" t="s">
+        <v>653</v>
+      </c>
+      <c r="F8" s="90" t="s">
+        <v>688</v>
+      </c>
+      <c r="G8" s="122">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
+      <formula1>"ExistingUser,logedOn_user"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="50" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="50" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="50"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="45">
+        <v>1</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>496</v>
+      </c>
+      <c r="C2" s="51">
+        <v>1</v>
+      </c>
+      <c r="D2" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="45">
+        <v>2</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>497</v>
+      </c>
+      <c r="C3" s="51">
+        <v>1</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="45">
+        <v>3</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>498</v>
+      </c>
+      <c r="C4" s="51">
+        <v>1</v>
+      </c>
+      <c r="D4" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="45">
+        <v>4</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>499</v>
+      </c>
+      <c r="C5" s="51">
+        <v>1</v>
+      </c>
+      <c r="D5" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="45">
+        <v>5</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>500</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="45">
+        <v>6</v>
+      </c>
+      <c r="B7" s="46" t="s">
+        <v>501</v>
+      </c>
+      <c r="C7" s="51">
+        <v>1</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="45">
+        <v>7</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>502</v>
+      </c>
+      <c r="C8" s="51">
+        <v>1</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="45">
+        <v>8</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>503</v>
+      </c>
+      <c r="C9" s="51">
+        <v>1</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="45">
+        <v>9</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>504</v>
+      </c>
+      <c r="C10" s="51">
+        <v>1</v>
+      </c>
+      <c r="D10" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="45">
+        <v>10</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="C11" s="51">
+        <v>1</v>
+      </c>
+      <c r="D11" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="45">
+        <v>11</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="C12" s="51">
+        <v>1</v>
+      </c>
+      <c r="D12" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="45">
+        <v>12</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>521</v>
+      </c>
+      <c r="C13" s="51">
+        <v>1</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="45">
+        <v>13</v>
+      </c>
+      <c r="B14" s="45" t="s">
+        <v>522</v>
+      </c>
+      <c r="C14" s="51">
+        <v>1</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="45">
+        <v>14</v>
+      </c>
+      <c r="B15" s="45" t="s">
+        <v>523</v>
+      </c>
+      <c r="C15" s="51">
+        <v>1</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="45">
+        <v>15</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>505</v>
+      </c>
+      <c r="C16" s="51">
+        <v>1</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="45">
+        <v>16</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>506</v>
+      </c>
+      <c r="C17" s="51">
+        <v>1</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="45">
+        <v>17</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>548</v>
+      </c>
+      <c r="C18" s="51">
+        <v>1</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="45">
+        <v>18</v>
+      </c>
+      <c r="B19" s="45" t="s">
+        <v>524</v>
+      </c>
+      <c r="C19" s="51">
+        <v>1</v>
+      </c>
+      <c r="D19" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="45">
+        <v>19</v>
+      </c>
+      <c r="B20" s="45" t="s">
+        <v>525</v>
+      </c>
+      <c r="C20" s="51">
+        <v>1</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="45">
+        <v>20</v>
+      </c>
+      <c r="B21" s="45" t="s">
+        <v>526</v>
+      </c>
+      <c r="C21" s="51">
+        <v>1</v>
+      </c>
+      <c r="D21" s="51" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="45">
+        <v>31</v>
+      </c>
+      <c r="B22" s="45" t="s">
+        <v>507</v>
+      </c>
+      <c r="C22" s="51">
+        <v>1</v>
+      </c>
+      <c r="D22" s="51" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="47">
+        <v>39</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>508</v>
+      </c>
+      <c r="C23" s="51">
+        <v>1</v>
+      </c>
+      <c r="D23" s="51" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="47">
+        <v>40</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>509</v>
+      </c>
+      <c r="C24" s="51">
+        <v>1</v>
+      </c>
+      <c r="D24" s="51" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="47">
+        <v>41</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>510</v>
+      </c>
+      <c r="C25" s="51">
+        <v>1</v>
+      </c>
+      <c r="D25" s="51" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="130"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A21">
+    <cfRule type="duplicateValues" dxfId="88" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B21">
+    <cfRule type="duplicateValues" dxfId="87" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="duplicateValues" dxfId="86" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B22">
+    <cfRule type="duplicateValues" dxfId="85" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A23:A26">
+    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:B26">
+    <cfRule type="duplicateValues" dxfId="83" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>385</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="38">
+        <v>49</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>515</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="38">
+        <v>50</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>516</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="38">
+        <v>51</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>517</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D4" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>389</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:B4">
+    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="47">
+        <v>48</v>
+      </c>
+      <c r="B2" s="49" t="s">
+        <v>531</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>384</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>371</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>373</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>374</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>375</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="48">
+        <v>47</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>378</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>379</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="J3" s="40" t="s">
+        <v>380</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>381</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
+      <formula1>"Female,Male"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>344</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="48">
+        <v>47</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>348</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
+      <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>353</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36">
+        <v>1</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="I2" s="36">
+        <v>2313</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="48">
+        <v>47</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="36">
+        <v>1</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="I3" s="36">
+        <v>2313</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+      <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
+          </x14:formula1>
+          <xm:sqref>K2:K1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36">
+        <v>1</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>365</v>
+      </c>
+      <c r="E2" s="36">
+        <v>2</v>
+      </c>
+      <c r="F2" s="36">
+        <v>3</v>
+      </c>
+      <c r="G2" s="36">
+        <v>34221</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="48">
+        <v>47</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="36">
+        <v>1</v>
+      </c>
+      <c r="D3" s="41" t="s">
+        <v>365</v>
+      </c>
+      <c r="E3" s="36">
+        <v>2</v>
+      </c>
+      <c r="F3" s="36">
+        <v>3</v>
+      </c>
+      <c r="G3" s="36">
+        <v>34221</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>366</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="36"/>
+    <col min="15" max="15" width="23.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>306</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>308</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>309</v>
+      </c>
+      <c r="H1" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="I1" s="36" t="s">
+        <v>311</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>312</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="L1" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="M1" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="N1" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="O1" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="P1" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="Q1" s="36" t="s">
+        <v>319</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>320</v>
+      </c>
+      <c r="S1" s="36" t="s">
+        <v>321</v>
+      </c>
+      <c r="T1" s="36" t="s">
+        <v>322</v>
+      </c>
+      <c r="U1" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="K2" s="36" t="s">
+        <v>326</v>
+      </c>
+      <c r="L2" s="36" t="s">
+        <v>327</v>
+      </c>
+      <c r="M2" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="N2" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="O2" s="36" t="s">
+        <v>329</v>
+      </c>
+      <c r="P2" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q2" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="S2" s="40" t="s">
+        <v>332</v>
+      </c>
+      <c r="T2" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="U2" s="36" t="s">
+        <v>333</v>
+      </c>
+      <c r="V2" s="36" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" s="48">
+        <v>47</v>
+      </c>
+      <c r="B3" s="49" t="s">
+        <v>413</v>
+      </c>
+      <c r="C3" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="K3" s="36" t="s">
+        <v>336</v>
+      </c>
+      <c r="L3" s="36" t="s">
+        <v>337</v>
+      </c>
+      <c r="M3" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="N3" s="36" t="s">
+        <v>328</v>
+      </c>
+      <c r="O3" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="P3" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="Q3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" s="36" t="s">
+        <v>331</v>
+      </c>
+      <c r="S3" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="T3" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="U3" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="V3" s="36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A3">
+    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B3">
+    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
+  </conditionalFormatting>
+  <dataValidations count="7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
+      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
+      <formula1>"African,Asian,Coloured,White,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
+      <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
+      <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
+      <formula1>"Female,Male"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
+      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="36"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>301</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>302</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="48">
+        <v>46</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>514</v>
+      </c>
+      <c r="C2" s="36">
+        <v>1</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>712</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>305</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4959,7 +6847,7 @@
         <v>495</v>
       </c>
       <c r="F2" s="123" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G2" s="125" t="s">
         <v>108</v>
@@ -4999,7 +6887,7 @@
         <v>495</v>
       </c>
       <c r="F3" s="123" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="125" t="s">
         <v>108</v>
@@ -8670,1481 +10558,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="50" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="50"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="51" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="45">
-        <v>1</v>
-      </c>
-      <c r="B2" s="45" t="s">
-        <v>496</v>
-      </c>
-      <c r="C2" s="51">
-        <v>1</v>
-      </c>
-      <c r="D2" s="51" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="45">
-        <v>2</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>497</v>
-      </c>
-      <c r="C3" s="51">
-        <v>1</v>
-      </c>
-      <c r="D3" s="51" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="45">
-        <v>3</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>498</v>
-      </c>
-      <c r="C4" s="51">
-        <v>1</v>
-      </c>
-      <c r="D4" s="51" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="45">
-        <v>4</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>499</v>
-      </c>
-      <c r="C5" s="51">
-        <v>1</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="45">
-        <v>5</v>
-      </c>
-      <c r="B6" s="45" t="s">
-        <v>500</v>
-      </c>
-      <c r="C6" s="51">
-        <v>1</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="45">
-        <v>6</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>501</v>
-      </c>
-      <c r="C7" s="51">
-        <v>1</v>
-      </c>
-      <c r="D7" s="51" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="45">
-        <v>7</v>
-      </c>
-      <c r="B8" s="45" t="s">
-        <v>502</v>
-      </c>
-      <c r="C8" s="51">
-        <v>1</v>
-      </c>
-      <c r="D8" s="51" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="45">
-        <v>8</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>503</v>
-      </c>
-      <c r="C9" s="51">
-        <v>1</v>
-      </c>
-      <c r="D9" s="51" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="45">
-        <v>9</v>
-      </c>
-      <c r="B10" s="45" t="s">
-        <v>504</v>
-      </c>
-      <c r="C10" s="51">
-        <v>1</v>
-      </c>
-      <c r="D10" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="45">
-        <v>10</v>
-      </c>
-      <c r="B11" s="45" t="s">
-        <v>519</v>
-      </c>
-      <c r="C11" s="51">
-        <v>1</v>
-      </c>
-      <c r="D11" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="45">
-        <v>11</v>
-      </c>
-      <c r="B12" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="C12" s="51">
-        <v>1</v>
-      </c>
-      <c r="D12" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="45">
-        <v>12</v>
-      </c>
-      <c r="B13" s="45" t="s">
-        <v>521</v>
-      </c>
-      <c r="C13" s="51">
-        <v>1</v>
-      </c>
-      <c r="D13" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="45">
-        <v>13</v>
-      </c>
-      <c r="B14" s="45" t="s">
-        <v>522</v>
-      </c>
-      <c r="C14" s="51">
-        <v>1</v>
-      </c>
-      <c r="D14" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="45">
-        <v>14</v>
-      </c>
-      <c r="B15" s="45" t="s">
-        <v>523</v>
-      </c>
-      <c r="C15" s="51">
-        <v>1</v>
-      </c>
-      <c r="D15" s="51" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" s="45">
-        <v>15</v>
-      </c>
-      <c r="B16" s="45" t="s">
-        <v>505</v>
-      </c>
-      <c r="C16" s="51">
-        <v>1</v>
-      </c>
-      <c r="D16" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="45">
-        <v>16</v>
-      </c>
-      <c r="B17" s="45" t="s">
-        <v>506</v>
-      </c>
-      <c r="C17" s="51">
-        <v>1</v>
-      </c>
-      <c r="D17" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" s="45">
-        <v>17</v>
-      </c>
-      <c r="B18" s="45" t="s">
-        <v>548</v>
-      </c>
-      <c r="C18" s="51">
-        <v>1</v>
-      </c>
-      <c r="D18" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" s="45">
-        <v>18</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>524</v>
-      </c>
-      <c r="C19" s="51">
-        <v>1</v>
-      </c>
-      <c r="D19" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="45">
-        <v>19</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>525</v>
-      </c>
-      <c r="C20" s="51">
-        <v>1</v>
-      </c>
-      <c r="D20" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="45">
-        <v>20</v>
-      </c>
-      <c r="B21" s="45" t="s">
-        <v>526</v>
-      </c>
-      <c r="C21" s="51">
-        <v>1</v>
-      </c>
-      <c r="D21" s="51" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="45">
-        <v>31</v>
-      </c>
-      <c r="B22" s="45" t="s">
-        <v>507</v>
-      </c>
-      <c r="C22" s="51">
-        <v>1</v>
-      </c>
-      <c r="D22" s="51" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="47">
-        <v>39</v>
-      </c>
-      <c r="B23" s="47" t="s">
-        <v>508</v>
-      </c>
-      <c r="C23" s="51">
-        <v>1</v>
-      </c>
-      <c r="D23" s="51" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="47">
-        <v>40</v>
-      </c>
-      <c r="B24" s="47" t="s">
-        <v>509</v>
-      </c>
-      <c r="C24" s="51">
-        <v>1</v>
-      </c>
-      <c r="D24" s="51" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="47">
-        <v>41</v>
-      </c>
-      <c r="B25" s="47" t="s">
-        <v>510</v>
-      </c>
-      <c r="C25" s="51">
-        <v>1</v>
-      </c>
-      <c r="D25" s="51" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="130"/>
-      <c r="B26" s="130"/>
-      <c r="C26" s="90"/>
-      <c r="D26" s="90"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="88" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="87" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="86" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="85" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="83" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>385</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="38">
-        <v>49</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>515</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="38">
-        <v>50</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>516</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="38">
-        <v>51</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>517</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>389</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>382</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="47">
-        <v>48</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>531</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>383</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>384</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>367</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>368</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>369</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>370</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>371</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>372</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>373</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>374</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>375</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>378</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>379</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="J2" s="40" t="s">
-        <v>380</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="48">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>377</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>379</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="J3" s="40" t="s">
-        <v>380</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>381</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
-      <formula1>"Female,Male"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>341</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>342</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>343</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>344</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>345</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>347</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>348</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>350</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="48">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>347</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>348</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>349</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>350</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
-      <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
-      <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.28515625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>351</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>352</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>353</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>354</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36">
-        <v>1</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>356</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>357</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>358</v>
-      </c>
-      <c r="I2" s="36">
-        <v>2313</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="48">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="36">
-        <v>1</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>356</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>357</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>73</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>358</v>
-      </c>
-      <c r="I3" s="36">
-        <v>2313</v>
-      </c>
-      <c r="J3" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>359</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
-      <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
-          </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>360</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>361</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>362</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>363</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36">
-        <v>1</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>365</v>
-      </c>
-      <c r="E2" s="36">
-        <v>2</v>
-      </c>
-      <c r="F2" s="36">
-        <v>3</v>
-      </c>
-      <c r="G2" s="36">
-        <v>34221</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="48">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="36">
-        <v>1</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>365</v>
-      </c>
-      <c r="E3" s="36">
-        <v>2</v>
-      </c>
-      <c r="F3" s="36">
-        <v>3</v>
-      </c>
-      <c r="G3" s="36">
-        <v>34221</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>366</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
-      <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.42578125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" style="36"/>
-    <col min="15" max="15" width="23.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>306</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>307</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>308</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>309</v>
-      </c>
-      <c r="H1" s="36" t="s">
-        <v>310</v>
-      </c>
-      <c r="I1" s="36" t="s">
-        <v>311</v>
-      </c>
-      <c r="J1" s="36" t="s">
-        <v>312</v>
-      </c>
-      <c r="K1" s="36" t="s">
-        <v>313</v>
-      </c>
-      <c r="L1" s="36" t="s">
-        <v>314</v>
-      </c>
-      <c r="M1" s="36" t="s">
-        <v>315</v>
-      </c>
-      <c r="N1" s="36" t="s">
-        <v>316</v>
-      </c>
-      <c r="O1" s="36" t="s">
-        <v>317</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>318</v>
-      </c>
-      <c r="Q1" s="36" t="s">
-        <v>319</v>
-      </c>
-      <c r="R1" s="36" t="s">
-        <v>320</v>
-      </c>
-      <c r="S1" s="36" t="s">
-        <v>321</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>322</v>
-      </c>
-      <c r="U1" s="36" t="s">
-        <v>323</v>
-      </c>
-      <c r="V1" s="36" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="H2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="36" t="s">
-        <v>325</v>
-      </c>
-      <c r="K2" s="36" t="s">
-        <v>326</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>327</v>
-      </c>
-      <c r="M2" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="N2" s="36" t="s">
-        <v>328</v>
-      </c>
-      <c r="O2" s="36" t="s">
-        <v>329</v>
-      </c>
-      <c r="P2" s="36" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q2" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="R2" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="S2" s="40" t="s">
-        <v>332</v>
-      </c>
-      <c r="T2" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="U2" s="36" t="s">
-        <v>333</v>
-      </c>
-      <c r="V2" s="36" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" s="48">
-        <v>47</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>413</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="H3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="I3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="J3" s="36" t="s">
-        <v>335</v>
-      </c>
-      <c r="K3" s="36" t="s">
-        <v>336</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>337</v>
-      </c>
-      <c r="M3" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="N3" s="36" t="s">
-        <v>328</v>
-      </c>
-      <c r="O3" s="36" t="s">
-        <v>338</v>
-      </c>
-      <c r="P3" s="36" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q3" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="R3" s="36" t="s">
-        <v>331</v>
-      </c>
-      <c r="S3" s="36" t="s">
-        <v>339</v>
-      </c>
-      <c r="T3" s="36" t="s">
-        <v>295</v>
-      </c>
-      <c r="U3" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="V3" s="36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
-  </conditionalFormatting>
-  <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
-      <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
-      <formula1>"African,Asian,Coloured,White,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
-      <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
-      <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
-      <formula1>"Female,Male"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
-      <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="36"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>301</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>302</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="48">
-        <v>46</v>
-      </c>
-      <c r="B2" s="47" t="s">
-        <v>514</v>
-      </c>
-      <c r="C2" s="36">
-        <v>1</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>712</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>304</v>
-      </c>
-      <c r="F2" s="36" t="s">
-        <v>305</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -10199,130 +10613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="7.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.140625" style="31"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:20" s="130" customFormat="1">
-      <c r="A1" s="172" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="86" t="s">
-        <v>518</v>
-      </c>
-      <c r="C1" s="172" t="s">
-        <v>215</v>
-      </c>
-      <c r="D1" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="86" t="s">
-        <v>85</v>
-      </c>
-      <c r="F1" s="86" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="86" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="86" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="86" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="86" t="s">
-        <v>21</v>
-      </c>
-      <c r="L1" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="86" t="s">
-        <v>24</v>
-      </c>
-      <c r="O1" s="86" t="s">
-        <v>25</v>
-      </c>
-      <c r="P1" s="86" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="86" t="s">
-        <v>297</v>
-      </c>
-      <c r="R1" s="144" t="s">
-        <v>667</v>
-      </c>
-      <c r="S1" s="144" t="s">
-        <v>668</v>
-      </c>
-      <c r="T1" s="144" t="s">
-        <v>734</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" s="130" customFormat="1">
-      <c r="A2" s="141">
-        <v>1</v>
-      </c>
-      <c r="B2" s="130" t="s">
-        <v>496</v>
-      </c>
-      <c r="C2" s="173" t="s">
-        <v>249</v>
-      </c>
-      <c r="D2" s="130" t="s">
-        <v>121</v>
-      </c>
-      <c r="E2" s="130" t="s">
-        <v>495</v>
-      </c>
-      <c r="F2" s="130" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="130" t="s">
-        <v>779</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B2">
-    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -10413,7 +10704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -11081,7 +11372,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
@@ -11748,7 +12039,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
@@ -12208,195 +12499,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="111" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" s="111" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A3" s="111">
-        <v>2</v>
-      </c>
-      <c r="B3" s="111" t="s">
-        <v>778</v>
-      </c>
-      <c r="C3" s="111" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="111" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="111" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="111" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A4" s="111">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A5" s="111">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A6" s="111">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A7" s="111">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A8" s="111">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14313,61 +14415,124 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="7.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="122" customFormat="1">
-      <c r="A1" s="86" t="s">
-        <v>34</v>
+    <row r="1" spans="1:20" s="130" customFormat="1">
+      <c r="A1" s="172" t="s">
+        <v>15</v>
       </c>
       <c r="B1" s="86" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="86" t="s">
-        <v>35</v>
+        <v>518</v>
+      </c>
+      <c r="C1" s="172" t="s">
+        <v>215</v>
       </c>
       <c r="D1" s="86" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="E1" s="86" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="113">
-        <v>1</v>
-      </c>
-      <c r="B2" s="113" t="s">
-        <v>505</v>
-      </c>
-      <c r="C2" s="113">
-        <v>1</v>
-      </c>
-      <c r="D2" s="113" t="s">
-        <v>726</v>
-      </c>
-      <c r="E2" s="138" t="s">
-        <v>167</v>
+        <v>85</v>
+      </c>
+      <c r="F1" s="86" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="86" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="86" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="86" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="86" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="86" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="86" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" s="86" t="s">
+        <v>25</v>
+      </c>
+      <c r="P1" s="86" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" s="86" t="s">
+        <v>297</v>
+      </c>
+      <c r="R1" s="144" t="s">
+        <v>667</v>
+      </c>
+      <c r="S1" s="144" t="s">
+        <v>668</v>
+      </c>
+      <c r="T1" s="144" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="130" customFormat="1">
+      <c r="A2" s="141">
+        <v>1</v>
+      </c>
+      <c r="B2" s="130" t="s">
+        <v>496</v>
+      </c>
+      <c r="C2" s="173" t="s">
+        <v>249</v>
+      </c>
+      <c r="D2" s="130" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="130" t="s">
+        <v>495</v>
+      </c>
+      <c r="F2" s="130" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="130" t="s">
+        <v>779</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-  </hyperlinks>
+  <conditionalFormatting sqref="A2">
+    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B2">
+    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17554,215 +17719,60 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="90" t="s">
+    <row r="1" spans="1:5" s="122" customFormat="1">
+      <c r="A1" s="86" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="90" t="s">
+      <c r="C1" s="86" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="90" t="s">
-        <v>182</v>
-      </c>
-      <c r="E1" s="90" t="s">
-        <v>755</v>
-      </c>
-      <c r="F1" s="90" t="s">
-        <v>756</v>
-      </c>
-      <c r="G1" s="90" t="s">
-        <v>757</v>
-      </c>
-      <c r="H1" s="90" t="s">
-        <v>758</v>
-      </c>
-      <c r="I1" s="90" t="s">
-        <v>761</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="90">
-        <v>87</v>
-      </c>
-      <c r="B2" s="130" t="s">
-        <v>764</v>
-      </c>
-      <c r="C2" s="90">
-        <v>1</v>
-      </c>
-      <c r="D2" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E2" s="90" t="s">
-        <v>759</v>
-      </c>
-      <c r="F2" s="90" t="s">
-        <v>760</v>
-      </c>
-      <c r="G2" s="90"/>
-      <c r="H2" s="90"/>
-      <c r="I2" s="90" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="90">
-        <v>88</v>
-      </c>
-      <c r="B3" s="130" t="s">
-        <v>762</v>
-      </c>
-      <c r="C3" s="90">
-        <v>2</v>
-      </c>
-      <c r="D3" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E3" s="90" t="s">
-        <v>768</v>
-      </c>
-      <c r="F3" s="90" t="s">
-        <v>773</v>
-      </c>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="90">
-        <v>89</v>
-      </c>
-      <c r="B4" s="130" t="s">
-        <v>763</v>
-      </c>
-      <c r="C4" s="90">
-        <v>3</v>
-      </c>
-      <c r="D4" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E4" s="90" t="s">
-        <v>769</v>
-      </c>
-      <c r="F4" s="90" t="s">
-        <v>774</v>
-      </c>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="90">
-        <v>90</v>
-      </c>
-      <c r="B5" s="130" t="s">
-        <v>765</v>
-      </c>
-      <c r="C5" s="90">
-        <v>4</v>
-      </c>
-      <c r="D5" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E5" s="90" t="s">
-        <v>770</v>
-      </c>
-      <c r="F5" s="90" t="s">
-        <v>775</v>
-      </c>
-      <c r="G5" s="90"/>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="90">
-        <v>91</v>
-      </c>
-      <c r="B6" s="130" t="s">
-        <v>766</v>
-      </c>
-      <c r="C6" s="90">
-        <v>5</v>
-      </c>
-      <c r="D6" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E6" s="90" t="s">
-        <v>771</v>
-      </c>
-      <c r="F6" s="90" t="s">
-        <v>776</v>
-      </c>
-      <c r="G6" s="90"/>
-      <c r="H6" s="90">
-        <v>99.998999999999995</v>
-      </c>
-      <c r="I6" s="90" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="90">
-        <v>92</v>
-      </c>
-      <c r="B7" s="130" t="s">
-        <v>767</v>
-      </c>
-      <c r="C7" s="90">
-        <v>6</v>
-      </c>
-      <c r="D7" s="90" t="s">
-        <v>754</v>
-      </c>
-      <c r="E7" s="90" t="s">
-        <v>772</v>
-      </c>
-      <c r="F7" s="90" t="s">
-        <v>775</v>
-      </c>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90">
-        <v>99.998999999999995</v>
-      </c>
-      <c r="I7" s="90" t="s">
-        <v>115</v>
+      <c r="D1" s="86" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="113">
+        <v>1</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>505</v>
+      </c>
+      <c r="C2" s="113">
+        <v>1</v>
+      </c>
+      <c r="D2" s="113" t="s">
+        <v>726</v>
+      </c>
+      <c r="E2" s="138" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
-  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19558,19 +19568,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="A1" s="90" t="s">
         <v>34</v>
       </c>
@@ -19580,28 +19597,186 @@
       <c r="C1" s="90" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="162" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>704</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="112" t="s">
-        <v>711</v>
+      <c r="D1" s="90" t="s">
+        <v>182</v>
+      </c>
+      <c r="E1" s="90" t="s">
+        <v>755</v>
+      </c>
+      <c r="F1" s="90" t="s">
+        <v>756</v>
+      </c>
+      <c r="G1" s="90" t="s">
+        <v>757</v>
+      </c>
+      <c r="H1" s="90" t="s">
+        <v>758</v>
+      </c>
+      <c r="I1" s="90" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="90">
+        <v>87</v>
+      </c>
+      <c r="B2" s="130" t="s">
+        <v>764</v>
+      </c>
+      <c r="C2" s="90">
+        <v>1</v>
+      </c>
+      <c r="D2" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E2" s="90" t="s">
+        <v>759</v>
+      </c>
+      <c r="F2" s="90" t="s">
+        <v>760</v>
+      </c>
+      <c r="G2" s="90"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="90">
+        <v>88</v>
+      </c>
+      <c r="B3" s="130" t="s">
+        <v>762</v>
+      </c>
+      <c r="C3" s="90">
+        <v>2</v>
+      </c>
+      <c r="D3" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E3" s="90" t="s">
+        <v>768</v>
+      </c>
+      <c r="F3" s="90" t="s">
+        <v>773</v>
+      </c>
+      <c r="G3" s="90"/>
+      <c r="H3" s="90"/>
+      <c r="I3" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="90">
+        <v>89</v>
+      </c>
+      <c r="B4" s="130" t="s">
+        <v>763</v>
+      </c>
+      <c r="C4" s="90">
+        <v>3</v>
+      </c>
+      <c r="D4" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E4" s="90" t="s">
+        <v>769</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>774</v>
+      </c>
+      <c r="G4" s="90"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="90">
+        <v>90</v>
+      </c>
+      <c r="B5" s="130" t="s">
+        <v>765</v>
+      </c>
+      <c r="C5" s="90">
+        <v>4</v>
+      </c>
+      <c r="D5" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E5" s="90" t="s">
+        <v>770</v>
+      </c>
+      <c r="F5" s="90" t="s">
+        <v>775</v>
+      </c>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90"/>
+      <c r="I5" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="90">
+        <v>91</v>
+      </c>
+      <c r="B6" s="130" t="s">
+        <v>766</v>
+      </c>
+      <c r="C6" s="90">
+        <v>5</v>
+      </c>
+      <c r="D6" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E6" s="90" t="s">
+        <v>771</v>
+      </c>
+      <c r="F6" s="90" t="s">
+        <v>776</v>
+      </c>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90">
+        <v>99.998999999999995</v>
+      </c>
+      <c r="I6" s="90" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="90">
+        <v>92</v>
+      </c>
+      <c r="B7" s="130" t="s">
+        <v>767</v>
+      </c>
+      <c r="C7" s="90">
+        <v>6</v>
+      </c>
+      <c r="D7" s="90" t="s">
+        <v>754</v>
+      </c>
+      <c r="E7" s="90" t="s">
+        <v>772</v>
+      </c>
+      <c r="F7" s="90" t="s">
+        <v>775</v>
+      </c>
+      <c r="G7" s="90"/>
+      <c r="H7" s="90">
+        <v>99.998999999999995</v>
+      </c>
+      <c r="I7" s="90" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-  </hyperlinks>
+  <conditionalFormatting sqref="B2:B6">
+    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7">
+    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21887,6 +22062,56 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="90" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="90" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="162" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="112" t="s">
+        <v>711</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21941,7 +22166,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -22046,7 +22271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -22207,231 +22432,6 @@
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="5" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" style="73" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" style="73" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="73" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="73" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="73"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="73" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="73" t="s">
-        <v>414</v>
-      </c>
-      <c r="E1" s="73" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="73" t="s">
-        <v>83</v>
-      </c>
-      <c r="G1" s="73" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="72">
-        <v>52</v>
-      </c>
-      <c r="B2" s="72" t="s">
-        <v>530</v>
-      </c>
-      <c r="C2" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>417</v>
-      </c>
-      <c r="F2" s="73" t="s">
-        <v>418</v>
-      </c>
-      <c r="G2" s="73">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="72">
-        <v>53</v>
-      </c>
-      <c r="B3" s="72" t="s">
-        <v>529</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E3" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F3" s="73" t="s">
-        <v>666</v>
-      </c>
-      <c r="G3" s="73">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="57">
-        <v>54</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>606</v>
-      </c>
-      <c r="C4" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F4" s="90" t="s">
-        <v>666</v>
-      </c>
-      <c r="G4" s="73">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="57">
-        <v>55</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>605</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E5" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F5" s="90" t="s">
-        <v>666</v>
-      </c>
-      <c r="G5" s="71">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="57">
-        <v>56</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>607</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E6" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F6" s="90" t="s">
-        <v>666</v>
-      </c>
-      <c r="G6" s="71">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" s="71">
-        <v>70</v>
-      </c>
-      <c r="B7" s="64" t="s">
-        <v>619</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="D7" s="73" t="s">
-        <v>416</v>
-      </c>
-      <c r="E7" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F7" s="90" t="s">
-        <v>666</v>
-      </c>
-      <c r="G7" s="71">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="90" customFormat="1">
-      <c r="A8" s="122">
-        <v>73</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>619</v>
-      </c>
-      <c r="C8" s="90">
-        <v>1</v>
-      </c>
-      <c r="D8" s="90" t="s">
-        <v>416</v>
-      </c>
-      <c r="E8" s="58" t="s">
-        <v>653</v>
-      </c>
-      <c r="F8" s="90" t="s">
-        <v>688</v>
-      </c>
-      <c r="G8" s="122">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
-  </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
-      <formula1>"ExistingUser,logedOn_user"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com"/>
-    <hyperlink ref="E8" r:id="rId4"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updated xpath for existing account error
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E7877C8-562E-4558-928F-4A2D8295C872}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6198B354-EFD5-4F40-AA57-90BCB6EA844B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="49" activeTab="51" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IC" sheetId="23" r:id="rId1"/>
@@ -4984,25 +4984,25 @@
       <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11" style="61" customWidth="1"/>
-    <col min="2" max="2" width="93.54296875" style="130" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="61" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="90.7265625" style="130" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="130" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.1796875" style="130" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.26953125" style="130" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.54296875" style="130" customWidth="1"/>
-    <col min="9" max="9" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.7265625" style="130" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="27.1796875" style="130" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="31.453125" style="130" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.26953125" style="130" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.1796875" style="130" customWidth="1"/>
-    <col min="19" max="16384" width="9.1796875" style="130"/>
+    <col min="2" max="2" width="93.5703125" style="130" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="61" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="90.7109375" style="130" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="130" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="130" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" style="130" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.5703125" style="130" customWidth="1"/>
+    <col min="9" max="9" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="31.7109375" style="130" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="27.140625" style="130" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="31.42578125" style="130" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.28515625" style="130" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.140625" style="130" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="130"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -5067,7 +5067,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="29">
+    <row r="2" spans="1:20" ht="30">
       <c r="A2" s="139">
         <v>1</v>
       </c>
@@ -5107,7 +5107,7 @@
       <c r="O2" s="123"/>
       <c r="P2" s="123"/>
     </row>
-    <row r="3" spans="1:20" ht="29">
+    <row r="3" spans="1:20" ht="30">
       <c r="A3" s="139">
         <v>2</v>
       </c>
@@ -5148,7 +5148,7 @@
       <c r="P3" s="123"/>
       <c r="Q3" s="123"/>
     </row>
-    <row r="4" spans="1:20" ht="29">
+    <row r="4" spans="1:20" ht="30">
       <c r="A4" s="139">
         <v>3</v>
       </c>
@@ -5187,7 +5187,7 @@
       <c r="P4" s="123"/>
       <c r="Q4" s="123"/>
     </row>
-    <row r="5" spans="1:20" ht="29">
+    <row r="5" spans="1:20" ht="30">
       <c r="A5" s="139">
         <v>4</v>
       </c>
@@ -5228,7 +5228,7 @@
       <c r="P5" s="123"/>
       <c r="Q5" s="123"/>
     </row>
-    <row r="6" spans="1:20" ht="29">
+    <row r="6" spans="1:20" ht="30">
       <c r="A6" s="139">
         <v>5</v>
       </c>
@@ -5269,7 +5269,7 @@
       <c r="P6" s="123"/>
       <c r="Q6" s="123"/>
     </row>
-    <row r="7" spans="1:20" ht="29">
+    <row r="7" spans="1:20" ht="30">
       <c r="A7" s="136">
         <v>6</v>
       </c>
@@ -5308,7 +5308,7 @@
       <c r="P7" s="123"/>
       <c r="Q7" s="123"/>
     </row>
-    <row r="8" spans="1:20" ht="29">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="136">
         <v>7</v>
       </c>
@@ -5347,7 +5347,7 @@
       <c r="P8" s="123"/>
       <c r="Q8" s="123"/>
     </row>
-    <row r="9" spans="1:20" ht="29">
+    <row r="9" spans="1:20" ht="30">
       <c r="A9" s="136">
         <v>8</v>
       </c>
@@ -5384,7 +5384,7 @@
       <c r="P9" s="123"/>
       <c r="Q9" s="123"/>
     </row>
-    <row r="10" spans="1:20" ht="29">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="136">
         <v>9</v>
       </c>
@@ -5423,7 +5423,7 @@
       <c r="P10" s="123"/>
       <c r="Q10" s="123"/>
     </row>
-    <row r="11" spans="1:20" ht="29">
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" s="136">
         <v>10</v>
       </c>
@@ -5462,7 +5462,7 @@
       <c r="P11" s="123"/>
       <c r="Q11" s="123"/>
     </row>
-    <row r="12" spans="1:20" ht="29">
+    <row r="12" spans="1:20" ht="30">
       <c r="A12" s="136">
         <v>11</v>
       </c>
@@ -5501,7 +5501,7 @@
       <c r="P12" s="123"/>
       <c r="Q12" s="123"/>
     </row>
-    <row r="13" spans="1:20" ht="29">
+    <row r="13" spans="1:20" ht="30">
       <c r="A13" s="136">
         <v>12</v>
       </c>
@@ -5540,7 +5540,7 @@
       <c r="P13" s="123"/>
       <c r="Q13" s="123"/>
     </row>
-    <row r="14" spans="1:20" ht="29">
+    <row r="14" spans="1:20" ht="30">
       <c r="A14" s="139">
         <v>13</v>
       </c>
@@ -5579,7 +5579,7 @@
       <c r="P14" s="123"/>
       <c r="Q14" s="123"/>
     </row>
-    <row r="15" spans="1:20" ht="29">
+    <row r="15" spans="1:20" ht="30">
       <c r="A15" s="139">
         <v>14</v>
       </c>
@@ -5618,7 +5618,7 @@
       <c r="P15" s="123"/>
       <c r="Q15" s="123"/>
     </row>
-    <row r="16" spans="1:20" ht="29">
+    <row r="16" spans="1:20" ht="30">
       <c r="A16" s="146">
         <v>15</v>
       </c>
@@ -5661,7 +5661,7 @@
       <c r="P16" s="123"/>
       <c r="Q16" s="123"/>
     </row>
-    <row r="17" spans="1:17" ht="29">
+    <row r="17" spans="1:17" ht="30">
       <c r="A17" s="146">
         <v>16</v>
       </c>
@@ -5704,7 +5704,7 @@
       <c r="P17" s="123"/>
       <c r="Q17" s="123"/>
     </row>
-    <row r="18" spans="1:17" ht="29">
+    <row r="18" spans="1:17" ht="30">
       <c r="A18" s="146">
         <v>17</v>
       </c>
@@ -5747,7 +5747,7 @@
       <c r="P18" s="123"/>
       <c r="Q18" s="123"/>
     </row>
-    <row r="19" spans="1:17" ht="29">
+    <row r="19" spans="1:17" ht="30">
       <c r="A19" s="146">
         <v>18</v>
       </c>
@@ -5790,7 +5790,7 @@
       <c r="P19" s="123"/>
       <c r="Q19" s="123"/>
     </row>
-    <row r="20" spans="1:17" ht="29">
+    <row r="20" spans="1:17" ht="30">
       <c r="A20" s="146">
         <v>19</v>
       </c>
@@ -5833,7 +5833,7 @@
       <c r="P20" s="123"/>
       <c r="Q20" s="123"/>
     </row>
-    <row r="21" spans="1:17" ht="29">
+    <row r="21" spans="1:17" ht="30">
       <c r="A21" s="146">
         <v>20</v>
       </c>
@@ -6597,7 +6597,7 @@
       <c r="O39" s="123"/>
       <c r="P39" s="123"/>
     </row>
-    <row r="40" spans="1:20" ht="29">
+    <row r="40" spans="1:20" ht="45">
       <c r="A40" s="141">
         <v>39</v>
       </c>
@@ -6655,7 +6655,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="29">
+    <row r="41" spans="1:20" ht="45">
       <c r="A41" s="141">
         <v>40</v>
       </c>
@@ -6713,7 +6713,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="29">
+    <row r="42" spans="1:20" ht="45">
       <c r="A42" s="141">
         <v>41</v>
       </c>
@@ -8801,16 +8801,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="73" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="73" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="73" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="73" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="73" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" style="73" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.54296875" style="73" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="73" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" style="73" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="73"/>
+    <col min="8" max="16384" width="9.140625" style="73"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -9028,13 +9028,13 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="50" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="50"/>
+    <col min="5" max="16384" width="9.140625" style="50"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -9427,14 +9427,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9521,14 +9521,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="15.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -9584,22 +9584,22 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="36"/>
+    <col min="13" max="13" width="17.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13">
@@ -9752,18 +9752,18 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="29.26953125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="22.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.28515625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -9883,21 +9883,21 @@
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.26953125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="36"/>
+    <col min="10" max="10" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -10041,17 +10041,17 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.453125" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="36"/>
+    <col min="8" max="8" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -10157,31 +10157,31 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="44.453125" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="44.42578125" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.1796875" style="36" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.140625" style="36" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.1796875" style="36"/>
-    <col min="15" max="15" width="23.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.7265625" style="36" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.1796875" style="36"/>
+    <col min="14" max="14" width="9.140625" style="36"/>
+    <col min="15" max="15" width="23.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -10431,15 +10431,15 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="36" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="36" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="36"/>
+    <col min="4" max="4" width="20.140625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -10498,26 +10498,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="48.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7265625" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="31" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="7.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="16" max="20" width="8.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="31"/>
+    <col min="7" max="7" width="20.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="7.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="16" max="20" width="8.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="130" customFormat="1">
@@ -10645,7 +10645,7 @@
         <v>195</v>
       </c>
       <c r="F4" s="31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="31" t="s">
         <v>802</v>
@@ -10668,7 +10668,7 @@
         <v>195</v>
       </c>
       <c r="F5" s="31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G5" s="31" t="s">
         <v>802</v>
@@ -10692,10 +10692,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.81640625" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="35" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="35"/>
@@ -10749,18 +10749,18 @@
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1796875" style="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1796875" style="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" style="29" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="29" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18" style="29" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="29"/>
+    <col min="10" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -10844,42 +10844,42 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.81640625" style="11" customWidth="1"/>
-    <col min="14" max="14" width="20.26953125" style="11" customWidth="1"/>
-    <col min="15" max="15" width="31.453125" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="28.54296875" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="11" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="11" customWidth="1"/>
+    <col min="15" max="15" width="31.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.26953125" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.81640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="30" style="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="30.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" style="11" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="27.1796875" style="11" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.1796875" style="11" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="11.54296875" style="11" customWidth="1"/>
-    <col min="31" max="16384" width="8.7265625" style="11"/>
+    <col min="27" max="27" width="23.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="27.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.140625" style="11" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" style="11" customWidth="1"/>
+    <col min="31" max="16384" width="8.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" ht="30">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -11506,38 +11506,38 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" style="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.26953125" style="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.54296875" style="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="28.1796875" style="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="27.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="28.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18" style="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="25" style="12" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.81640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.453125" style="12" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.7265625" style="12" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="30.26953125" style="12" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.7109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="30.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="20" style="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="27.1796875" style="12" bestFit="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.7265625" style="12"/>
+    <col min="28" max="28" width="23.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="27.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.7109375" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -12179,14 +12179,14 @@
       <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.7265625" style="1"/>
+    <col min="4" max="4" width="43.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12638,15 +12638,15 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -12825,19 +12825,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.26953125" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="38" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.54296875" style="38" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" style="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" style="38" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="38" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="38" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.1796875" style="38"/>
+    <col min="11" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="55" customFormat="1">
@@ -13272,12 +13272,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -13511,26 +13511,26 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.54296875" style="29" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.81640625" style="29" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="4" customFormat="1" ht="29">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A1" s="37" t="s">
         <v>34</v>
       </c>
@@ -13780,7 +13780,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:16" s="4" customFormat="1">
+    <row r="6" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -13830,7 +13830,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="29">
+    <row r="7" spans="1:16" s="4" customFormat="1" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -14393,11 +14393,11 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.1796875" style="29"/>
+    <col min="1" max="1" width="21.140625" style="29"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="21.1796875" style="29"/>
+    <col min="3" max="3" width="21.140625" style="29"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -14417,7 +14417,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="45">
         <v>1</v>
       </c>
@@ -14428,7 +14428,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="45">
         <v>2</v>
       </c>
@@ -14439,7 +14439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="45">
         <v>3</v>
       </c>
@@ -14450,7 +14450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="29">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="45">
         <v>4</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="45">
         <v>5</v>
       </c>
@@ -14516,7 +14516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" ht="30">
       <c r="A11" s="45">
         <v>19</v>
       </c>
@@ -14563,21 +14563,21 @@
       <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" customWidth="1"/>
-    <col min="9" max="9" width="13.08984375" customWidth="1"/>
-    <col min="13" max="14" width="12.08984375" customWidth="1"/>
-    <col min="15" max="15" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7265625" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" customWidth="1"/>
+    <col min="15" max="15" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1">
+    <row r="1" spans="1:17" s="4" customFormat="1" ht="30">
       <c r="A1" s="120" t="s">
         <v>34</v>
       </c>
@@ -14695,20 +14695,20 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.81640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.7265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="6"/>
+    <col min="4" max="4" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -14870,12 +14870,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.7265625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" style="11" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -14892,7 +14892,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -14906,7 +14906,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="29">
+    <row r="3" spans="1:4" s="1" customFormat="1" ht="45">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -14920,7 +14920,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -14948,7 +14948,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -14962,7 +14962,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -15018,7 +15018,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29">
+    <row r="11" spans="1:4" ht="30">
       <c r="A11" s="142">
         <v>40</v>
       </c>
@@ -15032,7 +15032,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="29">
+    <row r="12" spans="1:4" ht="45">
       <c r="A12" s="61">
         <v>41</v>
       </c>
@@ -15107,14 +15107,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -15367,14 +15367,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="38" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="38" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="38" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="38" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="38"/>
+    <col min="5" max="5" width="13.5703125" style="38" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -15454,7 +15454,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="29">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -15630,14 +15630,14 @@
       <selection pane="bottomRight" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="1"/>
+    <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -16309,13 +16309,13 @@
       <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.26953125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="11"/>
+    <col min="4" max="4" width="7.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -16332,7 +16332,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29">
+    <row r="2" spans="1:4" ht="30">
       <c r="A2" s="16">
         <v>26</v>
       </c>
@@ -16344,7 +16344,7 @@
       </c>
       <c r="D2" s="16"/>
     </row>
-    <row r="3" spans="1:4" ht="29">
+    <row r="3" spans="1:4" ht="45">
       <c r="A3" s="16">
         <v>27</v>
       </c>
@@ -16356,7 +16356,7 @@
       </c>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:4" ht="29">
+    <row r="4" spans="1:4" ht="45">
       <c r="A4" s="16">
         <v>28</v>
       </c>
@@ -16368,7 +16368,7 @@
       </c>
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:4" ht="29">
+    <row r="5" spans="1:4" ht="30">
       <c r="A5" s="16">
         <v>29</v>
       </c>
@@ -16380,7 +16380,7 @@
       </c>
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="29">
+    <row r="6" spans="1:4" ht="30">
       <c r="A6" s="16">
         <v>30</v>
       </c>
@@ -16392,7 +16392,7 @@
       </c>
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:4" ht="29">
+    <row r="7" spans="1:4" ht="30">
       <c r="A7" s="16">
         <v>31</v>
       </c>
@@ -16452,7 +16452,7 @@
       </c>
       <c r="D11" s="115"/>
     </row>
-    <row r="12" spans="1:4" ht="29">
+    <row r="12" spans="1:4" ht="30">
       <c r="A12" s="16">
         <v>39</v>
       </c>
@@ -16464,7 +16464,7 @@
       </c>
       <c r="D12" s="16"/>
     </row>
-    <row r="13" spans="1:4" ht="29">
+    <row r="13" spans="1:4" ht="30">
       <c r="A13" s="16">
         <v>40</v>
       </c>
@@ -16476,7 +16476,7 @@
       </c>
       <c r="D13" s="16"/>
     </row>
-    <row r="14" spans="1:4" ht="43.5">
+    <row r="14" spans="1:4" ht="45">
       <c r="A14" s="16">
         <v>41</v>
       </c>
@@ -16546,23 +16546,23 @@
       <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="82" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="82" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="82" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="82" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.54296875" style="82" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" style="82" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.81640625" style="82" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7265625" style="82" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.26953125" style="82" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.26953125" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="82"/>
+    <col min="4" max="4" width="20.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="102.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="82" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="82" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" style="82" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" style="82" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="82"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="30">
       <c r="A1" s="78" t="s">
         <v>34</v>
       </c>
@@ -16661,7 +16661,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="29">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="83">
         <v>28</v>
       </c>
@@ -16757,7 +16757,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="12.65" customHeight="1">
+    <row r="7" spans="1:11" ht="12.6" customHeight="1">
       <c r="A7" s="83">
         <v>31</v>
       </c>
@@ -17301,7 +17301,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="29">
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="85">
         <v>61</v>
       </c>
@@ -17558,7 +17558,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="113" customFormat="1" ht="29">
+    <row r="32" spans="1:11" s="113" customFormat="1" ht="30">
       <c r="A32" s="113">
         <v>78</v>
       </c>
@@ -17688,13 +17688,13 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -17751,9 +17751,9 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" style="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.28515625" style="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -17859,14 +17859,14 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="31"/>
+    <col min="4" max="4" width="18.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -17969,14 +17969,14 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.1796875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" style="31" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="31"/>
+    <col min="4" max="4" width="22.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="122" customFormat="1">
@@ -18029,14 +18029,14 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -18113,14 +18113,14 @@
       <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="96" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="96" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="96" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="96" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="96" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.1796875" style="96" customWidth="1"/>
-    <col min="6" max="16384" width="9.1796875" style="96"/>
+    <col min="5" max="5" width="23.140625" style="96" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="96"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18480,7 +18480,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="14.15" customHeight="1">
+    <row r="22" spans="1:5" ht="14.1" customHeight="1">
       <c r="A22" s="57">
         <v>64</v>
       </c>
@@ -18610,10 +18610,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -18786,15 +18786,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -18883,13 +18883,13 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -18939,20 +18939,20 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -19047,14 +19047,14 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -19179,19 +19179,19 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -19316,12 +19316,12 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1">
@@ -19338,7 +19338,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24.65" customHeight="1">
+    <row r="2" spans="1:4" ht="24.6" customHeight="1">
       <c r="A2" s="3">
         <v>9</v>
       </c>
@@ -19349,7 +19349,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="111" customFormat="1" ht="24.65" customHeight="1">
+    <row r="3" spans="1:4" s="111" customFormat="1" ht="24.6" customHeight="1">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -19373,24 +19373,24 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.1796875" style="1"/>
+    <col min="12" max="12" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29">
+    <row r="1" spans="1:12" ht="30">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -19496,7 +19496,7 @@
       </c>
       <c r="L3" s="16"/>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" s="16">
         <v>8</v>
       </c>
@@ -19861,17 +19861,17 @@
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -20076,9 +20076,9 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -20120,28 +20120,28 @@
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="121" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.1796875" style="121" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.140625" style="121" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="121" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.81640625" style="121" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.7265625" style="121" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="121" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" style="121" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11" style="121" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.81640625" style="121" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7265625" style="121" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.26953125" style="121" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.1796875" style="121" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.54296875" style="121" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.7265625" style="121" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.453125" style="121" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.1796875" style="121" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="9.1796875" style="121"/>
+    <col min="12" max="12" width="20.85546875" style="121" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" style="121" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.28515625" style="121" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" style="121" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" style="121" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" style="121" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.42578125" style="121" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" style="121" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="121"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -20640,7 +20640,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" ht="30">
       <c r="A9" s="115">
         <v>23</v>
       </c>
@@ -20702,7 +20702,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" ht="30">
       <c r="A10" s="115">
         <v>24</v>
       </c>
@@ -21295,31 +21295,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BA059A5-BADB-4EB7-9063-D7858E2E7132}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="67.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="121" customFormat="1">
@@ -21659,14 +21659,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="13" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1">
@@ -21763,12 +21763,12 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1">
@@ -21967,14 +21967,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -22071,14 +22071,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -22175,9 +22175,9 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -22548,14 +22548,14 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -22652,14 +22652,14 @@
       <selection activeCell="Y27" sqref="Y27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="12" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1">
@@ -22756,10 +22756,10 @@
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -22806,10 +22806,10 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -22862,12 +22862,12 @@
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="81" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="81" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="81" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="81" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.1796875" style="81"/>
+    <col min="4" max="16384" width="9.140625" style="81"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -22967,13 +22967,13 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="76" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.81640625" style="76" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="76" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="76" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.26953125" style="76" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="76"/>
+    <col min="4" max="4" width="19.28515625" style="76" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="76"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -23125,15 +23125,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -23142,7 +23133,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -23291,24 +23282,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -23316,7 +23299,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -23333,4 +23316,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
testing 432 and 423
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425" firstSheet="45" activeTab="47"/>
+    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425" firstSheet="8" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="evs_SAP_OrderRelated++" sheetId="93" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3608" uniqueCount="849">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3619" uniqueCount="851">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2755,6 +2755,12 @@
   </si>
   <si>
     <t>Credit Card (Processed By PayU)|Visa Checkout|EFT Pro (Processed By PayU)|Masterpass|Zapper, SnapScan &amp; Card (PayGate)|Cash Deposits</t>
+  </si>
+  <si>
+    <t>Clear Shopping Cart</t>
+  </si>
+  <si>
+    <t>evs_ClearCart</t>
   </si>
 </sst>
 </file>
@@ -3483,7 +3489,47 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="168">
+  <dxfs count="172">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5778,7 +5824,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="114" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -6368,7 +6414,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -6455,7 +6501,36 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="E3" s="163"/>
+      <c r="A3" s="101">
+        <v>8</v>
+      </c>
+      <c r="B3" s="63" t="s">
+        <v>849</v>
+      </c>
+      <c r="C3" s="110">
+        <v>1</v>
+      </c>
+      <c r="D3" s="184" t="s">
+        <v>147</v>
+      </c>
+      <c r="E3" s="184" t="s">
+        <v>835</v>
+      </c>
+      <c r="F3" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="G3" s="110" t="s">
+        <v>395</v>
+      </c>
+      <c r="H3" s="110">
+        <v>2</v>
+      </c>
+      <c r="I3" s="110">
+        <v>6</v>
+      </c>
+      <c r="J3" s="110" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="4" spans="1:11">
       <c r="E4" s="163"/>
@@ -6465,10 +6540,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="113" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F3">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6485,7 +6563,7 @@
           <x14:formula1>
             <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D1048576</xm:sqref>
+          <xm:sqref>D4:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7782,34 +7860,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="112" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="111" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="110" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="109" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="108" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="107" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="106" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="105" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="104" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="103" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
@@ -9089,22 +9167,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="102" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="101" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="98" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="97" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
@@ -9537,10 +9615,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9748,10 +9826,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="94" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="93" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="69"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9902,16 +9980,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="92" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="91" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
@@ -10127,10 +10205,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -10522,22 +10600,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="86" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="85" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="84" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="83" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -10634,7 +10712,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10694,10 +10772,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10987,10 +11065,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11115,10 +11193,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11267,10 +11345,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -11394,10 +11472,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11650,10 +11728,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
@@ -11745,10 +11823,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11800,10 +11878,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12533,22 +12611,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="63" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="62" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="60" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="59" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="58" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
@@ -13209,22 +13287,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="53" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
@@ -13770,10 +13848,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -14282,13 +14360,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -14552,13 +14630,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -15526,16 +15604,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="43" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="41" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -15710,16 +15788,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16138,10 +16216,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -16440,13 +16518,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -16459,7 +16537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15:E17"/>
     </sheetView>
   </sheetViews>
@@ -16742,13 +16820,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -16991,22 +17069,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="29" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="28" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="27" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="25" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="24" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -17599,31 +17677,31 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="167" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="166" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="165" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="164" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="163" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="duplicateValues" dxfId="162" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="161" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="160" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="159" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -18565,25 +18643,25 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="23" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="20" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="19" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="18" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="17" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -18822,25 +18900,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="16" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="15" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="14" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="13" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -20075,22 +20153,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="8" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="5" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="4" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
@@ -24607,121 +24685,121 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="158" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="157" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="156" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="155" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="154" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="153" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="152" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="151" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="150" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="149" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="148" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="147" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="146" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="145" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="144" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="143" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="142" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="141" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="140" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="139" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="138" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="137" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="136" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="135" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="134" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="133" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="132" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="131" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="130" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="129" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="128" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="127" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:I91">
-    <cfRule type="duplicateValues" dxfId="126" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="125" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="124" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="123" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="122" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92:G93">
-    <cfRule type="duplicateValues" dxfId="121" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="duplicateValues" dxfId="120" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
@@ -25148,13 +25226,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25480,21 +25558,50 @@
         <v>834</v>
       </c>
     </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="185">
+        <v>8</v>
+      </c>
+      <c r="B9" s="186" t="s">
+        <v>849</v>
+      </c>
+      <c r="C9" s="33">
+        <v>423</v>
+      </c>
+      <c r="D9" s="186" t="s">
+        <v>849</v>
+      </c>
+      <c r="F9" s="186" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="116" t="s">
+        <v>800</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>850</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="119" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="118" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="duplicateValues" dxfId="117" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
-    <cfRule type="duplicateValues" dxfId="116" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="115" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="99"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D9">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
@@ -25509,6 +25616,7 @@
     <hyperlink ref="O2" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
     <hyperlink ref="L2" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
     <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -25516,15 +25624,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -25533,7 +25632,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25682,24 +25781,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -25707,7 +25798,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25724,4 +25815,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add TA515_TA437  changes to main
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="-3510" yWindow="-10905" windowWidth="19425" windowHeight="10425" firstSheet="13" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="evs_SAP_OrderRelated++" sheetId="93" r:id="rId1"/>
@@ -200,7 +200,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3630" uniqueCount="853">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3662" uniqueCount="859">
   <si>
     <t>testSuitID</t>
   </si>
@@ -2767,6 +2767,24 @@
   </si>
   <si>
     <t>evs_IncreaseQuanityInCart</t>
+  </si>
+  <si>
+    <t>Remove some items from the cart and verify</t>
+  </si>
+  <si>
+    <t>evs_RemoveItemsFromCart</t>
+  </si>
+  <si>
+    <t>JOST Steel Wire Ironing Board 02A#Sleepmasters Santiago 152cm (Queen) Firm Bed Set#Ottawa Dining Chair</t>
+  </si>
+  <si>
+    <t>Add One Item to the Cart and Verify</t>
+  </si>
+  <si>
+    <t>Add the same Item multiple Times and Verify</t>
+  </si>
+  <si>
+    <t>Ottawa Dining Chair</t>
   </si>
 </sst>
 </file>
@@ -3024,7 +3042,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3420,9 +3438,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3437,9 +3452,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3468,12 +3480,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -3487,6 +3493,15 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3495,7 +3510,57 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="172">
+  <dxfs count="177">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5593,7 +5658,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -5648,7 +5713,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="54" customFormat="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="174" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="53" t="s">
@@ -5683,31 +5748,31 @@
       <c r="A2" s="103">
         <v>1</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="167" t="s">
         <v>829</v>
       </c>
-      <c r="C2" s="169">
-        <v>1</v>
-      </c>
-      <c r="D2" s="169" t="s">
+      <c r="C2" s="168">
+        <v>1</v>
+      </c>
+      <c r="D2" s="168" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="169" t="s">
+      <c r="E2" s="168" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="169" t="s">
+      <c r="F2" s="168" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="169" t="s">
+      <c r="G2" s="168" t="s">
         <v>78</v>
       </c>
-      <c r="H2" s="169" t="s">
+      <c r="H2" s="168" t="s">
         <v>79</v>
       </c>
-      <c r="I2" s="169" t="s">
+      <c r="I2" s="168" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="169"/>
+      <c r="J2" s="168"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -5733,7 +5798,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="173" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -5750,13 +5815,13 @@
       <c r="A2" s="103">
         <v>1</v>
       </c>
-      <c r="B2" s="168" t="s">
+      <c r="B2" s="167" t="s">
         <v>829</v>
       </c>
-      <c r="C2" s="168">
-        <v>1</v>
-      </c>
-      <c r="D2" s="168" t="s">
+      <c r="C2" s="167">
+        <v>1</v>
+      </c>
+      <c r="D2" s="167" t="s">
         <v>830</v>
       </c>
     </row>
@@ -5791,7 +5856,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -5811,7 +5876,7 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="170" t="s">
+      <c r="A2" s="169" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="42" t="s">
@@ -5830,7 +5895,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="114" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -5865,7 +5930,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="4" customFormat="1" ht="30">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="171" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="108" t="s">
@@ -5963,7 +6028,7 @@
       <c r="O2" s="100" t="s">
         <v>828</v>
       </c>
-      <c r="P2" s="166" t="s">
+      <c r="P2" s="165" t="s">
         <v>816</v>
       </c>
       <c r="Q2" s="99" t="s">
@@ -6011,7 +6076,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="109" customFormat="1">
-      <c r="A1" s="174" t="s">
+      <c r="A1" s="172" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="81" t="s">
@@ -6103,7 +6168,7 @@
       <c r="J2" s="30">
         <v>11117</v>
       </c>
-      <c r="K2" s="171" t="s">
+      <c r="K2" s="170" t="s">
         <v>805</v>
       </c>
       <c r="L2" s="30" t="s">
@@ -6115,7 +6180,7 @@
       <c r="N2" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="O2" s="171" t="s">
+      <c r="O2" s="170" t="s">
         <v>807</v>
       </c>
       <c r="P2" s="30" t="s">
@@ -6165,7 +6230,7 @@
       <c r="J3" s="30">
         <v>11117</v>
       </c>
-      <c r="K3" s="171" t="s">
+      <c r="K3" s="170" t="s">
         <v>809</v>
       </c>
       <c r="L3" s="30" t="s">
@@ -6177,7 +6242,7 @@
       <c r="N3" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="O3" s="171" t="s">
+      <c r="O3" s="170" t="s">
         <v>810</v>
       </c>
       <c r="P3" s="30" t="s">
@@ -6414,60 +6479,60 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5" style="101" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.140625" style="101" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" style="101" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45" style="101" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" style="101" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" style="101" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="102.5703125" style="101" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="101" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="101" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" style="101" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.7109375" style="101" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="101" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="109.42578125" style="101" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" style="101" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="101" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" style="101" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="101" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.28515625" style="101" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" style="101" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="101" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="101"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30">
-      <c r="A1" s="173" t="s">
+    <row r="1" spans="1:11">
+      <c r="A1" s="184" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="162" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="165" t="s">
+      <c r="C1" s="162" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="165" t="s">
+      <c r="D1" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="E1" s="183" t="s">
+      <c r="E1" s="186" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="165" t="s">
+      <c r="F1" s="162" t="s">
         <v>396</v>
       </c>
-      <c r="G1" s="165" t="s">
+      <c r="G1" s="162" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="165" t="s">
+      <c r="H1" s="162" t="s">
         <v>145</v>
       </c>
-      <c r="I1" s="165" t="s">
+      <c r="I1" s="162" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="165" t="s">
+      <c r="J1" s="162" t="s">
         <v>561</v>
       </c>
       <c r="K1" s="133" t="s">
@@ -6484,10 +6549,10 @@
       <c r="C2" s="110">
         <v>1</v>
       </c>
-      <c r="D2" s="184" t="s">
+      <c r="D2" s="187" t="s">
         <v>147</v>
       </c>
-      <c r="E2" s="184" t="s">
+      <c r="E2" s="187" t="s">
         <v>835</v>
       </c>
       <c r="F2" s="101" t="s">
@@ -6516,10 +6581,10 @@
       <c r="C3" s="110">
         <v>1</v>
       </c>
-      <c r="D3" s="184" t="s">
+      <c r="D3" s="187" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="184" t="s">
+      <c r="E3" s="187" t="s">
         <v>835</v>
       </c>
       <c r="F3" s="101" t="s">
@@ -6548,10 +6613,10 @@
       <c r="C4" s="110">
         <v>1</v>
       </c>
-      <c r="D4" s="184" t="s">
+      <c r="D4" s="187" t="s">
         <v>147</v>
       </c>
-      <c r="E4" s="184" t="s">
+      <c r="E4" s="187" t="s">
         <v>835</v>
       </c>
       <c r="F4" s="101" t="s">
@@ -6571,20 +6636,116 @@
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="E5" s="163"/>
+      <c r="A5" s="101">
+        <v>10</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>853</v>
+      </c>
+      <c r="C5" s="110">
+        <v>1</v>
+      </c>
+      <c r="D5" s="187" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="187" t="s">
+        <v>855</v>
+      </c>
+      <c r="F5" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="G5" s="110" t="s">
+        <v>395</v>
+      </c>
+      <c r="H5" s="110" t="s">
+        <v>583</v>
+      </c>
+      <c r="I5" s="110">
+        <v>6</v>
+      </c>
+      <c r="J5" s="110" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="101">
+        <v>11</v>
+      </c>
+      <c r="B6" s="99" t="s">
+        <v>856</v>
+      </c>
+      <c r="C6" s="110">
+        <v>1</v>
+      </c>
+      <c r="D6" s="188" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="188" t="s">
+        <v>835</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="G6" s="110" t="s">
+        <v>395</v>
+      </c>
+      <c r="H6" s="110">
+        <v>1</v>
+      </c>
+      <c r="I6" s="110">
+        <v>6</v>
+      </c>
+      <c r="J6" s="110" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="101">
+        <v>12</v>
+      </c>
+      <c r="B7" s="99" t="s">
+        <v>857</v>
+      </c>
+      <c r="C7" s="110">
+        <v>1</v>
+      </c>
+      <c r="D7" s="188" t="s">
+        <v>147</v>
+      </c>
+      <c r="E7" s="188" t="s">
+        <v>858</v>
+      </c>
+      <c r="F7" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="G7" s="110" t="s">
+        <v>395</v>
+      </c>
+      <c r="H7" s="110">
+        <v>3</v>
+      </c>
+      <c r="I7" s="110">
+        <v>6</v>
+      </c>
+      <c r="J7" s="110" t="s">
+        <v>563</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="113" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="112" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="111" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5">
+    <cfRule type="duplicateValues" dxfId="113" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F7">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6601,7 +6762,7 @@
           <x14:formula1>
             <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>D5:D1048576</xm:sqref>
+          <xm:sqref>D8:D1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6633,7 +6794,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="188" t="s">
+      <c r="A1" s="184" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="162" t="s">
@@ -7898,34 +8059,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="110" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="109" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="108" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="107" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="106" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="105" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="104" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="103" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="102" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="101" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
@@ -9205,22 +9366,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="100" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="99" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="97" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="96" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="95" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
@@ -9358,7 +9519,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="171" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="108" t="s">
@@ -9653,10 +9814,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="94" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9864,10 +10025,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="92" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="91" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="69"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10018,16 +10179,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="90" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="89" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
@@ -10243,10 +10404,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="86" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -10638,22 +10799,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="84" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="83" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="82" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="81" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="79" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -10750,7 +10911,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10810,10 +10971,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10896,7 +11057,7 @@
       <c r="A5" s="101" t="s">
         <v>782</v>
       </c>
-      <c r="B5" s="182">
+      <c r="B5" s="180">
         <v>225504</v>
       </c>
       <c r="C5" s="30" t="s">
@@ -10924,7 +11085,7 @@
       <c r="A7" s="101" t="s">
         <v>783</v>
       </c>
-      <c r="B7" s="182">
+      <c r="B7" s="180">
         <v>225504</v>
       </c>
       <c r="C7" s="30" t="s">
@@ -11103,10 +11264,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11231,10 +11392,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11383,10 +11544,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -11510,10 +11671,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -11766,10 +11927,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
@@ -11861,10 +12022,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11916,10 +12077,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12649,22 +12810,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="61" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="60" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="57" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="56" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
@@ -13325,22 +13486,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="55" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="54" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="53" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="52" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="51" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="50" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
@@ -13370,7 +13531,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="178" t="s">
+      <c r="A1" s="176" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="31" t="s">
@@ -13396,13 +13557,13 @@
       <c r="B2" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="C2" s="182">
-        <v>1</v>
-      </c>
-      <c r="D2" s="182" t="s">
+      <c r="C2" s="180">
+        <v>1</v>
+      </c>
+      <c r="D2" s="180" t="s">
         <v>783</v>
       </c>
-      <c r="E2" s="182">
+      <c r="E2" s="180">
         <v>225504</v>
       </c>
       <c r="F2" s="30" t="s">
@@ -13886,10 +14047,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -13922,7 +14083,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="54" customFormat="1">
-      <c r="A1" s="176" t="s">
+      <c r="A1" s="174" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="53" t="s">
@@ -14398,13 +14559,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="47" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -14429,7 +14590,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="175" t="s">
+      <c r="A1" s="173" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -14668,13 +14829,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="44" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="43" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -14714,7 +14875,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="4" customFormat="1" ht="30">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="171" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="36" t="s">
@@ -15642,16 +15803,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="41" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="40" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="39" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="38" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -15826,16 +15987,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="36" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16033,7 +16194,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -16254,10 +16415,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="33" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -16283,7 +16444,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -16556,13 +16717,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="31" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="30" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="29" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -16590,7 +16751,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="172" t="s">
+      <c r="A1" s="171" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="36" t="s">
@@ -16858,13 +17019,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="27" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="26" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -16894,7 +17055,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
       <c r="B1" s="19" t="s">
@@ -17107,22 +17268,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="25" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="21" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="20" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -17240,7 +17401,7 @@
       <c r="A7" s="101">
         <v>6</v>
       </c>
-      <c r="B7" s="179" t="s">
+      <c r="B7" s="177" t="s">
         <v>498</v>
       </c>
       <c r="C7" s="101">
@@ -17531,7 +17692,7 @@
       </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="180">
+      <c r="A28" s="178">
         <v>32</v>
       </c>
       <c r="B28" s="101" t="s">
@@ -17545,7 +17706,7 @@
       </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="180">
+      <c r="A29" s="178">
         <v>33</v>
       </c>
       <c r="B29" s="21" t="s">
@@ -17559,7 +17720,7 @@
       </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="180">
+      <c r="A30" s="178">
         <v>34</v>
       </c>
       <c r="B30" s="21" t="s">
@@ -17601,7 +17762,7 @@
       </c>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="181" t="s">
+      <c r="A33" s="179" t="s">
         <v>296</v>
       </c>
       <c r="B33" s="21" t="s">
@@ -17615,7 +17776,7 @@
       </c>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="181" t="s">
+      <c r="A34" s="179" t="s">
         <v>408</v>
       </c>
       <c r="B34" s="21" t="s">
@@ -17629,7 +17790,7 @@
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="181" t="s">
+      <c r="A35" s="179" t="s">
         <v>409</v>
       </c>
       <c r="B35" s="21" t="s">
@@ -17677,10 +17838,10 @@
       <c r="B38" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="C38" s="182">
-        <v>1</v>
-      </c>
-      <c r="D38" s="182" t="s">
+      <c r="C38" s="180">
+        <v>1</v>
+      </c>
+      <c r="D38" s="180" t="s">
         <v>783</v>
       </c>
     </row>
@@ -17715,31 +17876,31 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="171" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="170" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="169" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="168" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="167" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="duplicateValues" dxfId="166" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="165" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="164" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="163" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -18681,25 +18842,25 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="19" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="17" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -18938,25 +19099,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="12" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="11" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -19360,7 +19521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -20191,22 +20352,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
@@ -24606,13 +24767,13 @@
       <c r="E92" s="118" t="s">
         <v>193</v>
       </c>
-      <c r="F92" s="189" t="s">
+      <c r="F92" s="185" t="s">
         <v>8</v>
       </c>
       <c r="G92" s="118" t="s">
         <v>772</v>
       </c>
-      <c r="H92" s="187" t="s">
+      <c r="H92" s="183" t="s">
         <v>843</v>
       </c>
       <c r="I92" s="116" t="s">
@@ -24723,121 +24884,121 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="162" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="161" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="160" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="159" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="158" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="157" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="156" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="155" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="154" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="153" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="152" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="151" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="150" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="149" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="148" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="147" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="146" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="145" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="144" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="143" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="142" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="141" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="140" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="139" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="138" priority="90"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="90"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="137" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="136" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="135" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="134" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="133" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="132" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="131" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:I91">
-    <cfRule type="duplicateValues" dxfId="130" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="129" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="128" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="127" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="126" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G92:G93">
-    <cfRule type="duplicateValues" dxfId="125" priority="99"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="duplicateValues" dxfId="124" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H3" location="'Login_magento++'!A1" display="Login_magento"/>
@@ -25264,13 +25425,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25282,7 +25443,7 @@
     <col min="5" max="5" width="9.7109375" style="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8" style="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20" style="30" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" style="30" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27.85546875" style="30" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" style="30" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.7109375" style="30" bestFit="1" customWidth="1"/>
@@ -25397,7 +25558,7 @@
       <c r="N2" s="122" t="s">
         <v>818</v>
       </c>
-      <c r="O2" s="167" t="s">
+      <c r="O2" s="166" t="s">
         <v>833</v>
       </c>
       <c r="P2" s="21"/>
@@ -25423,7 +25584,7 @@
       <c r="F3" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="167" t="s">
+      <c r="G3" s="166" t="s">
         <v>813</v>
       </c>
       <c r="H3" s="21"/>
@@ -25457,7 +25618,7 @@
       <c r="F4" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="167" t="s">
+      <c r="G4" s="166" t="s">
         <v>813</v>
       </c>
       <c r="H4" s="21"/>
@@ -25491,7 +25652,7 @@
       <c r="F5" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="167" t="s">
+      <c r="G5" s="166" t="s">
         <v>813</v>
       </c>
       <c r="H5" s="21"/>
@@ -25525,7 +25686,7 @@
       <c r="F6" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="167" t="s">
+      <c r="G6" s="166" t="s">
         <v>813</v>
       </c>
       <c r="H6" s="21"/>
@@ -25559,7 +25720,7 @@
       <c r="F7" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="167" t="s">
+      <c r="G7" s="166" t="s">
         <v>813</v>
       </c>
       <c r="H7" s="21"/>
@@ -25577,19 +25738,19 @@
       <c r="T7" s="21"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="185">
+      <c r="A8" s="181">
         <v>7</v>
       </c>
-      <c r="B8" s="186" t="s">
+      <c r="B8" s="182" t="s">
         <v>836</v>
       </c>
       <c r="C8" s="33">
         <v>421</v>
       </c>
-      <c r="D8" s="186" t="s">
+      <c r="D8" s="182" t="s">
         <v>837</v>
       </c>
-      <c r="F8" s="186" t="s">
+      <c r="F8" s="182" t="s">
         <v>9</v>
       </c>
       <c r="G8" s="116" t="s">
@@ -25597,20 +25758,20 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="185">
+      <c r="A9" s="181">
         <v>8</v>
       </c>
-      <c r="B9" s="186" t="s">
+      <c r="B9" s="182" t="s">
         <v>849</v>
       </c>
       <c r="C9" s="33">
         <v>423</v>
       </c>
-      <c r="D9" s="186" t="s">
+      <c r="D9" s="182" t="s">
         <v>849</v>
       </c>
-      <c r="F9" s="186" t="s">
-        <v>8</v>
+      <c r="F9" s="182" t="s">
+        <v>9</v>
       </c>
       <c r="G9" s="116" t="s">
         <v>800</v>
@@ -25620,20 +25781,20 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="185">
+      <c r="A10" s="181">
         <v>9</v>
       </c>
-      <c r="B10" s="186" t="s">
+      <c r="B10" s="182" t="s">
         <v>851</v>
       </c>
       <c r="C10" s="33">
         <v>432</v>
       </c>
-      <c r="D10" s="186" t="s">
+      <c r="D10" s="182" t="s">
         <v>851</v>
       </c>
-      <c r="F10" s="186" t="s">
-        <v>8</v>
+      <c r="F10" s="182" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="116" t="s">
         <v>800</v>
@@ -25642,33 +25803,105 @@
         <v>852</v>
       </c>
     </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="181">
+        <v>10</v>
+      </c>
+      <c r="B11" s="182" t="s">
+        <v>853</v>
+      </c>
+      <c r="C11" s="33">
+        <v>440</v>
+      </c>
+      <c r="D11" s="182" t="s">
+        <v>853</v>
+      </c>
+      <c r="F11" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="116" t="s">
+        <v>800</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="181">
+        <v>11</v>
+      </c>
+      <c r="B12" s="182" t="s">
+        <v>856</v>
+      </c>
+      <c r="C12" s="33">
+        <v>427</v>
+      </c>
+      <c r="D12" s="99" t="s">
+        <v>856</v>
+      </c>
+      <c r="F12" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" s="116" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="181">
+        <v>12</v>
+      </c>
+      <c r="B13" s="182" t="s">
+        <v>857</v>
+      </c>
+      <c r="C13" s="33">
+        <v>436</v>
+      </c>
+      <c r="D13" s="99" t="s">
+        <v>857</v>
+      </c>
+      <c r="F13" s="182" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="116" t="s">
+        <v>800</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="123" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="122" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="duplicateValues" dxfId="121" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
-    <cfRule type="duplicateValues" dxfId="120" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="119" priority="101"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="104"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="118" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="duplicateValues" dxfId="117" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="116" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="duplicateValues" dxfId="115" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11">
+    <cfRule type="duplicateValues" dxfId="119" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="duplicateValues" dxfId="118" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:B13">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
@@ -25685,6 +25918,9 @@
     <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
     <hyperlink ref="G9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
     <hyperlink ref="G10" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G11" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G12" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G13" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -25692,6 +25928,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -25700,7 +25945,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -25849,16 +26094,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -25866,7 +26119,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25883,21 +26136,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="38ec8e4d-8506-4d8b-b040-96d37469ddf9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update TA586 to accomdate syncronization.
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2643C81-1240-48BE-9A80-908C0D0BC74D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="EVS" sheetId="82" r:id="rId1"/>
@@ -117,12 +116,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -140,12 +139,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2400-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2400-000002000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -184,12 +183,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2500-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -206,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-2500-000002000000}">
+    <comment ref="I1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -228,12 +227,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-5300-000001000000}">
+    <comment ref="F1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -251,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5406" uniqueCount="1022">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5406" uniqueCount="1021">
   <si>
     <t>testSuitID</t>
   </si>
@@ -3286,9 +3285,6 @@
   </si>
   <si>
     <t>Different_payment_options_to_display_on_checkout</t>
-  </si>
-  <si>
-    <t>evs_LaunchPortal</t>
   </si>
   <si>
     <t>evs_ExistingAddress</t>
@@ -3330,7 +3326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -4200,9 +4196,9 @@
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="4"/>
+    <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
   <dxfs count="324">
     <dxf>
@@ -7475,156 +7471,10 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="evs_SAP_OrderRelated++"/>
-      <sheetName val="evs_OrderStatusSearch++"/>
-      <sheetName val="URL++"/>
-      <sheetName val="EVS_Login_magento++"/>
-      <sheetName val="Login_magento++"/>
-      <sheetName val="Suites"/>
-      <sheetName val="IC"/>
-      <sheetName val="EVS"/>
-      <sheetName val="validatePaymentOption++"/>
-      <sheetName val="evs_RetriveOrderID++"/>
-      <sheetName val="evs_PayUPagePayment++"/>
-      <sheetName val="evs_CheckoutpaymentOption++"/>
-      <sheetName val="evs_GenerateOrderSAPnumber++"/>
-      <sheetName val="evs_DeliveryPopulation++"/>
-      <sheetName val="evs_AccountCreation++"/>
-      <sheetName val="evs_ProductSearch++"/>
-      <sheetName val="ProductSearch++"/>
-      <sheetName val="accountCreation++"/>
-      <sheetName val="parrallel_ic_Login++"/>
-      <sheetName val="evs_Login++"/>
-      <sheetName val="SapRSIGetDataFromSAPDB++"/>
-      <sheetName val="icInvalidEmailNewsLetter++"/>
-      <sheetName val="ic_SubscribeNewsletter++"/>
-      <sheetName val="evs_RemoveFromcart++"/>
-      <sheetName val="ic_RemoveFromcart++"/>
-      <sheetName val="IC_ClearWishList++"/>
-      <sheetName val="evs_ClearWishList++"/>
-      <sheetName val="evs_NavigetoWishlist++"/>
-      <sheetName val="ic_NavigetoWishlist++"/>
-      <sheetName val="Magento_UserInfoVerification++"/>
-      <sheetName val="IC_ProductsSortBy++"/>
-      <sheetName val="ic_SubscribeNews_DupliEmailID++"/>
-      <sheetName val="EnterSpouseInfor++"/>
-      <sheetName val="EnterContact++"/>
-      <sheetName val="CreditEnterAddressDetails++"/>
-      <sheetName val="CreditEnterEmploymentDetails++"/>
-      <sheetName val="EnterBasicDetails++"/>
-      <sheetName val="CreditStatusVerification++"/>
-      <sheetName val="CreditApp_NavigateFilter++"/>
-      <sheetName val="giftCardReport++"/>
-      <sheetName val="adminUserUpdate++"/>
-      <sheetName val="ICUpdateUser++"/>
-      <sheetName val="SapCustomer++"/>
-      <sheetName val="PayUPagePayment++"/>
-      <sheetName val="CheckoutpaymentOption++"/>
-      <sheetName val="deliveryPopulation++"/>
-      <sheetName val="RetrieveCustomerDetailsOld++"/>
-      <sheetName val="icGiftCardPurchase++"/>
-      <sheetName val="SAP_OrderRelated++"/>
-      <sheetName val="GenerateOrderSAPnumber++"/>
-      <sheetName val="OrderStatusSearch++"/>
-      <sheetName val="ic_RetriveOrderID++"/>
-      <sheetName val="evs_WishlistToCart++"/>
-      <sheetName val="IC_WishlistToCart++"/>
       <sheetName val="Products_Category"/>
-      <sheetName val="icRedeemGiftCard++"/>
-      <sheetName val="VeriyGiftcardUsableity++"/>
-      <sheetName val="ic_login++"/>
-      <sheetName val="ClearCart++"/>
-      <sheetName val="ic_invalidCredslogin++"/>
-      <sheetName val="SendWishlistToEmail++"/>
-      <sheetName val="icEmailWishlistverification++"/>
-      <sheetName val="DB_connection_master++"/>
-      <sheetName val="icGiftCardVerificationSender++"/>
-      <sheetName val="ic_CashDepositPayment++"/>
-      <sheetName val="CreateaccountBackend++"/>
-      <sheetName val="icSearchNoResultsReturned++"/>
-      <sheetName val="Russels"/>
-      <sheetName val="Login++"/>
-      <sheetName val="Bradlows"/>
-      <sheetName val="Rochester"/>
-      <sheetName val="Preferred Store"/>
-      <sheetName val="Sleepmasters"/>
-      <sheetName val="HiFiCorp"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7686,7 +7536,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7719,26 +7569,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -7771,23 +7604,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7963,11 +7779,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C44" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="D46" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9299,7 +9115,7 @@
       <c r="F38" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G38" s="99" t="s">
+      <c r="G38" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H38" s="57" t="s">
@@ -9337,7 +9153,7 @@
       <c r="F39" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G39" s="99" t="s">
+      <c r="G39" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H39" s="57" t="s">
@@ -9374,7 +9190,7 @@
       <c r="F40" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G40" s="99" t="s">
+      <c r="G40" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H40" s="57" t="s">
@@ -9397,7 +9213,7 @@
       <c r="F41" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G41" s="99" t="s">
+      <c r="G41" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H41" s="116" t="s">
@@ -9426,7 +9242,7 @@
       <c r="F42" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G42" s="99" t="s">
+      <c r="G42" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H42" s="116" t="s">
@@ -9465,7 +9281,7 @@
       <c r="F43" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G43" s="99" t="s">
+      <c r="G43" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H43" s="116" t="s">
@@ -9503,7 +9319,7 @@
       <c r="F44" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G44" s="99" t="s">
+      <c r="G44" s="100" t="s">
         <v>983</v>
       </c>
       <c r="H44" s="116" t="s">
@@ -9735,8 +9551,8 @@
       <c r="F52" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G52" s="113" t="s">
-        <v>1009</v>
+      <c r="G52" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H52" s="118" t="s">
         <v>981</v>
@@ -9789,8 +9605,8 @@
       <c r="F53" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G53" s="113" t="s">
-        <v>1009</v>
+      <c r="G53" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H53" s="118" t="s">
         <v>981</v>
@@ -9843,8 +9659,8 @@
       <c r="F54" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G54" s="113" t="s">
-        <v>1009</v>
+      <c r="G54" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H54" s="116" t="s">
         <v>964</v>
@@ -9874,8 +9690,8 @@
       <c r="F55" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="113" t="s">
-        <v>1009</v>
+      <c r="G55" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H55" s="224" t="s">
         <v>966</v>
@@ -9901,8 +9717,8 @@
       <c r="F56" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G56" s="113" t="s">
-        <v>1009</v>
+      <c r="G56" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H56" s="224" t="s">
         <v>967</v>
@@ -9928,8 +9744,8 @@
       <c r="F57" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G57" s="113" t="s">
-        <v>1009</v>
+      <c r="G57" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H57" s="194" t="s">
         <v>896</v>
@@ -9984,8 +9800,8 @@
       <c r="F58" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G58" s="113" t="s">
-        <v>1009</v>
+      <c r="G58" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H58" s="116" t="s">
         <v>795</v>
@@ -10034,8 +9850,8 @@
       <c r="F59" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G59" s="113" t="s">
-        <v>1009</v>
+      <c r="G59" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H59" s="194" t="s">
         <v>896</v>
@@ -10090,11 +9906,11 @@
       <c r="F60" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G60" s="113" t="s">
-        <v>1009</v>
+      <c r="G60" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H60" s="116" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="I60" s="117"/>
       <c r="J60" s="117"/>
@@ -10112,25 +9928,25 @@
         <v>100</v>
       </c>
       <c r="B61" s="117" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C61" s="231">
         <v>586</v>
       </c>
       <c r="D61" s="117" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="E61" s="111" t="s">
         <v>963</v>
       </c>
       <c r="F61" s="118" t="s">
-        <v>9</v>
-      </c>
-      <c r="G61" s="113" t="s">
-        <v>1009</v>
+        <v>8</v>
+      </c>
+      <c r="G61" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H61" s="159" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="I61" s="117"/>
       <c r="L61" s="117"/>
@@ -10146,25 +9962,25 @@
         <v>101</v>
       </c>
       <c r="B62" s="118" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C62" s="60">
         <v>587</v>
       </c>
       <c r="D62" s="118" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="E62" s="118" t="s">
         <v>963</v>
       </c>
       <c r="F62" s="118" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="113" t="s">
-        <v>1009</v>
+        <v>9</v>
+      </c>
+      <c r="G62" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H62" s="159" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="63" spans="1:21" s="118" customFormat="1">
@@ -10186,8 +10002,8 @@
       <c r="F63" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G63" s="113" t="s">
-        <v>1009</v>
+      <c r="G63" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H63" s="116" t="s">
         <v>896</v>
@@ -10231,8 +10047,8 @@
       <c r="F64" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="G64" s="113" t="s">
-        <v>1009</v>
+      <c r="G64" s="100" t="s">
+        <v>983</v>
       </c>
       <c r="H64" s="116" t="s">
         <v>896</v>
@@ -10244,10 +10060,10 @@
         <v>795</v>
       </c>
       <c r="K64" s="118" t="s">
+        <v>1009</v>
+      </c>
+      <c r="L64" s="100" t="s">
         <v>1010</v>
-      </c>
-      <c r="L64" s="100" t="s">
-        <v>1011</v>
       </c>
     </row>
   </sheetData>
@@ -10381,141 +10197,141 @@
     <cfRule type="duplicateValues" dxfId="281" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="I2" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J2" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="K2" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="L2" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="N2" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="O2" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="H3" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="H4:H7" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="P2" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="M2" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="H9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="H10" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="H11" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="H12" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="H13" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="G14" location="'parallel_evs_Login++'!A1" display="parallel_evs_Login" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="H15" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="H16" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="H17" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="H18:H20" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="I17" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="I18:I20" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="L17" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="K17" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="K18:K20" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="L18:L20" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="H21" location="'evs_Login++'!A1" display="evs_ForgotPassword" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="H22" location="'evs_Login++'!A1" display="evs_ForgotPasswordLink" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H23" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="J24" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="H24" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="L24" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="G25" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="G26:G27" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H25" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="H26:H27" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="I25" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="I26:I27" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="J25" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="J26:J27" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="H28" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="H29:H32" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="I28" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="I29:I32" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="J28" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="J29:J32" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="L28" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="L29:L32" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="M28" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="M29:M32" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="G33" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="H33" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="I33" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="J33" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="G34:G37" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="H34:H37" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="I34:I37" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="J34:J37" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="H39" location="'evs_NavigetoWishlist++'!A1" display="evs_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="H41:H42" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="K42" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="M42" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="L43" location="'evs_WishlistToCart++'!A1" display="evs_WishlistToCart" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="H44" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="H43" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="I41" location="'evs_ClearWishList++'!A1" display="evs_ClearWishList" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="J39" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="I41:I44" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="J43:J44" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="H40" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="K39" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="G45" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="J52" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="K52" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="L52" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="M52" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="O52" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="P52" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="N52" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="J53" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="K53" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="L53" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="M53" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="O53" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="P53" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="N53" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="H48:H51" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="G48" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="G49:G51" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="I52" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="I53" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="H58" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="I58" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="J58" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="K58" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="M58" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="O58" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="P58" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="H57" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="H59" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="J57" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="K57" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="L57" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="N57" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="P57" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="Q57" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="R57" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="O57" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="J59" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="K59" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
-    <hyperlink ref="L59" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
-    <hyperlink ref="M59" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
-    <hyperlink ref="O59" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="Q59" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="R59" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="N59" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
-    <hyperlink ref="L58" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
-    <hyperlink ref="M57" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
-    <hyperlink ref="H63" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="J63" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
-    <hyperlink ref="H64" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
-    <hyperlink ref="J64" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
-    <hyperlink ref="G64" location="'EVS_LaunchPortal++'!A1" display="evs_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="G52:G63" location="'EVS_LaunchPortal++'!A1" display="evs_LaunchPortal" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
-    <hyperlink ref="L64" location="'evs_validatePaymentOption++'!A1" display="evs_validatePaymentOption" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
-    <hyperlink ref="H56" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="H55" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="H54" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="H60" location="'evs_PopularSearch++'!A1" display="icPopularSearch" xr:uid="{DAFB2D4A-4709-4012-AC48-9B6DE6B1927C}"/>
-    <hyperlink ref="G60:G61" location="'evs_LaunchPortal++'!A1" display="evs_LaunchPortal++" xr:uid="{5AFE1EFF-A3E6-4C32-9C5D-4157CF05D92F}"/>
-    <hyperlink ref="G62" location="'evs_LaunchPortal++'!A1" display="evs_LaunchPortal++" xr:uid="{B63A3B91-4704-4072-BC98-F93BB4385875}"/>
-    <hyperlink ref="H61" location="'evs_SearchNoResultsReturned++'!A1" display="evs_SearchNoResultsReturned" xr:uid="{C0AFDCAA-9383-49A1-8130-D3A481DABBA0}"/>
-    <hyperlink ref="H62" location="'evs_SearchTextResults++'!A1" display="evs_SearchTextResults" xr:uid="{861ECC0E-5F52-4ADE-A43A-1EB2CE9C92F2}"/>
+    <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="I2" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="J2" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="K2" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="L2" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="N2" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="O2" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="H3" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="H4:H7" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="P2" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="M2" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G8" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H9" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H10" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H11" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H12" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H13" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G14" location="'parallel_evs_Login++'!A1" display="parallel_evs_Login"/>
+    <hyperlink ref="H15" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin"/>
+    <hyperlink ref="H16" location="'evs_invalidCredslogin++'!A1" display="evs_invalidCredslogin"/>
+    <hyperlink ref="H17" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="H18:H20" location="'evs_AccountCreation++'!A1" display="evs_AccountCreation"/>
+    <hyperlink ref="I17" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="I18:I20" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L17" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="K17" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="K18:K20" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="L18:L20" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H21" location="'evs_Login++'!A1" display="evs_ForgotPassword"/>
+    <hyperlink ref="H22" location="'evs_Login++'!A1" display="evs_ForgotPasswordLink"/>
+    <hyperlink ref="H23" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="J24" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H24" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="L24" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="G25" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G26:G27" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H25" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend"/>
+    <hyperlink ref="H26:H27" location="'evs_CreateaccountBackend++'!A1" display="evs_CreateaccountBackend"/>
+    <hyperlink ref="I25" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="I26:I27" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J25" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="J26:J27" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H28" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="H29:H32" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="I28" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser"/>
+    <hyperlink ref="I29:I32" location="'evs_UpdateUser++'!A1" display="evs_UpdateUser"/>
+    <hyperlink ref="J28" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J29:J32" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L28" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="L29:L32" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="M28" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="M29:M32" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="G33" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H33" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate"/>
+    <hyperlink ref="I33" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J33" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="G34:G37" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H34:H37" location="'evs_adminUserUpdate++'!A1" display="evs_adminUserUpdate"/>
+    <hyperlink ref="I34:I37" location="'evs_Magento_UserInfoVerify++'!A1" display="evs_Magento_UserInfoVerify"/>
+    <hyperlink ref="J34:J37" location="'EVS_SapCustomer++'!A1" display="evs_SapCustomer"/>
+    <hyperlink ref="H39" location="'evs_NavigetoWishlist++'!A1" display="evs_NavigetoWishlist"/>
+    <hyperlink ref="H41:H42" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="K42" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="M42" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="L43" location="'evs_WishlistToCart++'!A1" display="evs_WishlistToCart"/>
+    <hyperlink ref="H44" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="H43" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I41" location="'evs_ClearWishList++'!A1" display="evs_ClearWishList"/>
+    <hyperlink ref="J39" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart"/>
+    <hyperlink ref="I41:I44" location="'evs_RemoveFromcart++'!A1" display="evs_RemoveFromcart"/>
+    <hyperlink ref="J43:J44" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H40" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K39" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="G45" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login"/>
+    <hyperlink ref="J52" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="K52" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="L52" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="M52" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O52" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="P52" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="N52" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J53" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="K53" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="L53" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="M53" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O53" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="P53" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="N53" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="H48:H51" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="G48" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="G49:G51" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="I52" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct"/>
+    <hyperlink ref="I53" location="'evs_ProductSearch++'!A1" display="EVS_skuProduct"/>
+    <hyperlink ref="H58" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="I58" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="J58" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="K58" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="M58" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="O58" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="P58" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="H57" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="H59" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="J57" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K57" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="L57" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="N57" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="P57" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="Q57" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="R57" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="O57" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="J59" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="K59" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation"/>
+    <hyperlink ref="L59" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption"/>
+    <hyperlink ref="M59" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID"/>
+    <hyperlink ref="O59" location="'evs_OrderStatusSearch++'!A1" display="evs_OrderStatusSearch"/>
+    <hyperlink ref="Q59" location="'evs_GenerateOrderSAPnumber++'!A1" display="evs_GenerateOrderSAPnumber"/>
+    <hyperlink ref="R59" location="'evs_SAP_OrderRelated++'!A1" display="evs_SAP_OrderRelated"/>
+    <hyperlink ref="N59" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="L58" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento"/>
+    <hyperlink ref="M57" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment"/>
+    <hyperlink ref="H63" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="J63" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="H64" location="'evs_Login++'!A1" display="evs_Login"/>
+    <hyperlink ref="J64" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
+    <hyperlink ref="L64" location="'evs_validatePaymentOption++'!A1" display="evs_validatePaymentOption"/>
+    <hyperlink ref="H56" location="'evs_SubscribeNewsletter++'!A1" display="ic_SubscribeNewsletter"/>
+    <hyperlink ref="H55" location="'evs_InvalidEmailNewsLetter++'!A1" display="evs_InvalidEmailNewsLetter"/>
+    <hyperlink ref="H54" location="'evs_SubscribeNews_DupEmailID++'!A1" display="evs_SubscribeNews_DupEmailID"/>
+    <hyperlink ref="H60" location="'evs_PopularSearch++'!A1" display="icPopularSearch"/>
+    <hyperlink ref="H61" location="'evs_SearchNoResultsReturned++'!A1" display="evs_SearchNoResultsReturned"/>
+    <hyperlink ref="H62" location="'evs_SearchTextResults++'!A1" display="evs_SearchTextResults"/>
+    <hyperlink ref="G43" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G38:G42" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G44" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
+    <hyperlink ref="G52:G64" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -10523,7 +10339,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -10617,14 +10433,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
@@ -10740,16 +10556,16 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
-    <hyperlink ref="D7" r:id="rId3" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
-    <hyperlink ref="C2" r:id="rId5" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
-    <hyperlink ref="D3" r:id="rId7" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
-    <hyperlink ref="C3" r:id="rId8" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
-    <hyperlink ref="D4" r:id="rId9" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
-    <hyperlink ref="C4" r:id="rId10" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D6" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="D4" r:id="rId9"/>
+    <hyperlink ref="C4" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
@@ -10757,7 +10573,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -11191,14 +11007,14 @@
     <cfRule type="duplicateValues" dxfId="271" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11839,7 +11655,7 @@
     <cfRule type="duplicateValues" dxfId="261" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11847,12 +11663,10 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -12806,7 +12620,7 @@
         <v>100</v>
       </c>
       <c r="B68" s="117" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="C68" s="101">
         <v>1</v>
@@ -12820,7 +12634,7 @@
         <v>101</v>
       </c>
       <c r="B69" s="118" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="C69" s="101">
         <v>1</v>
@@ -12931,19 +12745,19 @@
     <cfRule type="duplicateValues" dxfId="237" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0A00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13858,12 +13672,12 @@
     <cfRule type="duplicateValues" dxfId="222" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -13871,7 +13685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -14055,7 +13869,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" location="EVS!A1" display="EVS" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="B3" location="EVS!A1" display="EVS"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14063,7 +13877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA96"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -17959,302 +17773,302 @@
     <cfRule type="duplicateValues" dxfId="182" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
-    <hyperlink ref="H3" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000001000000}"/>
-    <hyperlink ref="I4" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000002000000}"/>
-    <hyperlink ref="H4" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000003000000}"/>
-    <hyperlink ref="I5" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000004000000}"/>
-    <hyperlink ref="H5" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000005000000}"/>
-    <hyperlink ref="I6" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000006000000}"/>
-    <hyperlink ref="H6" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000007000000}"/>
-    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000008000000}"/>
-    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000009000000}"/>
-    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0D00-00000A000000}"/>
-    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend" xr:uid="{00000000-0004-0000-0D00-00000B000000}"/>
-    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00000C000000}"/>
-    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00000D000000}"/>
-    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0D00-00000E000000}"/>
-    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0D00-00000F000000}"/>
-    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000010000000}"/>
-    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate" xr:uid="{00000000-0004-0000-0D00-000011000000}"/>
-    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000012000000}"/>
-    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-000013000000}"/>
-    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000014000000}"/>
-    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000015000000}"/>
-    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000016000000}"/>
-    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000017000000}"/>
-    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000018000000}"/>
-    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-000019000000}"/>
-    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-00001A000000}"/>
-    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-00001B000000}"/>
-    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-00001C000000}"/>
-    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00001D000000}"/>
-    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00001E000000}"/>
-    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00001F000000}"/>
-    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000020000000}"/>
-    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000021000000}"/>
-    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser" xr:uid="{00000000-0004-0000-0D00-000022000000}"/>
-    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000023000000}"/>
-    <hyperlink ref="H27" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000024000000}"/>
-    <hyperlink ref="I27" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000025000000}"/>
-    <hyperlink ref="M27" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000026000000}"/>
-    <hyperlink ref="O27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000027000000}"/>
-    <hyperlink ref="H24" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000028000000}"/>
-    <hyperlink ref="H25" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000029000000}"/>
-    <hyperlink ref="H22" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-00002A000000}"/>
-    <hyperlink ref="H23" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-00002B000000}"/>
-    <hyperlink ref="H26" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-00002C000000}"/>
-    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00002D000000}"/>
-    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00002E000000}"/>
-    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00002F000000}"/>
-    <hyperlink ref="J27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-000030000000}"/>
-    <hyperlink ref="K27" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000031000000}"/>
-    <hyperlink ref="N27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-000032000000}"/>
-    <hyperlink ref="L27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-000033000000}"/>
-    <hyperlink ref="P27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000034000000}"/>
-    <hyperlink ref="H28" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000035000000}"/>
-    <hyperlink ref="H30" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000036000000}"/>
-    <hyperlink ref="I28" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000037000000}"/>
-    <hyperlink ref="I30" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000038000000}"/>
-    <hyperlink ref="M28" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000039000000}"/>
-    <hyperlink ref="M30" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00003A000000}"/>
-    <hyperlink ref="O28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-00003B000000}"/>
-    <hyperlink ref="O30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-00003C000000}"/>
-    <hyperlink ref="J28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00003D000000}"/>
-    <hyperlink ref="J30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00003E000000}"/>
-    <hyperlink ref="K28" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-00003F000000}"/>
-    <hyperlink ref="K30" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000040000000}"/>
-    <hyperlink ref="N28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-000041000000}"/>
-    <hyperlink ref="N30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-000042000000}"/>
-    <hyperlink ref="L28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-000043000000}"/>
-    <hyperlink ref="L30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-000044000000}"/>
-    <hyperlink ref="P28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000045000000}"/>
-    <hyperlink ref="P30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000046000000}"/>
-    <hyperlink ref="H31" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000047000000}"/>
-    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000048000000}"/>
-    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000049000000}"/>
-    <hyperlink ref="O31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-00004A000000}"/>
-    <hyperlink ref="J31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00004B000000}"/>
-    <hyperlink ref="M31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-00004C000000}"/>
-    <hyperlink ref="K31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-00004D000000}"/>
-    <hyperlink ref="P31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-00004E000000}"/>
-    <hyperlink ref="H29" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-00004F000000}"/>
-    <hyperlink ref="I29" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000050000000}"/>
-    <hyperlink ref="M29" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000051000000}"/>
-    <hyperlink ref="O29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000052000000}"/>
-    <hyperlink ref="J29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-000053000000}"/>
-    <hyperlink ref="K29" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000054000000}"/>
-    <hyperlink ref="N29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-000055000000}"/>
-    <hyperlink ref="L29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-000056000000}"/>
-    <hyperlink ref="P29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000057000000}"/>
-    <hyperlink ref="H32" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000058000000}"/>
-    <hyperlink ref="I32" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-000059000000}"/>
-    <hyperlink ref="M32" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00005A000000}"/>
-    <hyperlink ref="J32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00005B000000}"/>
-    <hyperlink ref="K32" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-00005C000000}"/>
-    <hyperlink ref="N32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-00005D000000}"/>
-    <hyperlink ref="L32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-00005E000000}"/>
-    <hyperlink ref="P32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-00005F000000}"/>
-    <hyperlink ref="Q32" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-000060000000}"/>
-    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000061000000}"/>
-    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000062000000}"/>
-    <hyperlink ref="I37" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-000063000000}"/>
-    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-000064000000}"/>
-    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000065000000}"/>
-    <hyperlink ref="L33" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000066000000}"/>
-    <hyperlink ref="M33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-000067000000}"/>
-    <hyperlink ref="N33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000068000000}"/>
-    <hyperlink ref="O33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000069000000}"/>
-    <hyperlink ref="H33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0D00-00006A000000}"/>
-    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase" xr:uid="{00000000-0004-0000-0D00-00006B000000}"/>
-    <hyperlink ref="I34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00006C000000}"/>
-    <hyperlink ref="J34" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-00006D000000}"/>
-    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00006E000000}"/>
-    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-00006F000000}"/>
-    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000070000000}"/>
-    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000071000000}"/>
-    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0D00-000072000000}"/>
-    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails" xr:uid="{00000000-0004-0000-0D00-000073000000}"/>
-    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor" xr:uid="{00000000-0004-0000-0D00-000074000000}"/>
-    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0D00-000075000000}"/>
-    <hyperlink ref="I48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails" xr:uid="{00000000-0004-0000-0D00-000076000000}"/>
-    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000077000000}"/>
-    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000078000000}"/>
-    <hyperlink ref="H49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID" xr:uid="{00000000-0004-0000-0D00-000079000000}"/>
-    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-00007A000000}"/>
-    <hyperlink ref="N40" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00007B000000}"/>
-    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-00007C000000}"/>
-    <hyperlink ref="K54" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-00007D000000}"/>
-    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00007E000000}"/>
-    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter" xr:uid="{00000000-0004-0000-0D00-00007F000000}"/>
-    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification" xr:uid="{00000000-0004-0000-0D00-000080000000}"/>
-    <hyperlink ref="O32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000081000000}"/>
-    <hyperlink ref="K48" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0D00-000082000000}"/>
-    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact" xr:uid="{00000000-0004-0000-0D00-000083000000}"/>
-    <hyperlink ref="J48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0D00-000084000000}"/>
-    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails" xr:uid="{00000000-0004-0000-0D00-000085000000}"/>
-    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000086000000}"/>
-    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000087000000}"/>
-    <hyperlink ref="H53:H54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0D00-000088000000}"/>
-    <hyperlink ref="I53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-000089000000}"/>
-    <hyperlink ref="J53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-00008A000000}"/>
-    <hyperlink ref="J35" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0D00-00008B000000}"/>
-    <hyperlink ref="H36" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-00008C000000}"/>
-    <hyperlink ref="J36" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-00008D000000}"/>
-    <hyperlink ref="K36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00008E000000}"/>
-    <hyperlink ref="L37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00008F000000}"/>
-    <hyperlink ref="J37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0D00-000090000000}"/>
-    <hyperlink ref="L36" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000091000000}"/>
-    <hyperlink ref="M37" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000092000000}"/>
-    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0D00-000093000000}"/>
-    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport" xr:uid="{00000000-0004-0000-0D00-000094000000}"/>
-    <hyperlink ref="H50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0D00-000095000000}"/>
-    <hyperlink ref="H50:H52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy" xr:uid="{00000000-0004-0000-0D00-000096000000}"/>
-    <hyperlink ref="I2" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-000097000000}"/>
-    <hyperlink ref="L2" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-000098000000}"/>
-    <hyperlink ref="H2" location="'accountCreation++'!A1" display="accountCreation" xr:uid="{00000000-0004-0000-0D00-000099000000}"/>
-    <hyperlink ref="K2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-00009A000000}"/>
-    <hyperlink ref="L3" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00009B000000}"/>
-    <hyperlink ref="L5" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-00009C000000}"/>
-    <hyperlink ref="K3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-00009D000000}"/>
-    <hyperlink ref="K4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-00009E000000}"/>
-    <hyperlink ref="K5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-00009F000000}"/>
-    <hyperlink ref="L6" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-0000A0000000}"/>
-    <hyperlink ref="K6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000A1000000}"/>
-    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000A2000000}"/>
-    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000A3000000}"/>
-    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0D00-0000A4000000}"/>
-    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0D00-0000A5000000}"/>
-    <hyperlink ref="J2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0D00-0000A6000000}"/>
-    <hyperlink ref="J3:J6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails" xr:uid="{00000000-0004-0000-0D00-0000A7000000}"/>
-    <hyperlink ref="K55" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000A8000000}"/>
-    <hyperlink ref="J55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-0000A9000000}"/>
-    <hyperlink ref="H55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0D00-0000AA000000}"/>
-    <hyperlink ref="L55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart" xr:uid="{00000000-0004-0000-0D00-0000AB000000}"/>
-    <hyperlink ref="K56" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000AC000000}"/>
-    <hyperlink ref="K57" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000AD000000}"/>
-    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000AE000000}"/>
-    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-0000AF000000}"/>
-    <hyperlink ref="H69" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000B0000000}"/>
-    <hyperlink ref="L71" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000B1000000}"/>
-    <hyperlink ref="I71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0D00-0000B2000000}"/>
-    <hyperlink ref="J71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000B3000000}"/>
-    <hyperlink ref="K71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-0000B4000000}"/>
-    <hyperlink ref="M71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail" xr:uid="{00000000-0004-0000-0D00-0000B5000000}"/>
-    <hyperlink ref="N71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification" xr:uid="{00000000-0004-0000-0D00-0000B6000000}"/>
-    <hyperlink ref="H56:H57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist" xr:uid="{00000000-0004-0000-0D00-0000B7000000}"/>
-    <hyperlink ref="J56:J57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-0000B8000000}"/>
-    <hyperlink ref="H63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0D00-0000B9000000}"/>
-    <hyperlink ref="H64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin" xr:uid="{00000000-0004-0000-0D00-0000BA000000}"/>
-    <hyperlink ref="H70" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000BB000000}"/>
-    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0D00-0000BC000000}"/>
-    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000BD000000}"/>
-    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000BE000000}"/>
-    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0D00-0000BF000000}"/>
-    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-0000C0000000}"/>
-    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-0000C1000000}"/>
-    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-0000C2000000}"/>
-    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-0000C3000000}"/>
-    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-0000C4000000}"/>
-    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-0000C5000000}"/>
-    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-0000C6000000}"/>
-    <hyperlink ref="N41" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000C7000000}"/>
-    <hyperlink ref="O41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-0000C8000000}"/>
-    <hyperlink ref="O40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-0000C9000000}"/>
-    <hyperlink ref="O42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-0000CA000000}"/>
-    <hyperlink ref="P42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-0000CB000000}"/>
-    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-0000CC000000}"/>
-    <hyperlink ref="R41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000CD000000}"/>
-    <hyperlink ref="R40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000CE000000}"/>
-    <hyperlink ref="R42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification" xr:uid="{00000000-0004-0000-0D00-0000CF000000}"/>
-    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-0000D0000000}"/>
-    <hyperlink ref="M54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-0000D1000000}"/>
-    <hyperlink ref="I55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000D2000000}"/>
-    <hyperlink ref="I56:I57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000D3000000}"/>
-    <hyperlink ref="L57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000D4000000}"/>
-    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000D5000000}"/>
-    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart" xr:uid="{00000000-0004-0000-0D00-0000D6000000}"/>
-    <hyperlink ref="L54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem" xr:uid="{00000000-0004-0000-0D00-0000D7000000}"/>
-    <hyperlink ref="H74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear" xr:uid="{00000000-0004-0000-0D00-0000D8000000}"/>
-    <hyperlink ref="H78" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000D9000000}"/>
-    <hyperlink ref="H79" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000DA000000}"/>
-    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000DB000000}"/>
-    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-0000DC000000}"/>
-    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000DD000000}"/>
-    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000DE000000}"/>
-    <hyperlink ref="H75" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000DF000000}"/>
-    <hyperlink ref="H76:H77" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000E0000000}"/>
-    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000E1000000}"/>
-    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-0000E2000000}"/>
-    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000E3000000}"/>
-    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000E4000000}"/>
-    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000E5000000}"/>
-    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++" xr:uid="{00000000-0004-0000-0D00-0000E6000000}"/>
-    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000E7000000}"/>
-    <hyperlink ref="G35" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000E8000000}"/>
-    <hyperlink ref="I36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard" xr:uid="{00000000-0004-0000-0D00-0000E9000000}"/>
-    <hyperlink ref="I35" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000EA000000}"/>
-    <hyperlink ref="G85" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login" xr:uid="{00000000-0004-0000-0D00-0000EB000000}"/>
-    <hyperlink ref="I88" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000EC000000}"/>
-    <hyperlink ref="I89" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000ED000000}"/>
-    <hyperlink ref="I90" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000EE000000}"/>
-    <hyperlink ref="I91" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000EF000000}"/>
-    <hyperlink ref="N92" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000F0000000}"/>
-    <hyperlink ref="K92" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-0000F1000000}"/>
-    <hyperlink ref="J92" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-0000F2000000}"/>
-    <hyperlink ref="L92" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-0000F3000000}"/>
-    <hyperlink ref="O92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-0000F4000000}"/>
-    <hyperlink ref="N93" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-0000F5000000}"/>
-    <hyperlink ref="I93" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000F6000000}"/>
-    <hyperlink ref="K93" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-0000F7000000}"/>
-    <hyperlink ref="J93" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-0000F8000000}"/>
-    <hyperlink ref="L93" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-0000F9000000}"/>
-    <hyperlink ref="O93" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-0000FA000000}"/>
-    <hyperlink ref="G94" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-0000FB000000}"/>
-    <hyperlink ref="H94" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-0000FC000000}"/>
-    <hyperlink ref="I94" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-0000FD000000}"/>
-    <hyperlink ref="K94" location="'validatePaymentOption++'!A1" display="validatePaymentOption" xr:uid="{00000000-0004-0000-0D00-0000FE000000}"/>
-    <hyperlink ref="M93" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-0000FF000000}"/>
-    <hyperlink ref="P92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000000010000}"/>
-    <hyperlink ref="G44" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000001010000}"/>
-    <hyperlink ref="G2:G6" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000002010000}"/>
-    <hyperlink ref="G22:G33" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000003010000}"/>
-    <hyperlink ref="G36" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000004010000}"/>
-    <hyperlink ref="G45:G46" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000005010000}"/>
-    <hyperlink ref="G49:G57" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000006010000}"/>
-    <hyperlink ref="G63:G79" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000007010000}"/>
-    <hyperlink ref="G81:G84" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000008010000}"/>
-    <hyperlink ref="G86:G93" location="'LaunchPortal++'!A1" display="LaunchPortal" xr:uid="{00000000-0004-0000-0D00-000009010000}"/>
-    <hyperlink ref="G95" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-00000A010000}"/>
-    <hyperlink ref="J95" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-00000B010000}"/>
-    <hyperlink ref="L95" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00000C010000}"/>
-    <hyperlink ref="M95" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-00000D010000}"/>
-    <hyperlink ref="N95" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-00000E010000}"/>
-    <hyperlink ref="O95" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00000F010000}"/>
-    <hyperlink ref="P95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000010010000}"/>
-    <hyperlink ref="S95" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000011010000}"/>
-    <hyperlink ref="T95" location="'srs_Login++'!A1" display="srs_Login" xr:uid="{00000000-0004-0000-0D00-000012010000}"/>
-    <hyperlink ref="U95" location="'SRSLogonStore++'!A1" display="SRSLogonStore" xr:uid="{00000000-0004-0000-0D00-000013010000}"/>
-    <hyperlink ref="V95" location="'srs_salesOrder_DeliverStatus++'!A1" display="srs_salesOrder_DeliverStatus" xr:uid="{00000000-0004-0000-0D00-000014010000}"/>
-    <hyperlink ref="I95" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-000015010000}"/>
-    <hyperlink ref="R95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000016010000}"/>
-    <hyperlink ref="T42" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-000017010000}"/>
-    <hyperlink ref="T40" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-000018010000}"/>
-    <hyperlink ref="T41" location="'SapCustomer++'!A1" display="SapCustomer" xr:uid="{00000000-0004-0000-0D00-000019010000}"/>
-    <hyperlink ref="S40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-00001A010000}"/>
-    <hyperlink ref="N96" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-0D00-00001B010000}"/>
-    <hyperlink ref="O96" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch" xr:uid="{00000000-0004-0000-0D00-00001C010000}"/>
-    <hyperlink ref="I96" location="'ProductSearch++'!A1" display="ProductSearch" xr:uid="{00000000-0004-0000-0D00-00001D010000}"/>
-    <hyperlink ref="K96" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption" xr:uid="{00000000-0004-0000-0D00-00001E010000}"/>
-    <hyperlink ref="J96" location="'deliveryPopulation++'!A1" display="deliveryPopulation" xr:uid="{00000000-0004-0000-0D00-00001F010000}"/>
-    <hyperlink ref="L96" location="'PayUPagePayment++'!A1" display="PayUPagePayment" xr:uid="{00000000-0004-0000-0D00-000020010000}"/>
-    <hyperlink ref="M96" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID" xr:uid="{00000000-0004-0000-0D00-000021010000}"/>
-    <hyperlink ref="G96" location="'ic_login++'!A1" display="ic_login" xr:uid="{00000000-0004-0000-0D00-000022010000}"/>
-    <hyperlink ref="H96" location="'ClearCart++'!A1" display="ClearCart" xr:uid="{00000000-0004-0000-0D00-000023010000}"/>
-    <hyperlink ref="P96" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber" xr:uid="{00000000-0004-0000-0D00-000024010000}"/>
-    <hyperlink ref="Q96" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated" xr:uid="{00000000-0004-0000-0D00-000025010000}"/>
-    <hyperlink ref="H88" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0D00-000026010000}"/>
-    <hyperlink ref="H89:H91" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB" xr:uid="{00000000-0004-0000-0D00-000027010000}"/>
+    <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H3" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I4" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H4" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I5" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H5" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="I6" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H6" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="G7" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G8:G9" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H7" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="H8:H9" location="'CreateaccountBackend++'!A1" display="CreateaccountBackend"/>
+    <hyperlink ref="J7" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G10:G14" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H10" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="H11:H14" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G15" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H15" location="'adminUserUpdate++'!A1" display="adminUserUpdate"/>
+    <hyperlink ref="G16" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H16" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I16" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G17" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G18" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G19" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G20" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H17" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H18" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H19" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="H20" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I17" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I18" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I19" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I20" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G21" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H21" location="'ICUpdateUser++'!A1" display="ICUpdateUser"/>
+    <hyperlink ref="I21" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H27" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I27" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M27" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O27" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="H24" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H25" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H22" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H23" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="H26" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="J10:J15" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L17:L21" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L16" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="J27" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K27" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N27" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L27" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P27" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H28" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H30" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I28" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="I30" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M28" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M30" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O28" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O30" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J28" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J30" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K28" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="K30" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N28" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N30" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L28" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="L30" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P28" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="P30" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H31" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I31" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L31" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O31" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J31" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="M31" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="K31" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P31" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H29" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I29" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M29" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O29" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="J29" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K29" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N29" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L29" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P29" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H32" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I32" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="M32" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="J32" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K32" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N32" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="L32" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P32" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="Q32" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="G34" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G37" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="I37" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I33" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J33" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L33" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M33" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N33" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O33" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H33" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="H34" location="'icGiftCardPurchase++'!A1" display="icGiftCardPurchase"/>
+    <hyperlink ref="I34" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J34" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L34" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="M34" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="N34" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O34" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H47" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="H48" location="'EnterBasicDetails++'!A1" display="EnterBasicDetails"/>
+    <hyperlink ref="I47" location="'EnterSpouseInfor++'!A1" display="EnterSpouseInfor"/>
+    <hyperlink ref="J47" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="I48" location="'CreditEnterEmploymentDetails++'!A1" display="CreditEnterEmploymentDetails"/>
+    <hyperlink ref="G47" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G48" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H49" location="'ic_SubscribeNews_DupliEmailID++'!A1" display="ic_SubscribeNews_DupliEmailID"/>
+    <hyperlink ref="G40" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="N40" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G41:G42" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="K54" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="M47" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N47" location="'CreditApp_NavigateFilter++'!A1" display="CreditApp_NavigateFilter"/>
+    <hyperlink ref="O47" location="'CreditStatusVerification++'!A1" display="CreditStatusVerification"/>
+    <hyperlink ref="O32" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="K48" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="L47" location="'EnterContact++'!A1" display="EnterContact"/>
+    <hyperlink ref="J48" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="K47" location="'CreditEnterAddressDetails++'!A1" display="CreditEnterAddressDetails"/>
+    <hyperlink ref="G39" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="G38" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="H53:H54" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="I53" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="J53" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="J35" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="H36" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J36" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="K36" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="L37" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J37" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="L36" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M37" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="H38" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H39" location="'giftCardReport++'!A1" display="giftCardReport"/>
+    <hyperlink ref="H50" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="H50:H52" location="'IC_ProductsSortBy++'!A1" display="IC_ProductsSortBy"/>
+    <hyperlink ref="I2" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="L2" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="H2" location="'accountCreation++'!A1" display="accountCreation"/>
+    <hyperlink ref="K2" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="L3" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="L5" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K3" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K4" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K5" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="L6" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="K6" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K16" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="K17:K21" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="J16" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J17:J21" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J2" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="J3:J6" location="'RetrieveCustomerDetails++'!A1" display="RetrieveCustomerDetails"/>
+    <hyperlink ref="K55" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="J55" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="H55" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="L55" location="'IC_WishlistToCart++'!A1" display="IC_WishlistToCart"/>
+    <hyperlink ref="K56" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K57" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G58" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="J58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="H69" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L71" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I71" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="J71" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="K71" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="M71" location="'SendWishlistToEmail++'!A1" display="SendWishlistToEmail"/>
+    <hyperlink ref="N71" location="'icEmailWishlistverification++'!A1" display="icEmailWishlistverification"/>
+    <hyperlink ref="H56:H57" location="'ic_NavigetoWishlist++'!A1" display="ic_NavigetoWishlist"/>
+    <hyperlink ref="J56:J57" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="H63" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="H64" location="'ic_invalidCredslogin++'!A1" display="ic_invalidCredslogin"/>
+    <hyperlink ref="H70" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H40" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I40" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I41:I42" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H41:H42" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="K41" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K42" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="K40" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J42" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="J40:J41" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L42" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="L40:L41" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N41" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O41" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="O40" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="O42" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="P42" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="O40:O41" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="R41" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R40" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R42" location="'Magento_UserInfoVerification++'!A1" display="Magento_UserInfoVerification"/>
+    <hyperlink ref="R41:R42" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="M54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="I55" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I56:I57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="L57" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="I54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="J54" location="'ic_RemoveFromcart++'!A1" display="ic_RemoveFromcart"/>
+    <hyperlink ref="L54" location="'ic_verifyWishlistItem++'!A1" display="ic_verifyWishlistItem"/>
+    <hyperlink ref="H74" location="'ic_NavigetoWishlist++'!A1" display="NavigateToWishlist_VerifyLoginPageAppear"/>
+    <hyperlink ref="H78" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H79" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G59:G62" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H58" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I58" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="I59:I62" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H75" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="H76:H77" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H80" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I80" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L80" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="G43" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H43" location="'ClearCart++'!A1" display="ClearCart++"/>
+    <hyperlink ref="I43" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G35" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="I36" location="'icRedeemGiftCard++'!A1" display="icRedeemGiftCard"/>
+    <hyperlink ref="I35" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="G85" location="'parrallel_ic_Login++'!A1" display="parrallel_ic_Login"/>
+    <hyperlink ref="I88" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I89" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I90" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I91" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="N92" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="K92" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J92" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L92" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="O92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="N93" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="I93" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K93" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J93" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L93" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="O93" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G94" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H94" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="I94" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K94" location="'validatePaymentOption++'!A1" display="validatePaymentOption"/>
+    <hyperlink ref="M93" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="P92" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="G44" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G2:G6" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G22:G33" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G36" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G45:G46" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G49:G57" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G63:G79" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G81:G84" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G86:G93" location="'LaunchPortal++'!A1" display="LaunchPortal"/>
+    <hyperlink ref="G95" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="J95" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="L95" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="M95" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="N95" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="O95" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="P95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="S95" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="T95" location="'srs_Login++'!A1" display="srs_Login"/>
+    <hyperlink ref="U95" location="'SRSLogonStore++'!A1" display="SRSLogonStore"/>
+    <hyperlink ref="V95" location="'srs_salesOrder_DeliverStatus++'!A1" display="srs_salesOrder_DeliverStatus"/>
+    <hyperlink ref="I95" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="R95" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="T42" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="T40" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="T41" location="'SapCustomer++'!A1" display="SapCustomer"/>
+    <hyperlink ref="S40" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="N96" location="'Login_magento++'!A1" display="Login_magento"/>
+    <hyperlink ref="O96" location="'OrderStatusSearch++'!A1" display="OrderStatusSearch"/>
+    <hyperlink ref="I96" location="'ProductSearch++'!A1" display="ProductSearch"/>
+    <hyperlink ref="K96" location="'CheckoutpaymentOption++'!A1" display="CheckoutpaymentOption"/>
+    <hyperlink ref="J96" location="'deliveryPopulation++'!A1" display="deliveryPopulation"/>
+    <hyperlink ref="L96" location="'PayUPagePayment++'!A1" display="PayUPagePayment"/>
+    <hyperlink ref="M96" location="'ic_RetriveOrderID++'!A1" display="ic_RetriveOrderID"/>
+    <hyperlink ref="G96" location="'ic_login++'!A1" display="ic_login"/>
+    <hyperlink ref="H96" location="'ClearCart++'!A1" display="ClearCart"/>
+    <hyperlink ref="P96" location="'GenerateOrderSAPnumber++'!A1" display="GenerateOrderSAPnumber"/>
+    <hyperlink ref="Q96" location="'SAP_OrderRelated++'!A1" display="SAP_OrderRelated"/>
+    <hyperlink ref="H88" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB"/>
+    <hyperlink ref="H89:H91" location="'SapRSIGetDataFromSAPDB++'!A1" display="SapRSIGetDataFromSAPDB"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18262,7 +18076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18298,14 +18112,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18342,14 +18156,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DBCBA8-8371-4E8A-89E7-DD862E72909E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18399,19 +18213,19 @@
     <cfRule type="duplicateValues" dxfId="279" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{2E01E73B-5236-4EED-82E9-0A8A9CB4EB1C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{FFB10F9A-9205-4C9F-AB6F-66955015CA4D}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18462,15 +18276,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" location="ZEccSRS-display" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1000-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1" location="ZEccSRS-display"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18521,12 +18335,12 @@
     <cfRule type="duplicateValues" dxfId="180" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"IC_frontend_QA_validUser,IC_frontend_QA_invalidUsername,IC_frontend_QA_invalidPassword,IC_magento_QA,EVS_frontend_QA,EVS_magento_QA"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18534,7 +18348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18810,19 +18624,19 @@
     <cfRule type="duplicateValues" dxfId="178" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{00000000-0002-0000-1200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18868,14 +18682,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -18949,14 +18763,14 @@
     <cfRule type="duplicateValues" dxfId="176" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19030,16 +18844,16 @@
     <cfRule type="duplicateValues" dxfId="174" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId2" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-1500-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="D3" r:id="rId2" display="automation13@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19121,7 +18935,7 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19245,14 +19059,14 @@
     <cfRule type="duplicateValues" dxfId="167" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19415,19 +19229,19 @@
     <cfRule type="duplicateValues" dxfId="160" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-1800-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -19622,18 +19436,18 @@
     <cfRule type="duplicateValues" dxfId="155" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1900-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-1900-000002000000}"/>
-    <hyperlink ref="E4:E7" r:id="rId4" display="MichaelGHand@teleworm.us" xr:uid="{00000000-0004-0000-1900-000003000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1900-000004000000}"/>
+    <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E4:E7" r:id="rId4" display="MichaelGHand@teleworm.us"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4F7395-4BDC-4DFE-BEDF-4192346F3655}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19667,7 +19481,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
     </row>
   </sheetData>
@@ -19682,7 +19496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20020,16 +19834,16 @@
     <cfRule type="duplicateValues" dxfId="154" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8" xr:uid="{00000000-0002-0000-1A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 G2:G7 I2:I7 K2:K7 M2:N7 U2:V7" xr:uid="{00000000-0002-0000-1A00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7 G2:G7 I2:I7 K2:K7 M2:N7 U2:V7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1A00-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -20037,7 +19851,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20316,12 +20130,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6 F2:F6 H2:H6 J2:J6 L2:L6 N2:N6" xr:uid="{00000000-0002-0000-1B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6 F2:F6 H2:H6 J2:J6 L2:L6 N2:N6">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -20329,7 +20143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20422,18 +20236,18 @@
     <cfRule type="duplicateValues" dxfId="153" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-1C00-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-1C00-000001000000}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{00000000-0004-0000-1C00-000002000000}"/>
-    <hyperlink ref="E2" r:id="rId4" xr:uid="{00000000-0004-0000-1C00-000003000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1C00-000004000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="E3" r:id="rId3"/>
+    <hyperlink ref="E2" r:id="rId4"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20521,15 +20335,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-1D00-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20604,14 +20418,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20728,14 +20542,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20821,19 +20635,19 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-2000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
       <formula1>"payUcreditcard"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2000-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -20946,14 +20760,14 @@
     <cfRule type="duplicateValues" dxfId="152" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -21244,11 +21058,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2200-000001000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-2200-000002000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-2200-000003000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-2200-000004000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -21256,7 +21070,7 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -22020,28 +21834,28 @@
     <cfRule type="duplicateValues" dxfId="151" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15" xr:uid="{00000000-0002-0000-2300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15">
       <formula1>"No,Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3 N11:N1048576" xr:uid="{00000000-0002-0000-2300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3 N11:N1048576">
       <formula1>"ID,Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3 I11:I1048576 M2:M1048576" xr:uid="{00000000-0002-0000-2300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3 I11:I1048576 M2:M1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N10" xr:uid="{00000000-0002-0000-2300-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N4:N10">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I10 P4:T6 P8:S9 Q7:S7 Q10:S10" xr:uid="{00000000-0002-0000-2300-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I10 P4:T6 P8:S9 Q7:S7 Q10:S10">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L6" xr:uid="{00000000-0002-0000-2300-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L6">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -22049,7 +21863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586266A-FF52-4B4A-9350-EC50F91BF86C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -22083,7 +21897,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="99" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
     </row>
   </sheetData>
@@ -22092,7 +21906,7 @@
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -22936,18 +22750,18 @@
     <cfRule type="duplicateValues" dxfId="136" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21" xr:uid="{00000000-0002-0000-2400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21" xr:uid="{00000000-0002-0000-2400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21" xr:uid="{00000000-0002-0000-2400-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2400-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -22955,21 +22769,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA421\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA403.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>D23:D1048576 E22</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\41066\git\Main_21_06\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA464.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[2]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E10:E15</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2400-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA599_TA600\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA464.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[3]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E18:E21</xm:sqref>
         </x14:dataValidation>
@@ -22980,7 +22794,7 @@
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
@@ -24371,18 +24185,18 @@
     <cfRule type="duplicateValues" dxfId="125" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16" xr:uid="{00000000-0002-0000-2500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G16" xr:uid="{00000000-0002-0000-2500-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G16">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K16" xr:uid="{00000000-0002-0000-2500-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K16">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -24390,21 +24204,21 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2500-000003000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$18</xm:f>
           </x14:formula1>
           <xm:sqref>E2:E36</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2500-000004000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Products_Category!$A$2:$A$7</xm:f>
           </x14:formula1>
           <xm:sqref>E39:E1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2500-000005000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA421\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA403.xlsx]Products_Category'!#REF!</xm:f>
+            <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>E37:E38</xm:sqref>
         </x14:dataValidation>
@@ -24415,7 +24229,7 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -25672,21 +25486,21 @@
     <cfRule type="duplicateValues" dxfId="119" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32" xr:uid="{00000000-0002-0000-2600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
       <formula1>"Main Website,Incredible Connection,Hifi Corporation,Russells,Sleepmasters,Rochester"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11 Q2:U11 J32 Q32:U32" xr:uid="{00000000-0002-0000-2600-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J11 Q2:U11 J32 Q32:U32">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O11 O31:O32" xr:uid="{00000000-0002-0000-2600-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O11 O31:O32">
       <formula1>"ID, Passport"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11 N31:N32" xr:uid="{00000000-0002-0000-2600-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N11 N31:N32">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
+    <hyperlink ref="G7" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
@@ -25694,7 +25508,7 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -25782,8 +25596,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-2700-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-2700-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -25791,7 +25605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26165,14 +25979,14 @@
     <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26391,14 +26205,14 @@
     <cfRule type="duplicateValues" dxfId="105" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26613,7 +26427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26656,14 +26470,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26712,14 +26526,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-2C00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26824,7 +26638,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26865,7 +26679,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="99" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
     </row>
   </sheetData>
@@ -26873,14 +26687,14 @@
     <cfRule type="duplicateValues" dxfId="276" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27036,7 +26850,7 @@
     <cfRule type="duplicateValues" dxfId="97" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-2E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
       <formula1>"All,Specific"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27045,7 +26859,7 @@
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27257,22 +27071,22 @@
     <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-2F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
       <formula1>"ExistingUser,logedOn_user"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-2F00-000001000000}"/>
-    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-2F00-000002000000}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{00000000-0004-0000-2F00-000003000000}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4:E7" r:id="rId3" display="watlevi41@gmail.com"/>
+    <hyperlink ref="E8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -27664,7 +27478,7 @@
     <cfRule type="duplicateValues" dxfId="89" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Update Account,Update Account Magento Admin,Create Account,Create Account Magento Admin,Guest Customer Creation,Registered customer from sales order"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27673,7 +27487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -27765,7 +27579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27828,7 +27642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -27984,10 +27798,10 @@
     <cfRule type="duplicateValues" dxfId="84" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{00000000-0002-0000-3300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
   </dataValidations>
@@ -27996,7 +27810,7 @@
 </file>
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28112,13 +27926,13 @@
     <cfRule type="duplicateValues" dxfId="82" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{00000000-0002-0000-3400-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
       <formula1>"ABSA,AFRICAN BANK,BIDVEST.CAPITEC,FNB,INVESTEC,NEDBANK,STANDARD BANK SA"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576" xr:uid="{00000000-0002-0000-3400-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H1048576">
       <formula1>"English,Afrikaans,Sesotho,Xhosa,Zulu"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28127,7 +27941,7 @@
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28264,7 +28078,7 @@
     <cfRule type="duplicateValues" dxfId="80" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-3500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28272,7 +28086,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-3500-000001000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Preferred Store'!$A$2:$A$71</xm:f>
           </x14:formula1>
@@ -28285,7 +28099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28391,7 +28205,7 @@
     <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3600-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Domestic Worker,Company Employed,Government Employed,Full-time Housewife,Self Employed - Company Owner,Self Employed - Informal Trader,Student,Unemployed,Pensioner/Retired,Contract Worker,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28401,7 +28215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28647,25 +28461,25 @@
     <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-3700-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3" xr:uid="{00000000-0002-0000-3700-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J3">
       <formula1>"Ms,Mr,Dr,Miss,Mrs,Prof,Rev,Adv,Honorable"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3" xr:uid="{00000000-0002-0000-3700-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N3">
       <formula1>"African,Asian,Coloured,White,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3" xr:uid="{00000000-0002-0000-3700-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:O3">
       <formula1>"Single,Married / Civil Partnership,Widowed,Divorced,Separated,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3" xr:uid="{00000000-0002-0000-3700-000004000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P3">
       <formula1>"ANC with Accrual,ANC without Accrual,In Community,Customary Union,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3" xr:uid="{00000000-0002-0000-3700-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:U3">
       <formula1>"Female,Male"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576" xr:uid="{00000000-0002-0000-3700-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2:V1048576">
       <formula1>"0,1,2,3,4,5,6,7,8,9"</formula1>
     </dataValidation>
   </dataValidations>
@@ -28675,7 +28489,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28739,16 +28553,16 @@
     <cfRule type="duplicateValues" dxfId="274" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="D3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28819,7 +28633,7 @@
 </file>
 
 <file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -28874,7 +28688,7 @@
 </file>
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -28965,7 +28779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -29615,25 +29429,25 @@
     <cfRule type="duplicateValues" dxfId="66" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-3B00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
       <formula1>"Eastern Cape,Free State,Gauteng,KwaZulu-Natal,Limpopo,Mpumalanga,Northern Cape,North-West,Western Cape"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7" xr:uid="{00000000-0002-0000-3B00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2:W10 I2:I10 K2:K10 M2:O10 G2:G10 E2:E10 F5:F7">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-3B00-000001000000}"/>
-    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3B00-000002000000}"/>
-    <hyperlink ref="D5:D6" r:id="rId4" display="original2Ic@automationjdg.co.za" xr:uid="{00000000-0004-0000-3B00-000003000000}"/>
+    <hyperlink ref="D6:D7" r:id="rId1" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D7" r:id="rId2"/>
+    <hyperlink ref="D2:D4" r:id="rId3" display="original2Ic@automationjdg.co.za"/>
+    <hyperlink ref="D5:D6" r:id="rId4" display="original2Ic@automationjdg.co.za"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
@@ -30291,7 +30105,7 @@
     <cfRule type="duplicateValues" dxfId="60" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-3C00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -30300,7 +30114,7 @@
 </file>
 
 <file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -30754,7 +30568,7 @@
     <cfRule type="duplicateValues" dxfId="58" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3D00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
@@ -30763,7 +30577,7 @@
 </file>
 
 <file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -31330,7 +31144,7 @@
     <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-3E00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -31338,7 +31152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -31634,19 +31448,19 @@
     <cfRule type="duplicateValues" dxfId="49" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3F00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"payUcreditcard,Cash_Deposits"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-3F00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -32661,18 +32475,18 @@
     <cfRule type="duplicateValues" dxfId="45" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-4000-000000000000}"/>
-    <hyperlink ref="O3" r:id="rId2" xr:uid="{00000000-0004-0000-4000-000001000000}"/>
-    <hyperlink ref="O4" r:id="rId3" xr:uid="{00000000-0004-0000-4000-000002000000}"/>
-    <hyperlink ref="O5" r:id="rId4" xr:uid="{00000000-0004-0000-4000-000003000000}"/>
-    <hyperlink ref="O8" r:id="rId5" xr:uid="{00000000-0004-0000-4000-000004000000}"/>
-    <hyperlink ref="O6" r:id="rId6" xr:uid="{00000000-0004-0000-4000-000005000000}"/>
-    <hyperlink ref="O7" r:id="rId7" xr:uid="{00000000-0004-0000-4000-000006000000}"/>
-    <hyperlink ref="O9" r:id="rId8" xr:uid="{00000000-0004-0000-4000-000007000000}"/>
-    <hyperlink ref="O34" r:id="rId9" xr:uid="{00000000-0004-0000-4000-000008000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4000-000009000000}"/>
-    <hyperlink ref="O35" r:id="rId10" xr:uid="{00000000-0004-0000-4000-00000A000000}"/>
-    <hyperlink ref="O36" r:id="rId11" xr:uid="{00000000-0004-0000-4000-00000B000000}"/>
+    <hyperlink ref="O2" r:id="rId1"/>
+    <hyperlink ref="O3" r:id="rId2"/>
+    <hyperlink ref="O4" r:id="rId3"/>
+    <hyperlink ref="O5" r:id="rId4"/>
+    <hyperlink ref="O8" r:id="rId5"/>
+    <hyperlink ref="O6" r:id="rId6"/>
+    <hyperlink ref="O7" r:id="rId7"/>
+    <hyperlink ref="O9" r:id="rId8"/>
+    <hyperlink ref="O34" r:id="rId9"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
+    <hyperlink ref="O35" r:id="rId10"/>
+    <hyperlink ref="O36" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId12"/>
@@ -32680,7 +32494,7 @@
 </file>
 
 <file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -32850,7 +32664,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33033,20 +32847,20 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L4">
       <formula1>"Default(General),Retailer,Wholesale"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K4">
       <formula1>"Main Website,Everyshop"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H4">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="F3:F4" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3:F4" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -33055,7 +32869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33218,19 +33032,19 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-4200-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{00000000-0004-0000-4200-000001000000}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{00000000-0004-0000-4200-000002000000}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{00000000-0004-0000-4200-000003000000}"/>
-    <hyperlink ref="J4" r:id="rId5" xr:uid="{00000000-0004-0000-4200-000004000000}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{00000000-0004-0000-4200-000005000000}"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="J3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="J4" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33487,14 +33301,14 @@
     <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-4300-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -33831,14 +33645,14 @@
     <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4400-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -34151,14 +33965,14 @@
     <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34427,14 +34241,14 @@
     <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4600-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34497,7 +34311,7 @@
 </file>
 
 <file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34605,7 +34419,7 @@
 </file>
 
 <file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -34705,7 +34519,7 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-4900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
       <formula1>"Reuse,Redeem"</formula1>
     </dataValidation>
   </dataValidations>
@@ -34715,7 +34529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -34799,7 +34613,7 @@
 </file>
 
 <file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -35451,44 +35265,44 @@
     <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-4B00-000000000000}"/>
-    <hyperlink ref="F8" r:id="rId2" xr:uid="{00000000-0004-0000-4B00-000001000000}"/>
-    <hyperlink ref="F13" r:id="rId3" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000002000000}"/>
-    <hyperlink ref="F22" r:id="rId4" xr:uid="{00000000-0004-0000-4B00-000003000000}"/>
-    <hyperlink ref="F23" r:id="rId5" xr:uid="{00000000-0004-0000-4B00-000004000000}"/>
-    <hyperlink ref="E13" r:id="rId6" xr:uid="{00000000-0004-0000-4B00-000005000000}"/>
-    <hyperlink ref="F14" r:id="rId7" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000006000000}"/>
-    <hyperlink ref="F12" r:id="rId8" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000007000000}"/>
-    <hyperlink ref="E14" r:id="rId9" xr:uid="{00000000-0004-0000-4B00-000008000000}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-4B00-000009000000}"/>
-    <hyperlink ref="F17" r:id="rId11" display="Password@123" xr:uid="{00000000-0004-0000-4B00-00000A000000}"/>
-    <hyperlink ref="E18" r:id="rId12" xr:uid="{00000000-0004-0000-4B00-00000B000000}"/>
-    <hyperlink ref="F18" r:id="rId13" display="Password@123" xr:uid="{00000000-0004-0000-4B00-00000C000000}"/>
-    <hyperlink ref="E20" r:id="rId14" xr:uid="{00000000-0004-0000-4B00-00000D000000}"/>
-    <hyperlink ref="E21" r:id="rId15" xr:uid="{00000000-0004-0000-4B00-00000E000000}"/>
-    <hyperlink ref="E24" r:id="rId16" xr:uid="{00000000-0004-0000-4B00-00000F000000}"/>
-    <hyperlink ref="E25" r:id="rId17" xr:uid="{00000000-0004-0000-4B00-000010000000}"/>
-    <hyperlink ref="E16" r:id="rId18" xr:uid="{00000000-0004-0000-4B00-000011000000}"/>
-    <hyperlink ref="F19" r:id="rId19" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000012000000}"/>
-    <hyperlink ref="E19" r:id="rId20" xr:uid="{00000000-0004-0000-4B00-000013000000}"/>
-    <hyperlink ref="E11" r:id="rId21" xr:uid="{00000000-0004-0000-4B00-000014000000}"/>
-    <hyperlink ref="F11" r:id="rId22" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000015000000}"/>
-    <hyperlink ref="E15" r:id="rId23" xr:uid="{00000000-0004-0000-4B00-000016000000}"/>
-    <hyperlink ref="F15" r:id="rId24" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000017000000}"/>
-    <hyperlink ref="E8" r:id="rId25" xr:uid="{00000000-0004-0000-4B00-000018000000}"/>
-    <hyperlink ref="E10" r:id="rId26" xr:uid="{00000000-0004-0000-4B00-000019000000}"/>
-    <hyperlink ref="F10" r:id="rId27" xr:uid="{00000000-0004-0000-4B00-00001A000000}"/>
-    <hyperlink ref="E9" r:id="rId28" xr:uid="{00000000-0004-0000-4B00-00001B000000}"/>
-    <hyperlink ref="F9" r:id="rId29" xr:uid="{00000000-0004-0000-4B00-00001C000000}"/>
-    <hyperlink ref="F3:F7" r:id="rId30" display="Password@123" xr:uid="{00000000-0004-0000-4B00-00001D000000}"/>
-    <hyperlink ref="F3" r:id="rId31" xr:uid="{00000000-0004-0000-4B00-00001E000000}"/>
-    <hyperlink ref="F4" r:id="rId32" xr:uid="{00000000-0004-0000-4B00-00001F000000}"/>
-    <hyperlink ref="F5" r:id="rId33" xr:uid="{00000000-0004-0000-4B00-000020000000}"/>
-    <hyperlink ref="F6" r:id="rId34" xr:uid="{00000000-0004-0000-4B00-000021000000}"/>
-    <hyperlink ref="F7" r:id="rId35" xr:uid="{00000000-0004-0000-4B00-000022000000}"/>
-    <hyperlink ref="F29" r:id="rId36" display="Password@123" xr:uid="{00000000-0004-0000-4B00-000023000000}"/>
-    <hyperlink ref="E29" r:id="rId37" xr:uid="{00000000-0004-0000-4B00-000024000000}"/>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4B00-000025000000}"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F8" r:id="rId2"/>
+    <hyperlink ref="F13" r:id="rId3" display="Password@123"/>
+    <hyperlink ref="F22" r:id="rId4"/>
+    <hyperlink ref="F23" r:id="rId5"/>
+    <hyperlink ref="E13" r:id="rId6"/>
+    <hyperlink ref="F14" r:id="rId7" display="Password@123"/>
+    <hyperlink ref="F12" r:id="rId8" display="Password@123"/>
+    <hyperlink ref="E14" r:id="rId9"/>
+    <hyperlink ref="E17" r:id="rId10"/>
+    <hyperlink ref="F17" r:id="rId11" display="Password@123"/>
+    <hyperlink ref="E18" r:id="rId12"/>
+    <hyperlink ref="F18" r:id="rId13" display="Password@123"/>
+    <hyperlink ref="E20" r:id="rId14"/>
+    <hyperlink ref="E21" r:id="rId15"/>
+    <hyperlink ref="E24" r:id="rId16"/>
+    <hyperlink ref="E25" r:id="rId17"/>
+    <hyperlink ref="E16" r:id="rId18"/>
+    <hyperlink ref="F19" r:id="rId19" display="Password@123"/>
+    <hyperlink ref="E19" r:id="rId20"/>
+    <hyperlink ref="E11" r:id="rId21"/>
+    <hyperlink ref="F11" r:id="rId22" display="Password@123"/>
+    <hyperlink ref="E15" r:id="rId23"/>
+    <hyperlink ref="F15" r:id="rId24" display="Password@123"/>
+    <hyperlink ref="E8" r:id="rId25"/>
+    <hyperlink ref="E10" r:id="rId26"/>
+    <hyperlink ref="F10" r:id="rId27"/>
+    <hyperlink ref="E9" r:id="rId28"/>
+    <hyperlink ref="F9" r:id="rId29"/>
+    <hyperlink ref="F3:F7" r:id="rId30" display="Password@123"/>
+    <hyperlink ref="F3" r:id="rId31"/>
+    <hyperlink ref="F4" r:id="rId32"/>
+    <hyperlink ref="F5" r:id="rId33"/>
+    <hyperlink ref="F6" r:id="rId34"/>
+    <hyperlink ref="F7" r:id="rId35"/>
+    <hyperlink ref="F29" r:id="rId36" display="Password@123"/>
+    <hyperlink ref="E29" r:id="rId37"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId38"/>
@@ -35496,7 +35310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -35822,19 +35636,19 @@
     <cfRule type="duplicateValues" dxfId="273" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
       <formula1>"Guest Customer Creation, Customer Creation, Customer Update,Customer Creation Magento Admin, Customer Update Magento Admin"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36076,14 +35890,14 @@
     <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4C00-000000000000}"/>
+    <hyperlink ref="A1" location="IC!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -36170,15 +35984,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-4D00-000000000000}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{00000000-0004-0000-4D00-000001000000}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36234,7 +36048,7 @@
 </file>
 
 <file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36335,14 +36149,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36466,8 +36280,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Welc0me@2021" xr:uid="{00000000-0004-0000-5000-000000000000}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{00000000-0004-0000-5000-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Welc0me@2021"/>
+    <hyperlink ref="F6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -36475,7 +36289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36602,9 +36416,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-5100-000000000000}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{00000000-0004-0000-5100-000001000000}"/>
-    <hyperlink ref="C5" r:id="rId3" xr:uid="{00000000-0004-0000-5100-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -36612,7 +36426,7 @@
 </file>
 
 <file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36669,7 +36483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37138,17 +36952,17 @@
     <cfRule type="duplicateValues" dxfId="0" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-5300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
       <formula1>"Main Website,Incredible Connection"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576" xr:uid="{00000000-0002-0000-5300-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G4 F5:F1048576">
       <formula1>"SAID,Passport"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5300-000000000000}"/>
-    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5300-000001000000}"/>
-    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com" xr:uid="{00000000-0004-0000-5300-000002000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F3" r:id="rId2" display="TestAutomation2@gmail.com"/>
+    <hyperlink ref="F4" r:id="rId3" display="TestAutomation2@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
@@ -37157,7 +36971,7 @@
 </file>
 
 <file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37198,7 +37012,7 @@
 </file>
 
 <file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37302,7 +37116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -37388,14 +37202,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37599,7 +37413,7 @@
 </file>
 
 <file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37703,7 +37517,7 @@
 </file>
 
 <file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -37807,7 +37621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38180,7 +37994,7 @@
 </file>
 
 <file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38284,7 +38098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView topLeftCell="L14" workbookViewId="0">

</xml_diff>

<commit_message>
removeing static variables from EVS_Delivery:Streetname,Cityname,Postalcode
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="39" activeTab="41"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="evs_RedeemGiftCard++" sheetId="121" r:id="rId1"/>
@@ -252,7 +252,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5724" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5762" uniqueCount="1064">
   <si>
     <t>testSuitID</t>
   </si>
@@ -3416,6 +3416,42 @@
   </si>
   <si>
     <t>Lio</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>39 Pritchard Street</t>
+  </si>
+  <si>
+    <t>Christ</t>
+  </si>
+  <si>
+    <t>Bowen</t>
+  </si>
+  <si>
+    <t>LarryMBruce@dayrep.com</t>
+  </si>
+  <si>
+    <t>Jerico</t>
+  </si>
+  <si>
+    <t>45 Zenith Drive</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>0845397015</t>
+  </si>
+  <si>
+    <t>Rustenburg</t>
+  </si>
+  <si>
+    <t>034</t>
   </si>
 </sst>
 </file>
@@ -3729,7 +3765,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="248">
+  <cellXfs count="251">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4328,6 +4364,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4336,7 +4377,127 @@
     <cellStyle name="Normal 2 2" xfId="4"/>
     <cellStyle name="Normal 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="366">
+  <dxfs count="378">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -8393,10 +8554,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="365" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="377" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="364" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="376" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
@@ -8787,7 +8948,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="305" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="317" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D18">
@@ -8808,9 +8969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -8963,13 +9122,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="304" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="316" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="303" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="315" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="302" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="314" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -9146,13 +9305,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="301" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="313" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="300" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="312" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="299" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="311" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -9166,7 +9325,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9794,19 +9953,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B15">
-    <cfRule type="duplicateValues" dxfId="298" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="310" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B25">
-    <cfRule type="duplicateValues" dxfId="297" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="309" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:A30">
-    <cfRule type="duplicateValues" dxfId="296" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="308" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="295" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="307" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="294" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="306" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -10427,34 +10586,34 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B33:B35">
-    <cfRule type="duplicateValues" dxfId="293" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="305" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36">
-    <cfRule type="duplicateValues" dxfId="292" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="304" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="291" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="303" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:A32">
-    <cfRule type="duplicateValues" dxfId="290" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="302" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31:B32">
-    <cfRule type="duplicateValues" dxfId="289" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="301" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="duplicateValues" dxfId="288" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="300" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="duplicateValues" dxfId="287" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="299" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="286" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="298" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="285" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="297" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="duplicateValues" dxfId="284" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="296" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -11559,91 +11718,91 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B49:B52 B29:B44 B18:B23 B2:B16">
-    <cfRule type="duplicateValues" dxfId="283" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="295" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="282" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="294" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B28">
-    <cfRule type="duplicateValues" dxfId="281" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="293" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="duplicateValues" dxfId="280" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="292" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="279" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="291" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="278" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="290" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="277" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="289" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="276" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="288" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="275" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="287" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="274" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="286" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B59">
-    <cfRule type="duplicateValues" dxfId="273" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="285" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="272" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="284" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A60">
-    <cfRule type="duplicateValues" dxfId="271" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="283" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A70">
-    <cfRule type="duplicateValues" dxfId="270" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="282" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="duplicateValues" dxfId="269" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="281" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="duplicateValues" dxfId="268" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="280" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="267" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="279" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62:B63">
-    <cfRule type="duplicateValues" dxfId="266" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="278" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="duplicateValues" dxfId="265" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="277" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B68">
-    <cfRule type="duplicateValues" dxfId="264" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="276" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B69">
-    <cfRule type="duplicateValues" dxfId="263" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="275" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A69">
-    <cfRule type="duplicateValues" dxfId="262" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="274" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A67">
-    <cfRule type="duplicateValues" dxfId="261" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="273" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="duplicateValues" dxfId="260" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="272" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A72">
-    <cfRule type="duplicateValues" dxfId="259" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="271" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72">
-    <cfRule type="duplicateValues" dxfId="258" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="270" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A73:A74">
-    <cfRule type="duplicateValues" dxfId="257" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="269" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="duplicateValues" dxfId="256" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="268" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74">
-    <cfRule type="duplicateValues" dxfId="255" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="267" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -12528,49 +12687,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B49:B52 B29:B44 B18:B23 B2:B16">
-    <cfRule type="duplicateValues" dxfId="254" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="266" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="253" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="265" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B28">
-    <cfRule type="duplicateValues" dxfId="252" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="duplicateValues" dxfId="251" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="250" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="249" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="248" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="260" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="247" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="246" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="245" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B59">
-    <cfRule type="duplicateValues" dxfId="244" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="256" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="243" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="255" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A60">
-    <cfRule type="duplicateValues" dxfId="242" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="254" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="241" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="253" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="duplicateValues" dxfId="240" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="252" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -16554,124 +16713,124 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="239" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="238" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="237" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="236" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="235" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="234" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="233" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="232" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="231" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="230" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="229" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="228" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="227" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="226" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="225" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="224" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="223" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="222" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="221" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="220" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="219" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="218" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="217" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="216" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="215" priority="91"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="91"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="214" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="213" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="225" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="212" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="224" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="211" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="210" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="209" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="208" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H88:J91">
-    <cfRule type="duplicateValues" dxfId="207" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="206" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="205" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="204" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="203" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H92:H93">
-    <cfRule type="duplicateValues" dxfId="202" priority="100"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="100"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="duplicateValues" dxfId="201" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="duplicateValues" dxfId="200" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento"/>
@@ -16980,8 +17139,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V70"/>
   <sheetViews>
-    <sheetView topLeftCell="E58" workbookViewId="0">
-      <selection activeCell="J68" sqref="J68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="M59" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -19607,148 +19769,148 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="363" priority="70"/>
+    <cfRule type="duplicateValues" dxfId="375" priority="70"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="duplicateValues" dxfId="362" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="374" priority="69"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="361" priority="68"/>
+    <cfRule type="duplicateValues" dxfId="373" priority="68"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D7">
-    <cfRule type="duplicateValues" dxfId="360" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="372" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1">
-    <cfRule type="duplicateValues" dxfId="359" priority="161"/>
+    <cfRule type="duplicateValues" dxfId="371" priority="161"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="358" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="370" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="357" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="369" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="356" priority="51"/>
+    <cfRule type="duplicateValues" dxfId="368" priority="51"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D23">
-    <cfRule type="duplicateValues" dxfId="355" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="367" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D32">
-    <cfRule type="duplicateValues" dxfId="354" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="366" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B32">
-    <cfRule type="duplicateValues" dxfId="353" priority="48"/>
+    <cfRule type="duplicateValues" dxfId="365" priority="48"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D33:D37">
-    <cfRule type="duplicateValues" dxfId="352" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="364" priority="47"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33:B37">
-    <cfRule type="duplicateValues" dxfId="351" priority="46"/>
+    <cfRule type="duplicateValues" dxfId="363" priority="46"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="350" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="362" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="duplicateValues" dxfId="349" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="361" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41:B42">
-    <cfRule type="duplicateValues" dxfId="348" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="360" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="duplicateValues" dxfId="347" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="359" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="duplicateValues" dxfId="346" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="358" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="345" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="357" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="344" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="356" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="343" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="355" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="342" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="354" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48:B52">
-    <cfRule type="duplicateValues" dxfId="341" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="353" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:G51 I48:I51">
-    <cfRule type="duplicateValues" dxfId="340" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="352" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="339" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="351" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48:D51">
-    <cfRule type="duplicateValues" dxfId="338" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="350" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="duplicateValues" dxfId="337" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="349" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52">
-    <cfRule type="duplicateValues" dxfId="336" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="348" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:H53">
-    <cfRule type="duplicateValues" dxfId="335" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="347" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="334" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="346" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55:B56">
-    <cfRule type="duplicateValues" dxfId="333" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="345" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="duplicateValues" dxfId="332" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="344" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56">
-    <cfRule type="duplicateValues" dxfId="331" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="343" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45">
-    <cfRule type="duplicateValues" dxfId="330" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="342" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63">
-    <cfRule type="duplicateValues" dxfId="329" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="341" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="duplicateValues" dxfId="328" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="340" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="duplicateValues" dxfId="327" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="339" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60">
-    <cfRule type="duplicateValues" dxfId="326" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="338" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B60">
-    <cfRule type="duplicateValues" dxfId="325" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="337" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61">
-    <cfRule type="duplicateValues" dxfId="324" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="336" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="duplicateValues" dxfId="323" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="335" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="duplicateValues" dxfId="322" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="334" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62">
-    <cfRule type="duplicateValues" dxfId="321" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="333" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65">
-    <cfRule type="duplicateValues" dxfId="320" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="332" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="duplicateValues" dxfId="319" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="331" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66:A67">
-    <cfRule type="duplicateValues" dxfId="318" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="330" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="duplicateValues" dxfId="317" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="329" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67">
-    <cfRule type="duplicateValues" dxfId="316" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="328" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="H2" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch"/>
@@ -20142,10 +20304,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="199" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="198" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -20471,10 +20633,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="197" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="196" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21">
@@ -20610,10 +20772,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="195" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="194" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -20691,10 +20853,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="193" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="192" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com"/>
@@ -20781,7 +20943,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="191" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20894,22 +21056,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="190" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="189" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="188" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="187" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="186" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="185" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -20932,8 +21094,8 @@
     <col min="4" max="4" width="12.5703125" style="99" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="99" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="20.5703125" style="99" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="99" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="99" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="99" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="99" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9.140625" style="99"/>
   </cols>
   <sheetData>
@@ -21035,13 +21197,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="315" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="327" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="314" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="326" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="313" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="325" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -21197,25 +21359,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="184" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="183" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="195" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B6">
-    <cfRule type="duplicateValues" dxfId="182" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="194" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="181" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="193" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="180" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="179" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="178" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9">
@@ -21410,19 +21572,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="177" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="176" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="175" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="174" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="173" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com"/>
@@ -21771,7 +21933,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="172" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8">
@@ -22173,7 +22335,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="171" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
@@ -22415,13 +22577,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="170" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="169" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="168" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -22707,13 +22869,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A4:A5">
-    <cfRule type="duplicateValues" dxfId="167" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="166" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="165" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -22879,13 +23041,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="164" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="163" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="162" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2">
@@ -23100,16 +23262,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="161" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="duplicateValues" dxfId="160" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="159" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="158" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -23163,10 +23325,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="312" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="324" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="311" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="323" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -23182,132 +23344,134 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="99"/>
-    <col min="2" max="2" width="86.5703125" style="99" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="99" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="99"/>
-    <col min="5" max="5" width="14.140625" style="99" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" style="99" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="99" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="99"/>
-    <col min="9" max="9" width="13.140625" style="99" customWidth="1"/>
-    <col min="10" max="12" width="9.140625" style="99"/>
-    <col min="13" max="14" width="12.140625" style="99" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="99" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.85546875" style="99" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="99" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="99"/>
+    <col min="1" max="1" width="5" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="30"/>
+    <col min="9" max="9" width="11" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.85546875" style="30" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="4" customFormat="1" ht="30">
-      <c r="A1" s="171" t="s">
+    <row r="1" spans="1:17" s="249" customFormat="1">
+      <c r="A1" s="186" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="108" t="s">
+      <c r="C1" s="80" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="108" t="s">
+      <c r="D1" s="80" t="s">
         <v>392</v>
       </c>
-      <c r="E1" s="108" t="s">
+      <c r="E1" s="80" t="s">
         <v>393</v>
       </c>
-      <c r="F1" s="108" t="s">
+      <c r="F1" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="G1" s="108" t="s">
+      <c r="G1" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="H1" s="108" t="s">
+      <c r="H1" s="80" t="s">
         <v>60</v>
       </c>
-      <c r="I1" s="108" t="s">
+      <c r="I1" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="108" t="s">
+      <c r="J1" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="108" t="s">
+      <c r="K1" s="80" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="108" t="s">
+      <c r="L1" s="80" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="108" t="s">
+      <c r="M1" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="108" t="s">
+      <c r="N1" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="O1" s="108" t="s">
+      <c r="O1" s="80" t="s">
         <v>67</v>
       </c>
-      <c r="P1" s="108" t="s">
+      <c r="P1" s="80" t="s">
         <v>68</v>
       </c>
-      <c r="Q1" s="108" t="s">
+      <c r="Q1" s="80" t="s">
         <v>809</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="99">
-        <v>1</v>
-      </c>
-      <c r="B2" s="99" t="s">
+      <c r="A2" s="30">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>806</v>
       </c>
-      <c r="C2" s="99">
-        <v>1</v>
-      </c>
-      <c r="D2" s="99" t="s">
+      <c r="C2" s="30">
+        <v>1</v>
+      </c>
+      <c r="D2" s="30" t="s">
         <v>565</v>
       </c>
-      <c r="E2" s="99" t="s">
+      <c r="E2" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="F2" s="99" t="s">
+      <c r="F2" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="G2" s="99" t="s">
+      <c r="G2" s="30" t="s">
         <v>810</v>
       </c>
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="30" t="s">
         <v>821</v>
       </c>
-      <c r="I2" s="99">
+      <c r="I2" s="30">
         <v>8358815893</v>
       </c>
-      <c r="J2" s="99" t="s">
+      <c r="J2" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="99" t="s">
+      <c r="K2" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L2" s="99" t="s">
+      <c r="L2" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="M2" s="99">
+      <c r="M2" s="30">
         <v>3820</v>
       </c>
-      <c r="N2" s="99">
+      <c r="N2" s="30">
         <v>435343</v>
       </c>
-      <c r="O2" s="100" t="s">
+      <c r="O2" s="161" t="s">
         <v>823</v>
       </c>
-      <c r="P2" s="165" t="s">
+      <c r="P2" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q2" s="99" t="s">
+      <c r="Q2" s="30" t="s">
         <v>812</v>
       </c>
     </row>
@@ -23318,49 +23482,49 @@
       <c r="B3" s="30" t="s">
         <v>984</v>
       </c>
-      <c r="C3" s="99">
-        <v>1</v>
-      </c>
-      <c r="D3" s="99" t="s">
+      <c r="C3" s="30">
+        <v>1</v>
+      </c>
+      <c r="D3" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="E3" s="99" t="s">
+      <c r="E3" s="30" t="s">
         <v>391</v>
       </c>
-      <c r="F3" s="99" t="s">
+      <c r="F3" s="30" t="s">
         <v>988</v>
       </c>
-      <c r="G3" s="99" t="s">
+      <c r="G3" s="30" t="s">
         <v>989</v>
       </c>
-      <c r="H3" s="99" t="s">
+      <c r="H3" s="30" t="s">
         <v>990</v>
       </c>
-      <c r="I3" s="165" t="s">
+      <c r="I3" s="170" t="s">
         <v>991</v>
       </c>
-      <c r="J3" s="99" t="s">
+      <c r="J3" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="99" t="s">
+      <c r="K3" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L3" s="99" t="s">
+      <c r="L3" s="30" t="s">
         <v>992</v>
       </c>
-      <c r="M3" s="99">
+      <c r="M3" s="30">
         <v>3378</v>
       </c>
-      <c r="N3" s="99">
+      <c r="N3" s="30">
         <v>38843</v>
       </c>
-      <c r="O3" s="100" t="s">
+      <c r="O3" s="161" t="s">
         <v>993</v>
       </c>
-      <c r="P3" s="165" t="s">
+      <c r="P3" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q3" s="99" t="s">
+      <c r="Q3" s="30" t="s">
         <v>994</v>
       </c>
     </row>
@@ -23371,49 +23535,49 @@
       <c r="B4" s="30" t="s">
         <v>985</v>
       </c>
-      <c r="C4" s="99">
-        <v>1</v>
-      </c>
-      <c r="D4" s="99" t="s">
+      <c r="C4" s="30">
+        <v>1</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>565</v>
       </c>
-      <c r="E4" s="99" t="s">
+      <c r="E4" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="F4" s="99" t="s">
+      <c r="F4" s="30" t="s">
         <v>995</v>
       </c>
-      <c r="G4" s="99" t="s">
+      <c r="G4" s="30" t="s">
         <v>996</v>
       </c>
-      <c r="H4" s="99" t="s">
+      <c r="H4" s="30" t="s">
         <v>997</v>
       </c>
-      <c r="I4" s="165" t="s">
+      <c r="I4" s="170" t="s">
         <v>998</v>
       </c>
-      <c r="J4" s="99" t="s">
+      <c r="J4" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="99" t="s">
+      <c r="K4" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L4" s="99" t="s">
+      <c r="L4" s="30" t="s">
         <v>355</v>
       </c>
-      <c r="M4" s="99">
+      <c r="M4" s="30">
         <v>8383</v>
       </c>
-      <c r="N4" s="99">
+      <c r="N4" s="30">
         <v>37382</v>
       </c>
-      <c r="O4" s="100" t="s">
+      <c r="O4" s="161" t="s">
         <v>999</v>
       </c>
-      <c r="P4" s="165" t="s">
+      <c r="P4" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q4" s="99" t="s">
+      <c r="Q4" s="30" t="s">
         <v>1000</v>
       </c>
     </row>
@@ -23424,49 +23588,49 @@
       <c r="B5" s="30" t="s">
         <v>987</v>
       </c>
-      <c r="C5" s="99">
-        <v>1</v>
-      </c>
-      <c r="D5" s="99" t="s">
+      <c r="C5" s="30">
+        <v>1</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="E5" s="99" t="s">
+      <c r="E5" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="F5" s="99" t="s">
+      <c r="F5" s="30" t="s">
         <v>820</v>
       </c>
-      <c r="G5" s="99" t="s">
+      <c r="G5" s="30" t="s">
         <v>1001</v>
       </c>
-      <c r="H5" s="99" t="s">
+      <c r="H5" s="30" t="s">
         <v>1002</v>
       </c>
-      <c r="I5" s="99">
+      <c r="I5" s="30">
         <v>8358815893</v>
       </c>
-      <c r="J5" s="99" t="s">
+      <c r="J5" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="99" t="s">
+      <c r="K5" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L5" s="99" t="s">
+      <c r="L5" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="M5" s="99">
+      <c r="M5" s="30">
         <v>3820</v>
       </c>
-      <c r="N5" s="99">
+      <c r="N5" s="30">
         <v>435343</v>
       </c>
-      <c r="O5" s="100" t="s">
+      <c r="O5" s="161" t="s">
         <v>1003</v>
       </c>
-      <c r="P5" s="165" t="s">
+      <c r="P5" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q5" s="99" t="s">
+      <c r="Q5" s="30" t="s">
         <v>812</v>
       </c>
     </row>
@@ -23477,49 +23641,49 @@
       <c r="B6" s="240" t="s">
         <v>1034</v>
       </c>
-      <c r="C6" s="99">
-        <v>1</v>
-      </c>
-      <c r="D6" s="99" t="s">
+      <c r="C6" s="30">
+        <v>1</v>
+      </c>
+      <c r="D6" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="E6" s="99" t="s">
+      <c r="E6" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="F6" s="99" t="s">
+      <c r="F6" s="30" t="s">
         <v>1037</v>
       </c>
-      <c r="G6" s="99" t="s">
+      <c r="G6" s="30" t="s">
         <v>1038</v>
       </c>
-      <c r="H6" s="99" t="s">
+      <c r="H6" s="30" t="s">
         <v>627</v>
       </c>
-      <c r="I6" s="165" t="s">
+      <c r="I6" s="170" t="s">
         <v>1039</v>
       </c>
-      <c r="J6" s="99" t="s">
+      <c r="J6" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="99" t="s">
+      <c r="K6" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L6" s="99" t="s">
+      <c r="L6" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="M6" s="99">
+      <c r="M6" s="30">
         <v>8493</v>
       </c>
-      <c r="N6" s="99">
+      <c r="N6" s="30">
         <v>332</v>
       </c>
-      <c r="O6" s="100" t="s">
+      <c r="O6" s="161" t="s">
         <v>1040</v>
       </c>
-      <c r="P6" s="165" t="s">
+      <c r="P6" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q6" s="99" t="s">
+      <c r="Q6" s="30" t="s">
         <v>1041</v>
       </c>
     </row>
@@ -23530,49 +23694,49 @@
       <c r="B7" s="33" t="s">
         <v>1035</v>
       </c>
-      <c r="C7" s="99">
-        <v>1</v>
-      </c>
-      <c r="D7" s="99" t="s">
+      <c r="C7" s="30">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="E7" s="99" t="s">
+      <c r="E7" s="30" t="s">
         <v>391</v>
       </c>
-      <c r="F7" s="99" t="s">
+      <c r="F7" s="30" t="s">
         <v>1042</v>
       </c>
-      <c r="G7" s="99" t="s">
+      <c r="G7" s="30" t="s">
         <v>1043</v>
       </c>
-      <c r="H7" s="99" t="s">
+      <c r="H7" s="30" t="s">
         <v>1044</v>
       </c>
-      <c r="I7" s="165" t="s">
+      <c r="I7" s="170" t="s">
         <v>1039</v>
       </c>
-      <c r="J7" s="99" t="s">
+      <c r="J7" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="99" t="s">
+      <c r="K7" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L7" s="99" t="s">
+      <c r="L7" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="M7" s="99">
+      <c r="M7" s="30">
         <v>8493</v>
       </c>
-      <c r="N7" s="99">
+      <c r="N7" s="30">
         <v>332</v>
       </c>
-      <c r="O7" s="100" t="s">
+      <c r="O7" s="161" t="s">
         <v>1045</v>
       </c>
-      <c r="P7" s="165" t="s">
+      <c r="P7" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q7" s="99" t="s">
+      <c r="Q7" s="30" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -23583,53 +23747,156 @@
       <c r="B8" s="33" t="s">
         <v>1036</v>
       </c>
-      <c r="C8" s="99">
-        <v>1</v>
-      </c>
-      <c r="D8" s="99" t="s">
+      <c r="C8" s="30">
+        <v>1</v>
+      </c>
+      <c r="D8" s="30" t="s">
         <v>388</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="30" t="s">
         <v>389</v>
       </c>
-      <c r="F8" s="99" t="s">
+      <c r="F8" s="30" t="s">
         <v>1047</v>
       </c>
-      <c r="G8" s="99" t="s">
+      <c r="G8" s="30" t="s">
         <v>1048</v>
       </c>
-      <c r="H8" s="99" t="s">
+      <c r="H8" s="30" t="s">
         <v>1049</v>
       </c>
-      <c r="I8" s="165" t="s">
+      <c r="I8" s="170" t="s">
         <v>1039</v>
       </c>
-      <c r="J8" s="99" t="s">
+      <c r="J8" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="K8" s="99" t="s">
+      <c r="K8" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="L8" s="99" t="s">
+      <c r="L8" s="30" t="s">
         <v>822</v>
       </c>
-      <c r="M8" s="99">
+      <c r="M8" s="30">
         <v>8493</v>
       </c>
-      <c r="N8" s="99">
+      <c r="N8" s="30">
         <v>332</v>
       </c>
-      <c r="O8" s="100" t="s">
+      <c r="O8" s="161" t="s">
         <v>1050</v>
       </c>
-      <c r="P8" s="165" t="s">
+      <c r="P8" s="170" t="s">
         <v>811</v>
       </c>
-      <c r="Q8" s="99" t="s">
+      <c r="Q8" s="30" t="s">
         <v>1051</v>
       </c>
     </row>
+    <row r="9" spans="1:17" s="109" customFormat="1">
+      <c r="A9" s="135">
+        <v>105</v>
+      </c>
+      <c r="B9" s="117" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C9" s="109">
+        <v>1</v>
+      </c>
+      <c r="D9" s="109" t="s">
+        <v>565</v>
+      </c>
+      <c r="E9" s="109" t="s">
+        <v>1052</v>
+      </c>
+      <c r="F9" s="163" t="s">
+        <v>1053</v>
+      </c>
+      <c r="G9" s="109" t="s">
+        <v>1054</v>
+      </c>
+      <c r="H9" s="109" t="s">
+        <v>1055</v>
+      </c>
+      <c r="I9" s="248" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="K9" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="L9" s="109" t="s">
+        <v>72</v>
+      </c>
+      <c r="M9" s="109">
+        <v>2000</v>
+      </c>
+      <c r="N9" s="109">
+        <v>434343</v>
+      </c>
+      <c r="O9" s="227" t="s">
+        <v>1056</v>
+      </c>
+      <c r="P9" s="170" t="s">
+        <v>811</v>
+      </c>
+      <c r="Q9" s="109" t="s">
+        <v>1057</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="228">
+        <v>106</v>
+      </c>
+      <c r="B10" s="164" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C10" s="30">
+        <v>1</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>388</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>1058</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>1059</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>1060</v>
+      </c>
+      <c r="I10" s="250" t="s">
+        <v>1061</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="30" t="s">
+        <v>1062</v>
+      </c>
+      <c r="M10" s="170" t="s">
+        <v>1063</v>
+      </c>
+      <c r="O10" s="30" t="s">
+        <v>925</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A9:A10">
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -23639,9 +23906,10 @@
     <hyperlink ref="O6" r:id="rId5"/>
     <hyperlink ref="O7" r:id="rId6"/>
     <hyperlink ref="O8" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8" display="tel:0845397015"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -24407,7 +24675,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B20">
-    <cfRule type="duplicateValues" dxfId="157" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15">
@@ -24440,13 +24708,13 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25376,66 +25644,145 @@
         <v>563</v>
       </c>
     </row>
+    <row r="27" spans="1:11" ht="14.45" customHeight="1">
+      <c r="A27" s="135">
+        <v>105</v>
+      </c>
+      <c r="B27" s="117" t="s">
+        <v>1023</v>
+      </c>
+      <c r="C27" s="110">
+        <v>1</v>
+      </c>
+      <c r="D27" s="101" t="s">
+        <v>776</v>
+      </c>
+      <c r="E27" s="101" t="s">
+        <v>147</v>
+      </c>
+      <c r="F27" s="184" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G27" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="H27" s="101" t="s">
+        <v>395</v>
+      </c>
+      <c r="I27" s="110">
+        <v>1</v>
+      </c>
+      <c r="J27" s="110">
+        <v>6</v>
+      </c>
+      <c r="K27" s="101" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.6" customHeight="1">
+      <c r="A28" s="228">
+        <v>106</v>
+      </c>
+      <c r="B28" s="164" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C28" s="110">
+        <v>1</v>
+      </c>
+      <c r="D28" s="101" t="s">
+        <v>776</v>
+      </c>
+      <c r="E28" s="101" t="s">
+        <v>147</v>
+      </c>
+      <c r="F28" s="184" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G28" s="101" t="s">
+        <v>394</v>
+      </c>
+      <c r="H28" s="101" t="s">
+        <v>395</v>
+      </c>
+      <c r="I28" s="110">
+        <v>1</v>
+      </c>
+      <c r="J28" s="110">
+        <v>6</v>
+      </c>
+      <c r="K28" s="101" t="s">
+        <v>563</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="156" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="155" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="154" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="153" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="152" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="151" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="150" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="149" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="148" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="147" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="146" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="145" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="duplicateValues" dxfId="144" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="143" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="142" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="duplicateValues" dxfId="141" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="140" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:A28">
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G23:G26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G23:G28">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H23:H26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H23:H28">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K23:K26">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K23:K28">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
   </dataValidations>
@@ -25452,7 +25799,7 @@
           <x14:formula1>
             <xm:f>[1]Products_Category!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E22 D27:D1048576</xm:sqref>
+          <xm:sqref>E22 D29:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -25464,7 +25811,7 @@
           <x14:formula1>
             <xm:f>[3]Products_Category!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E18:E21 E23:E26</xm:sqref>
+          <xm:sqref>E18:E21 E23:E28</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26831,37 +27178,37 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="139" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="138" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="137" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="136" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="135" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="134" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="133" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="132" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="131" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="130" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="129" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16">
@@ -28147,22 +28494,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="128" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="127" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="126" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="125" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="124" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="123" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32">
@@ -28287,8 +28634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -28646,7 +28993,7 @@
       <c r="C25" s="101">
         <v>1</v>
       </c>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="126" t="s">
         <v>776</v>
       </c>
     </row>
@@ -28694,55 +29041,56 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="duplicateValues" dxfId="122" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="121" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B13">
-    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="118" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="117" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="duplicateValues" dxfId="116" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="115" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="114" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="113" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="112" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="111" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="110" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="109" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="108" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="107" priority="162"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="162"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
+    <hyperlink ref="D25" location="'URL++'!A1" display="EVS_frontend_QA"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -28962,10 +29310,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="106" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="105" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -29180,10 +29528,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="104" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="103" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29279,10 +29627,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="310" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="322" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="309" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="321" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29440,10 +29788,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="102" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="101" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="69"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -29594,16 +29942,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="100" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="99" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
@@ -29821,10 +30169,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3">
@@ -30216,22 +30564,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="94" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="93" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="92" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="91" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -30328,7 +30676,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30388,10 +30736,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="86" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -30548,10 +30896,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="84" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -30676,10 +31024,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="83" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="82" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -30828,10 +31176,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
@@ -30998,10 +31346,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -31254,10 +31602,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3">
@@ -31349,10 +31697,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -31404,10 +31752,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -32137,22 +32485,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="71" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="70" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="67" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="66" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10">
@@ -32813,22 +33161,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="65" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="64" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="61" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="60" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576">
@@ -33288,10 +33636,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -33858,16 +34206,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="57" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -34159,19 +34507,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="53" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="52" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="51" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
@@ -34232,7 +34580,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="308" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="320" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -35245,16 +35593,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="48" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="47" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="46" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="45" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1"/>
@@ -35430,16 +35778,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="44" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="43" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35872,10 +36220,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID"/>
@@ -36210,16 +36558,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -36530,16 +36878,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="34" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="33" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -36794,28 +37142,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="30" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="29" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="27" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="26" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="25" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -37164,10 +37512,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="307" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="319" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="306" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="318" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
@@ -37891,28 +38239,28 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="22" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1"/>
@@ -38175,31 +38523,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID"/>
@@ -39246,22 +39594,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4">
@@ -40626,15 +40974,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -40783,7 +41122,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -40792,15 +41131,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED871C4-2A4D-4B74-98A2-587321F60978}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -40819,7 +41159,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D73877E0-ACC9-4E95-9DFE-6B4A6282CC78}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -40834,4 +41174,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{525C0858-3CD6-4044-8BEB-39A1DA4B5834}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated Sheet with EVS Bundle Article
</commit_message>
<xml_diff>
--- a/src/test/resources/data/jdgroupMAIN.xlsx
+++ b/src/test/resources/data/jdgroupMAIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E51E4E-0167-47DE-93CE-B5764685A306}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E34EC1-4980-434B-BF3A-7C1F43230FB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="24" activeTab="24" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-3510" yWindow="-10910" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EVS" sheetId="82" r:id="rId1"/>
@@ -261,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6096" uniqueCount="1106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6141" uniqueCount="1107">
   <si>
     <t>testSuitID</t>
   </si>
@@ -3587,6 +3587,9 @@
   </si>
   <si>
     <t>Reorder</t>
+  </si>
+  <si>
+    <t>EVS_Bundle_Article</t>
   </si>
 </sst>
 </file>
@@ -3903,7 +3906,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="288">
+  <cellXfs count="311">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4594,6 +4597,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9512,10 +9570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AC77"/>
+  <dimension ref="A1:AC78"/>
   <sheetViews>
-    <sheetView topLeftCell="D42" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="L63" workbookViewId="0">
+      <selection activeCell="P79" sqref="P79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -12820,6 +12878,52 @@
       </c>
       <c r="J77" s="118"/>
       <c r="K77" s="118"/>
+    </row>
+    <row r="78" spans="1:29">
+      <c r="A78" s="304">
+        <v>118</v>
+      </c>
+      <c r="B78" s="290" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C78" s="308">
+        <v>672</v>
+      </c>
+      <c r="D78" s="290" t="s">
+        <v>1106</v>
+      </c>
+      <c r="E78" s="310" t="s">
+        <v>492</v>
+      </c>
+      <c r="F78" s="305" t="s">
+        <v>9</v>
+      </c>
+      <c r="G78" s="309" t="s">
+        <v>971</v>
+      </c>
+      <c r="H78" s="299" t="s">
+        <v>891</v>
+      </c>
+      <c r="I78" s="298" t="s">
+        <v>843</v>
+      </c>
+      <c r="J78" s="298" t="s">
+        <v>794</v>
+      </c>
+      <c r="K78" s="299" t="s">
+        <v>806</v>
+      </c>
+      <c r="L78" s="299" t="s">
+        <v>815</v>
+      </c>
+      <c r="M78" s="299" t="s">
+        <v>816</v>
+      </c>
+      <c r="N78" s="299" t="s">
+        <v>817</v>
+      </c>
+      <c r="O78" s="289"/>
+      <c r="P78" s="289"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:U76" xr:uid="{55D3BFCF-5BB2-4597-90AF-71155E0BCD4E}"/>
@@ -13205,6 +13309,13 @@
     <hyperlink ref="I52" location="'evs_ProductSearch++'!A1" display="EVS_skuProductValidateOrderQuantity" xr:uid="{19E9B144-C65E-4B65-BBB4-1D02AA20EEBD}"/>
     <hyperlink ref="H77" location="'EVS_Login_magento++'!A1" display="EVS_Login_magento" xr:uid="{D6A95D8A-98CE-4ED5-91BE-9B4AF6C909E9}"/>
     <hyperlink ref="G77" location="'EVS_SapRSIGetDataFromSAPDB++'!A1" display="EVS_SapRSIGetDataFromSAPDB" xr:uid="{703B16CE-82AD-481A-86EE-1E5B5C04EA62}"/>
+    <hyperlink ref="J78" location="'evs_ProductSearch++'!A1" display="evs_ProductSearch" xr:uid="{E0CF3B00-C232-40B1-A8D7-39DBB80F3FC4}"/>
+    <hyperlink ref="H78" location="'evs_Login++'!A1" display="evs_Login" xr:uid="{C2127468-EF2A-4923-B30D-9A55C90819F7}"/>
+    <hyperlink ref="G78" location="'EVS_LaunchPortal++'!A1" display="EVS_LaunchPortal" xr:uid="{12E65B92-4946-4E32-8A70-6D13AD53BFBC}"/>
+    <hyperlink ref="K78" location="'evs_DeliveryPopulation++'!A1" display="evs_DeliveryPopulation" xr:uid="{1D5B856E-DECC-4A39-92D4-168EC4BA621E}"/>
+    <hyperlink ref="L78" location="'evs_CheckoutpaymentOption++'!A1" display="evs_CheckoutpaymentOption" xr:uid="{28C50DD2-F406-4731-9603-17C6A993CD2F}"/>
+    <hyperlink ref="N78" location="'evs_RetriveOrderID++'!A1" display="evs_RetriveOrderID" xr:uid="{68568407-C8E9-45AF-9935-6E6BC8B9656F}"/>
+    <hyperlink ref="M78" location="'evs_PayUPagePayment++'!A1" display="evs_PayUPagePayment" xr:uid="{57825AEC-62B9-4B4A-8772-DCC3CA66D978}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -15471,13 +15582,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A60" sqref="A60"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -16161,7 +16272,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:6">
       <c r="A49" s="60">
         <v>103</v>
       </c>
@@ -16175,7 +16286,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:6">
       <c r="A50" s="139">
         <v>104</v>
       </c>
@@ -16189,7 +16300,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:6">
       <c r="A51" s="135">
         <v>105</v>
       </c>
@@ -16203,7 +16314,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:6">
       <c r="A52" s="225">
         <v>106</v>
       </c>
@@ -16217,7 +16328,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:6">
       <c r="A53" s="232">
         <v>107</v>
       </c>
@@ -16231,7 +16342,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:6">
       <c r="A54" s="232">
         <v>108</v>
       </c>
@@ -16245,7 +16356,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:6">
       <c r="A55" s="232">
         <v>109</v>
       </c>
@@ -16259,7 +16370,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:6">
       <c r="A56" s="30">
         <v>110</v>
       </c>
@@ -16273,7 +16384,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:6">
       <c r="A57" s="30">
         <v>111</v>
       </c>
@@ -16287,7 +16398,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:6">
       <c r="A58" s="30">
         <v>112</v>
       </c>
@@ -16301,7 +16412,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:6">
       <c r="A59" s="30">
         <v>113</v>
       </c>
@@ -16315,7 +16426,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:6">
       <c r="A60" s="148">
         <v>116</v>
       </c>
@@ -16328,6 +16439,22 @@
       <c r="D60" s="84" t="s">
         <v>775</v>
       </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="304">
+        <v>118</v>
+      </c>
+      <c r="B61" s="290" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C61" s="297">
+        <v>1</v>
+      </c>
+      <c r="D61" s="295" t="s">
+        <v>775</v>
+      </c>
+      <c r="E61" s="293"/>
+      <c r="F61" s="293"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
@@ -17836,7 +17963,7 @@
     <cfRule type="duplicateValues" dxfId="289" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="288" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
@@ -18734,49 +18861,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B49:B52 B29:B44 B18:B23 B2:B16">
-    <cfRule type="duplicateValues" dxfId="288" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="287" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="287" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="286" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:B28">
-    <cfRule type="duplicateValues" dxfId="286" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="285" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:B26">
-    <cfRule type="duplicateValues" dxfId="285" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="284" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="duplicateValues" dxfId="284" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="283" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46">
-    <cfRule type="duplicateValues" dxfId="283" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="282" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="duplicateValues" dxfId="282" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="281" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B48">
-    <cfRule type="duplicateValues" dxfId="281" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="280" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="duplicateValues" dxfId="280" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="279" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54">
-    <cfRule type="duplicateValues" dxfId="279" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="278" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B56">
-    <cfRule type="duplicateValues" dxfId="278" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="277" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57">
-    <cfRule type="duplicateValues" dxfId="277" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="276" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57">
-    <cfRule type="duplicateValues" dxfId="276" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="275" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B55">
-    <cfRule type="duplicateValues" dxfId="275" priority="184"/>
+    <cfRule type="duplicateValues" dxfId="274" priority="184"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A56">
-    <cfRule type="duplicateValues" dxfId="274" priority="185"/>
+    <cfRule type="duplicateValues" dxfId="273" priority="185"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1500-000000000000}">
@@ -18988,7 +19115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AA99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -22851,136 +22978,136 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B53:B54">
-    <cfRule type="duplicateValues" dxfId="273" priority="57"/>
+    <cfRule type="duplicateValues" dxfId="272" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32">
-    <cfRule type="duplicateValues" dxfId="272" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="271" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="271" priority="55"/>
+    <cfRule type="duplicateValues" dxfId="270" priority="55"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B52">
-    <cfRule type="duplicateValues" dxfId="270" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="269" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="duplicateValues" dxfId="269" priority="50"/>
+    <cfRule type="duplicateValues" dxfId="268" priority="50"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:A54 A2:A31 A33:A49">
-    <cfRule type="duplicateValues" dxfId="268" priority="61"/>
+    <cfRule type="duplicateValues" dxfId="267" priority="61"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D32">
-    <cfRule type="duplicateValues" dxfId="267" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="266" priority="49"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D30">
-    <cfRule type="duplicateValues" dxfId="266" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="265" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="duplicateValues" dxfId="265" priority="44"/>
+    <cfRule type="duplicateValues" dxfId="264" priority="44"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D74">
-    <cfRule type="duplicateValues" dxfId="264" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="263" priority="43"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B76">
-    <cfRule type="duplicateValues" dxfId="263" priority="42"/>
+    <cfRule type="duplicateValues" dxfId="262" priority="42"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B77">
-    <cfRule type="duplicateValues" dxfId="262" priority="41"/>
+    <cfRule type="duplicateValues" dxfId="261" priority="41"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="duplicateValues" dxfId="261" priority="40"/>
+    <cfRule type="duplicateValues" dxfId="260" priority="40"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B79">
-    <cfRule type="duplicateValues" dxfId="260" priority="39"/>
+    <cfRule type="duplicateValues" dxfId="259" priority="39"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58">
-    <cfRule type="duplicateValues" dxfId="259" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="258" priority="38"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="duplicateValues" dxfId="258" priority="37"/>
+    <cfRule type="duplicateValues" dxfId="257" priority="37"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60">
-    <cfRule type="duplicateValues" dxfId="257" priority="36"/>
+    <cfRule type="duplicateValues" dxfId="256" priority="36"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="duplicateValues" dxfId="256" priority="35"/>
+    <cfRule type="duplicateValues" dxfId="255" priority="35"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="duplicateValues" dxfId="255" priority="34"/>
+    <cfRule type="duplicateValues" dxfId="254" priority="34"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D75">
-    <cfRule type="duplicateValues" dxfId="254" priority="33"/>
+    <cfRule type="duplicateValues" dxfId="253" priority="33"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76">
-    <cfRule type="duplicateValues" dxfId="253" priority="32"/>
+    <cfRule type="duplicateValues" dxfId="252" priority="32"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D77">
-    <cfRule type="duplicateValues" dxfId="252" priority="31"/>
+    <cfRule type="duplicateValues" dxfId="251" priority="31"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D78">
-    <cfRule type="duplicateValues" dxfId="251" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="250" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D79">
-    <cfRule type="duplicateValues" dxfId="250" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="249" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100:B1048576 B81:B84 B33:B49 B1:B31 B55:B75">
-    <cfRule type="duplicateValues" dxfId="249" priority="98"/>
+    <cfRule type="duplicateValues" dxfId="248" priority="98"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D72">
-    <cfRule type="duplicateValues" dxfId="248" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="247" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D73">
-    <cfRule type="duplicateValues" dxfId="247" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="246" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B86">
-    <cfRule type="duplicateValues" dxfId="246" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="245" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="duplicateValues" dxfId="245" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="244" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D87">
-    <cfRule type="duplicateValues" dxfId="244" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="243" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88:B92">
-    <cfRule type="duplicateValues" dxfId="243" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="242" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B93">
-    <cfRule type="duplicateValues" dxfId="242" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="241" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D88:D91">
-    <cfRule type="duplicateValues" dxfId="241" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="240" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D93">
-    <cfRule type="duplicateValues" dxfId="240" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="239" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D92">
-    <cfRule type="duplicateValues" dxfId="239" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="238" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="duplicateValues" dxfId="238" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="237" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="duplicateValues" dxfId="237" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="236" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
-    <cfRule type="duplicateValues" dxfId="236" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="235" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D85">
-    <cfRule type="duplicateValues" dxfId="235" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="234" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G88:I91">
-    <cfRule type="duplicateValues" dxfId="234" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="233" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D98">
-    <cfRule type="duplicateValues" dxfId="233" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="232" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="duplicateValues" dxfId="232" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="231" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G98:I98">
-    <cfRule type="duplicateValues" dxfId="231" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="230" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="229" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="I3" location="'Login_magento++'!A1" display="Login_magento" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
@@ -23491,10 +23618,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="230" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="228" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="229" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="227" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-1B00-000000000000}">
@@ -23939,10 +24066,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="228" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="226" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B18">
-    <cfRule type="duplicateValues" dxfId="227" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="225" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D21" xr:uid="{00000000-0002-0000-1C00-000000000000}">
@@ -24078,10 +24205,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="226" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="224" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="225" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="223" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
@@ -24159,10 +24286,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="224" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="222" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="223" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="221" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" display="automation13@gmail.com" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
@@ -24249,7 +24376,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="222" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="220" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24362,22 +24489,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="221" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="219" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="220" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="218" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="219" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="217" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="218" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="216" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="217" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="215" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="216" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="214" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2100-000000000000}"/>
@@ -24529,25 +24656,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="215" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="213" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="214" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="212" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4 B6">
-    <cfRule type="duplicateValues" dxfId="213" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="211" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="212" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="210" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="211" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="209" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="210" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="208" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="209" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="207" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-2200-000000000000}">
@@ -24742,19 +24869,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="208" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="206" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="207" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="205" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B5">
-    <cfRule type="duplicateValues" dxfId="206" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="204" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="205" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="203" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="204" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="202" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E2:E3" r:id="rId1" display="watlevi41@gmail.com" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
@@ -25103,7 +25230,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="203" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="201" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R8" xr:uid="{00000000-0002-0000-2400-000000000000}">
@@ -25606,7 +25733,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="202" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="200" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
@@ -25708,7 +25835,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="201" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="199" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{97EBD934-1E5E-4BD0-8466-30A3937F3E49}">
@@ -25725,9 +25852,11 @@
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -25738,7 +25867,7 @@
     <col min="5" max="16384" width="9.1796875" style="99"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" s="175" t="s">
         <v>34</v>
       </c>
@@ -25752,7 +25881,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="A2" s="103">
         <v>1</v>
       </c>
@@ -25764,7 +25893,7 @@
       </c>
       <c r="D2" s="103"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:7">
       <c r="A3" s="282">
         <v>91</v>
       </c>
@@ -25776,7 +25905,7 @@
       </c>
       <c r="D3" s="195"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="221">
         <v>96</v>
       </c>
@@ -25787,7 +25916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="221">
         <v>97</v>
       </c>
@@ -25798,7 +25927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7">
       <c r="A6" s="221">
         <v>98</v>
       </c>
@@ -25809,7 +25938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7" s="135">
         <v>105</v>
       </c>
@@ -25821,7 +25950,7 @@
       </c>
       <c r="D7" s="103"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:7">
       <c r="A8" s="225">
         <v>106</v>
       </c>
@@ -25833,7 +25962,7 @@
       </c>
       <c r="D8" s="103"/>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:7">
       <c r="A9" s="232">
         <v>107</v>
       </c>
@@ -25844,7 +25973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:7">
       <c r="A10" s="232">
         <v>108</v>
       </c>
@@ -25855,7 +25984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:7">
       <c r="A11" s="232">
         <v>109</v>
       </c>
@@ -25866,7 +25995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12" s="135">
         <v>111</v>
       </c>
@@ -25877,7 +26006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13" s="135">
         <v>112</v>
       </c>
@@ -25888,24 +26017,39 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="288">
+        <v>118</v>
+      </c>
+      <c r="B14" s="291" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C14" s="292">
+        <v>1</v>
+      </c>
+      <c r="D14" s="289"/>
+      <c r="E14" s="289"/>
+      <c r="F14" s="289"/>
+      <c r="G14" s="289"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="200" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="198" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="199" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="197" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="198" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="196" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="197" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="195" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="196" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="194" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="195" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="193" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2800-000000000000}"/>
@@ -25916,10 +26060,10 @@
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -26287,24 +26431,57 @@
       <c r="L11" s="54"/>
       <c r="M11" s="54"/>
     </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="288">
+        <v>118</v>
+      </c>
+      <c r="B12" s="291" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C12" s="301" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="301" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="301" t="s">
+        <v>80</v>
+      </c>
+      <c r="F12" s="301" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" s="301" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="301" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" s="301" t="s">
+        <v>52</v>
+      </c>
+      <c r="J12" s="301"/>
+      <c r="K12" s="296"/>
+      <c r="L12" s="296"/>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A5:A6">
-    <cfRule type="duplicateValues" dxfId="194" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="192" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="193" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="191" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="192" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="190" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="duplicateValues" dxfId="191" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="189" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="190" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="188" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="189" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="187" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2900-000000000000}"/>
@@ -26315,9 +26492,11 @@
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -26328,7 +26507,7 @@
     <col min="5" max="16384" width="9.1796875" style="99"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="173" t="s">
         <v>34</v>
       </c>
@@ -26342,7 +26521,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="103">
         <v>1</v>
       </c>
@@ -26356,7 +26535,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="282">
         <v>91</v>
       </c>
@@ -26370,7 +26549,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="221">
         <v>96</v>
       </c>
@@ -26384,7 +26563,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="221">
         <v>97</v>
       </c>
@@ -26398,7 +26577,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="221">
         <v>98</v>
       </c>
@@ -26412,7 +26591,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" s="135">
         <v>105</v>
       </c>
@@ -26426,7 +26605,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="225">
         <v>106</v>
       </c>
@@ -26440,7 +26619,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="232">
         <v>107</v>
       </c>
@@ -26454,7 +26633,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="232">
         <v>108</v>
       </c>
@@ -26468,7 +26647,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="232">
         <v>109</v>
       </c>
@@ -26482,7 +26661,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="135">
         <v>111</v>
       </c>
@@ -26496,7 +26675,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="135">
         <v>112</v>
       </c>
@@ -26510,27 +26689,42 @@
         <v>824</v>
       </c>
     </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="288">
+        <v>118</v>
+      </c>
+      <c r="B14" s="291" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C14" s="307">
+        <v>1</v>
+      </c>
+      <c r="D14" s="300" t="s">
+        <v>824</v>
+      </c>
+      <c r="E14" s="289"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="188" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="186" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="187" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="185" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="186" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="184" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="185" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="183" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="184" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="182" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="183" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="181" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D13 D2" xr:uid="{00000000-0002-0000-2A00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D14 D2" xr:uid="{00000000-0002-0000-2A00-000000000000}">
       <formula1>"payUcreditcard"</formula1>
     </dataValidation>
   </dataValidations>
@@ -26798,25 +26992,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="182" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="180" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8">
-    <cfRule type="duplicateValues" dxfId="181" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="179" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="180" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="178" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="179" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="177" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A13">
-    <cfRule type="duplicateValues" dxfId="178" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="176" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="177" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="175" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="176" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="174" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
@@ -26827,9 +27021,11 @@
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -26852,7 +27048,7 @@
     <col min="18" max="16384" width="9.1796875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="236" customFormat="1">
+    <row r="1" spans="1:20" s="236" customFormat="1">
       <c r="A1" s="185" t="s">
         <v>34</v>
       </c>
@@ -26905,7 +27101,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:20">
       <c r="A2" s="30">
         <v>1</v>
       </c>
@@ -26958,7 +27154,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="99" customFormat="1">
+    <row r="3" spans="1:20" s="99" customFormat="1">
       <c r="A3" s="99">
         <v>91</v>
       </c>
@@ -27011,7 +27207,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:20">
       <c r="A4" s="221">
         <v>96</v>
       </c>
@@ -27064,7 +27260,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:20">
       <c r="A5" s="221">
         <v>97</v>
       </c>
@@ -27117,7 +27313,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:20">
       <c r="A6" s="221">
         <v>98</v>
       </c>
@@ -27170,7 +27366,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:20">
       <c r="A7" s="232">
         <v>107</v>
       </c>
@@ -27223,7 +27419,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:20">
       <c r="A8" s="232">
         <v>108</v>
       </c>
@@ -27276,7 +27472,7 @@
         <v>1033</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:20">
       <c r="A9" s="232">
         <v>109</v>
       </c>
@@ -27329,7 +27525,7 @@
         <v>1038</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="109" customFormat="1">
+    <row r="10" spans="1:20" s="109" customFormat="1">
       <c r="A10" s="135">
         <v>105</v>
       </c>
@@ -27382,7 +27578,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:20">
       <c r="A11" s="225">
         <v>106</v>
       </c>
@@ -27423,7 +27619,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:20">
       <c r="A12" s="231">
         <v>111</v>
       </c>
@@ -27476,15 +27672,63 @@
         <v>1068</v>
       </c>
     </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="288">
+        <v>118</v>
+      </c>
+      <c r="B13" s="291" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C13" s="290">
+        <v>1</v>
+      </c>
+      <c r="D13" s="290" t="s">
+        <v>388</v>
+      </c>
+      <c r="E13" s="290" t="s">
+        <v>391</v>
+      </c>
+      <c r="F13" s="290" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G13" s="290" t="s">
+        <v>1046</v>
+      </c>
+      <c r="H13" s="290" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I13" s="306" t="s">
+        <v>1048</v>
+      </c>
+      <c r="J13" s="290" t="s">
+        <v>76</v>
+      </c>
+      <c r="K13" s="290" t="s">
+        <v>1049</v>
+      </c>
+      <c r="L13" s="290"/>
+      <c r="M13" s="302" t="s">
+        <v>1050</v>
+      </c>
+      <c r="N13" s="290"/>
+      <c r="O13" s="290" t="s">
+        <v>920</v>
+      </c>
+      <c r="P13" s="290"/>
+      <c r="Q13" s="290"/>
+      <c r="R13" s="290"/>
+      <c r="S13" s="290"/>
+      <c r="T13" s="290"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="175" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="173" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="174" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="172" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="duplicateValues" dxfId="173" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="171" priority="3"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-2C00-000000000000}"/>
@@ -27498,9 +27742,10 @@
     <hyperlink ref="I11" r:id="rId8" display="tel:0845397015" xr:uid="{00000000-0004-0000-2C00-000008000000}"/>
     <hyperlink ref="O12" r:id="rId9" xr:uid="{00000000-0004-0000-2C00-000009000000}"/>
     <hyperlink ref="O3" r:id="rId10" xr:uid="{76C67CE8-3474-4782-B235-A371A274BE14}"/>
+    <hyperlink ref="I13" r:id="rId11" display="tel:0845397015" xr:uid="{F16719AF-E6F9-4EA1-99A1-F78B8A7CE6EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
@@ -28268,7 +28513,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B20">
-    <cfRule type="duplicateValues" dxfId="172" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="170" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q21:R22 P7 P2:T3 P10:P1048576 T7:T10 Q11:R17 S11:S15" xr:uid="{00000000-0002-0000-2D00-000000000000}">
@@ -28301,13 +28546,13 @@
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
@@ -29447,87 +29692,127 @@
         <v>563</v>
       </c>
     </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="101">
+        <v>118</v>
+      </c>
+      <c r="B33" s="101" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C33" s="294">
+        <v>1</v>
+      </c>
+      <c r="D33" s="297" t="s">
+        <v>775</v>
+      </c>
+      <c r="E33" s="297" t="s">
+        <v>147</v>
+      </c>
+      <c r="F33" s="303" t="s">
+        <v>829</v>
+      </c>
+      <c r="G33" s="297" t="s">
+        <v>394</v>
+      </c>
+      <c r="H33" s="297" t="s">
+        <v>395</v>
+      </c>
+      <c r="I33" s="294">
+        <v>1</v>
+      </c>
+      <c r="J33" s="294">
+        <v>6</v>
+      </c>
+      <c r="K33" s="297" t="s">
+        <v>563</v>
+      </c>
+      <c r="L33" s="297"/>
+      <c r="M33" s="297"/>
+      <c r="N33" s="297"/>
+      <c r="O33" s="297"/>
+      <c r="P33" s="297"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="171" priority="30"/>
+    <cfRule type="duplicateValues" dxfId="169" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="170" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="168" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="169" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="167" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="168" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="166" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="167" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="165" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="duplicateValues" dxfId="166" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="164" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="duplicateValues" dxfId="165" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="163" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="164" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="162" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="163" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="161" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="162" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="160" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="duplicateValues" dxfId="161" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="159" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="duplicateValues" dxfId="160" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="158" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="159" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="157" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23">
-    <cfRule type="duplicateValues" dxfId="158" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="156" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="157" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="155" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:A28">
-    <cfRule type="duplicateValues" dxfId="156" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="154" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="155" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="153" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="154" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="152" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:A31">
-    <cfRule type="duplicateValues" dxfId="153" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="151" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="152" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="150" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="duplicateValues" dxfId="151" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="149" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32">
-    <cfRule type="duplicateValues" dxfId="150" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="148" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="149" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="147" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="148" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="146" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G23:G29" xr:uid="{00000000-0002-0000-2E00-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G21 G23:G29 G33" xr:uid="{00000000-0002-0000-2E00-000000000000}">
       <formula1>"ProductListingPage,ProductDetailPage"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H23:H28" xr:uid="{00000000-0002-0000-2E00-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H10:H15 H18:H21 H23:H28 H33" xr:uid="{00000000-0002-0000-2E00-000001000000}">
       <formula1>"Add_To_Cart,Add_To_Wishlist"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K23:K29" xr:uid="{00000000-0002-0000-2E00-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K10:K15 K18:K21 K23:K29 K33" xr:uid="{00000000-0002-0000-2E00-000002000000}">
       <formula1>"Yes_Wishlist,No_wishlist"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H29" xr:uid="{00000000-0002-0000-2E00-000003000000}">
@@ -29547,7 +29832,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA421\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA403.xlsx]Products_Category'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E22 E30:E31 D33:D1048576</xm:sqref>
+          <xm:sqref>E22 E30:E31 D34:D1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-2E00-000005000000}">
           <x14:formula1>
@@ -29559,7 +29844,7 @@
           <x14:formula1>
             <xm:f>'C:\Users\37601\Documents\JDGroupEVSBranchWorkSpaces\TA599_TA600\JD_IC_TestAutomation\src\test\resources\data\[jdgroupTA464.xlsx]Products_Category'!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E18:E21 E23:E29</xm:sqref>
+          <xm:sqref>E18:E21 E23:E29 E33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -30998,40 +31283,40 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B12:B15">
-    <cfRule type="duplicateValues" dxfId="147" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="145" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="146" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="144" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="duplicateValues" dxfId="145" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="143" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="144" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="142" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B33">
-    <cfRule type="duplicateValues" dxfId="143" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="141" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="duplicateValues" dxfId="142" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="140" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="141" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="139" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="duplicateValues" dxfId="140" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="138" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="duplicateValues" dxfId="139" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="137" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="duplicateValues" dxfId="138" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="136" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="duplicateValues" dxfId="137" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="135" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="134" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H16" xr:uid="{00000000-0002-0000-2F00-000000000000}">
@@ -32436,22 +32721,22 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A27">
-    <cfRule type="duplicateValues" dxfId="136" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="133" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="135" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="132" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:B31">
-    <cfRule type="duplicateValues" dxfId="134" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="131" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:A31">
-    <cfRule type="duplicateValues" dxfId="133" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="130" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B26">
-    <cfRule type="duplicateValues" dxfId="132" priority="65"/>
+    <cfRule type="duplicateValues" dxfId="129" priority="65"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12:A26">
-    <cfRule type="duplicateValues" dxfId="131" priority="66"/>
+    <cfRule type="duplicateValues" dxfId="128" priority="66"/>
   </conditionalFormatting>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M11 M32" xr:uid="{00000000-0002-0000-3000-000000000000}">
@@ -32574,9 +32859,11 @@
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
@@ -32811,7 +33098,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:6">
       <c r="A17" s="210">
         <v>41</v>
       </c>
@@ -32825,7 +33112,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:6">
       <c r="A18" s="210">
         <v>42</v>
       </c>
@@ -32839,7 +33126,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:6">
       <c r="A19" s="210">
         <v>43</v>
       </c>
@@ -32853,7 +33140,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:6">
       <c r="A20" s="221">
         <v>96</v>
       </c>
@@ -32867,7 +33154,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:6">
       <c r="A21" s="221">
         <v>98</v>
       </c>
@@ -32881,7 +33168,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:6">
       <c r="A22" s="135">
         <v>102</v>
       </c>
@@ -32895,7 +33182,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:6">
       <c r="A23" s="60">
         <v>103</v>
       </c>
@@ -32909,7 +33196,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:6">
       <c r="A24" s="124">
         <v>104</v>
       </c>
@@ -32923,7 +33210,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:6">
       <c r="A25" s="225">
         <v>106</v>
       </c>
@@ -32937,7 +33224,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:6">
       <c r="A26" s="232">
         <v>107</v>
       </c>
@@ -32951,7 +33238,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:6">
       <c r="A27" s="232">
         <v>108</v>
       </c>
@@ -32965,7 +33252,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:6">
       <c r="A28" s="232">
         <v>109</v>
       </c>
@@ -32979,7 +33266,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:6">
       <c r="A29" s="135">
         <v>112</v>
       </c>
@@ -32993,60 +33280,76 @@
         <v>775</v>
       </c>
     </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="304">
+        <v>118</v>
+      </c>
+      <c r="B30" s="290" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C30" s="297">
+        <v>1</v>
+      </c>
+      <c r="D30" s="297" t="s">
+        <v>775</v>
+      </c>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B4">
-    <cfRule type="duplicateValues" dxfId="130" priority="23"/>
+    <cfRule type="duplicateValues" dxfId="127" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="duplicateValues" dxfId="129" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="126" priority="22"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="128" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="125" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:B13">
-    <cfRule type="duplicateValues" dxfId="127" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="124" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="126" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="123" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="125" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="122" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B17">
-    <cfRule type="duplicateValues" dxfId="124" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="121" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="123" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="120" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="122" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="119" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="121" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="118" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="120" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="117" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23">
-    <cfRule type="duplicateValues" dxfId="119" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="116" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="118" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="115" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="117" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="114" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="duplicateValues" dxfId="116" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="113" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25">
-    <cfRule type="duplicateValues" dxfId="115" priority="167"/>
+    <cfRule type="duplicateValues" dxfId="112" priority="167"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29">
-    <cfRule type="duplicateValues" dxfId="114" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="duplicateValues" dxfId="113" priority="168"/>
+    <cfRule type="duplicateValues" dxfId="110" priority="168"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-3200-000000000000}"/>
@@ -33290,13 +33593,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="duplicateValues" dxfId="112" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="109" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="111" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="108" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="110" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="107" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-3300-000000000000}"/>
@@ -33535,16 +33838,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B5">
-    <cfRule type="duplicateValues" dxfId="109" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="106" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="108" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="105" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="duplicateValues" dxfId="107" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="104" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7">
-    <cfRule type="duplicateValues" dxfId="106" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="103" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33752,10 +34055,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="105" priority="67"/>
+    <cfRule type="duplicateValues" dxfId="102" priority="67"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="104" priority="69"/>
+    <cfRule type="duplicateValues" dxfId="101" priority="69"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33906,16 +34209,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2 B4">
-    <cfRule type="duplicateValues" dxfId="103" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="100" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2 A4">
-    <cfRule type="duplicateValues" dxfId="102" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="99" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="duplicateValues" dxfId="101" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="98" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="duplicateValues" dxfId="100" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="97" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4" xr:uid="{00000000-0002-0000-3800-000000000000}">
@@ -34133,10 +34436,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="99" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="96" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="98" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="95" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-3900-000000000000}">
@@ -34595,22 +34898,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A21">
-    <cfRule type="duplicateValues" dxfId="97" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="94" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B21">
-    <cfRule type="duplicateValues" dxfId="96" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="93" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="95" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="92" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="94" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="91" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A26">
-    <cfRule type="duplicateValues" dxfId="93" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B26">
-    <cfRule type="duplicateValues" dxfId="92" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3A00-000000000000}">
@@ -34707,7 +35010,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B4">
-    <cfRule type="duplicateValues" dxfId="91" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34767,10 +35070,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="90" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="87" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="89" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="86" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -34927,10 +35230,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="88" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="85" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="87" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="84" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3D00-000000000000}">
@@ -35055,10 +35358,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="86" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="83" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="85" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="82" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-3E00-000000000000}">
@@ -35207,10 +35510,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="84" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="81" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="83" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="80" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-3F00-000000000000}">
@@ -35334,10 +35637,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="82" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="79" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="81" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="78" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4000-000000000000}">
@@ -35590,10 +35893,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A3">
-    <cfRule type="duplicateValues" dxfId="80" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="77" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B3">
-    <cfRule type="duplicateValues" dxfId="79" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="76" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:I3 Q2:Q3" xr:uid="{00000000-0002-0000-4100-000000000000}">
@@ -35685,10 +35988,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="78" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="75" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="77" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="74" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -35740,10 +36043,10 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="76" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="73" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="duplicateValues" dxfId="75" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="72" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -36551,22 +36854,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="74" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="71" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="73" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="70" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="72" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="69" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="71" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="68" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="70" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="67" priority="45"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="69" priority="47"/>
+    <cfRule type="duplicateValues" dxfId="66" priority="47"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y10 Q2:Q10" xr:uid="{00000000-0002-0000-4500-000000000000}">
@@ -37227,22 +37530,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="68" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="65" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="67" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="64" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="66" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="63" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="65" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="62" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8:B21">
-    <cfRule type="duplicateValues" dxfId="64" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="61" priority="28"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A8:A21">
-    <cfRule type="duplicateValues" dxfId="63" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="60" priority="29"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576 F2:F1048576 H2:H1048576 J2:J1048576 L2:L1048576 N2:O1048576" xr:uid="{00000000-0002-0000-4600-000000000000}">
@@ -37702,10 +38005,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="62" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="59" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="61" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4700-000000000000}">
@@ -38274,16 +38577,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="duplicateValues" dxfId="60" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="57" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="59" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="56" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="58" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="55" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="54" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4800-000000000000}"/>
@@ -38577,19 +38880,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="57" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="53" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="56" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="52" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="55" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="51" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="54" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="50" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="5" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="49" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-4900-000000000000}">
@@ -39710,16 +40013,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B10:B12">
-    <cfRule type="duplicateValues" dxfId="53" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="48" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="52" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="47" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B33">
-    <cfRule type="duplicateValues" dxfId="51" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="46" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:A33">
-    <cfRule type="duplicateValues" dxfId="50" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="45" priority="6"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="O2" r:id="rId1" xr:uid="{00000000-0004-0000-4A00-000000000000}"/>
@@ -39897,16 +40200,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B6">
-    <cfRule type="duplicateValues" dxfId="49" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="44" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="duplicateValues" dxfId="48" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="43" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:B12">
-    <cfRule type="duplicateValues" dxfId="47" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="42" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A12">
-    <cfRule type="duplicateValues" dxfId="46" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -40351,10 +40654,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="45" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A13">
-    <cfRule type="duplicateValues" dxfId="44" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="2"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="EVS!A1" display="TCID" xr:uid="{00000000-0004-0000-4D00-000000000000}"/>
@@ -40765,16 +41068,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B11:B13">
-    <cfRule type="duplicateValues" dxfId="43" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="42" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="41" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4E00-000000000000}"/>
@@ -41113,16 +41416,16 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B15">
-    <cfRule type="duplicateValues" dxfId="40" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="39" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="38" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
@@ -41372,28 +41675,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B12">
-    <cfRule type="duplicateValues" dxfId="37" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B13">
-    <cfRule type="duplicateValues" dxfId="36" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="35" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="duplicateValues" dxfId="34" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="33" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="32" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="31" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5000-000000000000}"/>
@@ -42396,28 +42699,28 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B13:B16">
-    <cfRule type="duplicateValues" dxfId="30" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:A12">
-    <cfRule type="duplicateValues" dxfId="29" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11:B12">
-    <cfRule type="duplicateValues" dxfId="28" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="duplicateValues" dxfId="27" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="duplicateValues" dxfId="26" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="duplicateValues" dxfId="25" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="duplicateValues" dxfId="24" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="duplicateValues" dxfId="23" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-5500-000000000000}"/>
@@ -42680,31 +42983,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B9:B12">
-    <cfRule type="duplicateValues" dxfId="22" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9:A12">
-    <cfRule type="duplicateValues" dxfId="21" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="duplicateValues" dxfId="20" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B7">
-    <cfRule type="duplicateValues" dxfId="19" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="duplicateValues" dxfId="18" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B15">
-    <cfRule type="duplicateValues" dxfId="17" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="duplicateValues" dxfId="14" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="A1" location="IC!A1" display="TCID" xr:uid="{00000000-0004-0000-5600-000000000000}"/>
@@ -44001,22 +44304,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A22">
-    <cfRule type="duplicateValues" dxfId="13" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B25">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:A25">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5:B21">
-    <cfRule type="duplicateValues" dxfId="9" priority="54"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="54"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:A21">
-    <cfRule type="duplicateValues" dxfId="8" priority="56"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="56"/>
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J4" xr:uid="{00000000-0002-0000-5E00-000000000000}">
@@ -44387,6 +44690,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009E4315169E4449459811E1A2A421A5D2" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="484de8a0a7035cbf3240ac5ef037eda8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="38ec8e4d-8506-4d8b-b040-96d37469ddf9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="40b4f8b6fbe630a6badbf346a8d0e64c" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -44535,25 +44856,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>